<commit_message>
Chart features list update
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$591</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1154,9 +1154,9 @@
   <dimension ref="A1:J591"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1629,7 +1629,7 @@
         <v>210</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1655,7 +1655,7 @@
         <v>210</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1681,7 +1681,7 @@
         <v>210</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1709,7 +1709,7 @@
         <v>210</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1737,7 +1737,7 @@
         <v>210</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1765,7 +1765,7 @@
         <v>210</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1793,7 +1793,7 @@
         <v>210</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1845,7 +1845,7 @@
         <v>210</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1871,7 +1871,7 @@
         <v>210</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1923,7 +1923,7 @@
         <v>210</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1949,7 +1949,7 @@
         <v>210</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2053,7 +2053,7 @@
         <v>210</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2079,7 +2079,7 @@
         <v>210</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2105,7 +2105,7 @@
         <v>210</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2715,7 +2715,7 @@
         <v>210</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2741,7 +2741,7 @@
         <v>210</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2767,7 +2767,7 @@
         <v>210</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2793,7 +2793,7 @@
         <v>210</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2819,7 +2819,7 @@
         <v>210</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2845,7 +2845,7 @@
         <v>210</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>210</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2897,7 +2897,7 @@
         <v>210</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2923,7 +2923,7 @@
         <v>210</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2949,7 +2949,7 @@
         <v>210</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2975,7 +2975,7 @@
         <v>210</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3001,7 +3001,7 @@
         <v>210</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3027,7 +3027,7 @@
         <v>210</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -3053,7 +3053,7 @@
         <v>210</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -3079,7 +3079,7 @@
         <v>210</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -3105,7 +3105,7 @@
         <v>210</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -3131,7 +3131,7 @@
         <v>210</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3157,7 +3157,7 @@
         <v>210</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3183,7 +3183,7 @@
         <v>210</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3209,7 +3209,7 @@
         <v>210</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3235,7 +3235,7 @@
         <v>210</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3261,7 +3261,7 @@
         <v>210</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3287,7 +3287,7 @@
         <v>210</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3313,7 +3313,7 @@
         <v>210</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3339,7 +3339,7 @@
         <v>210</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3365,7 +3365,7 @@
         <v>210</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3391,7 +3391,7 @@
         <v>210</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3417,7 +3417,7 @@
         <v>210</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3443,7 +3443,7 @@
         <v>210</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3469,7 +3469,7 @@
         <v>210</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3495,7 +3495,7 @@
         <v>210</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3521,7 +3521,7 @@
         <v>210</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3547,7 +3547,7 @@
         <v>210</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3573,7 +3573,7 @@
         <v>210</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3599,7 +3599,7 @@
         <v>210</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3625,7 +3625,7 @@
         <v>210</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -3651,7 +3651,7 @@
         <v>210</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -4442,7 +4442,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1">
+    <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1">
+    <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1">
+    <row r="129" spans="1:10">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="130" spans="1:10" hidden="1">
+    <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="132" spans="1:10" hidden="1">
+    <row r="132" spans="1:10">
       <c r="A132" s="1" t="s">
         <v>0</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1">
+    <row r="133" spans="1:10">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1">
+    <row r="134" spans="1:10">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1">
+    <row r="135" spans="1:10">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="136" spans="1:10" hidden="1">
+    <row r="136" spans="1:10">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1">
+    <row r="137" spans="1:10">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="138" spans="1:10" hidden="1">
+    <row r="138" spans="1:10">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="1:10" hidden="1">
+    <row r="139" spans="1:10">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1">
+    <row r="140" spans="1:10">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="141" spans="1:10" hidden="1">
+    <row r="141" spans="1:10">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="142" spans="1:10" hidden="1">
+    <row r="142" spans="1:10">
       <c r="A142" s="1" t="s">
         <v>0</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="143" spans="1:10" hidden="1">
+    <row r="143" spans="1:10">
       <c r="A143" s="1" t="s">
         <v>0</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="144" spans="1:10" hidden="1">
+    <row r="144" spans="1:10">
       <c r="A144" s="1" t="s">
         <v>0</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1">
+    <row r="145" spans="1:10">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1">
+    <row r="146" spans="1:10">
       <c r="A146" s="1" t="s">
         <v>0</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1">
+    <row r="148" spans="1:10">
       <c r="A148" s="1" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1">
+    <row r="149" spans="1:10">
       <c r="A149" s="1" t="s">
         <v>0</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1">
+    <row r="150" spans="1:10">
       <c r="A150" s="1" t="s">
         <v>0</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1">
+    <row r="151" spans="1:10">
       <c r="A151" s="1" t="s">
         <v>0</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1">
+    <row r="152" spans="1:10">
       <c r="A152" s="1" t="s">
         <v>0</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1">
+    <row r="153" spans="1:10">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1">
+    <row r="154" spans="1:10">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1">
+    <row r="155" spans="1:10">
       <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1">
+    <row r="156" spans="1:10">
       <c r="A156" s="1" t="s">
         <v>0</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1">
+    <row r="158" spans="1:10">
       <c r="A158" s="1" t="s">
         <v>0</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1">
+    <row r="159" spans="1:10">
       <c r="A159" s="1" t="s">
         <v>0</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1">
+    <row r="160" spans="1:10">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1">
+    <row r="161" spans="1:10">
       <c r="A161" s="1" t="s">
         <v>0</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1">
+    <row r="162" spans="1:10">
       <c r="A162" s="1" t="s">
         <v>0</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1">
+    <row r="163" spans="1:10">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1">
+    <row r="164" spans="1:10">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1">
+    <row r="166" spans="1:10">
       <c r="A166" s="1" t="s">
         <v>0</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1">
+    <row r="167" spans="1:10">
       <c r="A167" s="1" t="s">
         <v>0</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1">
+    <row r="168" spans="1:10">
       <c r="A168" s="1" t="s">
         <v>0</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1">
+    <row r="169" spans="1:10">
       <c r="A169" s="1" t="s">
         <v>0</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1">
+    <row r="171" spans="1:10">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1">
+    <row r="172" spans="1:10">
       <c r="A172" s="1" t="s">
         <v>0</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1">
+    <row r="173" spans="1:10">
       <c r="A173" s="1" t="s">
         <v>0</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1">
+    <row r="174" spans="1:10">
       <c r="A174" s="1" t="s">
         <v>0</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1">
+    <row r="175" spans="1:10">
       <c r="A175" s="1" t="s">
         <v>0</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1">
+    <row r="176" spans="1:10">
       <c r="A176" s="1" t="s">
         <v>0</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1">
+    <row r="177" spans="1:10">
       <c r="A177" s="1" t="s">
         <v>0</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1">
+    <row r="178" spans="1:10">
       <c r="A178" s="1" t="s">
         <v>0</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1">
+    <row r="179" spans="1:10">
       <c r="A179" s="1" t="s">
         <v>0</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1">
+    <row r="180" spans="1:10">
       <c r="A180" s="1" t="s">
         <v>0</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1">
+    <row r="181" spans="1:10">
       <c r="A181" s="1" t="s">
         <v>0</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1">
+    <row r="182" spans="1:10">
       <c r="A182" s="1" t="s">
         <v>0</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1">
+    <row r="183" spans="1:10">
       <c r="A183" s="1" t="s">
         <v>0</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1">
+    <row r="184" spans="1:10">
       <c r="A184" s="1" t="s">
         <v>0</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1">
+    <row r="185" spans="1:10">
       <c r="A185" s="1" t="s">
         <v>0</v>
       </c>
@@ -6108,7 +6108,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1">
+    <row r="187" spans="1:10">
       <c r="A187" s="1" t="s">
         <v>0</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1">
+    <row r="188" spans="1:10">
       <c r="A188" s="1" t="s">
         <v>0</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1">
+    <row r="189" spans="1:10">
       <c r="A189" s="1" t="s">
         <v>0</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1">
+    <row r="190" spans="1:10">
       <c r="A190" s="1" t="s">
         <v>0</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1">
+    <row r="191" spans="1:10">
       <c r="A191" s="1" t="s">
         <v>0</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1">
+    <row r="192" spans="1:10">
       <c r="A192" s="1" t="s">
         <v>0</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1">
+    <row r="193" spans="1:10">
       <c r="A193" s="1" t="s">
         <v>0</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1">
+    <row r="194" spans="1:10">
       <c r="A194" s="1" t="s">
         <v>0</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1">
+    <row r="195" spans="1:10">
       <c r="A195" s="1" t="s">
         <v>0</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:10" hidden="1">
+    <row r="211" spans="1:10">
       <c r="A211" s="1" t="s">
         <v>0</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="1:10" hidden="1">
+    <row r="212" spans="1:10">
       <c r="A212" s="1" t="s">
         <v>0</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="213" spans="1:10" hidden="1">
+    <row r="213" spans="1:10">
       <c r="A213" s="1" t="s">
         <v>0</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="214" spans="1:10" hidden="1">
+    <row r="214" spans="1:10">
       <c r="A214" s="1" t="s">
         <v>0</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1">
+    <row r="215" spans="1:10">
       <c r="A215" s="1" t="s">
         <v>0</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="216" spans="1:10" hidden="1">
+    <row r="216" spans="1:10">
       <c r="A216" s="1" t="s">
         <v>0</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1">
+    <row r="217" spans="1:10">
       <c r="A217" s="1" t="s">
         <v>0</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1">
+    <row r="218" spans="1:10">
       <c r="A218" s="1" t="s">
         <v>0</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1">
+    <row r="219" spans="1:10">
       <c r="A219" s="1" t="s">
         <v>0</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1">
+    <row r="221" spans="1:10">
       <c r="A221" s="1" t="s">
         <v>0</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1">
+    <row r="222" spans="1:10">
       <c r="A222" s="1" t="s">
         <v>0</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="223" spans="1:10" hidden="1">
+    <row r="223" spans="1:10">
       <c r="A223" s="1" t="s">
         <v>0</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1">
+    <row r="224" spans="1:10">
       <c r="A224" s="1" t="s">
         <v>0</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1">
+    <row r="226" spans="1:10">
       <c r="A226" s="1" t="s">
         <v>0</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="227" spans="1:10" hidden="1">
+    <row r="227" spans="1:10">
       <c r="A227" s="1" t="s">
         <v>0</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="228" spans="1:10" hidden="1">
+    <row r="228" spans="1:10">
       <c r="A228" s="1" t="s">
         <v>0</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="229" spans="1:10" hidden="1">
+    <row r="229" spans="1:10">
       <c r="A229" s="1" t="s">
         <v>0</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="230" spans="1:10" hidden="1">
+    <row r="230" spans="1:10">
       <c r="A230" s="1" t="s">
         <v>0</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="231" spans="1:10" hidden="1">
+    <row r="231" spans="1:10">
       <c r="A231" s="1" t="s">
         <v>0</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="232" spans="1:10" hidden="1">
+    <row r="232" spans="1:10">
       <c r="A232" s="1" t="s">
         <v>0</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="233" spans="1:10" hidden="1">
+    <row r="233" spans="1:10">
       <c r="A233" s="1" t="s">
         <v>0</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="234" spans="1:10" hidden="1">
+    <row r="234" spans="1:10">
       <c r="A234" s="1" t="s">
         <v>0</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="235" spans="1:10" hidden="1">
+    <row r="235" spans="1:10">
       <c r="A235" s="1" t="s">
         <v>0</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="236" spans="1:10" hidden="1">
+    <row r="236" spans="1:10">
       <c r="A236" s="1" t="s">
         <v>0</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="237" spans="1:10" hidden="1">
+    <row r="237" spans="1:10">
       <c r="A237" s="1" t="s">
         <v>0</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="238" spans="1:10" hidden="1">
+    <row r="238" spans="1:10">
       <c r="A238" s="1" t="s">
         <v>0</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="239" spans="1:10" hidden="1">
+    <row r="239" spans="1:10">
       <c r="A239" s="1" t="s">
         <v>0</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="240" spans="1:10" hidden="1">
+    <row r="240" spans="1:10">
       <c r="A240" s="1" t="s">
         <v>0</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="242" spans="1:10" hidden="1">
+    <row r="242" spans="1:10">
       <c r="A242" s="1" t="s">
         <v>0</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="243" spans="1:10" hidden="1">
+    <row r="243" spans="1:10">
       <c r="A243" s="1" t="s">
         <v>0</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="244" spans="1:10" hidden="1">
+    <row r="244" spans="1:10">
       <c r="A244" s="1" t="s">
         <v>0</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="245" spans="1:10" hidden="1">
+    <row r="245" spans="1:10">
       <c r="A245" s="1" t="s">
         <v>0</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="246" spans="1:10" hidden="1">
+    <row r="246" spans="1:10">
       <c r="A246" s="1" t="s">
         <v>0</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="247" spans="1:10" hidden="1">
+    <row r="247" spans="1:10">
       <c r="A247" s="1" t="s">
         <v>0</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="248" spans="1:10" hidden="1">
+    <row r="248" spans="1:10">
       <c r="A248" s="1" t="s">
         <v>0</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="249" spans="1:10" hidden="1">
+    <row r="249" spans="1:10">
       <c r="A249" s="1" t="s">
         <v>0</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="250" spans="1:10" hidden="1">
+    <row r="250" spans="1:10">
       <c r="A250" s="1" t="s">
         <v>0</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="252" spans="1:10" hidden="1">
+    <row r="252" spans="1:10">
       <c r="A252" s="1" t="s">
         <v>0</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="253" spans="1:10" hidden="1">
+    <row r="253" spans="1:10">
       <c r="A253" s="1" t="s">
         <v>0</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="254" spans="1:10" hidden="1">
+    <row r="254" spans="1:10">
       <c r="A254" s="1" t="s">
         <v>0</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:10" hidden="1">
+    <row r="255" spans="1:10">
       <c r="A255" s="1" t="s">
         <v>0</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="257" spans="1:10" hidden="1">
+    <row r="257" spans="1:10">
       <c r="A257" s="1" t="s">
         <v>0</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="258" spans="1:10" hidden="1">
+    <row r="258" spans="1:10">
       <c r="A258" s="1" t="s">
         <v>0</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="259" spans="1:10" hidden="1">
+    <row r="259" spans="1:10">
       <c r="A259" s="1" t="s">
         <v>0</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="260" spans="1:10" hidden="1">
+    <row r="260" spans="1:10">
       <c r="A260" s="1" t="s">
         <v>0</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="261" spans="1:10" hidden="1">
+    <row r="261" spans="1:10">
       <c r="A261" s="1" t="s">
         <v>0</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="262" spans="1:10" hidden="1">
+    <row r="262" spans="1:10">
       <c r="A262" s="1" t="s">
         <v>0</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="263" spans="1:10" hidden="1">
+    <row r="263" spans="1:10">
       <c r="A263" s="1" t="s">
         <v>0</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="264" spans="1:10" hidden="1">
+    <row r="264" spans="1:10">
       <c r="A264" s="1" t="s">
         <v>0</v>
       </c>
@@ -8296,7 +8296,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="266" spans="1:10" hidden="1">
+    <row r="266" spans="1:10">
       <c r="A266" s="1" t="s">
         <v>0</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="267" spans="1:10" hidden="1">
+    <row r="267" spans="1:10">
       <c r="A267" s="1" t="s">
         <v>0</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="269" spans="1:10" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
         <v>0</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="270" spans="1:10" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
         <v>0</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="271" spans="1:10" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
         <v>0</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="272" spans="1:10" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
         <v>0</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="273" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="273" spans="1:10" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
         <v>0</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="274" spans="1:10" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
         <v>0</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="275" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="275" spans="1:10" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
         <v>0</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="276" spans="1:10" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
         <v>0</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="277" spans="1:10" hidden="1">
+    <row r="277" spans="1:10">
       <c r="A277" s="1" t="s">
         <v>0</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="279" spans="1:10" hidden="1">
+    <row r="279" spans="1:10">
       <c r="A279" s="1" t="s">
         <v>0</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="280" spans="1:10" hidden="1">
+    <row r="280" spans="1:10">
       <c r="A280" s="1" t="s">
         <v>0</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="281" spans="1:10" hidden="1">
+    <row r="281" spans="1:10">
       <c r="A281" s="1" t="s">
         <v>0</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="282" spans="1:10" hidden="1">
+    <row r="282" spans="1:10">
       <c r="A282" s="1" t="s">
         <v>0</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="284" spans="1:10" hidden="1">
+    <row r="284" spans="1:10">
       <c r="A284" s="1" t="s">
         <v>0</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="285" spans="1:10" hidden="1">
+    <row r="285" spans="1:10">
       <c r="A285" s="1" t="s">
         <v>0</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="286" spans="1:10" hidden="1">
+    <row r="286" spans="1:10">
       <c r="A286" s="1" t="s">
         <v>0</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="287" spans="1:10" hidden="1">
+    <row r="287" spans="1:10">
       <c r="A287" s="1" t="s">
         <v>0</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="288" spans="1:10" hidden="1">
+    <row r="288" spans="1:10">
       <c r="A288" s="1" t="s">
         <v>0</v>
       </c>
@@ -8930,7 +8930,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="289" spans="1:10" hidden="1">
+    <row r="289" spans="1:10">
       <c r="A289" s="1" t="s">
         <v>0</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="290" spans="1:10" hidden="1">
+    <row r="290" spans="1:10">
       <c r="A290" s="1" t="s">
         <v>0</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="291" spans="1:10" hidden="1">
+    <row r="291" spans="1:10">
       <c r="A291" s="1" t="s">
         <v>0</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="292" spans="1:10" hidden="1">
+    <row r="292" spans="1:10">
       <c r="A292" s="1" t="s">
         <v>0</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="293" spans="1:10" hidden="1">
+    <row r="293" spans="1:10">
       <c r="A293" s="1" t="s">
         <v>0</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="294" spans="1:10" hidden="1">
+    <row r="294" spans="1:10">
       <c r="A294" s="1" t="s">
         <v>0</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="295" spans="1:10" hidden="1">
+    <row r="295" spans="1:10">
       <c r="A295" s="1" t="s">
         <v>0</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="296" spans="1:10" hidden="1">
+    <row r="296" spans="1:10">
       <c r="A296" s="1" t="s">
         <v>0</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="297" spans="1:10" hidden="1">
+    <row r="297" spans="1:10">
       <c r="A297" s="1" t="s">
         <v>0</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="298" spans="1:10" hidden="1">
+    <row r="298" spans="1:10">
       <c r="A298" s="1" t="s">
         <v>0</v>
       </c>
@@ -9274,7 +9274,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="300" spans="1:10" hidden="1">
+    <row r="300" spans="1:10">
       <c r="A300" s="1" t="s">
         <v>0</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="301" spans="1:10" hidden="1">
+    <row r="301" spans="1:10">
       <c r="A301" s="1" t="s">
         <v>0</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="302" spans="1:10" hidden="1">
+    <row r="302" spans="1:10">
       <c r="A302" s="1" t="s">
         <v>0</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="303" spans="1:10" hidden="1">
+    <row r="303" spans="1:10">
       <c r="A303" s="1" t="s">
         <v>0</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="304" spans="1:10" hidden="1">
+    <row r="304" spans="1:10">
       <c r="A304" s="1" t="s">
         <v>0</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="305" spans="1:10" hidden="1">
+    <row r="305" spans="1:10">
       <c r="A305" s="1" t="s">
         <v>0</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="306" spans="1:10" hidden="1">
+    <row r="306" spans="1:10">
       <c r="A306" s="1" t="s">
         <v>0</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="307" spans="1:10" hidden="1">
+    <row r="307" spans="1:10">
       <c r="A307" s="1" t="s">
         <v>0</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="308" spans="1:10" hidden="1">
+    <row r="308" spans="1:10">
       <c r="A308" s="1" t="s">
         <v>0</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="310" spans="1:10" hidden="1">
+    <row r="310" spans="1:10">
       <c r="A310" s="1" t="s">
         <v>0</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="311" spans="1:10" hidden="1">
+    <row r="311" spans="1:10">
       <c r="A311" s="1" t="s">
         <v>0</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="312" spans="1:10" hidden="1">
+    <row r="312" spans="1:10">
       <c r="A312" s="1" t="s">
         <v>0</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="313" spans="1:10" hidden="1">
+    <row r="313" spans="1:10">
       <c r="A313" s="1" t="s">
         <v>0</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="315" spans="1:10" hidden="1">
+    <row r="315" spans="1:10">
       <c r="A315" s="1" t="s">
         <v>0</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="316" spans="1:10" hidden="1">
+    <row r="316" spans="1:10">
       <c r="A316" s="1" t="s">
         <v>0</v>
       </c>
@@ -9734,7 +9734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="317" spans="1:10" hidden="1">
+    <row r="317" spans="1:10">
       <c r="A317" s="1" t="s">
         <v>0</v>
       </c>
@@ -9760,7 +9760,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="318" spans="1:10" hidden="1">
+    <row r="318" spans="1:10">
       <c r="A318" s="1" t="s">
         <v>0</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="319" spans="1:10" hidden="1">
+    <row r="319" spans="1:10">
       <c r="A319" s="1" t="s">
         <v>0</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="320" spans="1:10" hidden="1">
+    <row r="320" spans="1:10">
       <c r="A320" s="1" t="s">
         <v>0</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="321" spans="1:10" hidden="1">
+    <row r="321" spans="1:10">
       <c r="A321" s="1" t="s">
         <v>0</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="322" spans="1:10" hidden="1">
+    <row r="322" spans="1:10">
       <c r="A322" s="1" t="s">
         <v>0</v>
       </c>
@@ -9918,7 +9918,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="324" spans="1:10" hidden="1">
+    <row r="324" spans="1:10">
       <c r="A324" s="1" t="s">
         <v>0</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="325" spans="1:10" hidden="1">
+    <row r="325" spans="1:10">
       <c r="A325" s="1" t="s">
         <v>0</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="327" spans="1:10" hidden="1">
+    <row r="327" spans="1:10">
       <c r="A327" s="1" t="s">
         <v>0</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="328" spans="1:10" hidden="1">
+    <row r="328" spans="1:10">
       <c r="A328" s="1" t="s">
         <v>0</v>
       </c>
@@ -10052,7 +10052,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="329" spans="1:10" hidden="1">
+    <row r="329" spans="1:10">
       <c r="A329" s="1" t="s">
         <v>0</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="330" spans="1:10" hidden="1">
+    <row r="330" spans="1:10">
       <c r="A330" s="1" t="s">
         <v>0</v>
       </c>
@@ -10108,7 +10108,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="331" spans="1:10" hidden="1">
+    <row r="331" spans="1:10">
       <c r="A331" s="1" t="s">
         <v>0</v>
       </c>
@@ -10136,7 +10136,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="332" spans="1:10" hidden="1">
+    <row r="332" spans="1:10">
       <c r="A332" s="1" t="s">
         <v>0</v>
       </c>
@@ -10164,7 +10164,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="333" spans="1:10" hidden="1">
+    <row r="333" spans="1:10">
       <c r="A333" s="1" t="s">
         <v>0</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="334" spans="1:10" hidden="1">
+    <row r="334" spans="1:10">
       <c r="A334" s="1" t="s">
         <v>0</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="335" spans="1:10" hidden="1">
+    <row r="335" spans="1:10">
       <c r="A335" s="1" t="s">
         <v>0</v>
       </c>
@@ -10274,7 +10274,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="337" spans="1:10" hidden="1">
+    <row r="337" spans="1:10">
       <c r="A337" s="1" t="s">
         <v>0</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="338" spans="1:10" hidden="1">
+    <row r="338" spans="1:10">
       <c r="A338" s="1" t="s">
         <v>0</v>
       </c>
@@ -10326,7 +10326,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="339" spans="1:10" hidden="1">
+    <row r="339" spans="1:10">
       <c r="A339" s="1" t="s">
         <v>0</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="340" spans="1:10" hidden="1">
+    <row r="340" spans="1:10">
       <c r="A340" s="1" t="s">
         <v>0</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="342" spans="1:10" hidden="1">
+    <row r="342" spans="1:10">
       <c r="A342" s="1" t="s">
         <v>0</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="343" spans="1:10" hidden="1">
+    <row r="343" spans="1:10">
       <c r="A343" s="1" t="s">
         <v>0</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="344" spans="1:10" hidden="1">
+    <row r="344" spans="1:10">
       <c r="A344" s="1" t="s">
         <v>0</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="345" spans="1:10" hidden="1">
+    <row r="345" spans="1:10">
       <c r="A345" s="1" t="s">
         <v>0</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="346" spans="1:10" hidden="1">
+    <row r="346" spans="1:10">
       <c r="A346" s="1" t="s">
         <v>0</v>
       </c>
@@ -10552,7 +10552,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="347" spans="1:10" hidden="1">
+    <row r="347" spans="1:10">
       <c r="A347" s="1" t="s">
         <v>0</v>
       </c>
@@ -10584,7 +10584,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="348" spans="1:10" hidden="1">
+    <row r="348" spans="1:10">
       <c r="A348" s="1" t="s">
         <v>0</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="349" spans="1:10" hidden="1">
+    <row r="349" spans="1:10">
       <c r="A349" s="1" t="s">
         <v>0</v>
       </c>
@@ -10648,7 +10648,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="350" spans="1:10" hidden="1">
+    <row r="350" spans="1:10">
       <c r="A350" s="1" t="s">
         <v>0</v>
       </c>
@@ -10678,7 +10678,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="351" spans="1:10" hidden="1">
+    <row r="351" spans="1:10">
       <c r="A351" s="1" t="s">
         <v>0</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="352" spans="1:10" hidden="1">
+    <row r="352" spans="1:10">
       <c r="A352" s="1" t="s">
         <v>0</v>
       </c>
@@ -10742,7 +10742,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="353" spans="1:10" hidden="1">
+    <row r="353" spans="1:10">
       <c r="A353" s="1" t="s">
         <v>0</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="354" spans="1:10" hidden="1">
+    <row r="354" spans="1:10">
       <c r="A354" s="1" t="s">
         <v>0</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="355" spans="1:10" hidden="1">
+    <row r="355" spans="1:10">
       <c r="A355" s="1" t="s">
         <v>0</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="356" spans="1:10" hidden="1">
+    <row r="356" spans="1:10">
       <c r="A356" s="1" t="s">
         <v>0</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="358" spans="1:10" hidden="1">
+    <row r="358" spans="1:10">
       <c r="A358" s="1" t="s">
         <v>0</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="359" spans="1:10" hidden="1">
+    <row r="359" spans="1:10">
       <c r="A359" s="1" t="s">
         <v>0</v>
       </c>
@@ -10950,7 +10950,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="360" spans="1:10" hidden="1">
+    <row r="360" spans="1:10">
       <c r="A360" s="1" t="s">
         <v>0</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="361" spans="1:10" hidden="1">
+    <row r="361" spans="1:10">
       <c r="A361" s="1" t="s">
         <v>0</v>
       </c>
@@ -11006,7 +11006,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="362" spans="1:10" hidden="1">
+    <row r="362" spans="1:10">
       <c r="A362" s="1" t="s">
         <v>0</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="363" spans="1:10" hidden="1">
+    <row r="363" spans="1:10">
       <c r="A363" s="1" t="s">
         <v>0</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="364" spans="1:10" hidden="1">
+    <row r="364" spans="1:10">
       <c r="A364" s="1" t="s">
         <v>0</v>
       </c>
@@ -11090,7 +11090,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="365" spans="1:10" hidden="1">
+    <row r="365" spans="1:10">
       <c r="A365" s="1" t="s">
         <v>0</v>
       </c>
@@ -11118,7 +11118,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="366" spans="1:10" hidden="1">
+    <row r="366" spans="1:10">
       <c r="A366" s="1" t="s">
         <v>0</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="368" spans="1:10" hidden="1">
+    <row r="368" spans="1:10">
       <c r="A368" s="1" t="s">
         <v>0</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="369" spans="1:10" hidden="1">
+    <row r="369" spans="1:10">
       <c r="A369" s="1" t="s">
         <v>0</v>
       </c>
@@ -11224,7 +11224,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="370" spans="1:10" hidden="1">
+    <row r="370" spans="1:10">
       <c r="A370" s="1" t="s">
         <v>0</v>
       </c>
@@ -11250,7 +11250,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="371" spans="1:10" hidden="1">
+    <row r="371" spans="1:10">
       <c r="A371" s="1" t="s">
         <v>0</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="373" spans="1:10" hidden="1">
+    <row r="373" spans="1:10">
       <c r="A373" s="1" t="s">
         <v>0</v>
       </c>
@@ -11328,7 +11328,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="374" spans="1:10" hidden="1">
+    <row r="374" spans="1:10">
       <c r="A374" s="1" t="s">
         <v>0</v>
       </c>
@@ -11356,7 +11356,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="375" spans="1:10" hidden="1">
+    <row r="375" spans="1:10">
       <c r="A375" s="1" t="s">
         <v>0</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="376" spans="1:10" hidden="1">
+    <row r="376" spans="1:10">
       <c r="A376" s="1" t="s">
         <v>0</v>
       </c>
@@ -11410,7 +11410,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="377" spans="1:10" hidden="1">
+    <row r="377" spans="1:10">
       <c r="A377" s="1" t="s">
         <v>0</v>
       </c>
@@ -11436,7 +11436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="378" spans="1:10" hidden="1">
+    <row r="378" spans="1:10">
       <c r="A378" s="1" t="s">
         <v>0</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="379" spans="1:10" hidden="1">
+    <row r="379" spans="1:10">
       <c r="A379" s="1" t="s">
         <v>0</v>
       </c>
@@ -11488,7 +11488,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="380" spans="1:10" hidden="1">
+    <row r="380" spans="1:10">
       <c r="A380" s="1" t="s">
         <v>0</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="382" spans="1:10" hidden="1">
+    <row r="382" spans="1:10">
       <c r="A382" s="1" t="s">
         <v>0</v>
       </c>
@@ -11566,7 +11566,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="383" spans="1:10" hidden="1">
+    <row r="383" spans="1:10">
       <c r="A383" s="1" t="s">
         <v>0</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="385" spans="1:10" hidden="1">
+    <row r="385" spans="1:10">
       <c r="A385" s="1" t="s">
         <v>0</v>
       </c>
@@ -11640,7 +11640,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="386" spans="1:10" hidden="1">
+    <row r="386" spans="1:10">
       <c r="A386" s="1" t="s">
         <v>0</v>
       </c>
@@ -11664,7 +11664,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="387" spans="1:10" hidden="1">
+    <row r="387" spans="1:10">
       <c r="A387" s="1" t="s">
         <v>0</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="388" spans="1:10" hidden="1">
+    <row r="388" spans="1:10">
       <c r="A388" s="1" t="s">
         <v>0</v>
       </c>
@@ -11736,7 +11736,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="390" spans="1:10" hidden="1">
+    <row r="390" spans="1:10">
       <c r="A390" s="1" t="s">
         <v>0</v>
       </c>
@@ -11762,7 +11762,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="391" spans="1:10" hidden="1">
+    <row r="391" spans="1:10">
       <c r="A391" s="1" t="s">
         <v>0</v>
       </c>
@@ -11788,7 +11788,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="392" spans="1:10" hidden="1">
+    <row r="392" spans="1:10">
       <c r="A392" s="1" t="s">
         <v>0</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="393" spans="1:10" hidden="1">
+    <row r="393" spans="1:10">
       <c r="A393" s="1" t="s">
         <v>0</v>
       </c>
@@ -11844,7 +11844,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="394" spans="1:10" hidden="1">
+    <row r="394" spans="1:10">
       <c r="A394" s="1" t="s">
         <v>0</v>
       </c>
@@ -11874,7 +11874,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="395" spans="1:10" hidden="1">
+    <row r="395" spans="1:10">
       <c r="A395" s="1" t="s">
         <v>0</v>
       </c>
@@ -11904,7 +11904,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="396" spans="1:10" hidden="1">
+    <row r="396" spans="1:10">
       <c r="A396" s="1" t="s">
         <v>0</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="397" spans="1:10" hidden="1">
+    <row r="397" spans="1:10">
       <c r="A397" s="1" t="s">
         <v>0</v>
       </c>
@@ -11964,7 +11964,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="398" spans="1:10" hidden="1">
+    <row r="398" spans="1:10">
       <c r="A398" s="1" t="s">
         <v>0</v>
       </c>
@@ -11992,7 +11992,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="399" spans="1:10" hidden="1">
+    <row r="399" spans="1:10">
       <c r="A399" s="1" t="s">
         <v>0</v>
       </c>
@@ -12022,7 +12022,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="400" spans="1:10" hidden="1">
+    <row r="400" spans="1:10">
       <c r="A400" s="1" t="s">
         <v>0</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="401" spans="1:10" hidden="1">
+    <row r="401" spans="1:10">
       <c r="A401" s="1" t="s">
         <v>0</v>
       </c>
@@ -12082,7 +12082,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="402" spans="1:10" hidden="1">
+    <row r="402" spans="1:10">
       <c r="A402" s="1" t="s">
         <v>0</v>
       </c>
@@ -12112,7 +12112,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="403" spans="1:10" hidden="1">
+    <row r="403" spans="1:10">
       <c r="A403" s="1" t="s">
         <v>0</v>
       </c>
@@ -12142,7 +12142,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="404" spans="1:10" hidden="1">
+    <row r="404" spans="1:10">
       <c r="A404" s="1" t="s">
         <v>0</v>
       </c>
@@ -12196,7 +12196,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="406" spans="1:10" hidden="1">
+    <row r="406" spans="1:10">
       <c r="A406" s="1" t="s">
         <v>0</v>
       </c>
@@ -12220,7 +12220,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="407" spans="1:10" hidden="1">
+    <row r="407" spans="1:10">
       <c r="A407" s="1" t="s">
         <v>0</v>
       </c>
@@ -12246,7 +12246,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="408" spans="1:10" hidden="1">
+    <row r="408" spans="1:10">
       <c r="A408" s="1" t="s">
         <v>0</v>
       </c>
@@ -12272,7 +12272,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="409" spans="1:10" hidden="1">
+    <row r="409" spans="1:10">
       <c r="A409" s="1" t="s">
         <v>0</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="410" spans="1:10" hidden="1">
+    <row r="410" spans="1:10">
       <c r="A410" s="1" t="s">
         <v>0</v>
       </c>
@@ -12324,7 +12324,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="411" spans="1:10" hidden="1">
+    <row r="411" spans="1:10">
       <c r="A411" s="1" t="s">
         <v>0</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="412" spans="1:10" hidden="1">
+    <row r="412" spans="1:10">
       <c r="A412" s="1" t="s">
         <v>0</v>
       </c>
@@ -12376,7 +12376,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="413" spans="1:10" hidden="1">
+    <row r="413" spans="1:10">
       <c r="A413" s="1" t="s">
         <v>0</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="414" spans="1:10" hidden="1">
+    <row r="414" spans="1:10">
       <c r="A414" s="1" t="s">
         <v>0</v>
       </c>
@@ -12452,7 +12452,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="416" spans="1:10" hidden="1">
+    <row r="416" spans="1:10">
       <c r="A416" s="1" t="s">
         <v>0</v>
       </c>
@@ -12476,7 +12476,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="417" spans="1:10" hidden="1">
+    <row r="417" spans="1:10">
       <c r="A417" s="1" t="s">
         <v>0</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="418" spans="1:10" hidden="1">
+    <row r="418" spans="1:10">
       <c r="A418" s="1" t="s">
         <v>0</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="419" spans="1:10" hidden="1">
+    <row r="419" spans="1:10">
       <c r="A419" s="1" t="s">
         <v>0</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="421" spans="1:10" hidden="1">
+    <row r="421" spans="1:10">
       <c r="A421" s="1" t="s">
         <v>0</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="422" spans="1:10" hidden="1">
+    <row r="422" spans="1:10">
       <c r="A422" s="1" t="s">
         <v>0</v>
       </c>
@@ -12622,7 +12622,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="423" spans="1:10" hidden="1">
+    <row r="423" spans="1:10">
       <c r="A423" s="1" t="s">
         <v>0</v>
       </c>
@@ -12646,7 +12646,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="424" spans="1:10" hidden="1">
+    <row r="424" spans="1:10">
       <c r="A424" s="1" t="s">
         <v>0</v>
       </c>
@@ -12672,7 +12672,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="425" spans="1:10" hidden="1">
+    <row r="425" spans="1:10">
       <c r="A425" s="1" t="s">
         <v>0</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="426" spans="1:10" hidden="1">
+    <row r="426" spans="1:10">
       <c r="A426" s="1" t="s">
         <v>0</v>
       </c>
@@ -12720,7 +12720,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="427" spans="1:10" hidden="1">
+    <row r="427" spans="1:10">
       <c r="A427" s="1" t="s">
         <v>0</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="428" spans="1:10" hidden="1">
+    <row r="428" spans="1:10">
       <c r="A428" s="1" t="s">
         <v>0</v>
       </c>
@@ -12814,7 +12814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="431" spans="1:10" hidden="1">
+    <row r="431" spans="1:10">
       <c r="A431" s="1" t="s">
         <v>0</v>
       </c>
@@ -12840,7 +12840,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="432" spans="1:10" hidden="1">
+    <row r="432" spans="1:10">
       <c r="A432" s="1" t="s">
         <v>0</v>
       </c>
@@ -12866,7 +12866,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="433" spans="1:10" hidden="1">
+    <row r="433" spans="1:10">
       <c r="A433" s="1" t="s">
         <v>0</v>
       </c>
@@ -12892,7 +12892,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="434" spans="1:10" hidden="1">
+    <row r="434" spans="1:10">
       <c r="A434" s="1" t="s">
         <v>0</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="435" spans="1:10" hidden="1">
+    <row r="435" spans="1:10">
       <c r="A435" s="1" t="s">
         <v>0</v>
       </c>
@@ -12944,7 +12944,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="436" spans="1:10" hidden="1">
+    <row r="436" spans="1:10">
       <c r="A436" s="1" t="s">
         <v>0</v>
       </c>
@@ -12970,7 +12970,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="437" spans="1:10" hidden="1">
+    <row r="437" spans="1:10">
       <c r="A437" s="1" t="s">
         <v>0</v>
       </c>
@@ -13022,7 +13022,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="439" spans="1:10" hidden="1">
+    <row r="439" spans="1:10">
       <c r="A439" s="1" t="s">
         <v>0</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="440" spans="1:10" hidden="1">
+    <row r="440" spans="1:10">
       <c r="A440" s="1" t="s">
         <v>0</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="441" spans="1:10" hidden="1">
+    <row r="441" spans="1:10">
       <c r="A441" s="1" t="s">
         <v>0</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="442" spans="1:10" hidden="1">
+    <row r="442" spans="1:10">
       <c r="A442" s="1" t="s">
         <v>0</v>
       </c>
@@ -13152,7 +13152,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="444" spans="1:10" hidden="1">
+    <row r="444" spans="1:10">
       <c r="A444" s="1" t="s">
         <v>0</v>
       </c>
@@ -13178,7 +13178,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="445" spans="1:10" hidden="1">
+    <row r="445" spans="1:10">
       <c r="A445" s="1" t="s">
         <v>0</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="446" spans="1:10" hidden="1">
+    <row r="446" spans="1:10">
       <c r="A446" s="1" t="s">
         <v>0</v>
       </c>
@@ -13230,7 +13230,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="447" spans="1:10" hidden="1">
+    <row r="447" spans="1:10">
       <c r="A447" s="1" t="s">
         <v>0</v>
       </c>
@@ -13282,7 +13282,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="449" spans="1:10" hidden="1">
+    <row r="449" spans="1:10">
       <c r="A449" s="1" t="s">
         <v>0</v>
       </c>
@@ -13308,7 +13308,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="450" spans="1:10" hidden="1">
+    <row r="450" spans="1:10">
       <c r="A450" s="1" t="s">
         <v>0</v>
       </c>
@@ -13336,7 +13336,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="451" spans="1:10" hidden="1">
+    <row r="451" spans="1:10">
       <c r="A451" s="1" t="s">
         <v>0</v>
       </c>
@@ -13362,7 +13362,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="452" spans="1:10" hidden="1">
+    <row r="452" spans="1:10">
       <c r="A452" s="1" t="s">
         <v>0</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="453" spans="1:10" hidden="1">
+    <row r="453" spans="1:10">
       <c r="A453" s="1" t="s">
         <v>0</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="454" spans="1:10" hidden="1">
+    <row r="454" spans="1:10">
       <c r="A454" s="1" t="s">
         <v>0</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="455" spans="1:10" hidden="1">
+    <row r="455" spans="1:10">
       <c r="A455" s="1" t="s">
         <v>0</v>
       </c>
@@ -13468,7 +13468,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="456" spans="1:10" hidden="1">
+    <row r="456" spans="1:10">
       <c r="A456" s="1" t="s">
         <v>0</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="457" spans="1:10" hidden="1">
+    <row r="457" spans="1:10">
       <c r="A457" s="1" t="s">
         <v>0</v>
       </c>
@@ -13520,7 +13520,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="458" spans="1:10" hidden="1">
+    <row r="458" spans="1:10">
       <c r="A458" s="1" t="s">
         <v>0</v>
       </c>
@@ -13546,7 +13546,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="459" spans="1:10" hidden="1">
+    <row r="459" spans="1:10">
       <c r="A459" s="1" t="s">
         <v>0</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="460" spans="1:10" hidden="1">
+    <row r="460" spans="1:10">
       <c r="A460" s="1" t="s">
         <v>0</v>
       </c>
@@ -13602,7 +13602,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="461" spans="1:10" hidden="1">
+    <row r="461" spans="1:10">
       <c r="A461" s="1" t="s">
         <v>0</v>
       </c>
@@ -13630,7 +13630,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="462" spans="1:10" hidden="1">
+    <row r="462" spans="1:10">
       <c r="A462" s="1" t="s">
         <v>0</v>
       </c>
@@ -13684,7 +13684,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="464" spans="1:10" hidden="1">
+    <row r="464" spans="1:10">
       <c r="A464" s="1" t="s">
         <v>0</v>
       </c>
@@ -13710,7 +13710,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="465" spans="1:10" hidden="1">
+    <row r="465" spans="1:10">
       <c r="A465" s="1" t="s">
         <v>0</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="466" spans="1:10" hidden="1">
+    <row r="466" spans="1:10">
       <c r="A466" s="1" t="s">
         <v>0</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="467" spans="1:10" hidden="1">
+    <row r="467" spans="1:10">
       <c r="A467" s="1" t="s">
         <v>0</v>
       </c>
@@ -13814,7 +13814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="469" spans="1:10" hidden="1">
+    <row r="469" spans="1:10">
       <c r="A469" s="1" t="s">
         <v>0</v>
       </c>
@@ -13840,7 +13840,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="470" spans="1:10" hidden="1">
+    <row r="470" spans="1:10">
       <c r="A470" s="1" t="s">
         <v>0</v>
       </c>
@@ -13866,7 +13866,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="471" spans="1:10" hidden="1">
+    <row r="471" spans="1:10">
       <c r="A471" s="1" t="s">
         <v>0</v>
       </c>
@@ -13892,7 +13892,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="472" spans="1:10" hidden="1">
+    <row r="472" spans="1:10">
       <c r="A472" s="1" t="s">
         <v>0</v>
       </c>
@@ -13944,7 +13944,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="474" spans="1:10" hidden="1">
+    <row r="474" spans="1:10">
       <c r="A474" s="1" t="s">
         <v>0</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="475" spans="1:10" hidden="1">
+    <row r="475" spans="1:10">
       <c r="A475" s="1" t="s">
         <v>0</v>
       </c>
@@ -13998,7 +13998,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="476" spans="1:10" hidden="1">
+    <row r="476" spans="1:10">
       <c r="A476" s="1" t="s">
         <v>0</v>
       </c>
@@ -14024,7 +14024,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="477" spans="1:10" hidden="1">
+    <row r="477" spans="1:10">
       <c r="A477" s="1" t="s">
         <v>0</v>
       </c>
@@ -14052,7 +14052,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="478" spans="1:10" hidden="1">
+    <row r="478" spans="1:10">
       <c r="A478" s="1" t="s">
         <v>0</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="479" spans="1:10" hidden="1">
+    <row r="479" spans="1:10">
       <c r="A479" s="1" t="s">
         <v>0</v>
       </c>
@@ -14104,7 +14104,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="480" spans="1:10" hidden="1">
+    <row r="480" spans="1:10">
       <c r="A480" s="1" t="s">
         <v>0</v>
       </c>
@@ -14130,7 +14130,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="481" spans="1:10" hidden="1">
+    <row r="481" spans="1:10">
       <c r="A481" s="1" t="s">
         <v>0</v>
       </c>
@@ -14830,7 +14830,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="506" spans="1:10" hidden="1">
+    <row r="506" spans="1:10">
       <c r="A506" s="1" t="s">
         <v>0</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="507" spans="1:10" hidden="1">
+    <row r="507" spans="1:10">
       <c r="A507" s="1" t="s">
         <v>0</v>
       </c>
@@ -14882,7 +14882,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="508" spans="1:10" hidden="1">
+    <row r="508" spans="1:10">
       <c r="A508" s="1" t="s">
         <v>0</v>
       </c>
@@ -14910,7 +14910,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="509" spans="1:10" hidden="1">
+    <row r="509" spans="1:10">
       <c r="A509" s="1" t="s">
         <v>0</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="510" spans="1:10" hidden="1">
+    <row r="510" spans="1:10">
       <c r="A510" s="1" t="s">
         <v>0</v>
       </c>
@@ -14966,7 +14966,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="511" spans="1:10" hidden="1">
+    <row r="511" spans="1:10">
       <c r="A511" s="1" t="s">
         <v>0</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="513" spans="1:10" hidden="1">
+    <row r="513" spans="1:10">
       <c r="A513" s="1" t="s">
         <v>0</v>
       </c>
@@ -15046,7 +15046,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="514" spans="1:10" hidden="1">
+    <row r="514" spans="1:10">
       <c r="A514" s="1" t="s">
         <v>0</v>
       </c>
@@ -15072,7 +15072,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="515" spans="1:10" hidden="1">
+    <row r="515" spans="1:10">
       <c r="A515" s="1" t="s">
         <v>0</v>
       </c>
@@ -15098,7 +15098,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="516" spans="1:10" hidden="1">
+    <row r="516" spans="1:10">
       <c r="A516" s="1" t="s">
         <v>0</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="518" spans="1:10" hidden="1">
+    <row r="518" spans="1:10">
       <c r="A518" s="1" t="s">
         <v>0</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="519" spans="1:10" hidden="1">
+    <row r="519" spans="1:10">
       <c r="A519" s="1" t="s">
         <v>0</v>
       </c>
@@ -15202,7 +15202,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="520" spans="1:10" hidden="1">
+    <row r="520" spans="1:10">
       <c r="A520" s="1" t="s">
         <v>0</v>
       </c>
@@ -15228,7 +15228,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="521" spans="1:10" hidden="1">
+    <row r="521" spans="1:10">
       <c r="A521" s="1" t="s">
         <v>0</v>
       </c>
@@ -15280,7 +15280,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="523" spans="1:10" hidden="1">
+    <row r="523" spans="1:10">
       <c r="A523" s="1" t="s">
         <v>0</v>
       </c>
@@ -15306,7 +15306,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="524" spans="1:10" hidden="1">
+    <row r="524" spans="1:10">
       <c r="A524" s="1" t="s">
         <v>0</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="525" spans="1:10" hidden="1">
+    <row r="525" spans="1:10">
       <c r="A525" s="1" t="s">
         <v>0</v>
       </c>
@@ -15360,7 +15360,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="526" spans="1:10" hidden="1">
+    <row r="526" spans="1:10">
       <c r="A526" s="1" t="s">
         <v>0</v>
       </c>
@@ -15388,7 +15388,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="527" spans="1:10" hidden="1">
+    <row r="527" spans="1:10">
       <c r="A527" s="1" t="s">
         <v>0</v>
       </c>
@@ -15414,7 +15414,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="528" spans="1:10" hidden="1">
+    <row r="528" spans="1:10">
       <c r="A528" s="1" t="s">
         <v>0</v>
       </c>
@@ -15440,7 +15440,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="529" spans="1:10" hidden="1">
+    <row r="529" spans="1:10">
       <c r="A529" s="1" t="s">
         <v>0</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="530" spans="1:10" hidden="1">
+    <row r="530" spans="1:10">
       <c r="A530" s="1" t="s">
         <v>0</v>
       </c>
@@ -15518,7 +15518,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="532" spans="1:10" hidden="1">
+    <row r="532" spans="1:10">
       <c r="A532" s="1" t="s">
         <v>0</v>
       </c>
@@ -15544,7 +15544,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="533" spans="1:10" hidden="1">
+    <row r="533" spans="1:10">
       <c r="A533" s="1" t="s">
         <v>0</v>
       </c>
@@ -15570,7 +15570,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="534" spans="1:10" hidden="1">
+    <row r="534" spans="1:10">
       <c r="A534" s="1" t="s">
         <v>0</v>
       </c>
@@ -15598,7 +15598,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="535" spans="1:10" hidden="1">
+    <row r="535" spans="1:10">
       <c r="A535" s="1" t="s">
         <v>0</v>
       </c>
@@ -15626,7 +15626,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="536" spans="1:10" hidden="1">
+    <row r="536" spans="1:10">
       <c r="A536" s="1" t="s">
         <v>0</v>
       </c>
@@ -15654,7 +15654,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="537" spans="1:10" hidden="1">
+    <row r="537" spans="1:10">
       <c r="A537" s="1" t="s">
         <v>0</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="539" spans="1:10" hidden="1">
+    <row r="539" spans="1:10">
       <c r="A539" s="1" t="s">
         <v>0</v>
       </c>
@@ -15734,7 +15734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="540" spans="1:10" hidden="1">
+    <row r="540" spans="1:10">
       <c r="A540" s="1" t="s">
         <v>0</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="541" spans="1:10" hidden="1">
+    <row r="541" spans="1:10">
       <c r="A541" s="1" t="s">
         <v>0</v>
       </c>
@@ -15786,7 +15786,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="542" spans="1:10" hidden="1">
+    <row r="542" spans="1:10">
       <c r="A542" s="1" t="s">
         <v>0</v>
       </c>
@@ -15838,7 +15838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="544" spans="1:10" hidden="1">
+    <row r="544" spans="1:10">
       <c r="A544" s="1" t="s">
         <v>0</v>
       </c>
@@ -15864,7 +15864,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="545" spans="1:10" hidden="1">
+    <row r="545" spans="1:10">
       <c r="A545" s="1" t="s">
         <v>0</v>
       </c>
@@ -15890,7 +15890,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="546" spans="1:10" hidden="1">
+    <row r="546" spans="1:10">
       <c r="A546" s="1" t="s">
         <v>0</v>
       </c>
@@ -15916,7 +15916,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="547" spans="1:10" hidden="1">
+    <row r="547" spans="1:10">
       <c r="A547" s="1" t="s">
         <v>0</v>
       </c>
@@ -15968,7 +15968,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="549" spans="1:10" hidden="1">
+    <row r="549" spans="1:10">
       <c r="A549" s="1" t="s">
         <v>0</v>
       </c>
@@ -15994,7 +15994,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="550" spans="1:10" hidden="1">
+    <row r="550" spans="1:10">
       <c r="A550" s="1" t="s">
         <v>0</v>
       </c>
@@ -16020,7 +16020,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="551" spans="1:10" hidden="1">
+    <row r="551" spans="1:10">
       <c r="A551" s="1" t="s">
         <v>0</v>
       </c>
@@ -16046,7 +16046,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="552" spans="1:10" hidden="1">
+    <row r="552" spans="1:10">
       <c r="A552" s="1" t="s">
         <v>0</v>
       </c>
@@ -16096,7 +16096,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="554" spans="1:10" hidden="1">
+    <row r="554" spans="1:10">
       <c r="A554" s="1" t="s">
         <v>0</v>
       </c>
@@ -16120,7 +16120,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="555" spans="1:10" hidden="1">
+    <row r="555" spans="1:10">
       <c r="A555" s="1" t="s">
         <v>0</v>
       </c>
@@ -16144,7 +16144,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="556" spans="1:10" hidden="1">
+    <row r="556" spans="1:10">
       <c r="A556" s="1" t="s">
         <v>0</v>
       </c>
@@ -16168,7 +16168,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="557" spans="1:10" hidden="1">
+    <row r="557" spans="1:10">
       <c r="A557" s="1" t="s">
         <v>0</v>
       </c>
@@ -16192,7 +16192,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="558" spans="1:10" hidden="1">
+    <row r="558" spans="1:10">
       <c r="A558" s="1" t="s">
         <v>0</v>
       </c>
@@ -16218,7 +16218,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="559" spans="1:10" hidden="1">
+    <row r="559" spans="1:10">
       <c r="A559" s="1" t="s">
         <v>0</v>
       </c>
@@ -16244,7 +16244,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="560" spans="1:10" hidden="1">
+    <row r="560" spans="1:10">
       <c r="A560" s="1" t="s">
         <v>0</v>
       </c>
@@ -16270,7 +16270,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="561" spans="1:10" hidden="1">
+    <row r="561" spans="1:10">
       <c r="A561" s="1" t="s">
         <v>0</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="563" spans="1:10" hidden="1">
+    <row r="563" spans="1:10">
       <c r="A563" s="1" t="s">
         <v>0</v>
       </c>
@@ -16344,7 +16344,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="564" spans="1:10" hidden="1">
+    <row r="564" spans="1:10">
       <c r="A564" s="1" t="s">
         <v>0</v>
       </c>
@@ -16368,7 +16368,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="565" spans="1:10" hidden="1">
+    <row r="565" spans="1:10">
       <c r="A565" s="1" t="s">
         <v>0</v>
       </c>
@@ -16392,7 +16392,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="566" spans="1:10" hidden="1">
+    <row r="566" spans="1:10">
       <c r="A566" s="1" t="s">
         <v>0</v>
       </c>
@@ -16440,7 +16440,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="568" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="568" spans="1:10" ht="15" customHeight="1">
       <c r="A568" s="1" t="s">
         <v>0</v>
       </c>
@@ -16464,7 +16464,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="569" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="569" spans="1:10" ht="15" customHeight="1">
       <c r="A569" s="1" t="s">
         <v>0</v>
       </c>
@@ -16490,7 +16490,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="570" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="570" spans="1:10" ht="15" customHeight="1">
       <c r="A570" s="1" t="s">
         <v>0</v>
       </c>
@@ -16514,7 +16514,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="571" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="571" spans="1:10" ht="15" customHeight="1">
       <c r="A571" s="1" t="s">
         <v>0</v>
       </c>
@@ -16540,7 +16540,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="572" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="572" spans="1:10" ht="15" customHeight="1">
       <c r="A572" s="1" t="s">
         <v>0</v>
       </c>
@@ -16564,7 +16564,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="573" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="573" spans="1:10" ht="15" customHeight="1">
       <c r="A573" s="1" t="s">
         <v>0</v>
       </c>
@@ -16588,7 +16588,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="574" spans="1:10" ht="15" hidden="1" customHeight="1">
+    <row r="574" spans="1:10" ht="15" customHeight="1">
       <c r="A574" s="1" t="s">
         <v>0</v>
       </c>
@@ -16612,7 +16612,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="575" spans="1:10" hidden="1">
+    <row r="575" spans="1:10">
       <c r="A575" s="1" t="s">
         <v>0</v>
       </c>
@@ -17059,7 +17059,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:J1"/>
+  <autoFilter ref="I1:J591"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added: Chart Type -> 2D -> Net (Reverse)
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="212">
   <si>
     <t>Chart</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1156,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J591"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2481,7 +2484,7 @@
         <v>210</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2507,7 +2510,7 @@
         <v>210</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2533,7 +2536,7 @@
         <v>209</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2559,7 +2562,7 @@
         <v>209</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2585,7 +2588,7 @@
         <v>209</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:10">

</xml_diff>

<commit_message>
Added Feature: Chart Area -> Area -> Fill -> Color
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -828,17 +828,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1162,9 +1162,9 @@
   <dimension ref="A1:N530"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M127" sqref="M127:M164"/>
+      <selection pane="bottomLeft" activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1183,16 +1183,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1288,7 +1288,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1313,7 +1313,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1338,7 +1338,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1363,7 +1363,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1388,7 +1388,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1413,7 +1413,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1438,7 +1438,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M10" s="11"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="11"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2356,7 +2356,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="10">
+      <c r="M43" s="11">
         <v>2</v>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="10"/>
+      <c r="M44" s="11"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2420,7 +2420,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="10"/>
+      <c r="M45" s="11"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2452,7 +2452,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="10"/>
+      <c r="M46" s="11"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2484,7 +2484,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="10"/>
+      <c r="M47" s="11"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2516,7 +2516,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="10"/>
+      <c r="M48" s="11"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2548,7 +2548,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="10"/>
+      <c r="M49" s="11"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2580,7 +2580,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="10"/>
+      <c r="M50" s="11"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2769,7 +2769,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="10">
+      <c r="M57" s="11">
         <v>3</v>
       </c>
     </row>
@@ -2798,7 +2798,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="10"/>
+      <c r="M58" s="11"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2825,7 +2825,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="10"/>
+      <c r="M59" s="11"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2852,7 +2852,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="10"/>
+      <c r="M60" s="11"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3950,7 +3950,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="10">
+      <c r="M98" s="11">
         <v>2</v>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="10"/>
+      <c r="M99" s="11"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
@@ -4002,7 +4002,7 @@
       <c r="J100" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M100" s="10"/>
+      <c r="M100" s="11"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4027,7 +4027,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="10"/>
+      <c r="M101" s="11"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4049,12 +4049,12 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M102" s="10"/>
+        <v>210</v>
+      </c>
+      <c r="M102" s="11"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4076,12 +4076,12 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M103" s="10"/>
+        <v>210</v>
+      </c>
+      <c r="M103" s="11"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4110,7 +4110,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="10"/>
+      <c r="M104" s="11"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4139,7 +4139,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="10"/>
+      <c r="M105" s="11"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4170,7 +4170,7 @@
       <c r="J106" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M106" s="10"/>
+      <c r="M106" s="11"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4201,7 +4201,7 @@
       <c r="J107" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M107" s="10"/>
+      <c r="M107" s="11"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4232,7 +4232,7 @@
       <c r="J108" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M108" s="10"/>
+      <c r="M108" s="11"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4263,7 +4263,7 @@
       <c r="J109" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M109" s="10"/>
+      <c r="M109" s="11"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4292,7 +4292,7 @@
       <c r="J110" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M110" s="10"/>
+      <c r="M110" s="11"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4323,7 +4323,7 @@
       <c r="J111" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M111" s="10"/>
+      <c r="M111" s="11"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4354,7 +4354,7 @@
       <c r="J112" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M112" s="10"/>
+      <c r="M112" s="11"/>
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="1" t="s">
@@ -4385,7 +4385,7 @@
       <c r="J113" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M113" s="10"/>
+      <c r="M113" s="11"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4416,7 +4416,7 @@
       <c r="J114" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M114" s="10"/>
+      <c r="M114" s="11"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4447,7 +4447,7 @@
       <c r="J115" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M115" s="10"/>
+      <c r="M115" s="11"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4478,7 +4478,7 @@
       <c r="J116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M116" s="10"/>
+      <c r="M116" s="11"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4503,7 +4503,7 @@
       <c r="J117" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M117" s="10"/>
+      <c r="M117" s="11"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4530,7 +4530,7 @@
       <c r="J118" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M118" s="10"/>
+      <c r="M118" s="11"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4764,7 +4764,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="10">
+      <c r="M127" s="11">
         <v>1</v>
       </c>
     </row>
@@ -4791,7 +4791,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="10"/>
+      <c r="M128" s="11"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4816,7 +4816,7 @@
       <c r="J129" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M129" s="10"/>
+      <c r="M129" s="11"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4841,7 +4841,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="10"/>
+      <c r="M130" s="11"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4866,7 +4866,7 @@
       <c r="J131" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M131" s="10"/>
+      <c r="M131" s="11"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4893,7 +4893,7 @@
       <c r="J132" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M132" s="10"/>
+      <c r="M132" s="11"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4920,7 +4920,7 @@
       <c r="J133" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M133" s="10"/>
+      <c r="M133" s="11"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -4949,7 +4949,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="10"/>
+      <c r="M134" s="11"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -4978,7 +4978,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="10"/>
+      <c r="M135" s="11"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5009,7 +5009,7 @@
       <c r="J136" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M136" s="10"/>
+      <c r="M136" s="11"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5040,7 +5040,7 @@
       <c r="J137" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M137" s="10"/>
+      <c r="M137" s="11"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5071,7 +5071,7 @@
       <c r="J138" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M138" s="10"/>
+      <c r="M138" s="11"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5102,7 +5102,7 @@
       <c r="J139" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M139" s="10"/>
+      <c r="M139" s="11"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5131,7 +5131,7 @@
       <c r="J140" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M140" s="10"/>
+      <c r="M140" s="11"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5162,7 +5162,7 @@
       <c r="J141" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M141" s="10"/>
+      <c r="M141" s="11"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5193,7 +5193,7 @@
       <c r="J142" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M142" s="10"/>
+      <c r="M142" s="11"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5224,7 +5224,7 @@
       <c r="J143" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M143" s="10"/>
+      <c r="M143" s="11"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5255,7 +5255,7 @@
       <c r="J144" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M144" s="10"/>
+      <c r="M144" s="11"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5286,7 +5286,7 @@
       <c r="J145" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M145" s="10"/>
+      <c r="M145" s="11"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5317,7 +5317,7 @@
       <c r="J146" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M146" s="10"/>
+      <c r="M146" s="11"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5342,7 +5342,7 @@
       <c r="J147" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M147" s="10"/>
+      <c r="M147" s="11"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5367,7 +5367,7 @@
       <c r="J148" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M148" s="10"/>
+      <c r="M148" s="11"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5394,7 +5394,7 @@
       <c r="J149" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M149" s="10"/>
+      <c r="M149" s="11"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5421,7 +5421,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="10"/>
+      <c r="M150" s="11"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5448,7 +5448,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="10"/>
+      <c r="M151" s="11"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5475,7 +5475,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="10"/>
+      <c r="M152" s="11"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5502,7 +5502,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="10"/>
+      <c r="M153" s="11"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5529,7 +5529,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="10"/>
+      <c r="M154" s="11"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5556,7 +5556,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="10"/>
+      <c r="M155" s="11"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5583,7 +5583,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="10"/>
+      <c r="M156" s="11"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5608,7 +5608,7 @@
       <c r="J157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M157" s="10"/>
+      <c r="M157" s="11"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5635,7 +5635,7 @@
       <c r="J158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M158" s="10"/>
+      <c r="M158" s="11"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5662,7 +5662,7 @@
       <c r="J159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M159" s="10"/>
+      <c r="M159" s="11"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5689,7 +5689,7 @@
       <c r="J160" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M160" s="10"/>
+      <c r="M160" s="11"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5716,7 +5716,7 @@
       <c r="J161" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M161" s="10"/>
+      <c r="M161" s="11"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5743,7 +5743,7 @@
       <c r="J162" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M162" s="10"/>
+      <c r="M162" s="11"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5770,7 +5770,7 @@
       <c r="J163" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M163" s="10"/>
+      <c r="M163" s="11"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5797,7 +5797,7 @@
       <c r="J164" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M164" s="10"/>
+      <c r="M164" s="11"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5827,7 +5827,7 @@
       <c r="J165" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M165" s="10">
+      <c r="M165" s="11">
         <v>1</v>
       </c>
     </row>
@@ -5856,7 +5856,7 @@
       <c r="J166" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M166" s="10"/>
+      <c r="M166" s="11"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5883,7 +5883,7 @@
       <c r="J167" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M167" s="10"/>
+      <c r="M167" s="11"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5910,7 +5910,7 @@
       <c r="J168" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M168" s="10"/>
+      <c r="M168" s="11"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -5937,7 +5937,7 @@
       <c r="J169" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M169" s="10"/>
+      <c r="M169" s="11"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -5964,7 +5964,7 @@
       <c r="J170" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M170" s="10"/>
+      <c r="M170" s="11"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -5993,7 +5993,7 @@
       <c r="J171" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="10"/>
+      <c r="M171" s="11"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6022,7 +6022,7 @@
       <c r="J172" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M172" s="10"/>
+      <c r="M172" s="11"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6053,7 +6053,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="10"/>
+      <c r="M173" s="11"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6084,7 +6084,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="10"/>
+      <c r="M174" s="11"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6117,7 +6117,7 @@
       <c r="J175" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M175" s="10"/>
+      <c r="M175" s="11"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6150,7 +6150,7 @@
       <c r="J176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M176" s="10"/>
+      <c r="M176" s="11"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6183,7 +6183,7 @@
       <c r="J177" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M177" s="10"/>
+      <c r="M177" s="11"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6216,7 +6216,7 @@
       <c r="J178" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M178" s="10"/>
+      <c r="M178" s="11"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6247,7 +6247,7 @@
       <c r="J179" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M179" s="10"/>
+      <c r="M179" s="11"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6280,7 +6280,7 @@
       <c r="J180" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M180" s="10"/>
+      <c r="M180" s="11"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6313,7 +6313,7 @@
       <c r="J181" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M181" s="10"/>
+      <c r="M181" s="11"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6346,7 +6346,7 @@
       <c r="J182" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M182" s="10"/>
+      <c r="M182" s="11"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6379,7 +6379,7 @@
       <c r="J183" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M183" s="10"/>
+      <c r="M183" s="11"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6412,7 +6412,7 @@
       <c r="J184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M184" s="10"/>
+      <c r="M184" s="11"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6445,7 +6445,7 @@
       <c r="J185" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M185" s="10"/>
+      <c r="M185" s="11"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6472,7 +6472,7 @@
       <c r="J186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M186" s="10"/>
+      <c r="M186" s="11"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6499,7 +6499,7 @@
       <c r="J187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M187" s="10"/>
+      <c r="M187" s="11"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6528,7 +6528,7 @@
       <c r="J188" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M188" s="10"/>
+      <c r="M188" s="11"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6751,7 +6751,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="10">
+      <c r="M196" s="11">
         <v>2</v>
       </c>
     </row>
@@ -6780,7 +6780,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="10"/>
+      <c r="M197" s="11"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6807,7 +6807,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="10"/>
+      <c r="M198" s="11"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6834,7 +6834,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="10"/>
+      <c r="M199" s="11"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6861,7 +6861,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="10"/>
+      <c r="M200" s="11"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6890,7 +6890,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="10"/>
+      <c r="M201" s="11"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6917,7 +6917,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="10"/>
+      <c r="M202" s="11"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -6946,7 +6946,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="10"/>
+      <c r="M203" s="11"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -6973,7 +6973,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="10"/>
+      <c r="M204" s="11"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7000,7 +7000,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="10"/>
+      <c r="M205" s="11"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7027,7 +7027,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="10"/>
+      <c r="M206" s="11"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7054,7 +7054,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="10"/>
+      <c r="M207" s="11"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7081,7 +7081,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="10"/>
+      <c r="M208" s="11"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7108,7 +7108,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="10"/>
+      <c r="M209" s="11"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7138,7 +7138,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="10">
+      <c r="M210" s="11">
         <v>0.5</v>
       </c>
     </row>
@@ -7169,7 +7169,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="10"/>
+      <c r="M211" s="11"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7198,7 +7198,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="10"/>
+      <c r="M212" s="11"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7227,7 +7227,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="10"/>
+      <c r="M213" s="11"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7256,7 +7256,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="10"/>
+      <c r="M214" s="11"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7285,7 +7285,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="10"/>
+      <c r="M215" s="11"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7314,7 +7314,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="10"/>
+      <c r="M216" s="11"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7343,7 +7343,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="10"/>
+      <c r="M217" s="11"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7372,7 +7372,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="10"/>
+      <c r="M218" s="11"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7401,7 +7401,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="10"/>
+      <c r="M219" s="11"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7428,7 +7428,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="10">
+      <c r="M220" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7457,7 +7457,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="10"/>
+      <c r="M221" s="11"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7484,7 +7484,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="10"/>
+      <c r="M222" s="11"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7511,7 +7511,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="10"/>
+      <c r="M223" s="11"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7538,7 +7538,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="10"/>
+      <c r="M224" s="11"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7565,7 +7565,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="10"/>
+      <c r="M225" s="11"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7594,7 +7594,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="10"/>
+      <c r="M226" s="11"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7623,7 +7623,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="10"/>
+      <c r="M227" s="11"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7654,7 +7654,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="10"/>
+      <c r="M228" s="11"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7685,7 +7685,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="10"/>
+      <c r="M229" s="11"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7718,7 +7718,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="10"/>
+      <c r="M230" s="11"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7751,7 +7751,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="10"/>
+      <c r="M231" s="11"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7784,7 +7784,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="10"/>
+      <c r="M232" s="11"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7817,7 +7817,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="10"/>
+      <c r="M233" s="11"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7848,7 +7848,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="10"/>
+      <c r="M234" s="11"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7881,7 +7881,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="10"/>
+      <c r="M235" s="11"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7914,7 +7914,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="10"/>
+      <c r="M236" s="11"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -7947,7 +7947,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="10"/>
+      <c r="M237" s="11"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -7980,7 +7980,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="10"/>
+      <c r="M238" s="11"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8013,7 +8013,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="10"/>
+      <c r="M239" s="11"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8046,7 +8046,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="10"/>
+      <c r="M240" s="11"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8073,7 +8073,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="10"/>
+      <c r="M241" s="11"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8100,7 +8100,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="10"/>
+      <c r="M242" s="11"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8129,7 +8129,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="10"/>
+      <c r="M243" s="11"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8158,7 +8158,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="10"/>
+      <c r="M244" s="11"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8187,7 +8187,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="10"/>
+      <c r="M245" s="11"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8216,7 +8216,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="10"/>
+      <c r="M246" s="11"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8245,7 +8245,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="10"/>
+      <c r="M247" s="11"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8274,7 +8274,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="10"/>
+      <c r="M248" s="11"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8303,7 +8303,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="10"/>
+      <c r="M249" s="11"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8332,7 +8332,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="10"/>
+      <c r="M250" s="11"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8359,7 +8359,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="10"/>
+      <c r="M251" s="11"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8386,7 +8386,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="10"/>
+      <c r="M252" s="11"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8413,7 +8413,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="10"/>
+      <c r="M253" s="11"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8440,7 +8440,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="10"/>
+      <c r="M254" s="11"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8467,7 +8467,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="10"/>
+      <c r="M255" s="11"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8494,7 +8494,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="10"/>
+      <c r="M256" s="11"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8521,7 +8521,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="10"/>
+      <c r="M257" s="11"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8550,7 +8550,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="10"/>
+      <c r="M258" s="11"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8577,7 +8577,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="10"/>
+      <c r="M259" s="11"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8606,7 +8606,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="10"/>
+      <c r="M260" s="11"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8633,7 +8633,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="10"/>
+      <c r="M261" s="11"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8660,7 +8660,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="10"/>
+      <c r="M262" s="11"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8687,7 +8687,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="10"/>
+      <c r="M263" s="11"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8714,7 +8714,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="10"/>
+      <c r="M264" s="11"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8741,7 +8741,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="10"/>
+      <c r="M265" s="11"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8768,7 +8768,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="10"/>
+      <c r="M266" s="11"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8795,7 +8795,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="10"/>
+      <c r="M267" s="11"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8822,7 +8822,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="10"/>
+      <c r="M268" s="11"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8851,7 +8851,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="10"/>
+      <c r="M269" s="11"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8880,7 +8880,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="10"/>
+      <c r="M270" s="11"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8909,7 +8909,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="10"/>
+      <c r="M271" s="11"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -8938,7 +8938,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="10"/>
+      <c r="M272" s="11"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -8967,7 +8967,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="10"/>
+      <c r="M273" s="11"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -8996,7 +8996,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="10"/>
+      <c r="M274" s="11"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9025,7 +9025,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="10"/>
+      <c r="M275" s="11"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9054,7 +9054,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="10"/>
+      <c r="M276" s="11"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9083,7 +9083,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="10"/>
+      <c r="M277" s="11"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9110,7 +9110,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="10"/>
+      <c r="M278" s="11"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9137,7 +9137,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="10"/>
+      <c r="M279" s="11"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9164,7 +9164,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="10"/>
+      <c r="M280" s="11"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9191,7 +9191,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="10"/>
+      <c r="M281" s="11"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9218,7 +9218,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="10"/>
+      <c r="M282" s="11"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9245,7 +9245,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="10"/>
+      <c r="M283" s="11"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9274,7 +9274,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="10"/>
+      <c r="M284" s="11"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9303,7 +9303,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="10"/>
+      <c r="M285" s="11"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9334,7 +9334,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="10"/>
+      <c r="M286" s="11"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9365,7 +9365,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="10"/>
+      <c r="M287" s="11"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9398,7 +9398,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="10"/>
+      <c r="M288" s="11"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9431,7 +9431,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="10"/>
+      <c r="M289" s="11"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9464,7 +9464,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="10"/>
+      <c r="M290" s="11"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9497,7 +9497,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="10"/>
+      <c r="M291" s="11"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9528,7 +9528,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="10"/>
+      <c r="M292" s="11"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9561,7 +9561,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="10"/>
+      <c r="M293" s="11"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9594,7 +9594,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="10"/>
+      <c r="M294" s="11"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9627,7 +9627,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="10"/>
+      <c r="M295" s="11"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9660,7 +9660,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="10"/>
+      <c r="M296" s="11"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9693,7 +9693,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="10"/>
+      <c r="M297" s="11"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9726,7 +9726,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="10"/>
+      <c r="M298" s="11"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9753,7 +9753,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="10"/>
+      <c r="M299" s="11"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9780,7 +9780,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="10"/>
+      <c r="M300" s="11"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9809,7 +9809,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="10"/>
+      <c r="M301" s="11"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9838,7 +9838,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="10"/>
+      <c r="M302" s="11"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9867,7 +9867,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="10"/>
+      <c r="M303" s="11"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9896,7 +9896,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="10"/>
+      <c r="M304" s="11"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -9925,7 +9925,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="10"/>
+      <c r="M305" s="11"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -9954,7 +9954,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="10"/>
+      <c r="M306" s="11"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -9983,7 +9983,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="10"/>
+      <c r="M307" s="11"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10012,7 +10012,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="10"/>
+      <c r="M308" s="11"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10039,7 +10039,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="10"/>
+      <c r="M309" s="11"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10066,7 +10066,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="10"/>
+      <c r="M310" s="11"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10093,7 +10093,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="10"/>
+      <c r="M311" s="11"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10120,7 +10120,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="10"/>
+      <c r="M312" s="11"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10147,7 +10147,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="10"/>
+      <c r="M313" s="11"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10174,7 +10174,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="10"/>
+      <c r="M314" s="11"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10201,7 +10201,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="10"/>
+      <c r="M315" s="11"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10230,7 +10230,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="10"/>
+      <c r="M316" s="11"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10257,7 +10257,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="10"/>
+      <c r="M317" s="11"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10286,7 +10286,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="10"/>
+      <c r="M318" s="11"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10313,7 +10313,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="10"/>
+      <c r="M319" s="11"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10340,7 +10340,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="10"/>
+      <c r="M320" s="11"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10367,7 +10367,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="10"/>
+      <c r="M321" s="11"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10394,7 +10394,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="10"/>
+      <c r="M322" s="11"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10421,7 +10421,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="10"/>
+      <c r="M323" s="11"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10448,7 +10448,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="10"/>
+      <c r="M324" s="11"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10475,7 +10475,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="10"/>
+      <c r="M325" s="11"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10502,7 +10502,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="10"/>
+      <c r="M326" s="11"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10531,7 +10531,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="10"/>
+      <c r="M327" s="11"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10560,7 +10560,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="10"/>
+      <c r="M328" s="11"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10589,7 +10589,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="10"/>
+      <c r="M329" s="11"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10618,7 +10618,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="10"/>
+      <c r="M330" s="11"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10647,7 +10647,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="10"/>
+      <c r="M331" s="11"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10676,7 +10676,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="10"/>
+      <c r="M332" s="11"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10705,7 +10705,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="10"/>
+      <c r="M333" s="11"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10734,7 +10734,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="10"/>
+      <c r="M334" s="11"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10763,7 +10763,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="10"/>
+      <c r="M335" s="11"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -10938,7 +10938,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="10">
+      <c r="M342" s="11">
         <v>1</v>
       </c>
     </row>
@@ -10965,7 +10965,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="10"/>
+      <c r="M343" s="11"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -10990,7 +10990,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="10"/>
+      <c r="M344" s="11"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11015,7 +11015,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="10"/>
+      <c r="M345" s="11"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11040,7 +11040,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="10"/>
+      <c r="M346" s="11"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11065,7 +11065,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="10"/>
+      <c r="M347" s="11"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11092,7 +11092,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="10"/>
+      <c r="M348" s="11"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11119,7 +11119,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="10"/>
+      <c r="M349" s="11"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11148,7 +11148,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="10"/>
+      <c r="M350" s="11"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11177,7 +11177,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="10"/>
+      <c r="M351" s="11"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11208,7 +11208,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="10"/>
+      <c r="M352" s="11"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11239,7 +11239,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="10"/>
+      <c r="M353" s="11"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11270,7 +11270,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="10"/>
+      <c r="M354" s="11"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11301,7 +11301,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="10"/>
+      <c r="M355" s="11"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11330,7 +11330,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="10"/>
+      <c r="M356" s="11"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11361,7 +11361,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="10"/>
+      <c r="M357" s="11"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11392,7 +11392,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="10"/>
+      <c r="M358" s="11"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11423,7 +11423,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="10"/>
+      <c r="M359" s="11"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11454,7 +11454,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="10"/>
+      <c r="M360" s="11"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11485,7 +11485,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="10"/>
+      <c r="M361" s="11"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11516,7 +11516,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="10"/>
+      <c r="M362" s="11"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11541,7 +11541,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="10"/>
+      <c r="M363" s="11"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11566,7 +11566,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="10"/>
+      <c r="M364" s="11"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11593,7 +11593,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="10"/>
+      <c r="M365" s="11"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11620,7 +11620,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="10"/>
+      <c r="M366" s="11"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11647,7 +11647,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="10"/>
+      <c r="M367" s="11"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11674,7 +11674,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="10"/>
+      <c r="M368" s="11"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11701,7 +11701,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="10"/>
+      <c r="M369" s="11"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11728,7 +11728,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="10"/>
+      <c r="M370" s="11"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11755,7 +11755,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="10"/>
+      <c r="M371" s="11"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11782,7 +11782,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="10"/>
+      <c r="M372" s="11"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11807,7 +11807,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="10"/>
+      <c r="M373" s="11"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11832,7 +11832,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="10"/>
+      <c r="M374" s="11"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11857,7 +11857,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="10"/>
+      <c r="M375" s="11"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11882,7 +11882,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="10"/>
+      <c r="M376" s="11"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11907,7 +11907,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="10"/>
+      <c r="M377" s="11"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -11932,7 +11932,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="10"/>
+      <c r="M378" s="11"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -11957,7 +11957,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="10"/>
+      <c r="M379" s="11"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -11984,7 +11984,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="10"/>
+      <c r="M380" s="11"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12009,7 +12009,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="10"/>
+      <c r="M381" s="11"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12036,7 +12036,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="10"/>
+      <c r="M382" s="11"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12061,7 +12061,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="10"/>
+      <c r="M383" s="11"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12086,7 +12086,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="10"/>
+      <c r="M384" s="11"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12111,7 +12111,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="10"/>
+      <c r="M385" s="11"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12136,7 +12136,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="10"/>
+      <c r="M386" s="11"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12209,7 +12209,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="10">
+      <c r="M389" s="11">
         <v>0.5</v>
       </c>
     </row>
@@ -12238,7 +12238,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="10"/>
+      <c r="M390" s="11"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12265,7 +12265,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="10"/>
+      <c r="M391" s="11"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12292,7 +12292,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="10"/>
+      <c r="M392" s="11"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12319,7 +12319,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="10"/>
+      <c r="M393" s="11"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12346,7 +12346,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="10"/>
+      <c r="M394" s="11"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12373,7 +12373,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="10"/>
+      <c r="M395" s="11"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12403,7 +12403,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="10">
+      <c r="M396" s="11">
         <v>1</v>
       </c>
     </row>
@@ -12432,7 +12432,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="10"/>
+      <c r="M397" s="11"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12459,7 +12459,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="10"/>
+      <c r="M398" s="11"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12486,7 +12486,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="10"/>
+      <c r="M399" s="11"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12513,7 +12513,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="10"/>
+      <c r="M400" s="11"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12540,7 +12540,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="10"/>
+      <c r="M401" s="11"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12567,7 +12567,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="10"/>
+      <c r="M402" s="11"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12594,7 +12594,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="10"/>
+      <c r="M403" s="11"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12621,7 +12621,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="10"/>
+      <c r="M404" s="11"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12648,7 +12648,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="10"/>
+      <c r="M405" s="11"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12675,7 +12675,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="10"/>
+      <c r="M406" s="11"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12702,7 +12702,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="10"/>
+      <c r="M407" s="11"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12731,7 +12731,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="10"/>
+      <c r="M408" s="11"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12758,7 +12758,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="10"/>
+      <c r="M409" s="11"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12787,7 +12787,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="10"/>
+      <c r="M410" s="11"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12814,7 +12814,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="10"/>
+      <c r="M411" s="11"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12841,7 +12841,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="10"/>
+      <c r="M412" s="11"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12868,7 +12868,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="10"/>
+      <c r="M413" s="11"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12895,7 +12895,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="10"/>
+      <c r="M414" s="11"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -12925,7 +12925,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="10">
+      <c r="M415" s="11">
         <v>0.5</v>
       </c>
     </row>
@@ -12954,7 +12954,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="10"/>
+      <c r="M416" s="11"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -12983,7 +12983,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="10"/>
+      <c r="M417" s="11"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13012,7 +13012,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="10"/>
+      <c r="M418" s="11"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13041,7 +13041,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="10"/>
+      <c r="M419" s="11"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13070,7 +13070,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="10"/>
+      <c r="M420" s="11"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13100,7 +13100,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="10">
+      <c r="M421" s="11">
         <v>1</v>
       </c>
     </row>
@@ -13129,7 +13129,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="10"/>
+      <c r="M422" s="11"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13156,7 +13156,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="10"/>
+      <c r="M423" s="11"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13183,7 +13183,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="10"/>
+      <c r="M424" s="11"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13210,7 +13210,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="10"/>
+      <c r="M425" s="11"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13237,7 +13237,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="10"/>
+      <c r="M426" s="11"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13264,7 +13264,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="10"/>
+      <c r="M427" s="11"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13291,7 +13291,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="10"/>
+      <c r="M428" s="11"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13318,7 +13318,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="10"/>
+      <c r="M429" s="11"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13345,7 +13345,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="10"/>
+      <c r="M430" s="11"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13372,7 +13372,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="10"/>
+      <c r="M431" s="11"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13399,7 +13399,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="10"/>
+      <c r="M432" s="11"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13428,7 +13428,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="10"/>
+      <c r="M433" s="11"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13455,7 +13455,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="10"/>
+      <c r="M434" s="11"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13484,7 +13484,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="10"/>
+      <c r="M435" s="11"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13511,7 +13511,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="10"/>
+      <c r="M436" s="11"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13538,7 +13538,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="10"/>
+      <c r="M437" s="11"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13565,7 +13565,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="10"/>
+      <c r="M438" s="11"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13592,7 +13592,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="10"/>
+      <c r="M439" s="11"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13626,7 +13626,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="10">
+      <c r="M440" s="11">
         <v>1</v>
       </c>
     </row>
@@ -13659,7 +13659,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="10"/>
+      <c r="M441" s="11"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13690,7 +13690,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="10"/>
+      <c r="M442" s="11"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13721,7 +13721,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="10"/>
+      <c r="M443" s="11"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13752,7 +13752,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="10"/>
+      <c r="M444" s="11"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13783,7 +13783,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="10"/>
+      <c r="M445" s="11"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13814,7 +13814,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="10"/>
+      <c r="M446" s="11"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13845,7 +13845,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="10"/>
+      <c r="M447" s="11"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13876,7 +13876,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="10"/>
+      <c r="M448" s="11"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13907,7 +13907,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="10"/>
+      <c r="M449" s="11"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -13936,7 +13936,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="10"/>
+      <c r="M450" s="11"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -13965,7 +13965,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="10"/>
+      <c r="M451" s="11"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -13994,7 +13994,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="10"/>
+      <c r="M452" s="11"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14023,7 +14023,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="10"/>
+      <c r="M453" s="11"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14052,7 +14052,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="10"/>
+      <c r="M454" s="11"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14079,7 +14079,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="10"/>
+      <c r="M455" s="11"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14106,7 +14106,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="10"/>
+      <c r="M456" s="11"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14133,7 +14133,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="10"/>
+      <c r="M457" s="11"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14162,7 +14162,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="10"/>
+      <c r="M458" s="11"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14191,7 +14191,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="10"/>
+      <c r="M459" s="11"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14220,7 +14220,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="10"/>
+      <c r="M460" s="11"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14249,7 +14249,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="10"/>
+      <c r="M461" s="11"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14583,7 +14583,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="9">
+      <c r="M474" s="12">
         <v>1</v>
       </c>
     </row>
@@ -14612,7 +14612,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="9"/>
+      <c r="M475" s="12"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14639,7 +14639,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="9"/>
+      <c r="M476" s="12"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14666,7 +14666,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="9"/>
+      <c r="M477" s="12"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14693,7 +14693,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="9"/>
+      <c r="M478" s="12"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14720,7 +14720,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="9"/>
+      <c r="M479" s="12"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14747,7 +14747,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="9"/>
+      <c r="M480" s="12"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14774,7 +14774,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="9"/>
+      <c r="M481" s="12"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14801,7 +14801,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="9"/>
+      <c r="M482" s="12"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14828,7 +14828,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="9"/>
+      <c r="M483" s="12"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -14988,7 +14988,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="9">
+      <c r="M489" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15015,7 +15015,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="9"/>
+      <c r="M490" s="12"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15040,7 +15040,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="9"/>
+      <c r="M491" s="12"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15065,7 +15065,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="9"/>
+      <c r="M492" s="12"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15090,7 +15090,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="9"/>
+      <c r="M493" s="12"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15117,7 +15117,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="9"/>
+      <c r="M494" s="12"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15144,7 +15144,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="9"/>
+      <c r="M495" s="12"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15171,7 +15171,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="9"/>
+      <c r="M496" s="12"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15198,7 +15198,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="9"/>
+      <c r="M497" s="12"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15251,7 +15251,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="9">
+      <c r="M499" s="12">
         <v>1</v>
       </c>
     </row>
@@ -15278,7 +15278,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="9"/>
+      <c r="M500" s="12"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15303,7 +15303,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="9"/>
+      <c r="M501" s="12"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15328,7 +15328,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="9"/>
+      <c r="M502" s="12"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15353,7 +15353,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="9"/>
+      <c r="M503" s="12"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15378,7 +15378,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="9"/>
+      <c r="M504" s="12"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15405,7 +15405,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="9"/>
+      <c r="M505" s="12"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15430,7 +15430,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="9"/>
+      <c r="M506" s="12"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15457,7 +15457,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="9"/>
+      <c r="M507" s="12"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15482,7 +15482,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="9"/>
+      <c r="M508" s="12"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15507,7 +15507,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="9"/>
+      <c r="M509" s="12"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15532,7 +15532,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="9"/>
+      <c r="M510" s="12"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15557,7 +15557,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="9"/>
+      <c r="M511" s="12"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15584,7 +15584,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="9"/>
+      <c r="M512" s="12"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15611,7 +15611,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="9"/>
+      <c r="M513" s="12"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15636,7 +15636,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="9"/>
+      <c r="M514" s="12"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15661,7 +15661,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="9"/>
+      <c r="M515" s="12"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15689,7 +15689,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="9">
+      <c r="M516" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15718,7 +15718,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="9"/>
+      <c r="M517" s="12"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15745,7 +15745,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="9"/>
+      <c r="M518" s="12"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15772,7 +15772,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="9"/>
+      <c r="M519" s="12"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15801,7 +15801,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="9"/>
+      <c r="M520" s="12"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15830,7 +15830,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="9"/>
+      <c r="M521" s="12"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15859,7 +15859,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="9"/>
+      <c r="M522" s="12"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15888,7 +15888,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="9"/>
+      <c r="M523" s="12"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15917,7 +15917,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="9"/>
+      <c r="M524" s="12"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -15946,7 +15946,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="9"/>
+      <c r="M525" s="12"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -15973,7 +15973,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="9"/>
+      <c r="M526" s="12"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16000,7 +16000,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="9"/>
+      <c r="M527" s="12"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16025,11 +16025,6 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16046,6 +16041,11 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added: Chart Area -> Area -> Fil -> Bitmap -> Position (reverse)
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3960" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="217">
   <si>
     <t>Chart</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Only bitmap with original size can be properly conversed</t>
   </si>
 </sst>
 </file>
@@ -812,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -828,18 +831,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,10 +1165,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I104" sqref="I104"/>
+      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1183,16 +1187,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1233,7 +1237,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1263,7 +1267,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="11"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1288,7 +1292,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="11"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1313,7 +1317,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1338,7 +1342,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="11"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1363,7 +1367,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="11"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1388,7 +1392,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="11"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1413,7 +1417,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1438,7 +1442,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="11"/>
+      <c r="M10" s="10"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2059,7 +2063,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="11">
+      <c r="M33" s="10">
         <v>1</v>
       </c>
     </row>
@@ -2091,7 +2095,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="11"/>
+      <c r="M34" s="10"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2356,7 +2360,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="11">
+      <c r="M43" s="10">
         <v>2</v>
       </c>
     </row>
@@ -2388,7 +2392,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="11"/>
+      <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2420,7 +2424,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="11"/>
+      <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2452,7 +2456,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="11"/>
+      <c r="M46" s="10"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2484,7 +2488,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="11"/>
+      <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2516,7 +2520,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="11"/>
+      <c r="M48" s="10"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2548,7 +2552,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="11"/>
+      <c r="M49" s="10"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2580,7 +2584,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="11"/>
+      <c r="M50" s="10"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2769,7 +2773,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="11">
+      <c r="M57" s="10">
         <v>3</v>
       </c>
     </row>
@@ -2798,7 +2802,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="11"/>
+      <c r="M58" s="10"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2825,7 +2829,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="11"/>
+      <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2852,7 +2856,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="11"/>
+      <c r="M60" s="10"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3950,7 +3954,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="11">
+      <c r="M98" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3977,7 +3981,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="11"/>
+      <c r="M99" s="10"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
@@ -4002,7 +4006,7 @@
       <c r="J100" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M100" s="11"/>
+      <c r="M100" s="10"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4027,7 +4031,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="11"/>
+      <c r="M101" s="10"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4054,7 +4058,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="11"/>
+      <c r="M102" s="10"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4081,7 +4085,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="11"/>
+      <c r="M103" s="10"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4110,7 +4114,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="11"/>
+      <c r="M104" s="10"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4139,7 +4143,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="11"/>
+      <c r="M105" s="10"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4170,7 +4174,10 @@
       <c r="J106" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M106" s="11"/>
+      <c r="K106" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="M106" s="10"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4196,12 +4203,12 @@
       </c>
       <c r="H107" s="1"/>
       <c r="I107" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J107" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M107" s="11"/>
+        <v>211</v>
+      </c>
+      <c r="M107" s="10"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4227,12 +4234,12 @@
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J108" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M108" s="11"/>
+        <v>211</v>
+      </c>
+      <c r="M108" s="10"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4258,12 +4265,12 @@
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J109" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M109" s="11"/>
+        <v>211</v>
+      </c>
+      <c r="M109" s="10"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4287,12 +4294,12 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
       <c r="I110" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J110" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M110" s="11"/>
+      <c r="M110" s="10"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4323,7 +4330,7 @@
       <c r="J111" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M111" s="11"/>
+      <c r="M111" s="10"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4354,7 +4361,7 @@
       <c r="J112" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M112" s="11"/>
+      <c r="M112" s="10"/>
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="1" t="s">
@@ -4385,7 +4392,7 @@
       <c r="J113" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M113" s="11"/>
+      <c r="M113" s="10"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4416,7 +4423,7 @@
       <c r="J114" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M114" s="11"/>
+      <c r="M114" s="10"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4447,7 +4454,7 @@
       <c r="J115" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M115" s="11"/>
+      <c r="M115" s="10"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4478,7 +4485,7 @@
       <c r="J116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M116" s="11"/>
+      <c r="M116" s="10"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4503,7 +4510,7 @@
       <c r="J117" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M117" s="11"/>
+      <c r="M117" s="10"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4530,7 +4537,7 @@
       <c r="J118" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M118" s="11"/>
+      <c r="M118" s="10"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4764,7 +4771,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="11">
+      <c r="M127" s="10">
         <v>1</v>
       </c>
     </row>
@@ -4791,7 +4798,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="11"/>
+      <c r="M128" s="10"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4816,7 +4823,7 @@
       <c r="J129" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M129" s="11"/>
+      <c r="M129" s="10"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4841,7 +4848,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="11"/>
+      <c r="M130" s="10"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4866,7 +4873,7 @@
       <c r="J131" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M131" s="11"/>
+      <c r="M131" s="10"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4893,7 +4900,7 @@
       <c r="J132" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M132" s="11"/>
+      <c r="M132" s="10"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4920,7 +4927,7 @@
       <c r="J133" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M133" s="11"/>
+      <c r="M133" s="10"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -4949,7 +4956,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="11"/>
+      <c r="M134" s="10"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -4978,7 +4985,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="11"/>
+      <c r="M135" s="10"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5009,7 +5016,7 @@
       <c r="J136" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M136" s="11"/>
+      <c r="M136" s="10"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5040,7 +5047,7 @@
       <c r="J137" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M137" s="11"/>
+      <c r="M137" s="10"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5071,7 +5078,7 @@
       <c r="J138" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M138" s="11"/>
+      <c r="M138" s="10"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5102,7 +5109,7 @@
       <c r="J139" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M139" s="11"/>
+      <c r="M139" s="10"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5131,7 +5138,7 @@
       <c r="J140" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M140" s="11"/>
+      <c r="M140" s="10"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5162,7 +5169,7 @@
       <c r="J141" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M141" s="11"/>
+      <c r="M141" s="10"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5193,7 +5200,7 @@
       <c r="J142" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M142" s="11"/>
+      <c r="M142" s="10"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5224,7 +5231,7 @@
       <c r="J143" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M143" s="11"/>
+      <c r="M143" s="10"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5255,7 +5262,7 @@
       <c r="J144" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M144" s="11"/>
+      <c r="M144" s="10"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5286,7 +5293,7 @@
       <c r="J145" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M145" s="11"/>
+      <c r="M145" s="10"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5317,7 +5324,7 @@
       <c r="J146" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M146" s="11"/>
+      <c r="M146" s="10"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5342,7 +5349,7 @@
       <c r="J147" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M147" s="11"/>
+      <c r="M147" s="10"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5367,7 +5374,7 @@
       <c r="J148" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M148" s="11"/>
+      <c r="M148" s="10"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5394,7 +5401,7 @@
       <c r="J149" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M149" s="11"/>
+      <c r="M149" s="10"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5421,7 +5428,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="11"/>
+      <c r="M150" s="10"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5448,7 +5455,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="11"/>
+      <c r="M151" s="10"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5475,7 +5482,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="11"/>
+      <c r="M152" s="10"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5502,7 +5509,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="11"/>
+      <c r="M153" s="10"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5529,7 +5536,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="11"/>
+      <c r="M154" s="10"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5556,7 +5563,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="11"/>
+      <c r="M155" s="10"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5583,7 +5590,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="11"/>
+      <c r="M156" s="10"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5608,7 +5615,7 @@
       <c r="J157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M157" s="11"/>
+      <c r="M157" s="10"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5635,7 +5642,7 @@
       <c r="J158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M158" s="11"/>
+      <c r="M158" s="10"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5662,7 +5669,7 @@
       <c r="J159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M159" s="11"/>
+      <c r="M159" s="10"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5689,7 +5696,7 @@
       <c r="J160" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M160" s="11"/>
+      <c r="M160" s="10"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5716,7 +5723,7 @@
       <c r="J161" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M161" s="11"/>
+      <c r="M161" s="10"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5743,7 +5750,7 @@
       <c r="J162" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M162" s="11"/>
+      <c r="M162" s="10"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5770,7 +5777,7 @@
       <c r="J163" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M163" s="11"/>
+      <c r="M163" s="10"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5797,7 +5804,7 @@
       <c r="J164" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M164" s="11"/>
+      <c r="M164" s="10"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5827,7 +5834,7 @@
       <c r="J165" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M165" s="11">
+      <c r="M165" s="10">
         <v>1</v>
       </c>
     </row>
@@ -5856,7 +5863,7 @@
       <c r="J166" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M166" s="11"/>
+      <c r="M166" s="10"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5883,7 +5890,7 @@
       <c r="J167" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M167" s="11"/>
+      <c r="M167" s="10"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5910,7 +5917,7 @@
       <c r="J168" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M168" s="11"/>
+      <c r="M168" s="10"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -5937,7 +5944,7 @@
       <c r="J169" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M169" s="11"/>
+      <c r="M169" s="10"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -5964,7 +5971,7 @@
       <c r="J170" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M170" s="11"/>
+      <c r="M170" s="10"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -5993,7 +6000,7 @@
       <c r="J171" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="11"/>
+      <c r="M171" s="10"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6022,7 +6029,7 @@
       <c r="J172" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M172" s="11"/>
+      <c r="M172" s="10"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6053,7 +6060,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="11"/>
+      <c r="M173" s="10"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6084,7 +6091,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="11"/>
+      <c r="M174" s="10"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6117,7 +6124,7 @@
       <c r="J175" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M175" s="11"/>
+      <c r="M175" s="10"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6150,7 +6157,7 @@
       <c r="J176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M176" s="11"/>
+      <c r="M176" s="10"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6183,7 +6190,7 @@
       <c r="J177" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M177" s="11"/>
+      <c r="M177" s="10"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6216,7 +6223,7 @@
       <c r="J178" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M178" s="11"/>
+      <c r="M178" s="10"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6247,7 +6254,7 @@
       <c r="J179" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M179" s="11"/>
+      <c r="M179" s="10"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6280,7 +6287,7 @@
       <c r="J180" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M180" s="11"/>
+      <c r="M180" s="10"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6313,7 +6320,7 @@
       <c r="J181" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M181" s="11"/>
+      <c r="M181" s="10"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6346,7 +6353,7 @@
       <c r="J182" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M182" s="11"/>
+      <c r="M182" s="10"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6379,7 +6386,7 @@
       <c r="J183" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M183" s="11"/>
+      <c r="M183" s="10"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6412,7 +6419,7 @@
       <c r="J184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M184" s="11"/>
+      <c r="M184" s="10"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6445,7 +6452,7 @@
       <c r="J185" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M185" s="11"/>
+      <c r="M185" s="10"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6472,7 +6479,7 @@
       <c r="J186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M186" s="11"/>
+      <c r="M186" s="10"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6499,7 +6506,7 @@
       <c r="J187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M187" s="11"/>
+      <c r="M187" s="10"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6528,7 +6535,7 @@
       <c r="J188" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M188" s="11"/>
+      <c r="M188" s="10"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6751,7 +6758,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="11">
+      <c r="M196" s="10">
         <v>2</v>
       </c>
     </row>
@@ -6780,7 +6787,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="11"/>
+      <c r="M197" s="10"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6807,7 +6814,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="11"/>
+      <c r="M198" s="10"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6834,7 +6841,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="11"/>
+      <c r="M199" s="10"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6861,7 +6868,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="11"/>
+      <c r="M200" s="10"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6890,7 +6897,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="11"/>
+      <c r="M201" s="10"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6917,7 +6924,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="11"/>
+      <c r="M202" s="10"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -6946,7 +6953,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="11"/>
+      <c r="M203" s="10"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -6973,7 +6980,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="11"/>
+      <c r="M204" s="10"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7000,7 +7007,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="11"/>
+      <c r="M205" s="10"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7027,7 +7034,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="11"/>
+      <c r="M206" s="10"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7054,7 +7061,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="11"/>
+      <c r="M207" s="10"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7081,7 +7088,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="11"/>
+      <c r="M208" s="10"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7108,7 +7115,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="11"/>
+      <c r="M209" s="10"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7138,7 +7145,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="11">
+      <c r="M210" s="10">
         <v>0.5</v>
       </c>
     </row>
@@ -7169,7 +7176,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="11"/>
+      <c r="M211" s="10"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7198,7 +7205,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="11"/>
+      <c r="M212" s="10"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7227,7 +7234,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="11"/>
+      <c r="M213" s="10"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7256,7 +7263,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="11"/>
+      <c r="M214" s="10"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7285,7 +7292,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="11"/>
+      <c r="M215" s="10"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7314,7 +7321,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="11"/>
+      <c r="M216" s="10"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7343,7 +7350,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="11"/>
+      <c r="M217" s="10"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7372,7 +7379,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="11"/>
+      <c r="M218" s="10"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7401,7 +7408,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="11"/>
+      <c r="M219" s="10"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7428,7 +7435,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="11">
+      <c r="M220" s="10">
         <v>1</v>
       </c>
     </row>
@@ -7457,7 +7464,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="11"/>
+      <c r="M221" s="10"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7484,7 +7491,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="11"/>
+      <c r="M222" s="10"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7511,7 +7518,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="11"/>
+      <c r="M223" s="10"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7538,7 +7545,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="11"/>
+      <c r="M224" s="10"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7565,7 +7572,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="11"/>
+      <c r="M225" s="10"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7594,7 +7601,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="11"/>
+      <c r="M226" s="10"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7623,7 +7630,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="11"/>
+      <c r="M227" s="10"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7654,7 +7661,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="11"/>
+      <c r="M228" s="10"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7685,7 +7692,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="11"/>
+      <c r="M229" s="10"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7718,7 +7725,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="11"/>
+      <c r="M230" s="10"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7751,7 +7758,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="11"/>
+      <c r="M231" s="10"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7784,7 +7791,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="11"/>
+      <c r="M232" s="10"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7817,7 +7824,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="11"/>
+      <c r="M233" s="10"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7848,7 +7855,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="11"/>
+      <c r="M234" s="10"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7881,7 +7888,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="11"/>
+      <c r="M235" s="10"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7914,7 +7921,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="11"/>
+      <c r="M236" s="10"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -7947,7 +7954,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="11"/>
+      <c r="M237" s="10"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -7980,7 +7987,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="11"/>
+      <c r="M238" s="10"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8013,7 +8020,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="11"/>
+      <c r="M239" s="10"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8046,7 +8053,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="11"/>
+      <c r="M240" s="10"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8073,7 +8080,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="11"/>
+      <c r="M241" s="10"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8100,7 +8107,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="11"/>
+      <c r="M242" s="10"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8129,7 +8136,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="11"/>
+      <c r="M243" s="10"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8158,7 +8165,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="11"/>
+      <c r="M244" s="10"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8187,7 +8194,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="11"/>
+      <c r="M245" s="10"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8216,7 +8223,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="11"/>
+      <c r="M246" s="10"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8245,7 +8252,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="11"/>
+      <c r="M247" s="10"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8274,7 +8281,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="11"/>
+      <c r="M248" s="10"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8303,7 +8310,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="11"/>
+      <c r="M249" s="10"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8332,7 +8339,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="11"/>
+      <c r="M250" s="10"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8359,7 +8366,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="11"/>
+      <c r="M251" s="10"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8386,7 +8393,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="11"/>
+      <c r="M252" s="10"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8413,7 +8420,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="11"/>
+      <c r="M253" s="10"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8440,7 +8447,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="11"/>
+      <c r="M254" s="10"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8467,7 +8474,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="11"/>
+      <c r="M255" s="10"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8494,7 +8501,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="11"/>
+      <c r="M256" s="10"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8521,7 +8528,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="11"/>
+      <c r="M257" s="10"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8550,7 +8557,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="11"/>
+      <c r="M258" s="10"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8577,7 +8584,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="11"/>
+      <c r="M259" s="10"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8606,7 +8613,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="11"/>
+      <c r="M260" s="10"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8633,7 +8640,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="11"/>
+      <c r="M261" s="10"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8660,7 +8667,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="11"/>
+      <c r="M262" s="10"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8687,7 +8694,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="11"/>
+      <c r="M263" s="10"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8714,7 +8721,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="11"/>
+      <c r="M264" s="10"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8741,7 +8748,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="11"/>
+      <c r="M265" s="10"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8768,7 +8775,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="11"/>
+      <c r="M266" s="10"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8795,7 +8802,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="11"/>
+      <c r="M267" s="10"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8822,7 +8829,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="11"/>
+      <c r="M268" s="10"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8851,7 +8858,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="11"/>
+      <c r="M269" s="10"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8880,7 +8887,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="11"/>
+      <c r="M270" s="10"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8909,7 +8916,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="11"/>
+      <c r="M271" s="10"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -8938,7 +8945,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="11"/>
+      <c r="M272" s="10"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -8967,7 +8974,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="11"/>
+      <c r="M273" s="10"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -8996,7 +9003,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="11"/>
+      <c r="M274" s="10"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9025,7 +9032,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="11"/>
+      <c r="M275" s="10"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9054,7 +9061,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="11"/>
+      <c r="M276" s="10"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9083,7 +9090,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="11"/>
+      <c r="M277" s="10"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9110,7 +9117,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="11"/>
+      <c r="M278" s="10"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9137,7 +9144,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="11"/>
+      <c r="M279" s="10"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9164,7 +9171,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="11"/>
+      <c r="M280" s="10"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9191,7 +9198,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="11"/>
+      <c r="M281" s="10"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9218,7 +9225,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="11"/>
+      <c r="M282" s="10"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9245,7 +9252,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="11"/>
+      <c r="M283" s="10"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9274,7 +9281,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="11"/>
+      <c r="M284" s="10"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9303,7 +9310,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="11"/>
+      <c r="M285" s="10"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9334,7 +9341,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="11"/>
+      <c r="M286" s="10"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9365,7 +9372,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="11"/>
+      <c r="M287" s="10"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9398,7 +9405,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="11"/>
+      <c r="M288" s="10"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9431,7 +9438,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="11"/>
+      <c r="M289" s="10"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9464,7 +9471,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="11"/>
+      <c r="M290" s="10"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9497,7 +9504,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="11"/>
+      <c r="M291" s="10"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9528,7 +9535,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="11"/>
+      <c r="M292" s="10"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9561,7 +9568,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="11"/>
+      <c r="M293" s="10"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9594,7 +9601,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="11"/>
+      <c r="M294" s="10"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9627,7 +9634,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="11"/>
+      <c r="M295" s="10"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9660,7 +9667,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="11"/>
+      <c r="M296" s="10"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9693,7 +9700,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="11"/>
+      <c r="M297" s="10"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9726,7 +9733,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="11"/>
+      <c r="M298" s="10"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9753,7 +9760,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="11"/>
+      <c r="M299" s="10"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9780,7 +9787,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="11"/>
+      <c r="M300" s="10"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9809,7 +9816,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="11"/>
+      <c r="M301" s="10"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9838,7 +9845,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="11"/>
+      <c r="M302" s="10"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9867,7 +9874,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="11"/>
+      <c r="M303" s="10"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9896,7 +9903,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="11"/>
+      <c r="M304" s="10"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -9925,7 +9932,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="11"/>
+      <c r="M305" s="10"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -9954,7 +9961,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="11"/>
+      <c r="M306" s="10"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -9983,7 +9990,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="11"/>
+      <c r="M307" s="10"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10012,7 +10019,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="11"/>
+      <c r="M308" s="10"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10039,7 +10046,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="11"/>
+      <c r="M309" s="10"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10066,7 +10073,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="11"/>
+      <c r="M310" s="10"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10093,7 +10100,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="11"/>
+      <c r="M311" s="10"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10120,7 +10127,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="11"/>
+      <c r="M312" s="10"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10147,7 +10154,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="11"/>
+      <c r="M313" s="10"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10174,7 +10181,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="11"/>
+      <c r="M314" s="10"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10201,7 +10208,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="11"/>
+      <c r="M315" s="10"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10230,7 +10237,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="11"/>
+      <c r="M316" s="10"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10257,7 +10264,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="11"/>
+      <c r="M317" s="10"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10286,7 +10293,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="11"/>
+      <c r="M318" s="10"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10313,7 +10320,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="11"/>
+      <c r="M319" s="10"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10340,7 +10347,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="11"/>
+      <c r="M320" s="10"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10367,7 +10374,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="11"/>
+      <c r="M321" s="10"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10394,7 +10401,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="11"/>
+      <c r="M322" s="10"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10421,7 +10428,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="11"/>
+      <c r="M323" s="10"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10448,7 +10455,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="11"/>
+      <c r="M324" s="10"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10475,7 +10482,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="11"/>
+      <c r="M325" s="10"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10502,7 +10509,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="11"/>
+      <c r="M326" s="10"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10531,7 +10538,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="11"/>
+      <c r="M327" s="10"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10560,7 +10567,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="11"/>
+      <c r="M328" s="10"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10589,7 +10596,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="11"/>
+      <c r="M329" s="10"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10618,7 +10625,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="11"/>
+      <c r="M330" s="10"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10647,7 +10654,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="11"/>
+      <c r="M331" s="10"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10676,7 +10683,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="11"/>
+      <c r="M332" s="10"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10705,7 +10712,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="11"/>
+      <c r="M333" s="10"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10734,7 +10741,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="11"/>
+      <c r="M334" s="10"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10763,7 +10770,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="11"/>
+      <c r="M335" s="10"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -10938,7 +10945,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="11">
+      <c r="M342" s="10">
         <v>1</v>
       </c>
     </row>
@@ -10965,7 +10972,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="11"/>
+      <c r="M343" s="10"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -10990,7 +10997,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="11"/>
+      <c r="M344" s="10"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11015,7 +11022,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="11"/>
+      <c r="M345" s="10"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11040,7 +11047,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="11"/>
+      <c r="M346" s="10"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11065,7 +11072,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="11"/>
+      <c r="M347" s="10"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11092,7 +11099,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="11"/>
+      <c r="M348" s="10"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11119,7 +11126,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="11"/>
+      <c r="M349" s="10"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11148,7 +11155,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="11"/>
+      <c r="M350" s="10"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11177,7 +11184,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="11"/>
+      <c r="M351" s="10"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11208,7 +11215,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="11"/>
+      <c r="M352" s="10"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11239,7 +11246,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="11"/>
+      <c r="M353" s="10"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11270,7 +11277,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="11"/>
+      <c r="M354" s="10"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11301,7 +11308,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="11"/>
+      <c r="M355" s="10"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11330,7 +11337,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="11"/>
+      <c r="M356" s="10"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11361,7 +11368,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="11"/>
+      <c r="M357" s="10"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11392,7 +11399,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="11"/>
+      <c r="M358" s="10"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11423,7 +11430,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="11"/>
+      <c r="M359" s="10"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11454,7 +11461,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="11"/>
+      <c r="M360" s="10"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11485,7 +11492,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="11"/>
+      <c r="M361" s="10"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11516,7 +11523,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="11"/>
+      <c r="M362" s="10"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11541,7 +11548,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="11"/>
+      <c r="M363" s="10"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11566,7 +11573,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="11"/>
+      <c r="M364" s="10"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11593,7 +11600,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="11"/>
+      <c r="M365" s="10"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11620,7 +11627,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="11"/>
+      <c r="M366" s="10"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11647,7 +11654,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="11"/>
+      <c r="M367" s="10"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11674,7 +11681,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="11"/>
+      <c r="M368" s="10"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11701,7 +11708,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="11"/>
+      <c r="M369" s="10"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11728,7 +11735,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="11"/>
+      <c r="M370" s="10"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11755,7 +11762,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="11"/>
+      <c r="M371" s="10"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11782,7 +11789,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="11"/>
+      <c r="M372" s="10"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11807,7 +11814,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="11"/>
+      <c r="M373" s="10"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11832,7 +11839,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="11"/>
+      <c r="M374" s="10"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11857,7 +11864,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="11"/>
+      <c r="M375" s="10"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11882,7 +11889,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="11"/>
+      <c r="M376" s="10"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11907,7 +11914,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="11"/>
+      <c r="M377" s="10"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -11932,7 +11939,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="11"/>
+      <c r="M378" s="10"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -11957,7 +11964,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="11"/>
+      <c r="M379" s="10"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -11984,7 +11991,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="11"/>
+      <c r="M380" s="10"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12009,7 +12016,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="11"/>
+      <c r="M381" s="10"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12036,7 +12043,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="11"/>
+      <c r="M382" s="10"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12061,7 +12068,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="11"/>
+      <c r="M383" s="10"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12086,7 +12093,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="11"/>
+      <c r="M384" s="10"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12111,7 +12118,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="11"/>
+      <c r="M385" s="10"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12136,7 +12143,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="11"/>
+      <c r="M386" s="10"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12209,7 +12216,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="11">
+      <c r="M389" s="10">
         <v>0.5</v>
       </c>
     </row>
@@ -12238,7 +12245,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="11"/>
+      <c r="M390" s="10"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12265,7 +12272,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="11"/>
+      <c r="M391" s="10"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12292,7 +12299,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="11"/>
+      <c r="M392" s="10"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12319,7 +12326,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="11"/>
+      <c r="M393" s="10"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12346,7 +12353,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="11"/>
+      <c r="M394" s="10"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12373,7 +12380,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="11"/>
+      <c r="M395" s="10"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12403,7 +12410,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="11">
+      <c r="M396" s="10">
         <v>1</v>
       </c>
     </row>
@@ -12432,7 +12439,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="11"/>
+      <c r="M397" s="10"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12459,7 +12466,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="11"/>
+      <c r="M398" s="10"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12486,7 +12493,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="11"/>
+      <c r="M399" s="10"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12513,7 +12520,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="11"/>
+      <c r="M400" s="10"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12540,7 +12547,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="11"/>
+      <c r="M401" s="10"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12567,7 +12574,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="11"/>
+      <c r="M402" s="10"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12594,7 +12601,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="11"/>
+      <c r="M403" s="10"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12621,7 +12628,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="11"/>
+      <c r="M404" s="10"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12648,7 +12655,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="11"/>
+      <c r="M405" s="10"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12675,7 +12682,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="11"/>
+      <c r="M406" s="10"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12702,7 +12709,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="11"/>
+      <c r="M407" s="10"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12731,7 +12738,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="11"/>
+      <c r="M408" s="10"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12758,7 +12765,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="11"/>
+      <c r="M409" s="10"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12787,7 +12794,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="11"/>
+      <c r="M410" s="10"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12814,7 +12821,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="11"/>
+      <c r="M411" s="10"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12841,7 +12848,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="11"/>
+      <c r="M412" s="10"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12868,7 +12875,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="11"/>
+      <c r="M413" s="10"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12895,7 +12902,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="11"/>
+      <c r="M414" s="10"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -12925,7 +12932,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="11">
+      <c r="M415" s="10">
         <v>0.5</v>
       </c>
     </row>
@@ -12954,7 +12961,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="11"/>
+      <c r="M416" s="10"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -12983,7 +12990,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="11"/>
+      <c r="M417" s="10"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13012,7 +13019,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="11"/>
+      <c r="M418" s="10"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13041,7 +13048,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="11"/>
+      <c r="M419" s="10"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13070,7 +13077,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="11"/>
+      <c r="M420" s="10"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13100,7 +13107,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="11">
+      <c r="M421" s="10">
         <v>1</v>
       </c>
     </row>
@@ -13129,7 +13136,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="11"/>
+      <c r="M422" s="10"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13156,7 +13163,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="11"/>
+      <c r="M423" s="10"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13183,7 +13190,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="11"/>
+      <c r="M424" s="10"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13210,7 +13217,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="11"/>
+      <c r="M425" s="10"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13237,7 +13244,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="11"/>
+      <c r="M426" s="10"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13264,7 +13271,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="11"/>
+      <c r="M427" s="10"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13291,7 +13298,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="11"/>
+      <c r="M428" s="10"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13318,7 +13325,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="11"/>
+      <c r="M429" s="10"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13345,7 +13352,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="11"/>
+      <c r="M430" s="10"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13372,7 +13379,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="11"/>
+      <c r="M431" s="10"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13399,7 +13406,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="11"/>
+      <c r="M432" s="10"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13428,7 +13435,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="11"/>
+      <c r="M433" s="10"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13455,7 +13462,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="11"/>
+      <c r="M434" s="10"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13484,7 +13491,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="11"/>
+      <c r="M435" s="10"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13511,7 +13518,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="11"/>
+      <c r="M436" s="10"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13538,7 +13545,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="11"/>
+      <c r="M437" s="10"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13565,7 +13572,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="11"/>
+      <c r="M438" s="10"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13592,7 +13599,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="11"/>
+      <c r="M439" s="10"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13626,7 +13633,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="11">
+      <c r="M440" s="10">
         <v>1</v>
       </c>
     </row>
@@ -13659,7 +13666,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="11"/>
+      <c r="M441" s="10"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13690,7 +13697,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="11"/>
+      <c r="M442" s="10"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13721,7 +13728,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="11"/>
+      <c r="M443" s="10"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13752,7 +13759,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="11"/>
+      <c r="M444" s="10"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13783,7 +13790,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="11"/>
+      <c r="M445" s="10"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13814,7 +13821,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="11"/>
+      <c r="M446" s="10"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13845,7 +13852,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="11"/>
+      <c r="M447" s="10"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13876,7 +13883,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="11"/>
+      <c r="M448" s="10"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13907,7 +13914,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="11"/>
+      <c r="M449" s="10"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -13936,7 +13943,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="11"/>
+      <c r="M450" s="10"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -13965,7 +13972,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="11"/>
+      <c r="M451" s="10"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -13994,7 +14001,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="11"/>
+      <c r="M452" s="10"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14023,7 +14030,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="11"/>
+      <c r="M453" s="10"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14052,7 +14059,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="11"/>
+      <c r="M454" s="10"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14079,7 +14086,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="11"/>
+      <c r="M455" s="10"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14106,7 +14113,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="11"/>
+      <c r="M456" s="10"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14133,7 +14140,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="11"/>
+      <c r="M457" s="10"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14162,7 +14169,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="11"/>
+      <c r="M458" s="10"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14191,7 +14198,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="11"/>
+      <c r="M459" s="10"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14220,7 +14227,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="11"/>
+      <c r="M460" s="10"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14249,7 +14256,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="11"/>
+      <c r="M461" s="10"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14583,7 +14590,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="12">
+      <c r="M474" s="9">
         <v>1</v>
       </c>
     </row>
@@ -14612,7 +14619,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="12"/>
+      <c r="M475" s="9"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14639,7 +14646,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="12"/>
+      <c r="M476" s="9"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14666,7 +14673,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="12"/>
+      <c r="M477" s="9"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14693,7 +14700,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="12"/>
+      <c r="M478" s="9"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14720,7 +14727,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="12"/>
+      <c r="M479" s="9"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14747,7 +14754,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="12"/>
+      <c r="M480" s="9"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14774,7 +14781,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="12"/>
+      <c r="M481" s="9"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14801,7 +14808,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="12"/>
+      <c r="M482" s="9"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14828,7 +14835,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="12"/>
+      <c r="M483" s="9"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -14988,7 +14995,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="12">
+      <c r="M489" s="9">
         <v>2</v>
       </c>
     </row>
@@ -15015,7 +15022,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="12"/>
+      <c r="M490" s="9"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15040,7 +15047,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="12"/>
+      <c r="M491" s="9"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15065,7 +15072,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="12"/>
+      <c r="M492" s="9"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15090,7 +15097,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="12"/>
+      <c r="M493" s="9"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15117,7 +15124,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="12"/>
+      <c r="M494" s="9"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15144,7 +15151,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="12"/>
+      <c r="M495" s="9"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15171,7 +15178,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="12"/>
+      <c r="M496" s="9"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15198,7 +15205,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="12"/>
+      <c r="M497" s="9"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15251,7 +15258,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="12">
+      <c r="M499" s="9">
         <v>1</v>
       </c>
     </row>
@@ -15278,7 +15285,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="12"/>
+      <c r="M500" s="9"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15303,7 +15310,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="12"/>
+      <c r="M501" s="9"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15328,7 +15335,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="12"/>
+      <c r="M502" s="9"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15353,7 +15360,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="12"/>
+      <c r="M503" s="9"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15378,7 +15385,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="12"/>
+      <c r="M504" s="9"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15405,7 +15412,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="12"/>
+      <c r="M505" s="9"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15430,7 +15437,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="12"/>
+      <c r="M506" s="9"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15457,7 +15464,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="12"/>
+      <c r="M507" s="9"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15482,7 +15489,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="12"/>
+      <c r="M508" s="9"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15507,7 +15514,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="12"/>
+      <c r="M509" s="9"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15532,7 +15539,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="12"/>
+      <c r="M510" s="9"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15557,7 +15564,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="12"/>
+      <c r="M511" s="9"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15584,7 +15591,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="12"/>
+      <c r="M512" s="9"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15611,7 +15618,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="12"/>
+      <c r="M513" s="9"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15636,7 +15643,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="12"/>
+      <c r="M514" s="9"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15661,7 +15668,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="12"/>
+      <c r="M515" s="9"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15689,7 +15696,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="12">
+      <c r="M516" s="9">
         <v>2</v>
       </c>
     </row>
@@ -15718,7 +15725,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="12"/>
+      <c r="M517" s="9"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15745,7 +15752,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="12"/>
+      <c r="M518" s="9"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15772,7 +15779,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="12"/>
+      <c r="M519" s="9"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15801,7 +15808,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="12"/>
+      <c r="M520" s="9"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15830,7 +15837,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="12"/>
+      <c r="M521" s="9"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15859,7 +15866,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="12"/>
+      <c r="M522" s="9"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15888,7 +15895,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="12"/>
+      <c r="M523" s="9"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15917,7 +15924,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="12"/>
+      <c r="M524" s="9"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -15946,7 +15953,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="12"/>
+      <c r="M525" s="9"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -15973,7 +15980,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="12"/>
+      <c r="M526" s="9"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16000,7 +16007,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="12"/>
+      <c r="M527" s="9"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16025,6 +16032,11 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16041,11 +16053,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added: Chart Area -> Area -> Fill -> Bitmap -> Position (direct)
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -831,19 +831,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,7 +1168,7 @@
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
+      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1187,16 +1187,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1292,7 +1292,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1317,7 +1317,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1342,7 +1342,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1367,7 +1367,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1392,7 +1392,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1417,7 +1417,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1442,7 +1442,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M10" s="12"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="12"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="10">
+      <c r="M43" s="12">
         <v>2</v>
       </c>
     </row>
@@ -2392,7 +2392,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="10"/>
+      <c r="M44" s="12"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2424,7 +2424,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="10"/>
+      <c r="M45" s="12"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2456,7 +2456,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="10"/>
+      <c r="M46" s="12"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2488,7 +2488,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="10"/>
+      <c r="M47" s="12"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2520,7 +2520,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="10"/>
+      <c r="M48" s="12"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2552,7 +2552,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="10"/>
+      <c r="M49" s="12"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2584,7 +2584,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="10"/>
+      <c r="M50" s="12"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2773,7 +2773,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="10">
+      <c r="M57" s="12">
         <v>3</v>
       </c>
     </row>
@@ -2802,7 +2802,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="10"/>
+      <c r="M58" s="12"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2829,7 +2829,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="10"/>
+      <c r="M59" s="12"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2856,7 +2856,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="10"/>
+      <c r="M60" s="12"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3954,7 +3954,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="10">
+      <c r="M98" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="10"/>
+      <c r="M99" s="12"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
@@ -4006,7 +4006,7 @@
       <c r="J100" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M100" s="10"/>
+      <c r="M100" s="12"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4031,7 +4031,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="10"/>
+      <c r="M101" s="12"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4058,7 +4058,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="10"/>
+      <c r="M102" s="12"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4085,7 +4085,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="10"/>
+      <c r="M103" s="12"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4114,7 +4114,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="10"/>
+      <c r="M104" s="12"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4143,7 +4143,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="10"/>
+      <c r="M105" s="12"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4174,10 +4174,10 @@
       <c r="J106" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="K106" s="13" t="s">
+      <c r="K106" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="10"/>
+      <c r="M106" s="12"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4208,7 +4208,7 @@
       <c r="J107" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M107" s="10"/>
+      <c r="M107" s="12"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4239,7 +4239,7 @@
       <c r="J108" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M108" s="10"/>
+      <c r="M108" s="12"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4270,7 +4270,7 @@
       <c r="J109" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M109" s="10"/>
+      <c r="M109" s="12"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4297,9 +4297,9 @@
         <v>210</v>
       </c>
       <c r="J110" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M110" s="10"/>
+        <v>210</v>
+      </c>
+      <c r="M110" s="12"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4330,7 +4330,7 @@
       <c r="J111" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M111" s="10"/>
+      <c r="M111" s="12"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4361,7 +4361,7 @@
       <c r="J112" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M112" s="10"/>
+      <c r="M112" s="12"/>
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="1" t="s">
@@ -4392,7 +4392,7 @@
       <c r="J113" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M113" s="10"/>
+      <c r="M113" s="12"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4423,7 +4423,7 @@
       <c r="J114" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M114" s="10"/>
+      <c r="M114" s="12"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4454,7 +4454,7 @@
       <c r="J115" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M115" s="10"/>
+      <c r="M115" s="12"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4485,7 +4485,7 @@
       <c r="J116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M116" s="10"/>
+      <c r="M116" s="12"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4510,7 +4510,7 @@
       <c r="J117" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M117" s="10"/>
+      <c r="M117" s="12"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4537,7 +4537,7 @@
       <c r="J118" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M118" s="10"/>
+      <c r="M118" s="12"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4771,7 +4771,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="10">
+      <c r="M127" s="12">
         <v>1</v>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="10"/>
+      <c r="M128" s="12"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4823,7 +4823,7 @@
       <c r="J129" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M129" s="10"/>
+      <c r="M129" s="12"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4848,7 +4848,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="10"/>
+      <c r="M130" s="12"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4873,7 +4873,7 @@
       <c r="J131" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M131" s="10"/>
+      <c r="M131" s="12"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4900,7 +4900,7 @@
       <c r="J132" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M132" s="10"/>
+      <c r="M132" s="12"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4927,7 +4927,7 @@
       <c r="J133" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M133" s="10"/>
+      <c r="M133" s="12"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -4956,7 +4956,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="10"/>
+      <c r="M134" s="12"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -4985,7 +4985,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="10"/>
+      <c r="M135" s="12"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5016,7 +5016,7 @@
       <c r="J136" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M136" s="10"/>
+      <c r="M136" s="12"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5047,7 +5047,7 @@
       <c r="J137" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M137" s="10"/>
+      <c r="M137" s="12"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5078,7 +5078,7 @@
       <c r="J138" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M138" s="10"/>
+      <c r="M138" s="12"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5109,7 +5109,7 @@
       <c r="J139" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M139" s="10"/>
+      <c r="M139" s="12"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5138,7 +5138,7 @@
       <c r="J140" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M140" s="10"/>
+      <c r="M140" s="12"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5169,7 +5169,7 @@
       <c r="J141" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M141" s="10"/>
+      <c r="M141" s="12"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5200,7 +5200,7 @@
       <c r="J142" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M142" s="10"/>
+      <c r="M142" s="12"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5231,7 +5231,7 @@
       <c r="J143" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M143" s="10"/>
+      <c r="M143" s="12"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5262,7 +5262,7 @@
       <c r="J144" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M144" s="10"/>
+      <c r="M144" s="12"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5293,7 +5293,7 @@
       <c r="J145" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M145" s="10"/>
+      <c r="M145" s="12"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5324,7 +5324,7 @@
       <c r="J146" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M146" s="10"/>
+      <c r="M146" s="12"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5349,7 +5349,7 @@
       <c r="J147" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M147" s="10"/>
+      <c r="M147" s="12"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5374,7 +5374,7 @@
       <c r="J148" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M148" s="10"/>
+      <c r="M148" s="12"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5401,7 +5401,7 @@
       <c r="J149" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M149" s="10"/>
+      <c r="M149" s="12"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5428,7 +5428,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="10"/>
+      <c r="M150" s="12"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5455,7 +5455,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="10"/>
+      <c r="M151" s="12"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5482,7 +5482,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="10"/>
+      <c r="M152" s="12"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5509,7 +5509,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="10"/>
+      <c r="M153" s="12"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5536,7 +5536,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="10"/>
+      <c r="M154" s="12"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5563,7 +5563,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="10"/>
+      <c r="M155" s="12"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5590,7 +5590,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="10"/>
+      <c r="M156" s="12"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5615,7 +5615,7 @@
       <c r="J157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M157" s="10"/>
+      <c r="M157" s="12"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5642,7 +5642,7 @@
       <c r="J158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M158" s="10"/>
+      <c r="M158" s="12"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5669,7 +5669,7 @@
       <c r="J159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M159" s="10"/>
+      <c r="M159" s="12"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5696,7 +5696,7 @@
       <c r="J160" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M160" s="10"/>
+      <c r="M160" s="12"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5723,7 +5723,7 @@
       <c r="J161" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M161" s="10"/>
+      <c r="M161" s="12"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5750,7 +5750,7 @@
       <c r="J162" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M162" s="10"/>
+      <c r="M162" s="12"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5777,7 +5777,7 @@
       <c r="J163" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M163" s="10"/>
+      <c r="M163" s="12"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5804,7 +5804,7 @@
       <c r="J164" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M164" s="10"/>
+      <c r="M164" s="12"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5834,7 +5834,7 @@
       <c r="J165" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M165" s="10">
+      <c r="M165" s="12">
         <v>1</v>
       </c>
     </row>
@@ -5863,7 +5863,7 @@
       <c r="J166" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M166" s="10"/>
+      <c r="M166" s="12"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5890,7 +5890,7 @@
       <c r="J167" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M167" s="10"/>
+      <c r="M167" s="12"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5917,7 +5917,7 @@
       <c r="J168" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M168" s="10"/>
+      <c r="M168" s="12"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -5944,7 +5944,7 @@
       <c r="J169" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M169" s="10"/>
+      <c r="M169" s="12"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -5971,7 +5971,7 @@
       <c r="J170" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M170" s="10"/>
+      <c r="M170" s="12"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6000,7 +6000,7 @@
       <c r="J171" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="10"/>
+      <c r="M171" s="12"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6029,7 +6029,7 @@
       <c r="J172" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M172" s="10"/>
+      <c r="M172" s="12"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6060,7 +6060,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="10"/>
+      <c r="M173" s="12"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6091,7 +6091,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="10"/>
+      <c r="M174" s="12"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6124,7 +6124,7 @@
       <c r="J175" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M175" s="10"/>
+      <c r="M175" s="12"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6157,7 +6157,7 @@
       <c r="J176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M176" s="10"/>
+      <c r="M176" s="12"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6190,7 +6190,7 @@
       <c r="J177" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M177" s="10"/>
+      <c r="M177" s="12"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6223,7 +6223,7 @@
       <c r="J178" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M178" s="10"/>
+      <c r="M178" s="12"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6254,7 +6254,7 @@
       <c r="J179" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M179" s="10"/>
+      <c r="M179" s="12"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6287,7 +6287,7 @@
       <c r="J180" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M180" s="10"/>
+      <c r="M180" s="12"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6320,7 +6320,7 @@
       <c r="J181" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M181" s="10"/>
+      <c r="M181" s="12"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6353,7 +6353,7 @@
       <c r="J182" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M182" s="10"/>
+      <c r="M182" s="12"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6386,7 +6386,7 @@
       <c r="J183" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M183" s="10"/>
+      <c r="M183" s="12"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6419,7 +6419,7 @@
       <c r="J184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M184" s="10"/>
+      <c r="M184" s="12"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6452,7 +6452,7 @@
       <c r="J185" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M185" s="10"/>
+      <c r="M185" s="12"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6479,7 +6479,7 @@
       <c r="J186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M186" s="10"/>
+      <c r="M186" s="12"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6506,7 +6506,7 @@
       <c r="J187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M187" s="10"/>
+      <c r="M187" s="12"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6535,7 +6535,7 @@
       <c r="J188" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M188" s="10"/>
+      <c r="M188" s="12"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6758,7 +6758,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="10">
+      <c r="M196" s="12">
         <v>2</v>
       </c>
     </row>
@@ -6787,7 +6787,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="10"/>
+      <c r="M197" s="12"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6814,7 +6814,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="10"/>
+      <c r="M198" s="12"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6841,7 +6841,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="10"/>
+      <c r="M199" s="12"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6868,7 +6868,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="10"/>
+      <c r="M200" s="12"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6897,7 +6897,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="10"/>
+      <c r="M201" s="12"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6924,7 +6924,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="10"/>
+      <c r="M202" s="12"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -6953,7 +6953,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="10"/>
+      <c r="M203" s="12"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -6980,7 +6980,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="10"/>
+      <c r="M204" s="12"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7007,7 +7007,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="10"/>
+      <c r="M205" s="12"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7034,7 +7034,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="10"/>
+      <c r="M206" s="12"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7061,7 +7061,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="10"/>
+      <c r="M207" s="12"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7088,7 +7088,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="10"/>
+      <c r="M208" s="12"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7115,7 +7115,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="10"/>
+      <c r="M209" s="12"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7145,7 +7145,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="10">
+      <c r="M210" s="12">
         <v>0.5</v>
       </c>
     </row>
@@ -7176,7 +7176,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="10"/>
+      <c r="M211" s="12"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7205,7 +7205,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="10"/>
+      <c r="M212" s="12"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7234,7 +7234,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="10"/>
+      <c r="M213" s="12"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7263,7 +7263,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="10"/>
+      <c r="M214" s="12"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7292,7 +7292,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="10"/>
+      <c r="M215" s="12"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7321,7 +7321,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="10"/>
+      <c r="M216" s="12"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7350,7 +7350,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="10"/>
+      <c r="M217" s="12"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7379,7 +7379,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="10"/>
+      <c r="M218" s="12"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7408,7 +7408,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="10"/>
+      <c r="M219" s="12"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7435,7 +7435,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="10">
+      <c r="M220" s="12">
         <v>1</v>
       </c>
     </row>
@@ -7464,7 +7464,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="10"/>
+      <c r="M221" s="12"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7491,7 +7491,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="10"/>
+      <c r="M222" s="12"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7518,7 +7518,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="10"/>
+      <c r="M223" s="12"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7545,7 +7545,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="10"/>
+      <c r="M224" s="12"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7572,7 +7572,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="10"/>
+      <c r="M225" s="12"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7601,7 +7601,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="10"/>
+      <c r="M226" s="12"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7630,7 +7630,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="10"/>
+      <c r="M227" s="12"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7661,7 +7661,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="10"/>
+      <c r="M228" s="12"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7692,7 +7692,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="10"/>
+      <c r="M229" s="12"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7725,7 +7725,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="10"/>
+      <c r="M230" s="12"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7758,7 +7758,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="10"/>
+      <c r="M231" s="12"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7791,7 +7791,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="10"/>
+      <c r="M232" s="12"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7824,7 +7824,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="10"/>
+      <c r="M233" s="12"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7855,7 +7855,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="10"/>
+      <c r="M234" s="12"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7888,7 +7888,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="10"/>
+      <c r="M235" s="12"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7921,7 +7921,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="10"/>
+      <c r="M236" s="12"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -7954,7 +7954,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="10"/>
+      <c r="M237" s="12"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -7987,7 +7987,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="10"/>
+      <c r="M238" s="12"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8020,7 +8020,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="10"/>
+      <c r="M239" s="12"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8053,7 +8053,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="10"/>
+      <c r="M240" s="12"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8080,7 +8080,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="10"/>
+      <c r="M241" s="12"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8107,7 +8107,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="10"/>
+      <c r="M242" s="12"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8136,7 +8136,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="10"/>
+      <c r="M243" s="12"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8165,7 +8165,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="10"/>
+      <c r="M244" s="12"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8194,7 +8194,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="10"/>
+      <c r="M245" s="12"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8223,7 +8223,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="10"/>
+      <c r="M246" s="12"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8252,7 +8252,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="10"/>
+      <c r="M247" s="12"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8281,7 +8281,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="10"/>
+      <c r="M248" s="12"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8310,7 +8310,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="10"/>
+      <c r="M249" s="12"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8339,7 +8339,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="10"/>
+      <c r="M250" s="12"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8366,7 +8366,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="10"/>
+      <c r="M251" s="12"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8393,7 +8393,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="10"/>
+      <c r="M252" s="12"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8420,7 +8420,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="10"/>
+      <c r="M253" s="12"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8447,7 +8447,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="10"/>
+      <c r="M254" s="12"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8474,7 +8474,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="10"/>
+      <c r="M255" s="12"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8501,7 +8501,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="10"/>
+      <c r="M256" s="12"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8528,7 +8528,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="10"/>
+      <c r="M257" s="12"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8557,7 +8557,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="10"/>
+      <c r="M258" s="12"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8584,7 +8584,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="10"/>
+      <c r="M259" s="12"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8613,7 +8613,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="10"/>
+      <c r="M260" s="12"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8640,7 +8640,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="10"/>
+      <c r="M261" s="12"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8667,7 +8667,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="10"/>
+      <c r="M262" s="12"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8694,7 +8694,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="10"/>
+      <c r="M263" s="12"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8721,7 +8721,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="10"/>
+      <c r="M264" s="12"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8748,7 +8748,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="10"/>
+      <c r="M265" s="12"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8775,7 +8775,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="10"/>
+      <c r="M266" s="12"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8802,7 +8802,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="10"/>
+      <c r="M267" s="12"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8829,7 +8829,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="10"/>
+      <c r="M268" s="12"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8858,7 +8858,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="10"/>
+      <c r="M269" s="12"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8887,7 +8887,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="10"/>
+      <c r="M270" s="12"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8916,7 +8916,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="10"/>
+      <c r="M271" s="12"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -8945,7 +8945,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="10"/>
+      <c r="M272" s="12"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -8974,7 +8974,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="10"/>
+      <c r="M273" s="12"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9003,7 +9003,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="10"/>
+      <c r="M274" s="12"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9032,7 +9032,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="10"/>
+      <c r="M275" s="12"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9061,7 +9061,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="10"/>
+      <c r="M276" s="12"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9090,7 +9090,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="10"/>
+      <c r="M277" s="12"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9117,7 +9117,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="10"/>
+      <c r="M278" s="12"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9144,7 +9144,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="10"/>
+      <c r="M279" s="12"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9171,7 +9171,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="10"/>
+      <c r="M280" s="12"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9198,7 +9198,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="10"/>
+      <c r="M281" s="12"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9225,7 +9225,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="10"/>
+      <c r="M282" s="12"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9252,7 +9252,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="10"/>
+      <c r="M283" s="12"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9281,7 +9281,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="10"/>
+      <c r="M284" s="12"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9310,7 +9310,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="10"/>
+      <c r="M285" s="12"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9341,7 +9341,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="10"/>
+      <c r="M286" s="12"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9372,7 +9372,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="10"/>
+      <c r="M287" s="12"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9405,7 +9405,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="10"/>
+      <c r="M288" s="12"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9438,7 +9438,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="10"/>
+      <c r="M289" s="12"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9471,7 +9471,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="10"/>
+      <c r="M290" s="12"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9504,7 +9504,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="10"/>
+      <c r="M291" s="12"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9535,7 +9535,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="10"/>
+      <c r="M292" s="12"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9568,7 +9568,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="10"/>
+      <c r="M293" s="12"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9601,7 +9601,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="10"/>
+      <c r="M294" s="12"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9634,7 +9634,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="10"/>
+      <c r="M295" s="12"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9667,7 +9667,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="10"/>
+      <c r="M296" s="12"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9700,7 +9700,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="10"/>
+      <c r="M297" s="12"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9733,7 +9733,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="10"/>
+      <c r="M298" s="12"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9760,7 +9760,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="10"/>
+      <c r="M299" s="12"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9787,7 +9787,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="10"/>
+      <c r="M300" s="12"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9816,7 +9816,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="10"/>
+      <c r="M301" s="12"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9845,7 +9845,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="10"/>
+      <c r="M302" s="12"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9874,7 +9874,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="10"/>
+      <c r="M303" s="12"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9903,7 +9903,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="10"/>
+      <c r="M304" s="12"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -9932,7 +9932,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="10"/>
+      <c r="M305" s="12"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -9961,7 +9961,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="10"/>
+      <c r="M306" s="12"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -9990,7 +9990,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="10"/>
+      <c r="M307" s="12"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10019,7 +10019,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="10"/>
+      <c r="M308" s="12"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10046,7 +10046,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="10"/>
+      <c r="M309" s="12"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10073,7 +10073,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="10"/>
+      <c r="M310" s="12"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10100,7 +10100,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="10"/>
+      <c r="M311" s="12"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10127,7 +10127,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="10"/>
+      <c r="M312" s="12"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10154,7 +10154,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="10"/>
+      <c r="M313" s="12"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10181,7 +10181,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="10"/>
+      <c r="M314" s="12"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10208,7 +10208,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="10"/>
+      <c r="M315" s="12"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10237,7 +10237,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="10"/>
+      <c r="M316" s="12"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10264,7 +10264,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="10"/>
+      <c r="M317" s="12"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10293,7 +10293,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="10"/>
+      <c r="M318" s="12"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10320,7 +10320,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="10"/>
+      <c r="M319" s="12"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10347,7 +10347,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="10"/>
+      <c r="M320" s="12"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10374,7 +10374,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="10"/>
+      <c r="M321" s="12"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10401,7 +10401,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="10"/>
+      <c r="M322" s="12"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10428,7 +10428,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="10"/>
+      <c r="M323" s="12"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10455,7 +10455,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="10"/>
+      <c r="M324" s="12"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10482,7 +10482,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="10"/>
+      <c r="M325" s="12"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10509,7 +10509,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="10"/>
+      <c r="M326" s="12"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10538,7 +10538,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="10"/>
+      <c r="M327" s="12"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10567,7 +10567,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="10"/>
+      <c r="M328" s="12"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10596,7 +10596,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="10"/>
+      <c r="M329" s="12"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10625,7 +10625,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="10"/>
+      <c r="M330" s="12"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10654,7 +10654,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="10"/>
+      <c r="M331" s="12"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10683,7 +10683,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="10"/>
+      <c r="M332" s="12"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10712,7 +10712,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="10"/>
+      <c r="M333" s="12"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10741,7 +10741,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="10"/>
+      <c r="M334" s="12"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10770,7 +10770,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="10"/>
+      <c r="M335" s="12"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -10945,7 +10945,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="10">
+      <c r="M342" s="12">
         <v>1</v>
       </c>
     </row>
@@ -10972,7 +10972,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="10"/>
+      <c r="M343" s="12"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -10997,7 +10997,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="10"/>
+      <c r="M344" s="12"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11022,7 +11022,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="10"/>
+      <c r="M345" s="12"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11047,7 +11047,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="10"/>
+      <c r="M346" s="12"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11072,7 +11072,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="10"/>
+      <c r="M347" s="12"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11099,7 +11099,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="10"/>
+      <c r="M348" s="12"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11126,7 +11126,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="10"/>
+      <c r="M349" s="12"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11155,7 +11155,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="10"/>
+      <c r="M350" s="12"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11184,7 +11184,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="10"/>
+      <c r="M351" s="12"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11215,7 +11215,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="10"/>
+      <c r="M352" s="12"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11246,7 +11246,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="10"/>
+      <c r="M353" s="12"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11277,7 +11277,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="10"/>
+      <c r="M354" s="12"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11308,7 +11308,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="10"/>
+      <c r="M355" s="12"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11337,7 +11337,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="10"/>
+      <c r="M356" s="12"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11368,7 +11368,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="10"/>
+      <c r="M357" s="12"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11399,7 +11399,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="10"/>
+      <c r="M358" s="12"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11430,7 +11430,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="10"/>
+      <c r="M359" s="12"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11461,7 +11461,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="10"/>
+      <c r="M360" s="12"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11492,7 +11492,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="10"/>
+      <c r="M361" s="12"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11523,7 +11523,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="10"/>
+      <c r="M362" s="12"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11548,7 +11548,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="10"/>
+      <c r="M363" s="12"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11573,7 +11573,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="10"/>
+      <c r="M364" s="12"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11600,7 +11600,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="10"/>
+      <c r="M365" s="12"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11627,7 +11627,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="10"/>
+      <c r="M366" s="12"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11654,7 +11654,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="10"/>
+      <c r="M367" s="12"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11681,7 +11681,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="10"/>
+      <c r="M368" s="12"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11708,7 +11708,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="10"/>
+      <c r="M369" s="12"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11735,7 +11735,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="10"/>
+      <c r="M370" s="12"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11762,7 +11762,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="10"/>
+      <c r="M371" s="12"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11789,7 +11789,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="10"/>
+      <c r="M372" s="12"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11814,7 +11814,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="10"/>
+      <c r="M373" s="12"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11839,7 +11839,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="10"/>
+      <c r="M374" s="12"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11864,7 +11864,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="10"/>
+      <c r="M375" s="12"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11889,7 +11889,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="10"/>
+      <c r="M376" s="12"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11914,7 +11914,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="10"/>
+      <c r="M377" s="12"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -11939,7 +11939,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="10"/>
+      <c r="M378" s="12"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -11964,7 +11964,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="10"/>
+      <c r="M379" s="12"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -11991,7 +11991,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="10"/>
+      <c r="M380" s="12"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12016,7 +12016,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="10"/>
+      <c r="M381" s="12"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12043,7 +12043,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="10"/>
+      <c r="M382" s="12"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12068,7 +12068,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="10"/>
+      <c r="M383" s="12"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12093,7 +12093,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="10"/>
+      <c r="M384" s="12"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12118,7 +12118,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="10"/>
+      <c r="M385" s="12"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12143,7 +12143,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="10"/>
+      <c r="M386" s="12"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12216,7 +12216,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="10">
+      <c r="M389" s="12">
         <v>0.5</v>
       </c>
     </row>
@@ -12245,7 +12245,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="10"/>
+      <c r="M390" s="12"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12272,7 +12272,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="10"/>
+      <c r="M391" s="12"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12299,7 +12299,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="10"/>
+      <c r="M392" s="12"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12326,7 +12326,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="10"/>
+      <c r="M393" s="12"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12353,7 +12353,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="10"/>
+      <c r="M394" s="12"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12380,7 +12380,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="10"/>
+      <c r="M395" s="12"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12410,7 +12410,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="10">
+      <c r="M396" s="12">
         <v>1</v>
       </c>
     </row>
@@ -12439,7 +12439,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="10"/>
+      <c r="M397" s="12"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12466,7 +12466,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="10"/>
+      <c r="M398" s="12"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12493,7 +12493,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="10"/>
+      <c r="M399" s="12"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12520,7 +12520,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="10"/>
+      <c r="M400" s="12"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12547,7 +12547,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="10"/>
+      <c r="M401" s="12"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12574,7 +12574,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="10"/>
+      <c r="M402" s="12"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12601,7 +12601,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="10"/>
+      <c r="M403" s="12"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12628,7 +12628,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="10"/>
+      <c r="M404" s="12"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12655,7 +12655,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="10"/>
+      <c r="M405" s="12"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12682,7 +12682,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="10"/>
+      <c r="M406" s="12"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12709,7 +12709,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="10"/>
+      <c r="M407" s="12"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12738,7 +12738,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="10"/>
+      <c r="M408" s="12"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12765,7 +12765,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="10"/>
+      <c r="M409" s="12"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12794,7 +12794,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="10"/>
+      <c r="M410" s="12"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12821,7 +12821,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="10"/>
+      <c r="M411" s="12"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12848,7 +12848,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="10"/>
+      <c r="M412" s="12"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12875,7 +12875,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="10"/>
+      <c r="M413" s="12"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12902,7 +12902,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="10"/>
+      <c r="M414" s="12"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -12932,7 +12932,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="10">
+      <c r="M415" s="12">
         <v>0.5</v>
       </c>
     </row>
@@ -12961,7 +12961,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="10"/>
+      <c r="M416" s="12"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -12990,7 +12990,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="10"/>
+      <c r="M417" s="12"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13019,7 +13019,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="10"/>
+      <c r="M418" s="12"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13048,7 +13048,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="10"/>
+      <c r="M419" s="12"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13077,7 +13077,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="10"/>
+      <c r="M420" s="12"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13107,7 +13107,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="10">
+      <c r="M421" s="12">
         <v>1</v>
       </c>
     </row>
@@ -13136,7 +13136,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="10"/>
+      <c r="M422" s="12"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13163,7 +13163,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="10"/>
+      <c r="M423" s="12"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13190,7 +13190,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="10"/>
+      <c r="M424" s="12"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13217,7 +13217,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="10"/>
+      <c r="M425" s="12"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13244,7 +13244,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="10"/>
+      <c r="M426" s="12"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13271,7 +13271,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="10"/>
+      <c r="M427" s="12"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13298,7 +13298,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="10"/>
+      <c r="M428" s="12"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13325,7 +13325,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="10"/>
+      <c r="M429" s="12"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13352,7 +13352,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="10"/>
+      <c r="M430" s="12"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13379,7 +13379,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="10"/>
+      <c r="M431" s="12"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13406,7 +13406,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="10"/>
+      <c r="M432" s="12"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13435,7 +13435,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="10"/>
+      <c r="M433" s="12"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13462,7 +13462,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="10"/>
+      <c r="M434" s="12"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13491,7 +13491,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="10"/>
+      <c r="M435" s="12"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13518,7 +13518,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="10"/>
+      <c r="M436" s="12"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13545,7 +13545,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="10"/>
+      <c r="M437" s="12"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13572,7 +13572,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="10"/>
+      <c r="M438" s="12"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13599,7 +13599,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="10"/>
+      <c r="M439" s="12"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13633,7 +13633,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="10">
+      <c r="M440" s="12">
         <v>1</v>
       </c>
     </row>
@@ -13666,7 +13666,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="10"/>
+      <c r="M441" s="12"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13697,7 +13697,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="10"/>
+      <c r="M442" s="12"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13728,7 +13728,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="10"/>
+      <c r="M443" s="12"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13759,7 +13759,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="10"/>
+      <c r="M444" s="12"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13790,7 +13790,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="10"/>
+      <c r="M445" s="12"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13821,7 +13821,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="10"/>
+      <c r="M446" s="12"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13852,7 +13852,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="10"/>
+      <c r="M447" s="12"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13883,7 +13883,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="10"/>
+      <c r="M448" s="12"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13914,7 +13914,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="10"/>
+      <c r="M449" s="12"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -13943,7 +13943,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="10"/>
+      <c r="M450" s="12"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -13972,7 +13972,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="10"/>
+      <c r="M451" s="12"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14001,7 +14001,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="10"/>
+      <c r="M452" s="12"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14030,7 +14030,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="10"/>
+      <c r="M453" s="12"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14059,7 +14059,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="10"/>
+      <c r="M454" s="12"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14086,7 +14086,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="10"/>
+      <c r="M455" s="12"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14113,7 +14113,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="10"/>
+      <c r="M456" s="12"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14140,7 +14140,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="10"/>
+      <c r="M457" s="12"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14169,7 +14169,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="10"/>
+      <c r="M458" s="12"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14198,7 +14198,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="10"/>
+      <c r="M459" s="12"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14227,7 +14227,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="10"/>
+      <c r="M460" s="12"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14256,7 +14256,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="10"/>
+      <c r="M461" s="12"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14590,7 +14590,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="9">
+      <c r="M474" s="13">
         <v>1</v>
       </c>
     </row>
@@ -14619,7 +14619,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="9"/>
+      <c r="M475" s="13"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14646,7 +14646,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="9"/>
+      <c r="M476" s="13"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14673,7 +14673,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="9"/>
+      <c r="M477" s="13"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14700,7 +14700,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="9"/>
+      <c r="M478" s="13"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14727,7 +14727,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="9"/>
+      <c r="M479" s="13"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14754,7 +14754,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="9"/>
+      <c r="M480" s="13"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14781,7 +14781,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="9"/>
+      <c r="M481" s="13"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14808,7 +14808,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="9"/>
+      <c r="M482" s="13"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14835,7 +14835,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="9"/>
+      <c r="M483" s="13"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -14995,7 +14995,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="9">
+      <c r="M489" s="13">
         <v>2</v>
       </c>
     </row>
@@ -15022,7 +15022,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="9"/>
+      <c r="M490" s="13"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15047,7 +15047,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="9"/>
+      <c r="M491" s="13"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15072,7 +15072,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="9"/>
+      <c r="M492" s="13"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15097,7 +15097,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="9"/>
+      <c r="M493" s="13"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15124,7 +15124,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="9"/>
+      <c r="M494" s="13"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15151,7 +15151,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="9"/>
+      <c r="M495" s="13"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15178,7 +15178,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="9"/>
+      <c r="M496" s="13"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15205,7 +15205,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="9"/>
+      <c r="M497" s="13"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15258,7 +15258,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="9">
+      <c r="M499" s="13">
         <v>1</v>
       </c>
     </row>
@@ -15285,7 +15285,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="9"/>
+      <c r="M500" s="13"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15310,7 +15310,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="9"/>
+      <c r="M501" s="13"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15335,7 +15335,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="9"/>
+      <c r="M502" s="13"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15360,7 +15360,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="9"/>
+      <c r="M503" s="13"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15385,7 +15385,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="9"/>
+      <c r="M504" s="13"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15412,7 +15412,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="9"/>
+      <c r="M505" s="13"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15437,7 +15437,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="9"/>
+      <c r="M506" s="13"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15464,7 +15464,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="9"/>
+      <c r="M507" s="13"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15489,7 +15489,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="9"/>
+      <c r="M508" s="13"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15514,7 +15514,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="9"/>
+      <c r="M509" s="13"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15539,7 +15539,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="9"/>
+      <c r="M510" s="13"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15564,7 +15564,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="9"/>
+      <c r="M511" s="13"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15591,7 +15591,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="9"/>
+      <c r="M512" s="13"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15618,7 +15618,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="9"/>
+      <c r="M513" s="13"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15643,7 +15643,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="9"/>
+      <c r="M514" s="13"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15668,7 +15668,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="9"/>
+      <c r="M515" s="13"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15696,7 +15696,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="9">
+      <c r="M516" s="13">
         <v>2</v>
       </c>
     </row>
@@ -15725,7 +15725,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="9"/>
+      <c r="M517" s="13"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15752,7 +15752,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="9"/>
+      <c r="M518" s="13"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15779,7 +15779,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="9"/>
+      <c r="M519" s="13"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15808,7 +15808,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="9"/>
+      <c r="M520" s="13"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15837,7 +15837,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="9"/>
+      <c r="M521" s="13"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15866,7 +15866,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="9"/>
+      <c r="M522" s="13"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15895,7 +15895,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="9"/>
+      <c r="M523" s="13"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15924,7 +15924,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="9"/>
+      <c r="M524" s="13"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -15953,7 +15953,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="9"/>
+      <c r="M525" s="13"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -15980,7 +15980,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="9"/>
+      <c r="M526" s="13"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16007,7 +16007,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="9"/>
+      <c r="M527" s="13"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16032,11 +16032,6 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16053,6 +16048,11 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Feature added: Chart Area -> Area -> Fill -> Bitmap -> Position -> Tile. Feature added: Chart Area -> Area -> Fill -> Bitmap -> Position -> Autofit.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="221">
   <si>
     <t>Chart</t>
   </si>
@@ -671,7 +671,20 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Only bitmap with original size can be properly conversed</t>
+    <t>Always checked because only bitmap with original size can be properly conversed</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1771441 ] Relative size of chart bitmap fill tile.</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1771438 ] Custom size of chart bitmap fill tile.</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1771442 ] Offset length of chart bitmap fill tile.</t>
+  </si>
+  <si>
+    <t>Reverse conversion not perfect due to incompatibilities
+Known Issues: [ 1771500 ] Chart area tiled bitmap fill.</t>
   </si>
 </sst>
 </file>
@@ -815,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -832,6 +845,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1165,10 +1181,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
+      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1178,25 +1194,26 @@
     <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="43.85546875" customWidth="1"/>
+    <col min="11" max="11" width="60.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1237,7 +1254,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1267,7 +1284,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1292,7 +1309,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="12"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1317,7 +1334,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="12"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1342,7 +1359,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="12"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1367,7 +1384,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1392,7 +1409,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="12"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1417,7 +1434,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="12"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1442,7 +1459,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="13"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2063,7 +2080,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="12">
+      <c r="M33" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2095,7 +2112,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="12"/>
+      <c r="M34" s="13"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2360,7 +2377,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="12">
+      <c r="M43" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2392,7 +2409,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="12"/>
+      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2424,7 +2441,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="12"/>
+      <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2456,7 +2473,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="12"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2488,7 +2505,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="12"/>
+      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2520,7 +2537,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="12"/>
+      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2552,7 +2569,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="12"/>
+      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2584,7 +2601,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="12"/>
+      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2773,7 +2790,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="12">
+      <c r="M57" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2802,7 +2819,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="12"/>
+      <c r="M58" s="13"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2829,7 +2846,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="12"/>
+      <c r="M59" s="13"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2856,7 +2873,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="12"/>
+      <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3954,7 +3971,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="12">
+      <c r="M98" s="13">
         <v>2</v>
       </c>
     </row>
@@ -3981,7 +3998,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="12"/>
+      <c r="M99" s="13"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
@@ -4006,7 +4023,7 @@
       <c r="J100" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M100" s="12"/>
+      <c r="M100" s="13"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4031,7 +4048,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="12"/>
+      <c r="M101" s="13"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4058,7 +4075,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="12"/>
+      <c r="M102" s="13"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4085,7 +4102,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="12"/>
+      <c r="M103" s="13"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4114,7 +4131,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="12"/>
+      <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4143,9 +4160,9 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="12"/>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="M105" s="13"/>
+    </row>
+    <row r="106" spans="1:13" ht="30">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -4169,15 +4186,15 @@
       </c>
       <c r="H106" s="1"/>
       <c r="I106" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="K106" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="12"/>
+      <c r="M106" s="13"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4208,7 +4225,10 @@
       <c r="J107" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M107" s="12"/>
+      <c r="K107" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M107" s="13"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4239,7 +4259,10 @@
       <c r="J108" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M108" s="12"/>
+      <c r="K108" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M108" s="13"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4270,7 +4293,10 @@
       <c r="J109" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M109" s="12"/>
+      <c r="K109" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M109" s="13"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4299,7 +4325,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="12"/>
+      <c r="M110" s="13"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4325,12 +4351,15 @@
       </c>
       <c r="H111" s="1"/>
       <c r="I111" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J111" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M111" s="12"/>
+        <v>211</v>
+      </c>
+      <c r="K111" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M111" s="13"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4356,14 +4385,17 @@
       </c>
       <c r="H112" s="1"/>
       <c r="I112" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M112" s="12"/>
-    </row>
-    <row r="113" spans="1:14">
+        <v>211</v>
+      </c>
+      <c r="K112" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M112" s="13"/>
+    </row>
+    <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -4387,12 +4419,15 @@
       </c>
       <c r="H113" s="1"/>
       <c r="I113" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J113" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M113" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="K113" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="M113" s="13"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4418,12 +4453,12 @@
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J114" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M114" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M114" s="13"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4454,7 +4489,7 @@
       <c r="J115" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M115" s="12"/>
+      <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4485,7 +4520,7 @@
       <c r="J116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M116" s="12"/>
+      <c r="M116" s="13"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4510,7 +4545,7 @@
       <c r="J117" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M117" s="12"/>
+      <c r="M117" s="13"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4537,7 +4572,7 @@
       <c r="J118" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M118" s="12"/>
+      <c r="M118" s="13"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4771,7 +4806,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="12">
+      <c r="M127" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4798,7 +4833,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="12"/>
+      <c r="M128" s="13"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4823,7 +4858,7 @@
       <c r="J129" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M129" s="12"/>
+      <c r="M129" s="13"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4848,7 +4883,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="12"/>
+      <c r="M130" s="13"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4873,7 +4908,7 @@
       <c r="J131" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M131" s="12"/>
+      <c r="M131" s="13"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4900,7 +4935,7 @@
       <c r="J132" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M132" s="12"/>
+      <c r="M132" s="13"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4927,7 +4962,7 @@
       <c r="J133" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M133" s="12"/>
+      <c r="M133" s="13"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -4956,7 +4991,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="12"/>
+      <c r="M134" s="13"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -4985,7 +5020,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="12"/>
+      <c r="M135" s="13"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5016,7 +5051,7 @@
       <c r="J136" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M136" s="12"/>
+      <c r="M136" s="13"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5047,7 +5082,7 @@
       <c r="J137" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M137" s="12"/>
+      <c r="M137" s="13"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5078,7 +5113,7 @@
       <c r="J138" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M138" s="12"/>
+      <c r="M138" s="13"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5109,7 +5144,7 @@
       <c r="J139" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M139" s="12"/>
+      <c r="M139" s="13"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5138,7 +5173,7 @@
       <c r="J140" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M140" s="12"/>
+      <c r="M140" s="13"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5169,7 +5204,7 @@
       <c r="J141" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M141" s="12"/>
+      <c r="M141" s="13"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5200,7 +5235,7 @@
       <c r="J142" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M142" s="12"/>
+      <c r="M142" s="13"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5231,7 +5266,7 @@
       <c r="J143" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M143" s="12"/>
+      <c r="M143" s="13"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5262,7 +5297,7 @@
       <c r="J144" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M144" s="12"/>
+      <c r="M144" s="13"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5293,7 +5328,7 @@
       <c r="J145" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M145" s="12"/>
+      <c r="M145" s="13"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5324,7 +5359,7 @@
       <c r="J146" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M146" s="12"/>
+      <c r="M146" s="13"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5349,7 +5384,7 @@
       <c r="J147" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M147" s="12"/>
+      <c r="M147" s="13"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5374,7 +5409,7 @@
       <c r="J148" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M148" s="12"/>
+      <c r="M148" s="13"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5401,7 +5436,7 @@
       <c r="J149" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M149" s="12"/>
+      <c r="M149" s="13"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5428,7 +5463,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="12"/>
+      <c r="M150" s="13"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5455,7 +5490,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="12"/>
+      <c r="M151" s="13"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5482,7 +5517,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="12"/>
+      <c r="M152" s="13"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5509,7 +5544,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="12"/>
+      <c r="M153" s="13"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5536,7 +5571,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="12"/>
+      <c r="M154" s="13"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5563,7 +5598,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="12"/>
+      <c r="M155" s="13"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5590,7 +5625,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="12"/>
+      <c r="M156" s="13"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5615,7 +5650,7 @@
       <c r="J157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M157" s="12"/>
+      <c r="M157" s="13"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5642,7 +5677,7 @@
       <c r="J158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M158" s="12"/>
+      <c r="M158" s="13"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5669,7 +5704,7 @@
       <c r="J159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M159" s="12"/>
+      <c r="M159" s="13"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5696,7 +5731,7 @@
       <c r="J160" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M160" s="12"/>
+      <c r="M160" s="13"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5723,7 +5758,7 @@
       <c r="J161" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M161" s="12"/>
+      <c r="M161" s="13"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5750,7 +5785,7 @@
       <c r="J162" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M162" s="12"/>
+      <c r="M162" s="13"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5777,7 +5812,7 @@
       <c r="J163" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M163" s="12"/>
+      <c r="M163" s="13"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5804,7 +5839,7 @@
       <c r="J164" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M164" s="12"/>
+      <c r="M164" s="13"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5834,7 +5869,7 @@
       <c r="J165" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M165" s="12">
+      <c r="M165" s="13">
         <v>1</v>
       </c>
     </row>
@@ -5863,7 +5898,7 @@
       <c r="J166" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M166" s="12"/>
+      <c r="M166" s="13"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5890,7 +5925,7 @@
       <c r="J167" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M167" s="12"/>
+      <c r="M167" s="13"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5917,7 +5952,7 @@
       <c r="J168" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M168" s="12"/>
+      <c r="M168" s="13"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -5944,7 +5979,7 @@
       <c r="J169" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M169" s="12"/>
+      <c r="M169" s="13"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -5971,7 +6006,7 @@
       <c r="J170" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M170" s="12"/>
+      <c r="M170" s="13"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6000,7 +6035,7 @@
       <c r="J171" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="12"/>
+      <c r="M171" s="13"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6029,7 +6064,7 @@
       <c r="J172" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M172" s="12"/>
+      <c r="M172" s="13"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6060,7 +6095,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="12"/>
+      <c r="M173" s="13"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6091,7 +6126,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="12"/>
+      <c r="M174" s="13"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6124,7 +6159,7 @@
       <c r="J175" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M175" s="12"/>
+      <c r="M175" s="13"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6157,7 +6192,7 @@
       <c r="J176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M176" s="12"/>
+      <c r="M176" s="13"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6190,7 +6225,7 @@
       <c r="J177" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M177" s="12"/>
+      <c r="M177" s="13"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6223,7 +6258,7 @@
       <c r="J178" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M178" s="12"/>
+      <c r="M178" s="13"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6254,7 +6289,7 @@
       <c r="J179" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M179" s="12"/>
+      <c r="M179" s="13"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6287,7 +6322,7 @@
       <c r="J180" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M180" s="12"/>
+      <c r="M180" s="13"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6320,7 +6355,7 @@
       <c r="J181" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M181" s="12"/>
+      <c r="M181" s="13"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6353,7 +6388,7 @@
       <c r="J182" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M182" s="12"/>
+      <c r="M182" s="13"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6386,7 +6421,7 @@
       <c r="J183" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M183" s="12"/>
+      <c r="M183" s="13"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6419,7 +6454,7 @@
       <c r="J184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M184" s="12"/>
+      <c r="M184" s="13"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6452,7 +6487,7 @@
       <c r="J185" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M185" s="12"/>
+      <c r="M185" s="13"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6479,7 +6514,7 @@
       <c r="J186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M186" s="12"/>
+      <c r="M186" s="13"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6506,7 +6541,7 @@
       <c r="J187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M187" s="12"/>
+      <c r="M187" s="13"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6535,7 +6570,7 @@
       <c r="J188" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M188" s="12"/>
+      <c r="M188" s="13"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6758,7 +6793,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="12">
+      <c r="M196" s="13">
         <v>2</v>
       </c>
     </row>
@@ -6787,7 +6822,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="12"/>
+      <c r="M197" s="13"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6814,7 +6849,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="12"/>
+      <c r="M198" s="13"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6841,7 +6876,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="12"/>
+      <c r="M199" s="13"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6868,7 +6903,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="12"/>
+      <c r="M200" s="13"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6897,7 +6932,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="12"/>
+      <c r="M201" s="13"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6924,7 +6959,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="12"/>
+      <c r="M202" s="13"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -6953,7 +6988,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="12"/>
+      <c r="M203" s="13"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -6980,7 +7015,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="12"/>
+      <c r="M204" s="13"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7007,7 +7042,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="12"/>
+      <c r="M205" s="13"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7034,7 +7069,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="12"/>
+      <c r="M206" s="13"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7061,7 +7096,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="12"/>
+      <c r="M207" s="13"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7088,7 +7123,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="12"/>
+      <c r="M208" s="13"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7115,7 +7150,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="12"/>
+      <c r="M209" s="13"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7145,7 +7180,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="12">
+      <c r="M210" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -7176,7 +7211,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="12"/>
+      <c r="M211" s="13"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7205,7 +7240,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="12"/>
+      <c r="M212" s="13"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7234,7 +7269,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="12"/>
+      <c r="M213" s="13"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7263,7 +7298,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="12"/>
+      <c r="M214" s="13"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7292,7 +7327,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="12"/>
+      <c r="M215" s="13"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7321,7 +7356,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="12"/>
+      <c r="M216" s="13"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7350,7 +7385,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="12"/>
+      <c r="M217" s="13"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7379,7 +7414,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="12"/>
+      <c r="M218" s="13"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7408,7 +7443,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="12"/>
+      <c r="M219" s="13"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7435,7 +7470,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="12">
+      <c r="M220" s="13">
         <v>1</v>
       </c>
     </row>
@@ -7464,7 +7499,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="12"/>
+      <c r="M221" s="13"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7491,7 +7526,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="12"/>
+      <c r="M222" s="13"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7518,7 +7553,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="12"/>
+      <c r="M223" s="13"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7545,7 +7580,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="12"/>
+      <c r="M224" s="13"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7572,7 +7607,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="12"/>
+      <c r="M225" s="13"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7601,7 +7636,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="12"/>
+      <c r="M226" s="13"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7630,7 +7665,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="12"/>
+      <c r="M227" s="13"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7661,7 +7696,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="12"/>
+      <c r="M228" s="13"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7692,7 +7727,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="12"/>
+      <c r="M229" s="13"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7725,7 +7760,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="12"/>
+      <c r="M230" s="13"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7758,7 +7793,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="12"/>
+      <c r="M231" s="13"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7791,7 +7826,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="12"/>
+      <c r="M232" s="13"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7824,7 +7859,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="12"/>
+      <c r="M233" s="13"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7855,7 +7890,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="12"/>
+      <c r="M234" s="13"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7888,7 +7923,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="12"/>
+      <c r="M235" s="13"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7921,7 +7956,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="12"/>
+      <c r="M236" s="13"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -7954,7 +7989,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="12"/>
+      <c r="M237" s="13"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -7987,7 +8022,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="12"/>
+      <c r="M238" s="13"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8020,7 +8055,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="12"/>
+      <c r="M239" s="13"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8053,7 +8088,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="12"/>
+      <c r="M240" s="13"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8080,7 +8115,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="12"/>
+      <c r="M241" s="13"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8107,7 +8142,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="12"/>
+      <c r="M242" s="13"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8136,7 +8171,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="12"/>
+      <c r="M243" s="13"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8165,7 +8200,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="12"/>
+      <c r="M244" s="13"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8194,7 +8229,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="12"/>
+      <c r="M245" s="13"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8223,7 +8258,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="12"/>
+      <c r="M246" s="13"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8252,7 +8287,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="12"/>
+      <c r="M247" s="13"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8281,7 +8316,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="12"/>
+      <c r="M248" s="13"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8310,7 +8345,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="12"/>
+      <c r="M249" s="13"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8339,7 +8374,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="12"/>
+      <c r="M250" s="13"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8366,7 +8401,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="12"/>
+      <c r="M251" s="13"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8393,7 +8428,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="12"/>
+      <c r="M252" s="13"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8420,7 +8455,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="12"/>
+      <c r="M253" s="13"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8447,7 +8482,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="12"/>
+      <c r="M254" s="13"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8474,7 +8509,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="12"/>
+      <c r="M255" s="13"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8501,7 +8536,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="12"/>
+      <c r="M256" s="13"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8528,7 +8563,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="12"/>
+      <c r="M257" s="13"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8557,7 +8592,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="12"/>
+      <c r="M258" s="13"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8584,7 +8619,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="12"/>
+      <c r="M259" s="13"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8613,7 +8648,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="12"/>
+      <c r="M260" s="13"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8640,7 +8675,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="12"/>
+      <c r="M261" s="13"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8667,7 +8702,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="12"/>
+      <c r="M262" s="13"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8694,7 +8729,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="12"/>
+      <c r="M263" s="13"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8721,7 +8756,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="12"/>
+      <c r="M264" s="13"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8748,7 +8783,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="12"/>
+      <c r="M265" s="13"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8775,7 +8810,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="12"/>
+      <c r="M266" s="13"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8802,7 +8837,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="12"/>
+      <c r="M267" s="13"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8829,7 +8864,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="12"/>
+      <c r="M268" s="13"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8858,7 +8893,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="12"/>
+      <c r="M269" s="13"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8887,7 +8922,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="12"/>
+      <c r="M270" s="13"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8916,7 +8951,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="12"/>
+      <c r="M271" s="13"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -8945,7 +8980,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="12"/>
+      <c r="M272" s="13"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -8974,7 +9009,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="12"/>
+      <c r="M273" s="13"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9003,7 +9038,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="12"/>
+      <c r="M274" s="13"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9032,7 +9067,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="12"/>
+      <c r="M275" s="13"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9061,7 +9096,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="12"/>
+      <c r="M276" s="13"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9090,7 +9125,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="12"/>
+      <c r="M277" s="13"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9117,7 +9152,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="12"/>
+      <c r="M278" s="13"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9144,7 +9179,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="12"/>
+      <c r="M279" s="13"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9171,7 +9206,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="12"/>
+      <c r="M280" s="13"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9198,7 +9233,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="12"/>
+      <c r="M281" s="13"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9225,7 +9260,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="12"/>
+      <c r="M282" s="13"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9252,7 +9287,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="12"/>
+      <c r="M283" s="13"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9281,7 +9316,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="12"/>
+      <c r="M284" s="13"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9310,7 +9345,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="12"/>
+      <c r="M285" s="13"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9341,7 +9376,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="12"/>
+      <c r="M286" s="13"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9372,7 +9407,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="12"/>
+      <c r="M287" s="13"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9405,7 +9440,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="12"/>
+      <c r="M288" s="13"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9438,7 +9473,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="12"/>
+      <c r="M289" s="13"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9471,7 +9506,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="12"/>
+      <c r="M290" s="13"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9504,7 +9539,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="12"/>
+      <c r="M291" s="13"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9535,7 +9570,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="12"/>
+      <c r="M292" s="13"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9568,7 +9603,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="12"/>
+      <c r="M293" s="13"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9601,7 +9636,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="12"/>
+      <c r="M294" s="13"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9634,7 +9669,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="12"/>
+      <c r="M295" s="13"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9667,7 +9702,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="12"/>
+      <c r="M296" s="13"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9700,7 +9735,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="12"/>
+      <c r="M297" s="13"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9733,7 +9768,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="12"/>
+      <c r="M298" s="13"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9760,7 +9795,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="12"/>
+      <c r="M299" s="13"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9787,7 +9822,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="12"/>
+      <c r="M300" s="13"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9816,7 +9851,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="12"/>
+      <c r="M301" s="13"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9845,7 +9880,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="12"/>
+      <c r="M302" s="13"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9874,7 +9909,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="12"/>
+      <c r="M303" s="13"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9903,7 +9938,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="12"/>
+      <c r="M304" s="13"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -9932,7 +9967,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="12"/>
+      <c r="M305" s="13"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -9961,7 +9996,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="12"/>
+      <c r="M306" s="13"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -9990,7 +10025,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="12"/>
+      <c r="M307" s="13"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10019,7 +10054,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="12"/>
+      <c r="M308" s="13"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10046,7 +10081,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="12"/>
+      <c r="M309" s="13"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10073,7 +10108,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="12"/>
+      <c r="M310" s="13"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10100,7 +10135,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="12"/>
+      <c r="M311" s="13"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10127,7 +10162,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="12"/>
+      <c r="M312" s="13"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10154,7 +10189,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="12"/>
+      <c r="M313" s="13"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10181,7 +10216,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="12"/>
+      <c r="M314" s="13"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10208,7 +10243,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="12"/>
+      <c r="M315" s="13"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10237,7 +10272,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="12"/>
+      <c r="M316" s="13"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10264,7 +10299,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="12"/>
+      <c r="M317" s="13"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10293,7 +10328,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="12"/>
+      <c r="M318" s="13"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10320,7 +10355,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="12"/>
+      <c r="M319" s="13"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10347,7 +10382,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="12"/>
+      <c r="M320" s="13"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10374,7 +10409,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="12"/>
+      <c r="M321" s="13"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10401,7 +10436,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="12"/>
+      <c r="M322" s="13"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10428,7 +10463,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="12"/>
+      <c r="M323" s="13"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10455,7 +10490,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="12"/>
+      <c r="M324" s="13"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10482,7 +10517,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="12"/>
+      <c r="M325" s="13"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10509,7 +10544,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="12"/>
+      <c r="M326" s="13"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10538,7 +10573,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="12"/>
+      <c r="M327" s="13"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10567,7 +10602,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="12"/>
+      <c r="M328" s="13"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10596,7 +10631,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="12"/>
+      <c r="M329" s="13"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10625,7 +10660,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="12"/>
+      <c r="M330" s="13"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10654,7 +10689,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="12"/>
+      <c r="M331" s="13"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10683,7 +10718,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="12"/>
+      <c r="M332" s="13"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10712,7 +10747,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="12"/>
+      <c r="M333" s="13"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10741,7 +10776,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="12"/>
+      <c r="M334" s="13"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10770,7 +10805,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="12"/>
+      <c r="M335" s="13"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -10945,7 +10980,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="12">
+      <c r="M342" s="13">
         <v>1</v>
       </c>
     </row>
@@ -10972,7 +11007,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="12"/>
+      <c r="M343" s="13"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -10997,7 +11032,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="12"/>
+      <c r="M344" s="13"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11022,7 +11057,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="12"/>
+      <c r="M345" s="13"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11047,7 +11082,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="12"/>
+      <c r="M346" s="13"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11072,7 +11107,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="12"/>
+      <c r="M347" s="13"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11099,7 +11134,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="12"/>
+      <c r="M348" s="13"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11126,7 +11161,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="12"/>
+      <c r="M349" s="13"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11155,7 +11190,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="12"/>
+      <c r="M350" s="13"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11184,7 +11219,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="12"/>
+      <c r="M351" s="13"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11215,7 +11250,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="12"/>
+      <c r="M352" s="13"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11246,7 +11281,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="12"/>
+      <c r="M353" s="13"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11277,7 +11312,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="12"/>
+      <c r="M354" s="13"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11308,7 +11343,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="12"/>
+      <c r="M355" s="13"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11337,7 +11372,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="12"/>
+      <c r="M356" s="13"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11368,7 +11403,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="12"/>
+      <c r="M357" s="13"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11399,7 +11434,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="12"/>
+      <c r="M358" s="13"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11430,7 +11465,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="12"/>
+      <c r="M359" s="13"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11461,7 +11496,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="12"/>
+      <c r="M360" s="13"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11492,7 +11527,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="12"/>
+      <c r="M361" s="13"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11523,7 +11558,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="12"/>
+      <c r="M362" s="13"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11548,7 +11583,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="12"/>
+      <c r="M363" s="13"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11573,7 +11608,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="12"/>
+      <c r="M364" s="13"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11600,7 +11635,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="12"/>
+      <c r="M365" s="13"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11627,7 +11662,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="12"/>
+      <c r="M366" s="13"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11654,7 +11689,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="12"/>
+      <c r="M367" s="13"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11681,7 +11716,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="12"/>
+      <c r="M368" s="13"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11708,7 +11743,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="12"/>
+      <c r="M369" s="13"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11735,7 +11770,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="12"/>
+      <c r="M370" s="13"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11762,7 +11797,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="12"/>
+      <c r="M371" s="13"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11789,7 +11824,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="12"/>
+      <c r="M372" s="13"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11814,7 +11849,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="12"/>
+      <c r="M373" s="13"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11839,7 +11874,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="12"/>
+      <c r="M374" s="13"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11864,7 +11899,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="12"/>
+      <c r="M375" s="13"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11889,7 +11924,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="12"/>
+      <c r="M376" s="13"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11914,7 +11949,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="12"/>
+      <c r="M377" s="13"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -11939,7 +11974,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="12"/>
+      <c r="M378" s="13"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -11964,7 +11999,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="12"/>
+      <c r="M379" s="13"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -11991,7 +12026,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="12"/>
+      <c r="M380" s="13"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12016,7 +12051,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="12"/>
+      <c r="M381" s="13"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12043,7 +12078,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="12"/>
+      <c r="M382" s="13"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12068,7 +12103,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="12"/>
+      <c r="M383" s="13"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12093,7 +12128,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="12"/>
+      <c r="M384" s="13"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12118,7 +12153,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="12"/>
+      <c r="M385" s="13"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12143,7 +12178,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="12"/>
+      <c r="M386" s="13"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12216,7 +12251,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="12">
+      <c r="M389" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -12245,7 +12280,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="12"/>
+      <c r="M390" s="13"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12272,7 +12307,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="12"/>
+      <c r="M391" s="13"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12299,7 +12334,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="12"/>
+      <c r="M392" s="13"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12326,7 +12361,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="12"/>
+      <c r="M393" s="13"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12353,7 +12388,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="12"/>
+      <c r="M394" s="13"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12380,7 +12415,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="12"/>
+      <c r="M395" s="13"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12410,7 +12445,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="12">
+      <c r="M396" s="13">
         <v>1</v>
       </c>
     </row>
@@ -12439,7 +12474,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="12"/>
+      <c r="M397" s="13"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12466,7 +12501,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="12"/>
+      <c r="M398" s="13"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12493,7 +12528,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="12"/>
+      <c r="M399" s="13"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12520,7 +12555,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="12"/>
+      <c r="M400" s="13"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12547,7 +12582,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="12"/>
+      <c r="M401" s="13"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12574,7 +12609,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="12"/>
+      <c r="M402" s="13"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12601,7 +12636,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="12"/>
+      <c r="M403" s="13"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12628,7 +12663,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="12"/>
+      <c r="M404" s="13"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12655,7 +12690,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="12"/>
+      <c r="M405" s="13"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12682,7 +12717,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="12"/>
+      <c r="M406" s="13"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12709,7 +12744,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="12"/>
+      <c r="M407" s="13"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12738,7 +12773,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="12"/>
+      <c r="M408" s="13"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12765,7 +12800,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="12"/>
+      <c r="M409" s="13"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12794,7 +12829,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="12"/>
+      <c r="M410" s="13"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12821,7 +12856,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="12"/>
+      <c r="M411" s="13"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12848,7 +12883,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="12"/>
+      <c r="M412" s="13"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12875,7 +12910,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="12"/>
+      <c r="M413" s="13"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12902,7 +12937,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="12"/>
+      <c r="M414" s="13"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -12932,7 +12967,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="12">
+      <c r="M415" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -12961,7 +12996,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="12"/>
+      <c r="M416" s="13"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -12990,7 +13025,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="12"/>
+      <c r="M417" s="13"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13019,7 +13054,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="12"/>
+      <c r="M418" s="13"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13048,7 +13083,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="12"/>
+      <c r="M419" s="13"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13077,7 +13112,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="12"/>
+      <c r="M420" s="13"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13107,7 +13142,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="12">
+      <c r="M421" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13136,7 +13171,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="12"/>
+      <c r="M422" s="13"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13163,7 +13198,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="12"/>
+      <c r="M423" s="13"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13190,7 +13225,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="12"/>
+      <c r="M424" s="13"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13217,7 +13252,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="12"/>
+      <c r="M425" s="13"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13244,7 +13279,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="12"/>
+      <c r="M426" s="13"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13271,7 +13306,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="12"/>
+      <c r="M427" s="13"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13298,7 +13333,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="12"/>
+      <c r="M428" s="13"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13325,7 +13360,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="12"/>
+      <c r="M429" s="13"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13352,7 +13387,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="12"/>
+      <c r="M430" s="13"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13379,7 +13414,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="12"/>
+      <c r="M431" s="13"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13406,7 +13441,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="12"/>
+      <c r="M432" s="13"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13435,7 +13470,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="12"/>
+      <c r="M433" s="13"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13462,7 +13497,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="12"/>
+      <c r="M434" s="13"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13491,7 +13526,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="12"/>
+      <c r="M435" s="13"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13518,7 +13553,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="12"/>
+      <c r="M436" s="13"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13545,7 +13580,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="12"/>
+      <c r="M437" s="13"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13572,7 +13607,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="12"/>
+      <c r="M438" s="13"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13599,7 +13634,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="12"/>
+      <c r="M439" s="13"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13633,7 +13668,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="12">
+      <c r="M440" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13666,7 +13701,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="12"/>
+      <c r="M441" s="13"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13697,7 +13732,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="12"/>
+      <c r="M442" s="13"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13728,7 +13763,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="12"/>
+      <c r="M443" s="13"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13759,7 +13794,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="12"/>
+      <c r="M444" s="13"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13790,7 +13825,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="12"/>
+      <c r="M445" s="13"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13821,7 +13856,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="12"/>
+      <c r="M446" s="13"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13852,7 +13887,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="12"/>
+      <c r="M447" s="13"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13883,7 +13918,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="12"/>
+      <c r="M448" s="13"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13914,7 +13949,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="12"/>
+      <c r="M449" s="13"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -13943,7 +13978,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="12"/>
+      <c r="M450" s="13"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -13972,7 +14007,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="12"/>
+      <c r="M451" s="13"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14001,7 +14036,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="12"/>
+      <c r="M452" s="13"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14030,7 +14065,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="12"/>
+      <c r="M453" s="13"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14059,7 +14094,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="12"/>
+      <c r="M454" s="13"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14086,7 +14121,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="12"/>
+      <c r="M455" s="13"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14113,7 +14148,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="12"/>
+      <c r="M456" s="13"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14140,7 +14175,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="12"/>
+      <c r="M457" s="13"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14169,7 +14204,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="12"/>
+      <c r="M458" s="13"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14198,7 +14233,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="12"/>
+      <c r="M459" s="13"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14227,7 +14262,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="12"/>
+      <c r="M460" s="13"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14256,7 +14291,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="12"/>
+      <c r="M461" s="13"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14590,7 +14625,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="13">
+      <c r="M474" s="14">
         <v>1</v>
       </c>
     </row>
@@ -14619,7 +14654,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="13"/>
+      <c r="M475" s="14"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14646,7 +14681,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="13"/>
+      <c r="M476" s="14"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14673,7 +14708,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="13"/>
+      <c r="M477" s="14"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14700,7 +14735,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="13"/>
+      <c r="M478" s="14"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14727,7 +14762,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="13"/>
+      <c r="M479" s="14"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14754,7 +14789,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="13"/>
+      <c r="M480" s="14"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14781,7 +14816,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="13"/>
+      <c r="M481" s="14"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14808,7 +14843,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="13"/>
+      <c r="M482" s="14"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14835,7 +14870,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="13"/>
+      <c r="M483" s="14"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -14995,7 +15030,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="13">
+      <c r="M489" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15022,7 +15057,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="13"/>
+      <c r="M490" s="14"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15047,7 +15082,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="13"/>
+      <c r="M491" s="14"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15072,7 +15107,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="13"/>
+      <c r="M492" s="14"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15097,7 +15132,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="13"/>
+      <c r="M493" s="14"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15124,7 +15159,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="13"/>
+      <c r="M494" s="14"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15151,7 +15186,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="13"/>
+      <c r="M495" s="14"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15178,7 +15213,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="13"/>
+      <c r="M496" s="14"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15205,7 +15240,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="13"/>
+      <c r="M497" s="14"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15258,7 +15293,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="13">
+      <c r="M499" s="14">
         <v>1</v>
       </c>
     </row>
@@ -15285,7 +15320,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="13"/>
+      <c r="M500" s="14"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15310,7 +15345,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="13"/>
+      <c r="M501" s="14"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15335,7 +15370,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="13"/>
+      <c r="M502" s="14"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15360,7 +15395,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="13"/>
+      <c r="M503" s="14"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15385,7 +15420,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="13"/>
+      <c r="M504" s="14"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15412,7 +15447,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="13"/>
+      <c r="M505" s="14"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15437,7 +15472,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="13"/>
+      <c r="M506" s="14"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15464,7 +15499,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="13"/>
+      <c r="M507" s="14"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15489,7 +15524,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="13"/>
+      <c r="M508" s="14"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15514,7 +15549,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="13"/>
+      <c r="M509" s="14"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15539,7 +15574,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="13"/>
+      <c r="M510" s="14"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15564,7 +15599,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="13"/>
+      <c r="M511" s="14"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15591,7 +15626,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="13"/>
+      <c r="M512" s="14"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15618,7 +15653,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="13"/>
+      <c r="M513" s="14"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15643,7 +15678,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="13"/>
+      <c r="M514" s="14"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15668,7 +15703,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="13"/>
+      <c r="M515" s="14"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15696,7 +15731,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="13">
+      <c r="M516" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15725,7 +15760,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="13"/>
+      <c r="M517" s="14"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15752,7 +15787,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="13"/>
+      <c r="M518" s="14"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15779,7 +15814,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="13"/>
+      <c r="M519" s="14"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15808,7 +15843,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="13"/>
+      <c r="M520" s="14"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15837,7 +15872,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="13"/>
+      <c r="M521" s="14"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15866,7 +15901,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="13"/>
+      <c r="M522" s="14"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15895,7 +15930,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="13"/>
+      <c r="M523" s="14"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15924,7 +15959,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="13"/>
+      <c r="M524" s="14"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -15953,7 +15988,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="13"/>
+      <c r="M525" s="14"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -15980,7 +16015,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="13"/>
+      <c r="M526" s="14"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16007,7 +16042,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="13"/>
+      <c r="M527" s="14"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">

</xml_diff>

<commit_message>
Added feature: Chart Area -> Transparency
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -1181,10 +1181,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
+      <selection pane="bottomLeft" activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4484,10 +4484,10 @@
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J115" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M115" s="13"/>
     </row>
@@ -4515,10 +4515,10 @@
       </c>
       <c r="H116" s="1"/>
       <c r="I116" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J116" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M116" s="13"/>
     </row>
@@ -4540,10 +4540,10 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
       <c r="I117" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M117" s="13"/>
     </row>
@@ -4567,10 +4567,10 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
       <c r="I118" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J118" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M118" s="13"/>
       <c r="N118">

</xml_diff>

<commit_message>
Added feature: Chart Wall -> Lines. Added feature: Chart Wall -> Area.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="223">
   <si>
     <t>Chart</t>
   </si>
@@ -684,7 +684,14 @@
   </si>
   <si>
     <t>Reverse conversion not perfect due to incompatibilities
-Known Issues: [ 1771500 ] Chart area tiled bitmap fill.</t>
+Known Issues: [ 1771500 ] Chart objects bitmap tile and border width display.</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1772876 ] Border width for chart area
+Known Issues: [ 1771500 ] Chart objects bitmap tile and border width display.</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1771500 ]Chart objects bitmap tile and border width display.</t>
   </si>
 </sst>
 </file>
@@ -828,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -846,6 +853,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1181,10 +1191,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K117" sqref="K117"/>
+      <selection pane="bottomLeft" activeCell="K143" sqref="K143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,22 +1208,22 @@
     <col min="8" max="8" width="14.140625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="60.28515625" customWidth="1"/>
+    <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.140625" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1254,7 +1264,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1284,7 +1294,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1309,7 +1319,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1334,7 +1344,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1359,7 +1369,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1384,7 +1394,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1409,7 +1419,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1434,7 +1444,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1459,7 +1469,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="13"/>
+      <c r="M10" s="14"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2080,7 +2090,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2112,7 +2122,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="13"/>
+      <c r="M34" s="14"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2377,7 +2387,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="13">
+      <c r="M43" s="14">
         <v>2</v>
       </c>
     </row>
@@ -2409,7 +2419,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="13"/>
+      <c r="M44" s="14"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2441,7 +2451,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="13"/>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2473,7 +2483,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="13"/>
+      <c r="M46" s="14"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2505,7 +2515,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="13"/>
+      <c r="M47" s="14"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2537,7 +2547,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="13"/>
+      <c r="M48" s="14"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2569,7 +2579,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="13"/>
+      <c r="M49" s="14"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2601,7 +2611,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="13"/>
+      <c r="M50" s="14"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2790,7 +2800,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="13">
+      <c r="M57" s="14">
         <v>3</v>
       </c>
     </row>
@@ -2819,7 +2829,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="13"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2846,7 +2856,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="13"/>
+      <c r="M59" s="14"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2873,7 +2883,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="13"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3971,7 +3981,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="13">
+      <c r="M98" s="14">
         <v>2</v>
       </c>
     </row>
@@ -3998,9 +4008,9 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="13"/>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="M99" s="14"/>
+    </row>
+    <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +4033,10 @@
       <c r="J100" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M100" s="13"/>
+      <c r="K100" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4048,7 +4061,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="13"/>
+      <c r="M101" s="14"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4075,7 +4088,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="13"/>
+      <c r="M102" s="14"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4102,7 +4115,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="13"/>
+      <c r="M103" s="14"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4131,7 +4144,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="13"/>
+      <c r="M104" s="14"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4160,9 +4173,9 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="13"/>
-    </row>
-    <row r="106" spans="1:13" ht="30">
+      <c r="M105" s="14"/>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -4194,7 +4207,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="13"/>
+      <c r="M106" s="14"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4228,7 +4241,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="13"/>
+      <c r="M107" s="14"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4262,7 +4275,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="13"/>
+      <c r="M108" s="14"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4296,7 +4309,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="13"/>
+      <c r="M109" s="14"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4325,7 +4338,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="13"/>
+      <c r="M110" s="14"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4359,7 +4372,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="13"/>
+      <c r="M111" s="14"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4393,7 +4406,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="13"/>
+      <c r="M112" s="14"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4427,7 +4440,7 @@
       <c r="K113" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="M113" s="13"/>
+      <c r="M113" s="14"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4458,7 +4471,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="13"/>
+      <c r="M114" s="14"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4489,7 +4502,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="13"/>
+      <c r="M115" s="14"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4520,7 +4533,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="13"/>
+      <c r="M116" s="14"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4545,7 +4558,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="13"/>
+      <c r="M117" s="14"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4572,7 +4585,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="13"/>
+      <c r="M118" s="14"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4806,7 +4819,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="13">
+      <c r="M127" s="14">
         <v>1</v>
       </c>
     </row>
@@ -4833,7 +4846,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="13"/>
+      <c r="M128" s="14"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4858,7 +4871,10 @@
       <c r="J129" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M129" s="13"/>
+      <c r="K129" t="s">
+        <v>222</v>
+      </c>
+      <c r="M129" s="14"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4883,7 +4899,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="13"/>
+      <c r="M130" s="14"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4903,12 +4919,12 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
       <c r="I131" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J131" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M131" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M131" s="14"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4930,12 +4946,12 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
       <c r="I132" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J132" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M132" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M132" s="14"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4957,12 +4973,12 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
       <c r="I133" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J133" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M133" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M133" s="14"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -4991,7 +5007,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="13"/>
+      <c r="M134" s="14"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5020,7 +5036,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="13"/>
+      <c r="M135" s="14"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5046,12 +5062,15 @@
       </c>
       <c r="H136" s="1"/>
       <c r="I136" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J136" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M136" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K136" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="M136" s="14"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5077,12 +5096,15 @@
       </c>
       <c r="H137" s="1"/>
       <c r="I137" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J137" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M137" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K137" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M137" s="14"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5108,12 +5130,15 @@
       </c>
       <c r="H138" s="1"/>
       <c r="I138" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J138" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M138" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K138" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M138" s="14"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5139,12 +5164,15 @@
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J139" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M139" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K139" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M139" s="14"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5168,12 +5196,12 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
       <c r="I140" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J140" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M140" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M140" s="14"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5199,12 +5227,15 @@
       </c>
       <c r="H141" s="1"/>
       <c r="I141" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J141" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M141" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K141" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M141" s="14"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5230,12 +5261,15 @@
       </c>
       <c r="H142" s="1"/>
       <c r="I142" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J142" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M142" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K142" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M142" s="14"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5261,12 +5295,13 @@
       </c>
       <c r="H143" s="1"/>
       <c r="I143" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J143" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M143" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K143" s="10"/>
+      <c r="M143" s="14"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5292,12 +5327,12 @@
       </c>
       <c r="H144" s="1"/>
       <c r="I144" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J144" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M144" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M144" s="14"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5323,12 +5358,12 @@
       </c>
       <c r="H145" s="1"/>
       <c r="I145" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J145" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M145" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M145" s="14"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5354,12 +5389,12 @@
       </c>
       <c r="H146" s="1"/>
       <c r="I146" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J146" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M146" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M146" s="14"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5379,12 +5414,12 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
       <c r="I147" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J147" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M147" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M147" s="14"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5404,12 +5439,12 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
       <c r="I148" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J148" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M148" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M148" s="14"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5431,12 +5466,12 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
       <c r="I149" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J149" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M149" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M149" s="14"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5463,7 +5498,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="13"/>
+      <c r="M150" s="14"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5490,7 +5525,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="13"/>
+      <c r="M151" s="14"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5517,7 +5552,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="13"/>
+      <c r="M152" s="14"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5544,7 +5579,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="13"/>
+      <c r="M153" s="14"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5571,7 +5606,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="13"/>
+      <c r="M154" s="14"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5598,7 +5633,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="13"/>
+      <c r="M155" s="14"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5625,7 +5660,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="13"/>
+      <c r="M156" s="14"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5650,7 +5685,7 @@
       <c r="J157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M157" s="13"/>
+      <c r="M157" s="14"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5677,7 +5712,7 @@
       <c r="J158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M158" s="13"/>
+      <c r="M158" s="14"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5704,7 +5739,7 @@
       <c r="J159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M159" s="13"/>
+      <c r="M159" s="14"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5731,7 +5766,7 @@
       <c r="J160" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M160" s="13"/>
+      <c r="M160" s="14"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5758,7 +5793,7 @@
       <c r="J161" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M161" s="13"/>
+      <c r="M161" s="14"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5785,7 +5820,7 @@
       <c r="J162" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M162" s="13"/>
+      <c r="M162" s="14"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5812,7 +5847,7 @@
       <c r="J163" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M163" s="13"/>
+      <c r="M163" s="14"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5839,7 +5874,7 @@
       <c r="J164" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M164" s="13"/>
+      <c r="M164" s="14"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5869,7 +5904,7 @@
       <c r="J165" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M165" s="13">
+      <c r="M165" s="14">
         <v>1</v>
       </c>
     </row>
@@ -5898,7 +5933,7 @@
       <c r="J166" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M166" s="13"/>
+      <c r="M166" s="14"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5925,7 +5960,7 @@
       <c r="J167" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M167" s="13"/>
+      <c r="M167" s="14"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5952,7 +5987,7 @@
       <c r="J168" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M168" s="13"/>
+      <c r="M168" s="14"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -5979,7 +6014,7 @@
       <c r="J169" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M169" s="13"/>
+      <c r="M169" s="14"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6006,7 +6041,7 @@
       <c r="J170" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M170" s="13"/>
+      <c r="M170" s="14"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6035,7 +6070,7 @@
       <c r="J171" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="13"/>
+      <c r="M171" s="14"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6064,7 +6099,7 @@
       <c r="J172" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M172" s="13"/>
+      <c r="M172" s="14"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6095,7 +6130,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="13"/>
+      <c r="M173" s="14"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6126,7 +6161,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="13"/>
+      <c r="M174" s="14"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6159,7 +6194,7 @@
       <c r="J175" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M175" s="13"/>
+      <c r="M175" s="14"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6192,7 +6227,7 @@
       <c r="J176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M176" s="13"/>
+      <c r="M176" s="14"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6225,7 +6260,7 @@
       <c r="J177" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M177" s="13"/>
+      <c r="M177" s="14"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6258,7 +6293,7 @@
       <c r="J178" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M178" s="13"/>
+      <c r="M178" s="14"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6289,7 +6324,7 @@
       <c r="J179" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M179" s="13"/>
+      <c r="M179" s="14"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6322,7 +6357,7 @@
       <c r="J180" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M180" s="13"/>
+      <c r="M180" s="14"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6355,7 +6390,7 @@
       <c r="J181" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M181" s="13"/>
+      <c r="M181" s="14"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6388,7 +6423,7 @@
       <c r="J182" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M182" s="13"/>
+      <c r="M182" s="14"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6421,7 +6456,7 @@
       <c r="J183" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M183" s="13"/>
+      <c r="M183" s="14"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6454,7 +6489,7 @@
       <c r="J184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M184" s="13"/>
+      <c r="M184" s="14"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6487,7 +6522,7 @@
       <c r="J185" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M185" s="13"/>
+      <c r="M185" s="14"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6514,7 +6549,7 @@
       <c r="J186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M186" s="13"/>
+      <c r="M186" s="14"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6541,7 +6576,7 @@
       <c r="J187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M187" s="13"/>
+      <c r="M187" s="14"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6570,7 +6605,7 @@
       <c r="J188" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M188" s="13"/>
+      <c r="M188" s="14"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6793,7 +6828,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="13">
+      <c r="M196" s="14">
         <v>2</v>
       </c>
     </row>
@@ -6822,7 +6857,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="13"/>
+      <c r="M197" s="14"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6849,7 +6884,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="13"/>
+      <c r="M198" s="14"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6876,7 +6911,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="13"/>
+      <c r="M199" s="14"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6903,7 +6938,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="13"/>
+      <c r="M200" s="14"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6932,7 +6967,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="13"/>
+      <c r="M201" s="14"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6959,7 +6994,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="13"/>
+      <c r="M202" s="14"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -6988,7 +7023,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="13"/>
+      <c r="M203" s="14"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7015,7 +7050,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="13"/>
+      <c r="M204" s="14"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7042,7 +7077,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="13"/>
+      <c r="M205" s="14"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7069,7 +7104,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="13"/>
+      <c r="M206" s="14"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7096,7 +7131,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="13"/>
+      <c r="M207" s="14"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7123,7 +7158,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="13"/>
+      <c r="M208" s="14"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7150,7 +7185,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="13"/>
+      <c r="M209" s="14"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7180,7 +7215,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="13">
+      <c r="M210" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -7211,7 +7246,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="13"/>
+      <c r="M211" s="14"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7240,7 +7275,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="13"/>
+      <c r="M212" s="14"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7269,7 +7304,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="13"/>
+      <c r="M213" s="14"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7298,7 +7333,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="13"/>
+      <c r="M214" s="14"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7327,7 +7362,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="13"/>
+      <c r="M215" s="14"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7356,7 +7391,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="13"/>
+      <c r="M216" s="14"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7385,7 +7420,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="13"/>
+      <c r="M217" s="14"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7414,7 +7449,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="13"/>
+      <c r="M218" s="14"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7443,7 +7478,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="13"/>
+      <c r="M219" s="14"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7470,7 +7505,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="13">
+      <c r="M220" s="14">
         <v>1</v>
       </c>
     </row>
@@ -7499,7 +7534,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="13"/>
+      <c r="M221" s="14"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7526,7 +7561,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="13"/>
+      <c r="M222" s="14"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7553,7 +7588,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="13"/>
+      <c r="M223" s="14"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7580,7 +7615,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="13"/>
+      <c r="M224" s="14"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7607,7 +7642,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="13"/>
+      <c r="M225" s="14"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7636,7 +7671,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="13"/>
+      <c r="M226" s="14"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7665,7 +7700,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="13"/>
+      <c r="M227" s="14"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7696,7 +7731,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="13"/>
+      <c r="M228" s="14"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7727,7 +7762,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="13"/>
+      <c r="M229" s="14"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7760,7 +7795,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="13"/>
+      <c r="M230" s="14"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7793,7 +7828,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="13"/>
+      <c r="M231" s="14"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7826,7 +7861,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="13"/>
+      <c r="M232" s="14"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7859,7 +7894,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="13"/>
+      <c r="M233" s="14"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7890,7 +7925,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="13"/>
+      <c r="M234" s="14"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7923,7 +7958,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="13"/>
+      <c r="M235" s="14"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7956,7 +7991,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="13"/>
+      <c r="M236" s="14"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -7989,7 +8024,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="13"/>
+      <c r="M237" s="14"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8022,7 +8057,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="13"/>
+      <c r="M238" s="14"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8055,7 +8090,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="13"/>
+      <c r="M239" s="14"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8088,7 +8123,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="13"/>
+      <c r="M240" s="14"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8115,7 +8150,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="13"/>
+      <c r="M241" s="14"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8142,7 +8177,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="13"/>
+      <c r="M242" s="14"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8171,7 +8206,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="13"/>
+      <c r="M243" s="14"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8200,7 +8235,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="13"/>
+      <c r="M244" s="14"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8229,7 +8264,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="13"/>
+      <c r="M245" s="14"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8258,7 +8293,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="13"/>
+      <c r="M246" s="14"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8287,7 +8322,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="13"/>
+      <c r="M247" s="14"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8316,7 +8351,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="13"/>
+      <c r="M248" s="14"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8345,7 +8380,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="13"/>
+      <c r="M249" s="14"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8374,7 +8409,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="13"/>
+      <c r="M250" s="14"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8401,7 +8436,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="13"/>
+      <c r="M251" s="14"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8428,7 +8463,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="13"/>
+      <c r="M252" s="14"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8455,7 +8490,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="13"/>
+      <c r="M253" s="14"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8482,7 +8517,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="13"/>
+      <c r="M254" s="14"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8509,7 +8544,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="13"/>
+      <c r="M255" s="14"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8536,7 +8571,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="13"/>
+      <c r="M256" s="14"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8563,7 +8598,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="13"/>
+      <c r="M257" s="14"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8592,7 +8627,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="13"/>
+      <c r="M258" s="14"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8619,7 +8654,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="13"/>
+      <c r="M259" s="14"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8648,7 +8683,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="13"/>
+      <c r="M260" s="14"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8675,7 +8710,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="13"/>
+      <c r="M261" s="14"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8702,7 +8737,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="13"/>
+      <c r="M262" s="14"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8729,7 +8764,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="13"/>
+      <c r="M263" s="14"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8756,7 +8791,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="13"/>
+      <c r="M264" s="14"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8783,7 +8818,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="13"/>
+      <c r="M265" s="14"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8810,7 +8845,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="13"/>
+      <c r="M266" s="14"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8837,7 +8872,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="13"/>
+      <c r="M267" s="14"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8864,7 +8899,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="13"/>
+      <c r="M268" s="14"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8893,7 +8928,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="13"/>
+      <c r="M269" s="14"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8922,7 +8957,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="13"/>
+      <c r="M270" s="14"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8951,7 +8986,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="13"/>
+      <c r="M271" s="14"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -8980,7 +9015,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="13"/>
+      <c r="M272" s="14"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9009,7 +9044,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="13"/>
+      <c r="M273" s="14"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9038,7 +9073,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="13"/>
+      <c r="M274" s="14"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9067,7 +9102,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="13"/>
+      <c r="M275" s="14"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9096,7 +9131,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="13"/>
+      <c r="M276" s="14"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9125,7 +9160,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="13"/>
+      <c r="M277" s="14"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9152,7 +9187,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="13"/>
+      <c r="M278" s="14"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9179,7 +9214,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="13"/>
+      <c r="M279" s="14"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9206,7 +9241,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="13"/>
+      <c r="M280" s="14"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9233,7 +9268,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="13"/>
+      <c r="M281" s="14"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9260,7 +9295,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="13"/>
+      <c r="M282" s="14"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9287,7 +9322,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="13"/>
+      <c r="M283" s="14"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9316,7 +9351,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="13"/>
+      <c r="M284" s="14"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9345,7 +9380,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="13"/>
+      <c r="M285" s="14"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9376,7 +9411,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="13"/>
+      <c r="M286" s="14"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9407,7 +9442,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="13"/>
+      <c r="M287" s="14"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9440,7 +9475,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="13"/>
+      <c r="M288" s="14"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9473,7 +9508,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="13"/>
+      <c r="M289" s="14"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9506,7 +9541,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="13"/>
+      <c r="M290" s="14"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9539,7 +9574,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="13"/>
+      <c r="M291" s="14"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9570,7 +9605,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="13"/>
+      <c r="M292" s="14"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9603,7 +9638,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="13"/>
+      <c r="M293" s="14"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9636,7 +9671,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="13"/>
+      <c r="M294" s="14"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9669,7 +9704,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="13"/>
+      <c r="M295" s="14"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9702,7 +9737,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="13"/>
+      <c r="M296" s="14"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9735,7 +9770,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="13"/>
+      <c r="M297" s="14"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9768,7 +9803,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="13"/>
+      <c r="M298" s="14"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9795,7 +9830,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="13"/>
+      <c r="M299" s="14"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9822,7 +9857,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="13"/>
+      <c r="M300" s="14"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9851,7 +9886,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="13"/>
+      <c r="M301" s="14"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9880,7 +9915,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="13"/>
+      <c r="M302" s="14"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9909,7 +9944,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="13"/>
+      <c r="M303" s="14"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9938,7 +9973,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="13"/>
+      <c r="M304" s="14"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -9967,7 +10002,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="13"/>
+      <c r="M305" s="14"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -9996,7 +10031,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="13"/>
+      <c r="M306" s="14"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10025,7 +10060,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="13"/>
+      <c r="M307" s="14"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10054,7 +10089,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="13"/>
+      <c r="M308" s="14"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10081,7 +10116,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="13"/>
+      <c r="M309" s="14"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10108,7 +10143,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="13"/>
+      <c r="M310" s="14"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10135,7 +10170,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="13"/>
+      <c r="M311" s="14"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10162,7 +10197,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="13"/>
+      <c r="M312" s="14"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10189,7 +10224,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="13"/>
+      <c r="M313" s="14"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10216,7 +10251,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="13"/>
+      <c r="M314" s="14"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10243,7 +10278,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="13"/>
+      <c r="M315" s="14"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10272,7 +10307,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="13"/>
+      <c r="M316" s="14"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10299,7 +10334,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="13"/>
+      <c r="M317" s="14"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10328,7 +10363,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="13"/>
+      <c r="M318" s="14"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10355,7 +10390,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="13"/>
+      <c r="M319" s="14"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10382,7 +10417,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="13"/>
+      <c r="M320" s="14"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10409,7 +10444,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="13"/>
+      <c r="M321" s="14"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10436,7 +10471,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="13"/>
+      <c r="M322" s="14"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10463,7 +10498,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="13"/>
+      <c r="M323" s="14"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10490,7 +10525,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="13"/>
+      <c r="M324" s="14"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10517,7 +10552,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="13"/>
+      <c r="M325" s="14"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10544,7 +10579,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="13"/>
+      <c r="M326" s="14"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10573,7 +10608,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="13"/>
+      <c r="M327" s="14"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10602,7 +10637,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="13"/>
+      <c r="M328" s="14"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10631,7 +10666,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="13"/>
+      <c r="M329" s="14"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10660,7 +10695,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="13"/>
+      <c r="M330" s="14"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10689,7 +10724,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="13"/>
+      <c r="M331" s="14"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10718,7 +10753,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="13"/>
+      <c r="M332" s="14"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10747,7 +10782,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="13"/>
+      <c r="M333" s="14"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10776,7 +10811,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="13"/>
+      <c r="M334" s="14"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10805,7 +10840,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="13"/>
+      <c r="M335" s="14"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -10980,7 +11015,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="13">
+      <c r="M342" s="14">
         <v>1</v>
       </c>
     </row>
@@ -11007,7 +11042,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="13"/>
+      <c r="M343" s="14"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11032,7 +11067,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="13"/>
+      <c r="M344" s="14"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11057,7 +11092,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="13"/>
+      <c r="M345" s="14"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11082,7 +11117,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="13"/>
+      <c r="M346" s="14"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11107,7 +11142,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="13"/>
+      <c r="M347" s="14"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11134,7 +11169,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="13"/>
+      <c r="M348" s="14"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11161,7 +11196,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="13"/>
+      <c r="M349" s="14"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11190,7 +11225,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="13"/>
+      <c r="M350" s="14"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11219,7 +11254,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="13"/>
+      <c r="M351" s="14"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11250,7 +11285,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="13"/>
+      <c r="M352" s="14"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11281,7 +11316,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="13"/>
+      <c r="M353" s="14"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11312,7 +11347,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="13"/>
+      <c r="M354" s="14"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11343,7 +11378,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="13"/>
+      <c r="M355" s="14"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11372,7 +11407,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="13"/>
+      <c r="M356" s="14"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11403,7 +11438,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="13"/>
+      <c r="M357" s="14"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11434,7 +11469,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="13"/>
+      <c r="M358" s="14"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11465,7 +11500,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="13"/>
+      <c r="M359" s="14"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11496,7 +11531,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="13"/>
+      <c r="M360" s="14"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11527,7 +11562,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="13"/>
+      <c r="M361" s="14"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11558,7 +11593,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="13"/>
+      <c r="M362" s="14"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11583,7 +11618,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="13"/>
+      <c r="M363" s="14"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11608,7 +11643,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="13"/>
+      <c r="M364" s="14"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11635,7 +11670,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="13"/>
+      <c r="M365" s="14"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11662,7 +11697,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="13"/>
+      <c r="M366" s="14"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11689,7 +11724,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="13"/>
+      <c r="M367" s="14"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11716,7 +11751,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="13"/>
+      <c r="M368" s="14"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11743,7 +11778,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="13"/>
+      <c r="M369" s="14"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11770,7 +11805,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="13"/>
+      <c r="M370" s="14"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11797,7 +11832,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="13"/>
+      <c r="M371" s="14"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11824,7 +11859,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="13"/>
+      <c r="M372" s="14"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11849,7 +11884,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="13"/>
+      <c r="M373" s="14"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11874,7 +11909,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="13"/>
+      <c r="M374" s="14"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11899,7 +11934,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="13"/>
+      <c r="M375" s="14"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11924,7 +11959,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="13"/>
+      <c r="M376" s="14"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11949,7 +11984,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="13"/>
+      <c r="M377" s="14"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -11974,7 +12009,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="13"/>
+      <c r="M378" s="14"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -11999,7 +12034,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="13"/>
+      <c r="M379" s="14"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12026,7 +12061,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="13"/>
+      <c r="M380" s="14"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12051,7 +12086,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="13"/>
+      <c r="M381" s="14"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12078,7 +12113,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="13"/>
+      <c r="M382" s="14"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12103,7 +12138,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="13"/>
+      <c r="M383" s="14"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12128,7 +12163,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="13"/>
+      <c r="M384" s="14"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12153,7 +12188,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="13"/>
+      <c r="M385" s="14"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12178,7 +12213,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="13"/>
+      <c r="M386" s="14"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12251,7 +12286,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="13">
+      <c r="M389" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -12280,7 +12315,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="13"/>
+      <c r="M390" s="14"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12307,7 +12342,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="13"/>
+      <c r="M391" s="14"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12334,7 +12369,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="13"/>
+      <c r="M392" s="14"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12361,7 +12396,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="13"/>
+      <c r="M393" s="14"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12388,7 +12423,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="13"/>
+      <c r="M394" s="14"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12415,7 +12450,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="13"/>
+      <c r="M395" s="14"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12445,7 +12480,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="13">
+      <c r="M396" s="14">
         <v>1</v>
       </c>
     </row>
@@ -12474,7 +12509,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="13"/>
+      <c r="M397" s="14"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12501,7 +12536,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="13"/>
+      <c r="M398" s="14"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12528,7 +12563,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="13"/>
+      <c r="M399" s="14"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12555,7 +12590,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="13"/>
+      <c r="M400" s="14"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12582,7 +12617,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="13"/>
+      <c r="M401" s="14"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12609,7 +12644,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="13"/>
+      <c r="M402" s="14"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12636,7 +12671,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="13"/>
+      <c r="M403" s="14"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12663,7 +12698,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="13"/>
+      <c r="M404" s="14"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12690,7 +12725,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="13"/>
+      <c r="M405" s="14"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12717,7 +12752,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="13"/>
+      <c r="M406" s="14"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12744,7 +12779,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="13"/>
+      <c r="M407" s="14"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12773,7 +12808,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="13"/>
+      <c r="M408" s="14"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12800,7 +12835,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="13"/>
+      <c r="M409" s="14"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12829,7 +12864,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="13"/>
+      <c r="M410" s="14"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12856,7 +12891,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="13"/>
+      <c r="M411" s="14"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12883,7 +12918,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="13"/>
+      <c r="M412" s="14"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12910,7 +12945,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="13"/>
+      <c r="M413" s="14"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12937,7 +12972,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="13"/>
+      <c r="M414" s="14"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -12967,7 +13002,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="13">
+      <c r="M415" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -12996,7 +13031,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="13"/>
+      <c r="M416" s="14"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13025,7 +13060,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="13"/>
+      <c r="M417" s="14"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13054,7 +13089,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="13"/>
+      <c r="M418" s="14"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13083,7 +13118,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="13"/>
+      <c r="M419" s="14"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13112,7 +13147,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="13"/>
+      <c r="M420" s="14"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13142,7 +13177,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="13">
+      <c r="M421" s="14">
         <v>1</v>
       </c>
     </row>
@@ -13171,7 +13206,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="13"/>
+      <c r="M422" s="14"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13198,7 +13233,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="13"/>
+      <c r="M423" s="14"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13225,7 +13260,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="13"/>
+      <c r="M424" s="14"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13252,7 +13287,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="13"/>
+      <c r="M425" s="14"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13279,7 +13314,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="13"/>
+      <c r="M426" s="14"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13306,7 +13341,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="13"/>
+      <c r="M427" s="14"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13333,7 +13368,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="13"/>
+      <c r="M428" s="14"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13360,7 +13395,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="13"/>
+      <c r="M429" s="14"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13387,7 +13422,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="13"/>
+      <c r="M430" s="14"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13414,7 +13449,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="13"/>
+      <c r="M431" s="14"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13441,7 +13476,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="13"/>
+      <c r="M432" s="14"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13470,7 +13505,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="13"/>
+      <c r="M433" s="14"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13497,7 +13532,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="13"/>
+      <c r="M434" s="14"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13526,7 +13561,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="13"/>
+      <c r="M435" s="14"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13553,7 +13588,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="13"/>
+      <c r="M436" s="14"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13580,7 +13615,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="13"/>
+      <c r="M437" s="14"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13607,7 +13642,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="13"/>
+      <c r="M438" s="14"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13634,7 +13669,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="13"/>
+      <c r="M439" s="14"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13668,7 +13703,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="13">
+      <c r="M440" s="14">
         <v>1</v>
       </c>
     </row>
@@ -13701,7 +13736,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="13"/>
+      <c r="M441" s="14"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13732,7 +13767,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="13"/>
+      <c r="M442" s="14"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13763,7 +13798,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="13"/>
+      <c r="M443" s="14"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13794,7 +13829,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="13"/>
+      <c r="M444" s="14"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13825,7 +13860,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="13"/>
+      <c r="M445" s="14"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13856,7 +13891,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="13"/>
+      <c r="M446" s="14"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13887,7 +13922,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="13"/>
+      <c r="M447" s="14"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13918,7 +13953,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="13"/>
+      <c r="M448" s="14"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13949,7 +13984,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="13"/>
+      <c r="M449" s="14"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -13978,7 +14013,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="13"/>
+      <c r="M450" s="14"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14007,7 +14042,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="13"/>
+      <c r="M451" s="14"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14036,7 +14071,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="13"/>
+      <c r="M452" s="14"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14065,7 +14100,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="13"/>
+      <c r="M453" s="14"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14094,7 +14129,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="13"/>
+      <c r="M454" s="14"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14121,7 +14156,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="13"/>
+      <c r="M455" s="14"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14148,7 +14183,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="13"/>
+      <c r="M456" s="14"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14175,7 +14210,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="13"/>
+      <c r="M457" s="14"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14204,7 +14239,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="13"/>
+      <c r="M458" s="14"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14233,7 +14268,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="13"/>
+      <c r="M459" s="14"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14262,7 +14297,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="13"/>
+      <c r="M460" s="14"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14291,7 +14326,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="13"/>
+      <c r="M461" s="14"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14625,7 +14660,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="14">
+      <c r="M474" s="15">
         <v>1</v>
       </c>
     </row>
@@ -14654,7 +14689,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="14"/>
+      <c r="M475" s="15"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14681,7 +14716,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="14"/>
+      <c r="M476" s="15"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14708,7 +14743,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="14"/>
+      <c r="M477" s="15"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14735,7 +14770,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="14"/>
+      <c r="M478" s="15"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14762,7 +14797,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="14"/>
+      <c r="M479" s="15"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14789,7 +14824,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="14"/>
+      <c r="M480" s="15"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14816,7 +14851,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="14"/>
+      <c r="M481" s="15"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14843,7 +14878,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="14"/>
+      <c r="M482" s="15"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14870,7 +14905,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="14"/>
+      <c r="M483" s="15"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15030,7 +15065,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="14">
+      <c r="M489" s="15">
         <v>2</v>
       </c>
     </row>
@@ -15057,7 +15092,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="14"/>
+      <c r="M490" s="15"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15082,7 +15117,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="14"/>
+      <c r="M491" s="15"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15107,7 +15142,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="14"/>
+      <c r="M492" s="15"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15132,7 +15167,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="14"/>
+      <c r="M493" s="15"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15159,7 +15194,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="14"/>
+      <c r="M494" s="15"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15186,7 +15221,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="14"/>
+      <c r="M495" s="15"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15213,7 +15248,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="14"/>
+      <c r="M496" s="15"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15240,7 +15275,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="14"/>
+      <c r="M497" s="15"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15293,7 +15328,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="14">
+      <c r="M499" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15320,7 +15355,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="14"/>
+      <c r="M500" s="15"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15345,7 +15380,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="14"/>
+      <c r="M501" s="15"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15370,7 +15405,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="14"/>
+      <c r="M502" s="15"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15395,7 +15430,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="14"/>
+      <c r="M503" s="15"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15420,7 +15455,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="14"/>
+      <c r="M504" s="15"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15447,7 +15482,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="14"/>
+      <c r="M505" s="15"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15472,7 +15507,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="14"/>
+      <c r="M506" s="15"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15499,7 +15534,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="14"/>
+      <c r="M507" s="15"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15524,7 +15559,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="14"/>
+      <c r="M508" s="15"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15549,7 +15584,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="14"/>
+      <c r="M509" s="15"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15574,7 +15609,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="14"/>
+      <c r="M510" s="15"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15599,7 +15634,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="14"/>
+      <c r="M511" s="15"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15626,7 +15661,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="14"/>
+      <c r="M512" s="15"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15653,7 +15688,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="14"/>
+      <c r="M513" s="15"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15678,7 +15713,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="14"/>
+      <c r="M514" s="15"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15703,7 +15738,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="14"/>
+      <c r="M515" s="15"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15731,7 +15766,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="14">
+      <c r="M516" s="15">
         <v>2</v>
       </c>
     </row>
@@ -15760,7 +15795,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="14"/>
+      <c r="M517" s="15"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15787,7 +15822,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="14"/>
+      <c r="M518" s="15"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15814,7 +15849,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="14"/>
+      <c r="M519" s="15"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15843,7 +15878,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="14"/>
+      <c r="M520" s="15"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15872,7 +15907,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="14"/>
+      <c r="M521" s="15"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15901,7 +15936,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="14"/>
+      <c r="M522" s="15"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15930,7 +15965,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="14"/>
+      <c r="M523" s="15"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15959,7 +15994,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="14"/>
+      <c r="M524" s="15"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -15988,7 +16023,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="14"/>
+      <c r="M525" s="15"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16015,7 +16050,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="14"/>
+      <c r="M526" s="15"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16042,7 +16077,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="14"/>
+      <c r="M527" s="15"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">

</xml_diff>

<commit_message>
Added feature: Chart Wall -> Transparency. Added feature: Chart Title -> Main Title -> Lines. Added feature: Chart Title -> Main Title -> Area. Added feature: Chart Title -> Main Title -> Transparency.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="225">
   <si>
     <t>Chart</t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t>Known Issues: [ 1771500 ]Chart objects bitmap tile and border width display.</t>
+  </si>
+  <si>
+    <t>Incompatible feature</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1772929 ] Chart objects' manual layout</t>
   </si>
 </sst>
 </file>
@@ -858,17 +864,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1191,10 +1197,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K143" sqref="K143"/>
+      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1204,8 +1210,8 @@
     <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
@@ -1214,16 +1220,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1264,7 +1270,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1294,7 +1300,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1319,7 +1325,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1344,7 +1350,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1369,7 +1375,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1394,7 +1400,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1419,7 +1425,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1444,7 +1450,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1469,7 +1475,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="13"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2090,7 +2096,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2122,7 +2128,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="14"/>
+      <c r="M34" s="13"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2387,7 +2393,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M43" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2419,7 +2425,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="14"/>
+      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2451,7 +2457,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="14"/>
+      <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2483,7 +2489,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="14"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2515,7 +2521,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="14"/>
+      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2547,7 +2553,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="14"/>
+      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2579,7 +2585,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="14"/>
+      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2611,7 +2617,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2800,7 +2806,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="14">
+      <c r="M57" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2829,7 +2835,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="14"/>
+      <c r="M58" s="13"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2856,7 +2862,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="14"/>
+      <c r="M59" s="13"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2883,7 +2889,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="14"/>
+      <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3981,7 +3987,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="14">
+      <c r="M98" s="13">
         <v>2</v>
       </c>
     </row>
@@ -4008,7 +4014,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="14"/>
+      <c r="M99" s="13"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4036,7 +4042,7 @@
       <c r="K100" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="M100" s="14"/>
+      <c r="M100" s="13"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4061,7 +4067,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="14"/>
+      <c r="M101" s="13"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4088,7 +4094,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="14"/>
+      <c r="M102" s="13"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4115,7 +4121,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="14"/>
+      <c r="M103" s="13"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4144,7 +4150,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="14"/>
+      <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4173,7 +4179,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="14"/>
+      <c r="M105" s="13"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4207,7 +4213,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="14"/>
+      <c r="M106" s="13"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4241,7 +4247,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="14"/>
+      <c r="M107" s="13"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4275,7 +4281,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="14"/>
+      <c r="M108" s="13"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4309,7 +4315,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="14"/>
+      <c r="M109" s="13"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4338,7 +4344,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="14"/>
+      <c r="M110" s="13"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4372,7 +4378,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="14"/>
+      <c r="M111" s="13"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4406,7 +4412,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="14"/>
+      <c r="M112" s="13"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4440,7 +4446,7 @@
       <c r="K113" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="M113" s="14"/>
+      <c r="M113" s="13"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4471,7 +4477,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="14"/>
+      <c r="M114" s="13"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4502,7 +4508,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="14"/>
+      <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4533,7 +4539,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="14"/>
+      <c r="M116" s="13"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4558,7 +4564,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="14"/>
+      <c r="M117" s="13"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4585,7 +4591,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="14"/>
+      <c r="M118" s="13"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4819,7 +4825,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="14">
+      <c r="M127" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4846,7 +4852,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="14"/>
+      <c r="M128" s="13"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4874,7 +4880,7 @@
       <c r="K129" t="s">
         <v>222</v>
       </c>
-      <c r="M129" s="14"/>
+      <c r="M129" s="13"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4899,7 +4905,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="14"/>
+      <c r="M130" s="13"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4924,7 +4930,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="14"/>
+      <c r="M131" s="13"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4951,7 +4957,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="14"/>
+      <c r="M132" s="13"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4978,7 +4984,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="14"/>
+      <c r="M133" s="13"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5007,7 +5013,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="14"/>
+      <c r="M134" s="13"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5036,7 +5042,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="14"/>
+      <c r="M135" s="13"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5070,7 +5076,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="14"/>
+      <c r="M136" s="13"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5104,7 +5110,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="14"/>
+      <c r="M137" s="13"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5138,7 +5144,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="14"/>
+      <c r="M138" s="13"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5172,7 +5178,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="14"/>
+      <c r="M139" s="13"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5201,7 +5207,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="14"/>
+      <c r="M140" s="13"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5235,7 +5241,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="14"/>
+      <c r="M141" s="13"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5269,7 +5275,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="14"/>
+      <c r="M142" s="13"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5301,7 +5307,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="14"/>
+      <c r="M143" s="13"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5332,7 +5338,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="14"/>
+      <c r="M144" s="13"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5363,7 +5369,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="14"/>
+      <c r="M145" s="13"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5394,7 +5400,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="14"/>
+      <c r="M146" s="13"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5419,7 +5425,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="14"/>
+      <c r="M147" s="13"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5444,7 +5450,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="14"/>
+      <c r="M148" s="13"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5471,7 +5477,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="14"/>
+      <c r="M149" s="13"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5498,7 +5504,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="14"/>
+      <c r="M150" s="13"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5525,7 +5531,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="14"/>
+      <c r="M151" s="13"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5552,7 +5558,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="14"/>
+      <c r="M152" s="13"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5579,7 +5585,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="14"/>
+      <c r="M153" s="13"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5606,7 +5612,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="14"/>
+      <c r="M154" s="13"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5633,7 +5639,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="14"/>
+      <c r="M155" s="13"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5660,7 +5666,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="14"/>
+      <c r="M156" s="13"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5680,12 +5686,15 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
       <c r="I157" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J157" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M157" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K157" t="s">
+        <v>223</v>
+      </c>
+      <c r="M157" s="13"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5707,12 +5716,15 @@
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
       <c r="I158" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J158" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M158" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K158" t="s">
+        <v>224</v>
+      </c>
+      <c r="M158" s="13"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5734,12 +5746,15 @@
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
       <c r="I159" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J159" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M159" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K159" t="s">
+        <v>224</v>
+      </c>
+      <c r="M159" s="13"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5761,12 +5776,15 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
       <c r="I160" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J160" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M160" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K160" t="s">
+        <v>224</v>
+      </c>
+      <c r="M160" s="13"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5788,12 +5806,15 @@
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
       <c r="I161" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J161" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M161" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K161" t="s">
+        <v>224</v>
+      </c>
+      <c r="M161" s="13"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5815,12 +5836,15 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
       <c r="I162" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J162" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M162" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K162" t="s">
+        <v>224</v>
+      </c>
+      <c r="M162" s="13"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5842,12 +5866,15 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
       <c r="I163" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J163" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M163" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K163" t="s">
+        <v>224</v>
+      </c>
+      <c r="M163" s="13"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5869,12 +5896,15 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J164" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M164" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K164" t="s">
+        <v>224</v>
+      </c>
+      <c r="M164" s="13"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5899,12 +5929,12 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
       <c r="I165" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J165" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M165" s="14">
+        <v>210</v>
+      </c>
+      <c r="M165" s="13">
         <v>1</v>
       </c>
     </row>
@@ -5928,12 +5958,12 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
       <c r="I166" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J166" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M166" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M166" s="13"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5955,12 +5985,12 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
       <c r="I167" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J167" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M167" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M167" s="13"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -5982,12 +6012,15 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
       <c r="I168" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J168" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M168" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K168" t="s">
+        <v>222</v>
+      </c>
+      <c r="M168" s="13"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6009,12 +6042,12 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
       <c r="I169" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J169" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M169" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M169" s="13"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6036,12 +6069,12 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
       <c r="I170" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J170" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M170" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M170" s="13"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6065,12 +6098,12 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
       <c r="I171" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J171" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M171" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M171" s="13"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6094,12 +6127,12 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
       <c r="I172" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J172" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M172" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M172" s="13"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6130,7 +6163,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="14"/>
+      <c r="M173" s="13"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6161,7 +6194,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="14"/>
+      <c r="M174" s="13"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6189,12 +6222,15 @@
         <v>94</v>
       </c>
       <c r="I175" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J175" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M175" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K175" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="M175" s="13"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6222,12 +6258,15 @@
         <v>95</v>
       </c>
       <c r="I176" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J176" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M176" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K176" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M176" s="13"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6255,12 +6294,15 @@
         <v>5</v>
       </c>
       <c r="I177" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J177" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M177" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K177" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M177" s="13"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6288,12 +6330,15 @@
         <v>6</v>
       </c>
       <c r="I178" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J178" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M178" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K178" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M178" s="13"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6319,12 +6364,12 @@
       </c>
       <c r="H179" s="1"/>
       <c r="I179" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J179" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M179" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M179" s="13"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6352,12 +6397,15 @@
         <v>96</v>
       </c>
       <c r="I180" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J180" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M180" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K180" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M180" s="13"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6385,12 +6433,15 @@
         <v>97</v>
       </c>
       <c r="I181" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J181" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M181" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K181" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M181" s="13"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6418,12 +6469,13 @@
         <v>98</v>
       </c>
       <c r="I182" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J182" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M182" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K182" s="10"/>
+      <c r="M182" s="13"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6451,12 +6503,12 @@
         <v>99</v>
       </c>
       <c r="I183" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J183" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M183" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M183" s="13"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6484,12 +6536,12 @@
         <v>101</v>
       </c>
       <c r="I184" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J184" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M184" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M184" s="13"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6517,12 +6569,12 @@
         <v>102</v>
       </c>
       <c r="I185" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J185" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M185" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M185" s="13"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6544,12 +6596,12 @@
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
       <c r="I186" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J186" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M186" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M186" s="13"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6571,12 +6623,12 @@
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
       <c r="I187" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J187" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M187" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M187" s="13"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6600,12 +6652,12 @@
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
       <c r="I188" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J188" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M188" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M188" s="13"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6828,7 +6880,7 @@
       <c r="J196" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M196" s="14">
+      <c r="M196" s="13">
         <v>2</v>
       </c>
     </row>
@@ -6857,7 +6909,7 @@
       <c r="J197" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M197" s="14"/>
+      <c r="M197" s="13"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6884,7 +6936,7 @@
       <c r="J198" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M198" s="14"/>
+      <c r="M198" s="13"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6911,7 +6963,7 @@
       <c r="J199" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M199" s="14"/>
+      <c r="M199" s="13"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6938,7 +6990,7 @@
       <c r="J200" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M200" s="14"/>
+      <c r="M200" s="13"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -6967,7 +7019,7 @@
       <c r="J201" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M201" s="14"/>
+      <c r="M201" s="13"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -6994,7 +7046,7 @@
       <c r="J202" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M202" s="14"/>
+      <c r="M202" s="13"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7023,7 +7075,7 @@
       <c r="J203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M203" s="14"/>
+      <c r="M203" s="13"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7050,7 +7102,7 @@
       <c r="J204" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M204" s="14"/>
+      <c r="M204" s="13"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7077,7 +7129,7 @@
       <c r="J205" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M205" s="14"/>
+      <c r="M205" s="13"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7104,7 +7156,7 @@
       <c r="J206" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M206" s="14"/>
+      <c r="M206" s="13"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7131,7 +7183,7 @@
       <c r="J207" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M207" s="14"/>
+      <c r="M207" s="13"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7158,7 +7210,7 @@
       <c r="J208" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M208" s="14"/>
+      <c r="M208" s="13"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7185,7 +7237,7 @@
       <c r="J209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M209" s="14"/>
+      <c r="M209" s="13"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7215,7 +7267,7 @@
       <c r="J210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M210" s="14">
+      <c r="M210" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -7246,7 +7298,7 @@
       <c r="J211" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M211" s="14"/>
+      <c r="M211" s="13"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7275,7 +7327,7 @@
       <c r="J212" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M212" s="14"/>
+      <c r="M212" s="13"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7304,7 +7356,7 @@
       <c r="J213" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M213" s="14"/>
+      <c r="M213" s="13"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7333,7 +7385,7 @@
       <c r="J214" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M214" s="14"/>
+      <c r="M214" s="13"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7362,7 +7414,7 @@
       <c r="J215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M215" s="14"/>
+      <c r="M215" s="13"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7391,7 +7443,7 @@
       <c r="J216" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M216" s="14"/>
+      <c r="M216" s="13"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7420,7 +7472,7 @@
       <c r="J217" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M217" s="14"/>
+      <c r="M217" s="13"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7449,7 +7501,7 @@
       <c r="J218" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M218" s="14"/>
+      <c r="M218" s="13"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7478,7 +7530,7 @@
       <c r="J219" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M219" s="14"/>
+      <c r="M219" s="13"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7505,7 +7557,7 @@
       <c r="J220" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M220" s="14">
+      <c r="M220" s="13">
         <v>1</v>
       </c>
     </row>
@@ -7534,7 +7586,7 @@
       <c r="J221" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M221" s="14"/>
+      <c r="M221" s="13"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7561,7 +7613,7 @@
       <c r="J222" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M222" s="14"/>
+      <c r="M222" s="13"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7588,7 +7640,7 @@
       <c r="J223" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M223" s="14"/>
+      <c r="M223" s="13"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7615,7 +7667,7 @@
       <c r="J224" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M224" s="14"/>
+      <c r="M224" s="13"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7642,7 +7694,7 @@
       <c r="J225" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M225" s="14"/>
+      <c r="M225" s="13"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7671,7 +7723,7 @@
       <c r="J226" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M226" s="14"/>
+      <c r="M226" s="13"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7700,7 +7752,7 @@
       <c r="J227" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M227" s="14"/>
+      <c r="M227" s="13"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7731,7 +7783,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="14"/>
+      <c r="M228" s="13"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7762,7 +7814,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="14"/>
+      <c r="M229" s="13"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7795,7 +7847,7 @@
       <c r="J230" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M230" s="14"/>
+      <c r="M230" s="13"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7828,7 +7880,7 @@
       <c r="J231" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M231" s="14"/>
+      <c r="M231" s="13"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7861,7 +7913,7 @@
       <c r="J232" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M232" s="14"/>
+      <c r="M232" s="13"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7894,7 +7946,7 @@
       <c r="J233" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M233" s="14"/>
+      <c r="M233" s="13"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7925,7 +7977,7 @@
       <c r="J234" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M234" s="14"/>
+      <c r="M234" s="13"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -7958,7 +8010,7 @@
       <c r="J235" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M235" s="14"/>
+      <c r="M235" s="13"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -7991,7 +8043,7 @@
       <c r="J236" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M236" s="14"/>
+      <c r="M236" s="13"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8024,7 +8076,7 @@
       <c r="J237" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M237" s="14"/>
+      <c r="M237" s="13"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8057,7 +8109,7 @@
       <c r="J238" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M238" s="14"/>
+      <c r="M238" s="13"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8090,7 +8142,7 @@
       <c r="J239" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M239" s="14"/>
+      <c r="M239" s="13"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8123,7 +8175,7 @@
       <c r="J240" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M240" s="14"/>
+      <c r="M240" s="13"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8150,7 +8202,7 @@
       <c r="J241" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M241" s="14"/>
+      <c r="M241" s="13"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8177,7 +8229,7 @@
       <c r="J242" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M242" s="14"/>
+      <c r="M242" s="13"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8206,7 +8258,7 @@
       <c r="J243" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M243" s="14"/>
+      <c r="M243" s="13"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8235,7 +8287,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="14"/>
+      <c r="M244" s="13"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8264,7 +8316,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="14"/>
+      <c r="M245" s="13"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8293,7 +8345,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="14"/>
+      <c r="M246" s="13"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8322,7 +8374,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="14"/>
+      <c r="M247" s="13"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8351,7 +8403,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="14"/>
+      <c r="M248" s="13"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8380,7 +8432,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="14"/>
+      <c r="M249" s="13"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8409,7 +8461,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="14"/>
+      <c r="M250" s="13"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8436,7 +8488,7 @@
       <c r="J251" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M251" s="14"/>
+      <c r="M251" s="13"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8463,7 +8515,7 @@
       <c r="J252" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M252" s="14"/>
+      <c r="M252" s="13"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8490,7 +8542,7 @@
       <c r="J253" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M253" s="14"/>
+      <c r="M253" s="13"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8517,7 +8569,7 @@
       <c r="J254" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M254" s="14"/>
+      <c r="M254" s="13"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8544,7 +8596,7 @@
       <c r="J255" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M255" s="14"/>
+      <c r="M255" s="13"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8571,7 +8623,7 @@
       <c r="J256" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M256" s="14"/>
+      <c r="M256" s="13"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8598,7 +8650,7 @@
       <c r="J257" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M257" s="14"/>
+      <c r="M257" s="13"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8627,7 +8679,7 @@
       <c r="J258" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M258" s="14"/>
+      <c r="M258" s="13"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8654,7 +8706,7 @@
       <c r="J259" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M259" s="14"/>
+      <c r="M259" s="13"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8683,7 +8735,7 @@
       <c r="J260" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M260" s="14"/>
+      <c r="M260" s="13"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8710,7 +8762,7 @@
       <c r="J261" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M261" s="14"/>
+      <c r="M261" s="13"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8737,7 +8789,7 @@
       <c r="J262" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M262" s="14"/>
+      <c r="M262" s="13"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8764,7 +8816,7 @@
       <c r="J263" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M263" s="14"/>
+      <c r="M263" s="13"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8791,7 +8843,7 @@
       <c r="J264" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M264" s="14"/>
+      <c r="M264" s="13"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8818,7 +8870,7 @@
       <c r="J265" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M265" s="14"/>
+      <c r="M265" s="13"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8845,7 +8897,7 @@
       <c r="J266" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M266" s="14"/>
+      <c r="M266" s="13"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8872,7 +8924,7 @@
       <c r="J267" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M267" s="14"/>
+      <c r="M267" s="13"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8899,7 +8951,7 @@
       <c r="J268" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M268" s="14"/>
+      <c r="M268" s="13"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8928,7 +8980,7 @@
       <c r="J269" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M269" s="14"/>
+      <c r="M269" s="13"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -8957,7 +9009,7 @@
       <c r="J270" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M270" s="14"/>
+      <c r="M270" s="13"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -8986,7 +9038,7 @@
       <c r="J271" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M271" s="14"/>
+      <c r="M271" s="13"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9015,7 +9067,7 @@
       <c r="J272" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M272" s="14"/>
+      <c r="M272" s="13"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9044,7 +9096,7 @@
       <c r="J273" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M273" s="14"/>
+      <c r="M273" s="13"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9073,7 +9125,7 @@
       <c r="J274" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M274" s="14"/>
+      <c r="M274" s="13"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9102,7 +9154,7 @@
       <c r="J275" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M275" s="14"/>
+      <c r="M275" s="13"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9131,7 +9183,7 @@
       <c r="J276" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M276" s="14"/>
+      <c r="M276" s="13"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9160,7 +9212,7 @@
       <c r="J277" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M277" s="14"/>
+      <c r="M277" s="13"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9187,7 +9239,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="14"/>
+      <c r="M278" s="13"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9214,7 +9266,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="14"/>
+      <c r="M279" s="13"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9241,7 +9293,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="14"/>
+      <c r="M280" s="13"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9268,7 +9320,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="14"/>
+      <c r="M281" s="13"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9295,7 +9347,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="14"/>
+      <c r="M282" s="13"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9322,7 +9374,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="14"/>
+      <c r="M283" s="13"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9351,7 +9403,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="14"/>
+      <c r="M284" s="13"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9380,7 +9432,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="14"/>
+      <c r="M285" s="13"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9411,7 +9463,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="14"/>
+      <c r="M286" s="13"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9442,7 +9494,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="14"/>
+      <c r="M287" s="13"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9475,7 +9527,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="14"/>
+      <c r="M288" s="13"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9508,7 +9560,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="14"/>
+      <c r="M289" s="13"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9541,7 +9593,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="14"/>
+      <c r="M290" s="13"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9574,7 +9626,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="14"/>
+      <c r="M291" s="13"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9605,7 +9657,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="14"/>
+      <c r="M292" s="13"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9638,7 +9690,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="14"/>
+      <c r="M293" s="13"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9671,7 +9723,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="14"/>
+      <c r="M294" s="13"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9704,7 +9756,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="14"/>
+      <c r="M295" s="13"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9737,7 +9789,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="14"/>
+      <c r="M296" s="13"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9770,7 +9822,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="14"/>
+      <c r="M297" s="13"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9803,7 +9855,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="14"/>
+      <c r="M298" s="13"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9830,7 +9882,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="14"/>
+      <c r="M299" s="13"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9857,7 +9909,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="14"/>
+      <c r="M300" s="13"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9886,7 +9938,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="14"/>
+      <c r="M301" s="13"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9915,7 +9967,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="14"/>
+      <c r="M302" s="13"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -9944,7 +9996,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="14"/>
+      <c r="M303" s="13"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -9973,7 +10025,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="14"/>
+      <c r="M304" s="13"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10002,7 +10054,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="14"/>
+      <c r="M305" s="13"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10031,7 +10083,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="14"/>
+      <c r="M306" s="13"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10060,7 +10112,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="14"/>
+      <c r="M307" s="13"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10089,7 +10141,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="14"/>
+      <c r="M308" s="13"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10116,7 +10168,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="14"/>
+      <c r="M309" s="13"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10143,7 +10195,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="14"/>
+      <c r="M310" s="13"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10170,7 +10222,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="14"/>
+      <c r="M311" s="13"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10197,7 +10249,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="14"/>
+      <c r="M312" s="13"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10224,7 +10276,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="14"/>
+      <c r="M313" s="13"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10251,7 +10303,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="14"/>
+      <c r="M314" s="13"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10278,7 +10330,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="14"/>
+      <c r="M315" s="13"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10307,7 +10359,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="14"/>
+      <c r="M316" s="13"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10334,7 +10386,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="14"/>
+      <c r="M317" s="13"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10363,7 +10415,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="14"/>
+      <c r="M318" s="13"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10390,7 +10442,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="14"/>
+      <c r="M319" s="13"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10417,7 +10469,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="14"/>
+      <c r="M320" s="13"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10444,7 +10496,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="14"/>
+      <c r="M321" s="13"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10471,7 +10523,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="14"/>
+      <c r="M322" s="13"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10498,7 +10550,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="14"/>
+      <c r="M323" s="13"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10525,7 +10577,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="14"/>
+      <c r="M324" s="13"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10552,7 +10604,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="14"/>
+      <c r="M325" s="13"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10579,7 +10631,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="14"/>
+      <c r="M326" s="13"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10608,7 +10660,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="14"/>
+      <c r="M327" s="13"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10637,7 +10689,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="14"/>
+      <c r="M328" s="13"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10666,7 +10718,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="14"/>
+      <c r="M329" s="13"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10695,7 +10747,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="14"/>
+      <c r="M330" s="13"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10724,7 +10776,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="14"/>
+      <c r="M331" s="13"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10753,7 +10805,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="14"/>
+      <c r="M332" s="13"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10782,7 +10834,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="14"/>
+      <c r="M333" s="13"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10811,7 +10863,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="14"/>
+      <c r="M334" s="13"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10840,7 +10892,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="14"/>
+      <c r="M335" s="13"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11015,7 +11067,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="14">
+      <c r="M342" s="13">
         <v>1</v>
       </c>
     </row>
@@ -11042,7 +11094,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="14"/>
+      <c r="M343" s="13"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11067,7 +11119,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="14"/>
+      <c r="M344" s="13"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11092,7 +11144,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="14"/>
+      <c r="M345" s="13"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11117,7 +11169,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="14"/>
+      <c r="M346" s="13"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11142,7 +11194,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="14"/>
+      <c r="M347" s="13"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11169,7 +11221,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="14"/>
+      <c r="M348" s="13"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11196,7 +11248,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="14"/>
+      <c r="M349" s="13"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11225,7 +11277,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="14"/>
+      <c r="M350" s="13"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11254,7 +11306,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="14"/>
+      <c r="M351" s="13"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11285,7 +11337,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="14"/>
+      <c r="M352" s="13"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11316,7 +11368,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="14"/>
+      <c r="M353" s="13"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11347,7 +11399,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="14"/>
+      <c r="M354" s="13"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11378,7 +11430,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="14"/>
+      <c r="M355" s="13"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11407,7 +11459,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="14"/>
+      <c r="M356" s="13"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11438,7 +11490,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="14"/>
+      <c r="M357" s="13"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11469,7 +11521,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="14"/>
+      <c r="M358" s="13"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11500,7 +11552,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="14"/>
+      <c r="M359" s="13"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11531,7 +11583,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="14"/>
+      <c r="M360" s="13"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11562,7 +11614,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="14"/>
+      <c r="M361" s="13"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11593,7 +11645,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="14"/>
+      <c r="M362" s="13"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11618,7 +11670,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="14"/>
+      <c r="M363" s="13"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11643,7 +11695,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="14"/>
+      <c r="M364" s="13"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11670,7 +11722,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="14"/>
+      <c r="M365" s="13"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11697,7 +11749,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="14"/>
+      <c r="M366" s="13"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11724,7 +11776,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="14"/>
+      <c r="M367" s="13"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11751,7 +11803,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="14"/>
+      <c r="M368" s="13"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11778,7 +11830,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="14"/>
+      <c r="M369" s="13"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11805,7 +11857,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="14"/>
+      <c r="M370" s="13"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11832,7 +11884,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="14"/>
+      <c r="M371" s="13"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11859,7 +11911,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="14"/>
+      <c r="M372" s="13"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11884,7 +11936,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="14"/>
+      <c r="M373" s="13"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11909,7 +11961,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="14"/>
+      <c r="M374" s="13"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11934,7 +11986,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="14"/>
+      <c r="M375" s="13"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -11959,7 +12011,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="14"/>
+      <c r="M376" s="13"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -11984,7 +12036,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="14"/>
+      <c r="M377" s="13"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12009,7 +12061,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="14"/>
+      <c r="M378" s="13"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12034,7 +12086,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="14"/>
+      <c r="M379" s="13"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12061,7 +12113,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="14"/>
+      <c r="M380" s="13"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12086,7 +12138,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="14"/>
+      <c r="M381" s="13"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12113,7 +12165,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="14"/>
+      <c r="M382" s="13"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12138,7 +12190,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="14"/>
+      <c r="M383" s="13"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12163,7 +12215,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="14"/>
+      <c r="M384" s="13"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12188,7 +12240,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="14"/>
+      <c r="M385" s="13"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12213,7 +12265,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="14"/>
+      <c r="M386" s="13"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12286,7 +12338,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="14">
+      <c r="M389" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -12315,7 +12367,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="14"/>
+      <c r="M390" s="13"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12342,7 +12394,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="14"/>
+      <c r="M391" s="13"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12369,7 +12421,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="14"/>
+      <c r="M392" s="13"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12396,7 +12448,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="14"/>
+      <c r="M393" s="13"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12423,7 +12475,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="14"/>
+      <c r="M394" s="13"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12450,7 +12502,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="14"/>
+      <c r="M395" s="13"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12480,7 +12532,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="14">
+      <c r="M396" s="13">
         <v>1</v>
       </c>
     </row>
@@ -12509,7 +12561,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="14"/>
+      <c r="M397" s="13"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12536,7 +12588,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="14"/>
+      <c r="M398" s="13"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12563,7 +12615,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="14"/>
+      <c r="M399" s="13"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12590,7 +12642,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="14"/>
+      <c r="M400" s="13"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12617,7 +12669,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="14"/>
+      <c r="M401" s="13"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12644,7 +12696,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="14"/>
+      <c r="M402" s="13"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12671,7 +12723,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="14"/>
+      <c r="M403" s="13"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12698,7 +12750,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="14"/>
+      <c r="M404" s="13"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12725,7 +12777,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="14"/>
+      <c r="M405" s="13"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12752,7 +12804,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="14"/>
+      <c r="M406" s="13"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12779,7 +12831,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="14"/>
+      <c r="M407" s="13"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12808,7 +12860,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="14"/>
+      <c r="M408" s="13"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12835,7 +12887,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="14"/>
+      <c r="M409" s="13"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12864,7 +12916,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="14"/>
+      <c r="M410" s="13"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12891,7 +12943,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="14"/>
+      <c r="M411" s="13"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12918,7 +12970,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="14"/>
+      <c r="M412" s="13"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -12945,7 +12997,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="14"/>
+      <c r="M413" s="13"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -12972,7 +13024,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="14"/>
+      <c r="M414" s="13"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13002,7 +13054,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="14">
+      <c r="M415" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -13031,7 +13083,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="14"/>
+      <c r="M416" s="13"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13060,7 +13112,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="14"/>
+      <c r="M417" s="13"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13089,7 +13141,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="14"/>
+      <c r="M418" s="13"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13118,7 +13170,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="14"/>
+      <c r="M419" s="13"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13147,7 +13199,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="14"/>
+      <c r="M420" s="13"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13177,7 +13229,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="14">
+      <c r="M421" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13206,7 +13258,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="14"/>
+      <c r="M422" s="13"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13233,7 +13285,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="14"/>
+      <c r="M423" s="13"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13260,7 +13312,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="14"/>
+      <c r="M424" s="13"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13287,7 +13339,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="14"/>
+      <c r="M425" s="13"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13314,7 +13366,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="14"/>
+      <c r="M426" s="13"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13341,7 +13393,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="14"/>
+      <c r="M427" s="13"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13368,7 +13420,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="14"/>
+      <c r="M428" s="13"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13395,7 +13447,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="14"/>
+      <c r="M429" s="13"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13422,7 +13474,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="14"/>
+      <c r="M430" s="13"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13449,7 +13501,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="14"/>
+      <c r="M431" s="13"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13476,7 +13528,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="14"/>
+      <c r="M432" s="13"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13505,7 +13557,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="14"/>
+      <c r="M433" s="13"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13532,7 +13584,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="14"/>
+      <c r="M434" s="13"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13561,7 +13613,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="14"/>
+      <c r="M435" s="13"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13588,7 +13640,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="14"/>
+      <c r="M436" s="13"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13615,7 +13667,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="14"/>
+      <c r="M437" s="13"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13642,7 +13694,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="14"/>
+      <c r="M438" s="13"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13669,7 +13721,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="14"/>
+      <c r="M439" s="13"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13703,7 +13755,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="14">
+      <c r="M440" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13736,7 +13788,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="14"/>
+      <c r="M441" s="13"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13767,7 +13819,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="14"/>
+      <c r="M442" s="13"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13798,7 +13850,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="14"/>
+      <c r="M443" s="13"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13829,7 +13881,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="14"/>
+      <c r="M444" s="13"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13860,7 +13912,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="14"/>
+      <c r="M445" s="13"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13891,7 +13943,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="14"/>
+      <c r="M446" s="13"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13922,7 +13974,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="14"/>
+      <c r="M447" s="13"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -13953,7 +14005,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="14"/>
+      <c r="M448" s="13"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -13984,7 +14036,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="14"/>
+      <c r="M449" s="13"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14013,7 +14065,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="14"/>
+      <c r="M450" s="13"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14042,7 +14094,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="14"/>
+      <c r="M451" s="13"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14071,7 +14123,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="14"/>
+      <c r="M452" s="13"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14100,7 +14152,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="14"/>
+      <c r="M453" s="13"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14129,7 +14181,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="14"/>
+      <c r="M454" s="13"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14156,7 +14208,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="14"/>
+      <c r="M455" s="13"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14183,7 +14235,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="14"/>
+      <c r="M456" s="13"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14210,7 +14262,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="14"/>
+      <c r="M457" s="13"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14239,7 +14291,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="14"/>
+      <c r="M458" s="13"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14268,7 +14320,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="14"/>
+      <c r="M459" s="13"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14297,7 +14349,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="14"/>
+      <c r="M460" s="13"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14326,7 +14378,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="14"/>
+      <c r="M461" s="13"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14660,7 +14712,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="15">
+      <c r="M474" s="12">
         <v>1</v>
       </c>
     </row>
@@ -14689,7 +14741,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="15"/>
+      <c r="M475" s="12"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14716,7 +14768,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="15"/>
+      <c r="M476" s="12"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14743,7 +14795,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="15"/>
+      <c r="M477" s="12"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14770,7 +14822,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="15"/>
+      <c r="M478" s="12"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14797,7 +14849,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="15"/>
+      <c r="M479" s="12"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14824,7 +14876,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="15"/>
+      <c r="M480" s="12"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14851,7 +14903,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="15"/>
+      <c r="M481" s="12"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14878,7 +14930,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="15"/>
+      <c r="M482" s="12"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14905,7 +14957,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="15"/>
+      <c r="M483" s="12"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15065,7 +15117,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="15">
+      <c r="M489" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15092,7 +15144,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="15"/>
+      <c r="M490" s="12"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15117,7 +15169,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="15"/>
+      <c r="M491" s="12"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15142,7 +15194,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="15"/>
+      <c r="M492" s="12"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15167,7 +15219,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="15"/>
+      <c r="M493" s="12"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15194,7 +15246,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="15"/>
+      <c r="M494" s="12"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15221,7 +15273,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="15"/>
+      <c r="M495" s="12"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15248,7 +15300,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="15"/>
+      <c r="M496" s="12"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15275,7 +15327,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="15"/>
+      <c r="M497" s="12"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15328,7 +15380,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="15">
+      <c r="M499" s="12">
         <v>1</v>
       </c>
     </row>
@@ -15355,7 +15407,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="15"/>
+      <c r="M500" s="12"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15380,7 +15432,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="15"/>
+      <c r="M501" s="12"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15405,7 +15457,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="15"/>
+      <c r="M502" s="12"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15430,7 +15482,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="15"/>
+      <c r="M503" s="12"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15455,7 +15507,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="15"/>
+      <c r="M504" s="12"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15482,7 +15534,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="15"/>
+      <c r="M505" s="12"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15507,7 +15559,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="15"/>
+      <c r="M506" s="12"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15534,7 +15586,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="15"/>
+      <c r="M507" s="12"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15559,7 +15611,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="15"/>
+      <c r="M508" s="12"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15584,7 +15636,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="15"/>
+      <c r="M509" s="12"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15609,7 +15661,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="15"/>
+      <c r="M510" s="12"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15634,7 +15686,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="15"/>
+      <c r="M511" s="12"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15661,7 +15713,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="15"/>
+      <c r="M512" s="12"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15688,7 +15740,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="15"/>
+      <c r="M513" s="12"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15713,7 +15765,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="15"/>
+      <c r="M514" s="12"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15738,7 +15790,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="15"/>
+      <c r="M515" s="12"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15766,7 +15818,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="15">
+      <c r="M516" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15795,7 +15847,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="15"/>
+      <c r="M517" s="12"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15822,7 +15874,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="15"/>
+      <c r="M518" s="12"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15849,7 +15901,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="15"/>
+      <c r="M519" s="12"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15878,7 +15930,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="15"/>
+      <c r="M520" s="12"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15907,7 +15959,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="15"/>
+      <c r="M521" s="12"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15936,7 +15988,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="15"/>
+      <c r="M522" s="12"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -15965,7 +16017,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="15"/>
+      <c r="M523" s="12"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -15994,7 +16046,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="15"/>
+      <c r="M524" s="12"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16023,7 +16075,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="15"/>
+      <c r="M525" s="12"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16050,7 +16102,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="15"/>
+      <c r="M526" s="12"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16077,7 +16129,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="15"/>
+      <c r="M527" s="12"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16102,6 +16154,11 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16118,11 +16175,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart Title -> Main Title -> Characters. Added feature: Chart Title -> Main Title -> Font Effects.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3992" uniqueCount="225">
   <si>
     <t>Chart</t>
   </si>
@@ -683,21 +683,21 @@
     <t>Known Issues: [ 1771442 ] Offset length of chart bitmap fill tile.</t>
   </si>
   <si>
+    <t>Incompatible feature</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1772929 ] Chart objects' manual layout</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1772876 ] Border width for chart area
+Known Issues: [ 1771500 ] Unexact chart display due to lack of chart size</t>
+  </si>
+  <si>
     <t>Reverse conversion not perfect due to incompatibilities
-Known Issues: [ 1771500 ] Chart objects bitmap tile and border width display.</t>
-  </si>
-  <si>
-    <t>Known Issues: [ 1772876 ] Border width for chart area
-Known Issues: [ 1771500 ] Chart objects bitmap tile and border width display.</t>
-  </si>
-  <si>
-    <t>Known Issues: [ 1771500 ]Chart objects bitmap tile and border width display.</t>
-  </si>
-  <si>
-    <t>Incompatible feature</t>
-  </si>
-  <si>
-    <t>Known Issues: [ 1772929 ] Chart objects' manual layout</t>
+Known Issues: [ 1771500 ] Unexact chart display due to lack of chart size</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1771500 ] Unexact chart display due to lack of chart size</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1197,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <selection pane="bottomLeft" activeCell="J208" sqref="J208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4040,7 +4040,7 @@
         <v>210</v>
       </c>
       <c r="K100" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M100" s="13"/>
     </row>
@@ -4444,7 +4444,7 @@
         <v>210</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="M113" s="13"/>
     </row>
@@ -4878,7 +4878,7 @@
         <v>210</v>
       </c>
       <c r="K129" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="M129" s="13"/>
     </row>
@@ -5692,7 +5692,7 @@
         <v>211</v>
       </c>
       <c r="K157" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M157" s="13"/>
     </row>
@@ -5722,7 +5722,7 @@
         <v>211</v>
       </c>
       <c r="K158" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M158" s="13"/>
     </row>
@@ -5752,7 +5752,7 @@
         <v>211</v>
       </c>
       <c r="K159" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M159" s="13"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>211</v>
       </c>
       <c r="K160" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M160" s="13"/>
     </row>
@@ -5812,7 +5812,7 @@
         <v>211</v>
       </c>
       <c r="K161" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M161" s="13"/>
     </row>
@@ -5842,7 +5842,7 @@
         <v>211</v>
       </c>
       <c r="K162" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M162" s="13"/>
     </row>
@@ -5872,7 +5872,7 @@
         <v>211</v>
       </c>
       <c r="K163" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M163" s="13"/>
     </row>
@@ -5902,7 +5902,7 @@
         <v>211</v>
       </c>
       <c r="K164" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M164" s="13"/>
       <c r="N164">
@@ -6018,7 +6018,7 @@
         <v>210</v>
       </c>
       <c r="K168" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="M168" s="13"/>
     </row>
@@ -6474,7 +6474,9 @@
       <c r="J182" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="K182" s="10"/>
+      <c r="K182" s="10" t="s">
+        <v>224</v>
+      </c>
       <c r="M182" s="13"/>
     </row>
     <row r="183" spans="1:13">
@@ -6875,10 +6877,10 @@
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
       <c r="I196" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J196" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M196" s="13">
         <v>2</v>
@@ -6904,10 +6906,10 @@
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
       <c r="I197" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J197" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M197" s="13"/>
     </row>
@@ -6931,10 +6933,13 @@
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
       <c r="I198" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J198" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="K198" t="s">
+        <v>224</v>
       </c>
       <c r="M198" s="13"/>
     </row>
@@ -6958,10 +6963,10 @@
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
       <c r="I199" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J199" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M199" s="13"/>
     </row>
@@ -6985,10 +6990,10 @@
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
       <c r="I200" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J200" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M200" s="13"/>
     </row>
@@ -7014,10 +7019,10 @@
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
       <c r="I201" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J201" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M201" s="13"/>
     </row>
@@ -7041,10 +7046,10 @@
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
       <c r="I202" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J202" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M202" s="13"/>
     </row>
@@ -7070,10 +7075,10 @@
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
       <c r="I203" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J203" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M203" s="13"/>
     </row>
@@ -7097,10 +7102,10 @@
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
       <c r="I204" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J204" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M204" s="13"/>
     </row>
@@ -7124,10 +7129,10 @@
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
       <c r="I205" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J205" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M205" s="13"/>
     </row>
@@ -7151,10 +7156,10 @@
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
       <c r="I206" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J206" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M206" s="13"/>
     </row>
@@ -7178,10 +7183,10 @@
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
       <c r="I207" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J207" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M207" s="13"/>
     </row>

</xml_diff>

<commit_message>
Feature added: Chart Title -> X Axis Title
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3992" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4022" uniqueCount="226">
   <si>
     <t>Chart</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>Known Issues: [ 1771500 ] Unexact chart display due to lack of chart size</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1773690 ] Chart titles angled text and vertical</t>
   </si>
 </sst>
 </file>
@@ -864,17 +867,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1197,10 +1200,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J208" sqref="J208"/>
+      <selection pane="bottomLeft" activeCell="I278" sqref="I278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1220,16 +1223,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1270,7 +1273,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1300,7 +1303,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1325,7 +1328,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1350,7 +1353,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1375,7 +1378,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1400,7 +1403,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1425,7 +1428,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1450,7 +1453,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1475,7 +1478,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="13"/>
+      <c r="M10" s="14"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2096,7 +2099,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2128,7 +2131,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="13"/>
+      <c r="M34" s="14"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2393,7 +2396,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="13">
+      <c r="M43" s="14">
         <v>2</v>
       </c>
     </row>
@@ -2425,7 +2428,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="13"/>
+      <c r="M44" s="14"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2457,7 +2460,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="13"/>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2489,7 +2492,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="13"/>
+      <c r="M46" s="14"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2521,7 +2524,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="13"/>
+      <c r="M47" s="14"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2553,7 +2556,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="13"/>
+      <c r="M48" s="14"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2585,7 +2588,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="13"/>
+      <c r="M49" s="14"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2617,7 +2620,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="13"/>
+      <c r="M50" s="14"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2806,7 +2809,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="13">
+      <c r="M57" s="14">
         <v>3</v>
       </c>
     </row>
@@ -2835,7 +2838,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="13"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2862,7 +2865,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="13"/>
+      <c r="M59" s="14"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2889,7 +2892,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="13"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3987,7 +3990,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="13">
+      <c r="M98" s="14">
         <v>2</v>
       </c>
     </row>
@@ -4014,7 +4017,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="13"/>
+      <c r="M99" s="14"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4042,7 +4045,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="13"/>
+      <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4067,7 +4070,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="13"/>
+      <c r="M101" s="14"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4094,7 +4097,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="13"/>
+      <c r="M102" s="14"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4121,7 +4124,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="13"/>
+      <c r="M103" s="14"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4150,7 +4153,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="13"/>
+      <c r="M104" s="14"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4179,7 +4182,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="13"/>
+      <c r="M105" s="14"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4213,7 +4216,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="13"/>
+      <c r="M106" s="14"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4247,7 +4250,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="13"/>
+      <c r="M107" s="14"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4281,7 +4284,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="13"/>
+      <c r="M108" s="14"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4315,7 +4318,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="13"/>
+      <c r="M109" s="14"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4344,7 +4347,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="13"/>
+      <c r="M110" s="14"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4378,7 +4381,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="13"/>
+      <c r="M111" s="14"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4412,7 +4415,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="13"/>
+      <c r="M112" s="14"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4446,7 +4449,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="13"/>
+      <c r="M113" s="14"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4477,7 +4480,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="13"/>
+      <c r="M114" s="14"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4508,7 +4511,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="13"/>
+      <c r="M115" s="14"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4539,7 +4542,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="13"/>
+      <c r="M116" s="14"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4564,7 +4567,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="13"/>
+      <c r="M117" s="14"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4591,7 +4594,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="13"/>
+      <c r="M118" s="14"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4825,7 +4828,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="13">
+      <c r="M127" s="14">
         <v>1</v>
       </c>
     </row>
@@ -4852,7 +4855,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="13"/>
+      <c r="M128" s="14"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4880,7 +4883,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="13"/>
+      <c r="M129" s="14"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4905,7 +4908,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="13"/>
+      <c r="M130" s="14"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4930,7 +4933,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="13"/>
+      <c r="M131" s="14"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4957,7 +4960,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="13"/>
+      <c r="M132" s="14"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4984,7 +4987,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="13"/>
+      <c r="M133" s="14"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5013,7 +5016,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="13"/>
+      <c r="M134" s="14"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5042,7 +5045,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="13"/>
+      <c r="M135" s="14"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5076,7 +5079,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="13"/>
+      <c r="M136" s="14"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5110,7 +5113,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="13"/>
+      <c r="M137" s="14"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5144,7 +5147,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="13"/>
+      <c r="M138" s="14"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5178,7 +5181,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="13"/>
+      <c r="M139" s="14"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5207,7 +5210,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="13"/>
+      <c r="M140" s="14"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5241,7 +5244,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="13"/>
+      <c r="M141" s="14"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5275,7 +5278,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="13"/>
+      <c r="M142" s="14"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5307,7 +5310,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="13"/>
+      <c r="M143" s="14"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5338,7 +5341,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="13"/>
+      <c r="M144" s="14"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5369,7 +5372,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="13"/>
+      <c r="M145" s="14"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5400,7 +5403,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="13"/>
+      <c r="M146" s="14"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5425,7 +5428,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="13"/>
+      <c r="M147" s="14"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5450,7 +5453,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="13"/>
+      <c r="M148" s="14"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5477,7 +5480,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="13"/>
+      <c r="M149" s="14"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5504,7 +5507,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="13"/>
+      <c r="M150" s="14"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5531,7 +5534,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="13"/>
+      <c r="M151" s="14"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5558,7 +5561,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="13"/>
+      <c r="M152" s="14"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5585,7 +5588,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="13"/>
+      <c r="M153" s="14"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5612,7 +5615,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="13"/>
+      <c r="M154" s="14"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5639,7 +5642,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="13"/>
+      <c r="M155" s="14"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5666,7 +5669,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="13"/>
+      <c r="M156" s="14"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5694,7 +5697,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="13"/>
+      <c r="M157" s="14"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5724,7 +5727,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="13"/>
+      <c r="M158" s="14"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5754,7 +5757,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="13"/>
+      <c r="M159" s="14"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5784,7 +5787,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="13"/>
+      <c r="M160" s="14"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5814,7 +5817,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="13"/>
+      <c r="M161" s="14"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5844,7 +5847,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="13"/>
+      <c r="M162" s="14"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5874,7 +5877,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="13"/>
+      <c r="M163" s="14"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5904,7 +5907,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="13"/>
+      <c r="M164" s="14"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5934,7 +5937,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="13">
+      <c r="M165" s="14">
         <v>1</v>
       </c>
     </row>
@@ -5963,7 +5966,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="13"/>
+      <c r="M166" s="14"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5990,7 +5993,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="13"/>
+      <c r="M167" s="14"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6020,7 +6023,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="13"/>
+      <c r="M168" s="14"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6047,7 +6050,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="13"/>
+      <c r="M169" s="14"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6074,7 +6077,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="13"/>
+      <c r="M170" s="14"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6103,7 +6106,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="13"/>
+      <c r="M171" s="14"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6132,7 +6135,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="13"/>
+      <c r="M172" s="14"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6163,7 +6166,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="13"/>
+      <c r="M173" s="14"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6194,7 +6197,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="13"/>
+      <c r="M174" s="14"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6230,7 +6233,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="13"/>
+      <c r="M175" s="14"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6266,7 +6269,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="13"/>
+      <c r="M176" s="14"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6302,7 +6305,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="13"/>
+      <c r="M177" s="14"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6338,7 +6341,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="13"/>
+      <c r="M178" s="14"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6369,7 +6372,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="13"/>
+      <c r="M179" s="14"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6405,7 +6408,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="13"/>
+      <c r="M180" s="14"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6441,7 +6444,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="13"/>
+      <c r="M181" s="14"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6477,7 +6480,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="13"/>
+      <c r="M182" s="14"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6510,7 +6513,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="13"/>
+      <c r="M183" s="14"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6543,7 +6546,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="13"/>
+      <c r="M184" s="14"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6576,7 +6579,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="13"/>
+      <c r="M185" s="14"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6603,7 +6606,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="13"/>
+      <c r="M186" s="14"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6630,7 +6633,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="13"/>
+      <c r="M187" s="14"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6659,7 +6662,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="13"/>
+      <c r="M188" s="14"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6882,7 +6885,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="13">
+      <c r="M196" s="14">
         <v>2</v>
       </c>
     </row>
@@ -6911,7 +6914,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="13"/>
+      <c r="M197" s="14"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6941,7 +6944,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="13"/>
+      <c r="M198" s="14"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6968,7 +6971,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="13"/>
+      <c r="M199" s="14"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6995,7 +6998,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="13"/>
+      <c r="M200" s="14"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7024,7 +7027,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="13"/>
+      <c r="M201" s="14"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7051,7 +7054,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="13"/>
+      <c r="M202" s="14"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7080,7 +7083,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="13"/>
+      <c r="M203" s="14"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7107,7 +7110,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="13"/>
+      <c r="M204" s="14"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7134,7 +7137,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="13"/>
+      <c r="M205" s="14"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7161,7 +7164,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="13"/>
+      <c r="M206" s="14"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7188,7 +7191,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="13"/>
+      <c r="M207" s="14"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7210,12 +7213,15 @@
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
       <c r="I208" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J208" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M208" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K208" t="s">
+        <v>225</v>
+      </c>
+      <c r="M208" s="14"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7237,12 +7243,15 @@
       <c r="G209" s="1"/>
       <c r="H209" s="1"/>
       <c r="I209" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J209" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M209" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K209" t="s">
+        <v>225</v>
+      </c>
+      <c r="M209" s="14"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7267,12 +7276,15 @@
       <c r="G210" s="1"/>
       <c r="H210" s="1"/>
       <c r="I210" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J210" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M210" s="13">
+        <v>211</v>
+      </c>
+      <c r="K210" t="s">
+        <v>220</v>
+      </c>
+      <c r="M210" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -7298,12 +7310,15 @@
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
       <c r="I211" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J211" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M211" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K211" t="s">
+        <v>221</v>
+      </c>
+      <c r="M211" s="14"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7327,12 +7342,15 @@
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
       <c r="I212" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J212" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M212" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K212" t="s">
+        <v>221</v>
+      </c>
+      <c r="M212" s="14"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7356,12 +7374,15 @@
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
       <c r="I213" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J213" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M213" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K213" t="s">
+        <v>221</v>
+      </c>
+      <c r="M213" s="14"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7385,12 +7406,15 @@
       <c r="G214" s="1"/>
       <c r="H214" s="1"/>
       <c r="I214" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J214" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M214" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K214" t="s">
+        <v>221</v>
+      </c>
+      <c r="M214" s="14"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7414,12 +7438,15 @@
       <c r="G215" s="1"/>
       <c r="H215" s="1"/>
       <c r="I215" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J215" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M215" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K215" t="s">
+        <v>221</v>
+      </c>
+      <c r="M215" s="14"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7443,12 +7470,15 @@
       <c r="G216" s="1"/>
       <c r="H216" s="1"/>
       <c r="I216" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J216" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M216" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K216" t="s">
+        <v>221</v>
+      </c>
+      <c r="M216" s="14"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7472,12 +7502,15 @@
       <c r="G217" s="1"/>
       <c r="H217" s="1"/>
       <c r="I217" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J217" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M217" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K217" t="s">
+        <v>221</v>
+      </c>
+      <c r="M217" s="14"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7501,12 +7534,12 @@
       <c r="G218" s="1"/>
       <c r="H218" s="1"/>
       <c r="I218" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J218" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M218" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M218" s="14"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7530,12 +7563,12 @@
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
       <c r="I219" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J219" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M219" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M219" s="14"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7557,12 +7590,12 @@
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
       <c r="I220" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J220" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M220" s="13">
+        <v>210</v>
+      </c>
+      <c r="M220" s="14">
         <v>1</v>
       </c>
     </row>
@@ -7586,12 +7619,12 @@
       <c r="G221" s="1"/>
       <c r="H221" s="1"/>
       <c r="I221" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J221" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M221" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M221" s="14"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7613,12 +7646,12 @@
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
       <c r="I222" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J222" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M222" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M222" s="14"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7640,12 +7673,15 @@
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
       <c r="I223" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J223" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M223" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K223" t="s">
+        <v>224</v>
+      </c>
+      <c r="M223" s="14"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7667,12 +7703,12 @@
       <c r="G224" s="1"/>
       <c r="H224" s="1"/>
       <c r="I224" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J224" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M224" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M224" s="14"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7694,12 +7730,12 @@
       <c r="G225" s="1"/>
       <c r="H225" s="1"/>
       <c r="I225" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J225" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M225" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M225" s="14"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7723,12 +7759,12 @@
       <c r="G226" s="1"/>
       <c r="H226" s="1"/>
       <c r="I226" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J226" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M226" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M226" s="14"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7752,12 +7788,12 @@
       <c r="G227" s="1"/>
       <c r="H227" s="1"/>
       <c r="I227" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J227" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M227" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M227" s="14"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7788,7 +7824,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="13"/>
+      <c r="M228" s="14"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7819,7 +7855,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="13"/>
+      <c r="M229" s="14"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7847,12 +7883,15 @@
         <v>94</v>
       </c>
       <c r="I230" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J230" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M230" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K230" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="M230" s="14"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7880,12 +7919,15 @@
         <v>95</v>
       </c>
       <c r="I231" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J231" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M231" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K231" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M231" s="14"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7913,12 +7955,15 @@
         <v>5</v>
       </c>
       <c r="I232" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J232" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M232" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K232" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M232" s="14"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7946,12 +7991,15 @@
         <v>6</v>
       </c>
       <c r="I233" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J233" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M233" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K233" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M233" s="14"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -7977,12 +8025,12 @@
       </c>
       <c r="H234" s="1"/>
       <c r="I234" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J234" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M234" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M234" s="14"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8010,12 +8058,15 @@
         <v>96</v>
       </c>
       <c r="I235" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J235" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M235" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K235" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M235" s="14"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8043,12 +8094,15 @@
         <v>97</v>
       </c>
       <c r="I236" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J236" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M236" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K236" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M236" s="14"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8076,12 +8130,15 @@
         <v>98</v>
       </c>
       <c r="I237" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J237" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M237" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K237" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="M237" s="14"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8109,12 +8166,12 @@
         <v>99</v>
       </c>
       <c r="I238" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J238" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M238" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M238" s="14"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8142,12 +8199,12 @@
         <v>101</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M239" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M239" s="14"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8175,12 +8232,12 @@
         <v>102</v>
       </c>
       <c r="I240" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J240" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M240" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M240" s="14"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8202,12 +8259,12 @@
       <c r="G241" s="1"/>
       <c r="H241" s="1"/>
       <c r="I241" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J241" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M241" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M241" s="14"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8229,12 +8286,12 @@
       <c r="G242" s="1"/>
       <c r="H242" s="1"/>
       <c r="I242" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J242" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M242" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M242" s="14"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8258,12 +8315,12 @@
       <c r="G243" s="1"/>
       <c r="H243" s="1"/>
       <c r="I243" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J243" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M243" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M243" s="14"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8292,7 +8349,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="13"/>
+      <c r="M244" s="14"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8321,7 +8378,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="13"/>
+      <c r="M245" s="14"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8350,7 +8407,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="13"/>
+      <c r="M246" s="14"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8379,7 +8436,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="13"/>
+      <c r="M247" s="14"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8408,7 +8465,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="13"/>
+      <c r="M248" s="14"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8437,7 +8494,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="13"/>
+      <c r="M249" s="14"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8466,7 +8523,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="13"/>
+      <c r="M250" s="14"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8488,12 +8545,12 @@
       <c r="G251" s="1"/>
       <c r="H251" s="1"/>
       <c r="I251" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J251" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M251" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M251" s="14"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8515,12 +8572,12 @@
       <c r="G252" s="1"/>
       <c r="H252" s="1"/>
       <c r="I252" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J252" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M252" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M252" s="14"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8542,12 +8599,12 @@
       <c r="G253" s="1"/>
       <c r="H253" s="1"/>
       <c r="I253" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J253" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M253" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M253" s="14"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8569,12 +8626,15 @@
       <c r="G254" s="1"/>
       <c r="H254" s="1"/>
       <c r="I254" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J254" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M254" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K254" t="s">
+        <v>224</v>
+      </c>
+      <c r="M254" s="14"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8596,12 +8656,12 @@
       <c r="G255" s="1"/>
       <c r="H255" s="1"/>
       <c r="I255" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J255" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M255" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M255" s="14"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8623,12 +8683,12 @@
       <c r="G256" s="1"/>
       <c r="H256" s="1"/>
       <c r="I256" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J256" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M256" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M256" s="14"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8650,12 +8710,12 @@
       <c r="G257" s="1"/>
       <c r="H257" s="1"/>
       <c r="I257" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J257" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M257" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M257" s="14"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8679,12 +8739,12 @@
       <c r="G258" s="1"/>
       <c r="H258" s="1"/>
       <c r="I258" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J258" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M258" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M258" s="14"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8706,12 +8766,12 @@
       <c r="G259" s="1"/>
       <c r="H259" s="1"/>
       <c r="I259" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J259" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M259" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M259" s="14"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8735,12 +8795,12 @@
       <c r="G260" s="1"/>
       <c r="H260" s="1"/>
       <c r="I260" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J260" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M260" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M260" s="14"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8762,12 +8822,12 @@
       <c r="G261" s="1"/>
       <c r="H261" s="1"/>
       <c r="I261" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J261" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M261" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M261" s="14"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8789,12 +8849,12 @@
       <c r="G262" s="1"/>
       <c r="H262" s="1"/>
       <c r="I262" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J262" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M262" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M262" s="14"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8816,12 +8876,12 @@
       <c r="G263" s="1"/>
       <c r="H263" s="1"/>
       <c r="I263" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J263" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M263" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M263" s="14"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8843,12 +8903,12 @@
       <c r="G264" s="1"/>
       <c r="H264" s="1"/>
       <c r="I264" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J264" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M264" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M264" s="14"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8870,12 +8930,15 @@
       <c r="G265" s="1"/>
       <c r="H265" s="1"/>
       <c r="I265" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J265" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M265" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K265" t="s">
+        <v>225</v>
+      </c>
+      <c r="M265" s="14"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8897,12 +8960,15 @@
       <c r="G266" s="1"/>
       <c r="H266" s="1"/>
       <c r="I266" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J266" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M266" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K266" t="s">
+        <v>225</v>
+      </c>
+      <c r="M266" s="14"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8924,12 +8990,15 @@
       <c r="G267" s="1"/>
       <c r="H267" s="1"/>
       <c r="I267" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J267" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M267" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K267" t="s">
+        <v>225</v>
+      </c>
+      <c r="M267" s="14"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -8951,12 +9020,15 @@
       <c r="G268" s="1"/>
       <c r="H268" s="1"/>
       <c r="I268" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J268" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M268" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K268" t="s">
+        <v>220</v>
+      </c>
+      <c r="M268" s="14"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -8980,12 +9052,15 @@
       <c r="G269" s="1"/>
       <c r="H269" s="1"/>
       <c r="I269" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J269" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M269" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K269" t="s">
+        <v>221</v>
+      </c>
+      <c r="M269" s="14"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9009,12 +9084,15 @@
       <c r="G270" s="1"/>
       <c r="H270" s="1"/>
       <c r="I270" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J270" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M270" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K270" t="s">
+        <v>221</v>
+      </c>
+      <c r="M270" s="14"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9038,12 +9116,15 @@
       <c r="G271" s="1"/>
       <c r="H271" s="1"/>
       <c r="I271" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J271" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M271" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K271" t="s">
+        <v>221</v>
+      </c>
+      <c r="M271" s="14"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9067,12 +9148,15 @@
       <c r="G272" s="1"/>
       <c r="H272" s="1"/>
       <c r="I272" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J272" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M272" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K272" t="s">
+        <v>221</v>
+      </c>
+      <c r="M272" s="14"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9096,12 +9180,15 @@
       <c r="G273" s="1"/>
       <c r="H273" s="1"/>
       <c r="I273" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J273" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M273" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K273" t="s">
+        <v>221</v>
+      </c>
+      <c r="M273" s="14"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9125,12 +9212,15 @@
       <c r="G274" s="1"/>
       <c r="H274" s="1"/>
       <c r="I274" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J274" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M274" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K274" t="s">
+        <v>221</v>
+      </c>
+      <c r="M274" s="14"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9154,12 +9244,15 @@
       <c r="G275" s="1"/>
       <c r="H275" s="1"/>
       <c r="I275" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J275" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M275" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K275" t="s">
+        <v>221</v>
+      </c>
+      <c r="M275" s="14"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9183,12 +9276,12 @@
       <c r="G276" s="1"/>
       <c r="H276" s="1"/>
       <c r="I276" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J276" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M276" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M276" s="14"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9212,12 +9305,12 @@
       <c r="G277" s="1"/>
       <c r="H277" s="1"/>
       <c r="I277" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J277" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M277" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M277" s="14"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9244,7 +9337,7 @@
       <c r="J278" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M278" s="13"/>
+      <c r="M278" s="14"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9271,7 +9364,7 @@
       <c r="J279" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M279" s="13"/>
+      <c r="M279" s="14"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9298,7 +9391,7 @@
       <c r="J280" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M280" s="13"/>
+      <c r="M280" s="14"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9325,7 +9418,7 @@
       <c r="J281" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M281" s="13"/>
+      <c r="M281" s="14"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9352,7 +9445,7 @@
       <c r="J282" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M282" s="13"/>
+      <c r="M282" s="14"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9379,7 +9472,7 @@
       <c r="J283" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M283" s="13"/>
+      <c r="M283" s="14"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9408,7 +9501,7 @@
       <c r="J284" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M284" s="13"/>
+      <c r="M284" s="14"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9437,7 +9530,7 @@
       <c r="J285" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M285" s="13"/>
+      <c r="M285" s="14"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9468,7 +9561,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="13"/>
+      <c r="M286" s="14"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9499,7 +9592,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="13"/>
+      <c r="M287" s="14"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9532,7 +9625,7 @@
       <c r="J288" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M288" s="13"/>
+      <c r="M288" s="14"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9565,7 +9658,7 @@
       <c r="J289" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M289" s="13"/>
+      <c r="M289" s="14"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9598,7 +9691,7 @@
       <c r="J290" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M290" s="13"/>
+      <c r="M290" s="14"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9631,7 +9724,7 @@
       <c r="J291" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M291" s="13"/>
+      <c r="M291" s="14"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9662,7 +9755,7 @@
       <c r="J292" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M292" s="13"/>
+      <c r="M292" s="14"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9695,7 +9788,7 @@
       <c r="J293" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M293" s="13"/>
+      <c r="M293" s="14"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9728,7 +9821,7 @@
       <c r="J294" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M294" s="13"/>
+      <c r="M294" s="14"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9761,7 +9854,7 @@
       <c r="J295" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M295" s="13"/>
+      <c r="M295" s="14"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9794,7 +9887,7 @@
       <c r="J296" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M296" s="13"/>
+      <c r="M296" s="14"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9827,7 +9920,7 @@
       <c r="J297" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M297" s="13"/>
+      <c r="M297" s="14"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9860,7 +9953,7 @@
       <c r="J298" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M298" s="13"/>
+      <c r="M298" s="14"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9887,7 +9980,7 @@
       <c r="J299" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M299" s="13"/>
+      <c r="M299" s="14"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -9914,7 +10007,7 @@
       <c r="J300" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M300" s="13"/>
+      <c r="M300" s="14"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -9943,7 +10036,7 @@
       <c r="J301" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M301" s="13"/>
+      <c r="M301" s="14"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -9972,7 +10065,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="13"/>
+      <c r="M302" s="14"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10001,7 +10094,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="13"/>
+      <c r="M303" s="14"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10030,7 +10123,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="13"/>
+      <c r="M304" s="14"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10059,7 +10152,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="13"/>
+      <c r="M305" s="14"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10088,7 +10181,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="13"/>
+      <c r="M306" s="14"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10117,7 +10210,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="13"/>
+      <c r="M307" s="14"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10146,7 +10239,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="13"/>
+      <c r="M308" s="14"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10173,7 +10266,7 @@
       <c r="J309" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M309" s="13"/>
+      <c r="M309" s="14"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10200,7 +10293,7 @@
       <c r="J310" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M310" s="13"/>
+      <c r="M310" s="14"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10227,7 +10320,7 @@
       <c r="J311" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M311" s="13"/>
+      <c r="M311" s="14"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10254,7 +10347,7 @@
       <c r="J312" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M312" s="13"/>
+      <c r="M312" s="14"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10281,7 +10374,7 @@
       <c r="J313" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M313" s="13"/>
+      <c r="M313" s="14"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10308,7 +10401,7 @@
       <c r="J314" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M314" s="13"/>
+      <c r="M314" s="14"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10335,7 +10428,7 @@
       <c r="J315" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M315" s="13"/>
+      <c r="M315" s="14"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10364,7 +10457,7 @@
       <c r="J316" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M316" s="13"/>
+      <c r="M316" s="14"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10391,7 +10484,7 @@
       <c r="J317" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M317" s="13"/>
+      <c r="M317" s="14"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10420,7 +10513,7 @@
       <c r="J318" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M318" s="13"/>
+      <c r="M318" s="14"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10447,7 +10540,7 @@
       <c r="J319" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M319" s="13"/>
+      <c r="M319" s="14"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10474,7 +10567,7 @@
       <c r="J320" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M320" s="13"/>
+      <c r="M320" s="14"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10501,7 +10594,7 @@
       <c r="J321" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M321" s="13"/>
+      <c r="M321" s="14"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10528,7 +10621,7 @@
       <c r="J322" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M322" s="13"/>
+      <c r="M322" s="14"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10555,7 +10648,7 @@
       <c r="J323" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M323" s="13"/>
+      <c r="M323" s="14"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10582,7 +10675,7 @@
       <c r="J324" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M324" s="13"/>
+      <c r="M324" s="14"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10609,7 +10702,7 @@
       <c r="J325" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M325" s="13"/>
+      <c r="M325" s="14"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10636,7 +10729,7 @@
       <c r="J326" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M326" s="13"/>
+      <c r="M326" s="14"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10665,7 +10758,7 @@
       <c r="J327" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M327" s="13"/>
+      <c r="M327" s="14"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10694,7 +10787,7 @@
       <c r="J328" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M328" s="13"/>
+      <c r="M328" s="14"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10723,7 +10816,7 @@
       <c r="J329" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M329" s="13"/>
+      <c r="M329" s="14"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10752,7 +10845,7 @@
       <c r="J330" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M330" s="13"/>
+      <c r="M330" s="14"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10781,7 +10874,7 @@
       <c r="J331" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M331" s="13"/>
+      <c r="M331" s="14"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10810,7 +10903,7 @@
       <c r="J332" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M332" s="13"/>
+      <c r="M332" s="14"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10839,7 +10932,7 @@
       <c r="J333" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M333" s="13"/>
+      <c r="M333" s="14"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10868,7 +10961,7 @@
       <c r="J334" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M334" s="13"/>
+      <c r="M334" s="14"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10897,7 +10990,7 @@
       <c r="J335" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M335" s="13"/>
+      <c r="M335" s="14"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11072,7 +11165,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="13">
+      <c r="M342" s="14">
         <v>1</v>
       </c>
     </row>
@@ -11099,7 +11192,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="13"/>
+      <c r="M343" s="14"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11124,7 +11217,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="13"/>
+      <c r="M344" s="14"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11149,7 +11242,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="13"/>
+      <c r="M345" s="14"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11174,7 +11267,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="13"/>
+      <c r="M346" s="14"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11199,7 +11292,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="13"/>
+      <c r="M347" s="14"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11226,7 +11319,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="13"/>
+      <c r="M348" s="14"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11253,7 +11346,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="13"/>
+      <c r="M349" s="14"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11282,7 +11375,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="13"/>
+      <c r="M350" s="14"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11311,7 +11404,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="13"/>
+      <c r="M351" s="14"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11342,7 +11435,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="13"/>
+      <c r="M352" s="14"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11373,7 +11466,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="13"/>
+      <c r="M353" s="14"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11404,7 +11497,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="13"/>
+      <c r="M354" s="14"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11435,7 +11528,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="13"/>
+      <c r="M355" s="14"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11464,7 +11557,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="13"/>
+      <c r="M356" s="14"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11495,7 +11588,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="13"/>
+      <c r="M357" s="14"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11526,7 +11619,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="13"/>
+      <c r="M358" s="14"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11557,7 +11650,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="13"/>
+      <c r="M359" s="14"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11588,7 +11681,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="13"/>
+      <c r="M360" s="14"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11619,7 +11712,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="13"/>
+      <c r="M361" s="14"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11650,7 +11743,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="13"/>
+      <c r="M362" s="14"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11675,7 +11768,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="13"/>
+      <c r="M363" s="14"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11700,7 +11793,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="13"/>
+      <c r="M364" s="14"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11727,7 +11820,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="13"/>
+      <c r="M365" s="14"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11754,7 +11847,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="13"/>
+      <c r="M366" s="14"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11781,7 +11874,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="13"/>
+      <c r="M367" s="14"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11808,7 +11901,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="13"/>
+      <c r="M368" s="14"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11835,7 +11928,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="13"/>
+      <c r="M369" s="14"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11862,7 +11955,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="13"/>
+      <c r="M370" s="14"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11889,7 +11982,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="13"/>
+      <c r="M371" s="14"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -11916,7 +12009,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="13"/>
+      <c r="M372" s="14"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -11941,7 +12034,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="13"/>
+      <c r="M373" s="14"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -11966,7 +12059,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="13"/>
+      <c r="M374" s="14"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -11991,7 +12084,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="13"/>
+      <c r="M375" s="14"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12016,7 +12109,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="13"/>
+      <c r="M376" s="14"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12041,7 +12134,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="13"/>
+      <c r="M377" s="14"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12066,7 +12159,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="13"/>
+      <c r="M378" s="14"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12091,7 +12184,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="13"/>
+      <c r="M379" s="14"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12118,7 +12211,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="13"/>
+      <c r="M380" s="14"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12143,7 +12236,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="13"/>
+      <c r="M381" s="14"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12170,7 +12263,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="13"/>
+      <c r="M382" s="14"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12195,7 +12288,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="13"/>
+      <c r="M383" s="14"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12220,7 +12313,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="13"/>
+      <c r="M384" s="14"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12245,7 +12338,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="13"/>
+      <c r="M385" s="14"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12270,7 +12363,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="13"/>
+      <c r="M386" s="14"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12343,7 +12436,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="13">
+      <c r="M389" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -12372,7 +12465,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="13"/>
+      <c r="M390" s="14"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12399,7 +12492,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="13"/>
+      <c r="M391" s="14"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12426,7 +12519,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="13"/>
+      <c r="M392" s="14"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12453,7 +12546,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="13"/>
+      <c r="M393" s="14"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12480,7 +12573,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="13"/>
+      <c r="M394" s="14"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12507,7 +12600,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="13"/>
+      <c r="M395" s="14"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12537,7 +12630,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="13">
+      <c r="M396" s="14">
         <v>1</v>
       </c>
     </row>
@@ -12566,7 +12659,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="13"/>
+      <c r="M397" s="14"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12593,7 +12686,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="13"/>
+      <c r="M398" s="14"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12620,7 +12713,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="13"/>
+      <c r="M399" s="14"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12647,7 +12740,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="13"/>
+      <c r="M400" s="14"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12674,7 +12767,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="13"/>
+      <c r="M401" s="14"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12701,7 +12794,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="13"/>
+      <c r="M402" s="14"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12728,7 +12821,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="13"/>
+      <c r="M403" s="14"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12755,7 +12848,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="13"/>
+      <c r="M404" s="14"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12782,7 +12875,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="13"/>
+      <c r="M405" s="14"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12809,7 +12902,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="13"/>
+      <c r="M406" s="14"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12836,7 +12929,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="13"/>
+      <c r="M407" s="14"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12865,7 +12958,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="13"/>
+      <c r="M408" s="14"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12892,7 +12985,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="13"/>
+      <c r="M409" s="14"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -12921,7 +13014,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="13"/>
+      <c r="M410" s="14"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -12948,7 +13041,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="13"/>
+      <c r="M411" s="14"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -12975,7 +13068,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="13"/>
+      <c r="M412" s="14"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13002,7 +13095,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="13"/>
+      <c r="M413" s="14"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13029,7 +13122,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="13"/>
+      <c r="M414" s="14"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13059,7 +13152,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="13">
+      <c r="M415" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -13088,7 +13181,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="13"/>
+      <c r="M416" s="14"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13117,7 +13210,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="13"/>
+      <c r="M417" s="14"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13146,7 +13239,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="13"/>
+      <c r="M418" s="14"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13175,7 +13268,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="13"/>
+      <c r="M419" s="14"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13204,7 +13297,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="13"/>
+      <c r="M420" s="14"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13234,7 +13327,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="13">
+      <c r="M421" s="14">
         <v>1</v>
       </c>
     </row>
@@ -13263,7 +13356,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="13"/>
+      <c r="M422" s="14"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13290,7 +13383,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="13"/>
+      <c r="M423" s="14"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13317,7 +13410,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="13"/>
+      <c r="M424" s="14"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13344,7 +13437,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="13"/>
+      <c r="M425" s="14"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13371,7 +13464,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="13"/>
+      <c r="M426" s="14"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13398,7 +13491,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="13"/>
+      <c r="M427" s="14"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13425,7 +13518,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="13"/>
+      <c r="M428" s="14"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13452,7 +13545,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="13"/>
+      <c r="M429" s="14"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13479,7 +13572,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="13"/>
+      <c r="M430" s="14"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13506,7 +13599,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="13"/>
+      <c r="M431" s="14"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13533,7 +13626,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="13"/>
+      <c r="M432" s="14"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13562,7 +13655,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="13"/>
+      <c r="M433" s="14"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13589,7 +13682,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="13"/>
+      <c r="M434" s="14"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13618,7 +13711,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="13"/>
+      <c r="M435" s="14"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13645,7 +13738,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="13"/>
+      <c r="M436" s="14"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13672,7 +13765,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="13"/>
+      <c r="M437" s="14"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13699,7 +13792,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="13"/>
+      <c r="M438" s="14"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13726,7 +13819,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="13"/>
+      <c r="M439" s="14"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13760,7 +13853,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="13">
+      <c r="M440" s="14">
         <v>1</v>
       </c>
     </row>
@@ -13793,7 +13886,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="13"/>
+      <c r="M441" s="14"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13824,7 +13917,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="13"/>
+      <c r="M442" s="14"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13855,7 +13948,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="13"/>
+      <c r="M443" s="14"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13886,7 +13979,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="13"/>
+      <c r="M444" s="14"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -13917,7 +14010,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="13"/>
+      <c r="M445" s="14"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -13948,7 +14041,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="13"/>
+      <c r="M446" s="14"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -13979,7 +14072,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="13"/>
+      <c r="M447" s="14"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14010,7 +14103,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="13"/>
+      <c r="M448" s="14"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14041,7 +14134,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="13"/>
+      <c r="M449" s="14"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14070,7 +14163,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="13"/>
+      <c r="M450" s="14"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14099,7 +14192,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="13"/>
+      <c r="M451" s="14"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14128,7 +14221,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="13"/>
+      <c r="M452" s="14"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14157,7 +14250,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="13"/>
+      <c r="M453" s="14"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14186,7 +14279,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="13"/>
+      <c r="M454" s="14"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14213,7 +14306,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="13"/>
+      <c r="M455" s="14"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14240,7 +14333,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="13"/>
+      <c r="M456" s="14"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14267,7 +14360,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="13"/>
+      <c r="M457" s="14"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14296,7 +14389,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="13"/>
+      <c r="M458" s="14"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14325,7 +14418,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="13"/>
+      <c r="M459" s="14"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14354,7 +14447,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="13"/>
+      <c r="M460" s="14"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14383,7 +14476,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="13"/>
+      <c r="M461" s="14"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14717,7 +14810,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="12">
+      <c r="M474" s="15">
         <v>1</v>
       </c>
     </row>
@@ -14746,7 +14839,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="12"/>
+      <c r="M475" s="15"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14773,7 +14866,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="12"/>
+      <c r="M476" s="15"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14800,7 +14893,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="12"/>
+      <c r="M477" s="15"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14827,7 +14920,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="12"/>
+      <c r="M478" s="15"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14854,7 +14947,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="12"/>
+      <c r="M479" s="15"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14881,7 +14974,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="12"/>
+      <c r="M480" s="15"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -14908,7 +15001,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="12"/>
+      <c r="M481" s="15"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -14935,7 +15028,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="12"/>
+      <c r="M482" s="15"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -14962,7 +15055,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="12"/>
+      <c r="M483" s="15"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15122,7 +15215,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="12">
+      <c r="M489" s="15">
         <v>2</v>
       </c>
     </row>
@@ -15149,7 +15242,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="12"/>
+      <c r="M490" s="15"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15174,7 +15267,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="12"/>
+      <c r="M491" s="15"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15199,7 +15292,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="12"/>
+      <c r="M492" s="15"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15224,7 +15317,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="12"/>
+      <c r="M493" s="15"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15251,7 +15344,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="12"/>
+      <c r="M494" s="15"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15278,7 +15371,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="12"/>
+      <c r="M495" s="15"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15305,7 +15398,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="12"/>
+      <c r="M496" s="15"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15332,7 +15425,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="12"/>
+      <c r="M497" s="15"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15385,7 +15478,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="12">
+      <c r="M499" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15412,7 +15505,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="12"/>
+      <c r="M500" s="15"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15437,7 +15530,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="12"/>
+      <c r="M501" s="15"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15462,7 +15555,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="12"/>
+      <c r="M502" s="15"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15487,7 +15580,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="12"/>
+      <c r="M503" s="15"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15512,7 +15605,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="12"/>
+      <c r="M504" s="15"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15539,7 +15632,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="12"/>
+      <c r="M505" s="15"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15564,7 +15657,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="12"/>
+      <c r="M506" s="15"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15591,7 +15684,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="12"/>
+      <c r="M507" s="15"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15616,7 +15709,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="12"/>
+      <c r="M508" s="15"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15641,7 +15734,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="12"/>
+      <c r="M509" s="15"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15666,7 +15759,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="12"/>
+      <c r="M510" s="15"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15691,7 +15784,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="12"/>
+      <c r="M511" s="15"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15718,7 +15811,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="12"/>
+      <c r="M512" s="15"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15745,7 +15838,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="12"/>
+      <c r="M513" s="15"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15770,7 +15863,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="12"/>
+      <c r="M514" s="15"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15795,7 +15888,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="12"/>
+      <c r="M515" s="15"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15823,7 +15916,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="12">
+      <c r="M516" s="15">
         <v>2</v>
       </c>
     </row>
@@ -15852,7 +15945,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="12"/>
+      <c r="M517" s="15"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15879,7 +15972,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="12"/>
+      <c r="M518" s="15"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15906,7 +15999,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="12"/>
+      <c r="M519" s="15"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -15935,7 +16028,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="12"/>
+      <c r="M520" s="15"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -15964,7 +16057,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="12"/>
+      <c r="M521" s="15"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -15993,7 +16086,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="12"/>
+      <c r="M522" s="15"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16022,7 +16115,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="12"/>
+      <c r="M523" s="15"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16051,7 +16144,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="12"/>
+      <c r="M524" s="15"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16080,7 +16173,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="12"/>
+      <c r="M525" s="15"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16107,7 +16200,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="12"/>
+      <c r="M526" s="15"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16134,7 +16227,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="12"/>
+      <c r="M527" s="15"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16159,11 +16252,6 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16180,6 +16268,11 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart Type -> 2D -> XY Chart (direct)
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4022" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4038" uniqueCount="226">
   <si>
     <t>Chart</t>
   </si>
@@ -867,17 +867,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,10 +1200,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I278" sqref="I278"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,16 +1223,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1328,7 +1328,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1353,7 +1353,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1378,7 +1378,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1403,7 +1403,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1428,7 +1428,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1453,7 +1453,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1478,7 +1478,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="13"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2099,7 +2099,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="14"/>
+      <c r="M34" s="13"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>209</v>
@@ -2396,7 +2396,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M43" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>209</v>
@@ -2428,7 +2428,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="14"/>
+      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2452,7 +2452,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>209</v>
@@ -2460,7 +2460,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="14"/>
+      <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2484,7 +2484,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>209</v>
@@ -2492,7 +2492,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="14"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2516,7 +2516,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>209</v>
@@ -2524,7 +2524,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="14"/>
+      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2548,7 +2548,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>209</v>
@@ -2556,7 +2556,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="14"/>
+      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2580,7 +2580,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>209</v>
@@ -2588,7 +2588,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="14"/>
+      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2612,7 +2612,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>209</v>
@@ -2620,7 +2620,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2809,7 +2809,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="14">
+      <c r="M57" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="14"/>
+      <c r="M58" s="13"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2865,7 +2865,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="14"/>
+      <c r="M59" s="13"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2892,7 +2892,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="14"/>
+      <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3990,7 +3990,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="14">
+      <c r="M98" s="13">
         <v>2</v>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="14"/>
+      <c r="M99" s="13"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4045,7 +4045,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="14"/>
+      <c r="M100" s="13"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4070,7 +4070,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="14"/>
+      <c r="M101" s="13"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4097,7 +4097,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="14"/>
+      <c r="M102" s="13"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4124,7 +4124,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="14"/>
+      <c r="M103" s="13"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4153,7 +4153,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="14"/>
+      <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4182,7 +4182,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="14"/>
+      <c r="M105" s="13"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4216,7 +4216,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="14"/>
+      <c r="M106" s="13"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4250,7 +4250,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="14"/>
+      <c r="M107" s="13"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4284,7 +4284,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="14"/>
+      <c r="M108" s="13"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4318,7 +4318,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="14"/>
+      <c r="M109" s="13"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4347,7 +4347,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="14"/>
+      <c r="M110" s="13"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4381,7 +4381,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="14"/>
+      <c r="M111" s="13"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4415,7 +4415,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="14"/>
+      <c r="M112" s="13"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4449,7 +4449,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="14"/>
+      <c r="M113" s="13"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4480,7 +4480,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="14"/>
+      <c r="M114" s="13"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4511,7 +4511,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="14"/>
+      <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4542,7 +4542,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="14"/>
+      <c r="M116" s="13"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4567,7 +4567,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="14"/>
+      <c r="M117" s="13"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4594,7 +4594,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="14"/>
+      <c r="M118" s="13"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4828,7 +4828,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="14">
+      <c r="M127" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4855,7 +4855,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="14"/>
+      <c r="M128" s="13"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4883,7 +4883,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="14"/>
+      <c r="M129" s="13"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4908,7 +4908,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="14"/>
+      <c r="M130" s="13"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4933,7 +4933,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="14"/>
+      <c r="M131" s="13"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4960,7 +4960,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="14"/>
+      <c r="M132" s="13"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4987,7 +4987,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="14"/>
+      <c r="M133" s="13"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5016,7 +5016,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="14"/>
+      <c r="M134" s="13"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5045,7 +5045,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="14"/>
+      <c r="M135" s="13"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5079,7 +5079,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="14"/>
+      <c r="M136" s="13"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5113,7 +5113,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="14"/>
+      <c r="M137" s="13"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5147,7 +5147,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="14"/>
+      <c r="M138" s="13"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5181,7 +5181,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="14"/>
+      <c r="M139" s="13"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5210,7 +5210,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="14"/>
+      <c r="M140" s="13"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5244,7 +5244,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="14"/>
+      <c r="M141" s="13"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5278,7 +5278,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="14"/>
+      <c r="M142" s="13"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5310,7 +5310,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="14"/>
+      <c r="M143" s="13"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5341,7 +5341,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="14"/>
+      <c r="M144" s="13"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5372,7 +5372,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="14"/>
+      <c r="M145" s="13"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5403,7 +5403,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="14"/>
+      <c r="M146" s="13"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5428,7 +5428,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="14"/>
+      <c r="M147" s="13"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5453,7 +5453,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="14"/>
+      <c r="M148" s="13"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5480,7 +5480,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="14"/>
+      <c r="M149" s="13"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5507,7 +5507,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="14"/>
+      <c r="M150" s="13"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5534,7 +5534,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="14"/>
+      <c r="M151" s="13"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5561,7 +5561,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="14"/>
+      <c r="M152" s="13"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5588,7 +5588,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="14"/>
+      <c r="M153" s="13"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5615,7 +5615,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="14"/>
+      <c r="M154" s="13"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5642,7 +5642,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="14"/>
+      <c r="M155" s="13"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5669,7 +5669,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="14"/>
+      <c r="M156" s="13"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5697,7 +5697,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="14"/>
+      <c r="M157" s="13"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5727,7 +5727,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="14"/>
+      <c r="M158" s="13"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5757,7 +5757,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="14"/>
+      <c r="M159" s="13"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5787,7 +5787,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="14"/>
+      <c r="M160" s="13"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5817,7 +5817,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="14"/>
+      <c r="M161" s="13"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5847,7 +5847,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="14"/>
+      <c r="M162" s="13"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5877,7 +5877,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="14"/>
+      <c r="M163" s="13"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5907,7 +5907,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="14"/>
+      <c r="M164" s="13"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5937,7 +5937,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="14">
+      <c r="M165" s="13">
         <v>1</v>
       </c>
     </row>
@@ -5966,7 +5966,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="14"/>
+      <c r="M166" s="13"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5993,7 +5993,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="14"/>
+      <c r="M167" s="13"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6023,7 +6023,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="14"/>
+      <c r="M168" s="13"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6050,7 +6050,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="14"/>
+      <c r="M169" s="13"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6077,7 +6077,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="14"/>
+      <c r="M170" s="13"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6106,7 +6106,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="14"/>
+      <c r="M171" s="13"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6135,7 +6135,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="14"/>
+      <c r="M172" s="13"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6166,7 +6166,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="14"/>
+      <c r="M173" s="13"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6197,7 +6197,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="14"/>
+      <c r="M174" s="13"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6233,7 +6233,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="14"/>
+      <c r="M175" s="13"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6269,7 +6269,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="14"/>
+      <c r="M176" s="13"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6305,7 +6305,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="14"/>
+      <c r="M177" s="13"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6341,7 +6341,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="14"/>
+      <c r="M178" s="13"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6372,7 +6372,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="14"/>
+      <c r="M179" s="13"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6408,7 +6408,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="14"/>
+      <c r="M180" s="13"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6444,7 +6444,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="14"/>
+      <c r="M181" s="13"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6480,7 +6480,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="14"/>
+      <c r="M182" s="13"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6513,7 +6513,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="14"/>
+      <c r="M183" s="13"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6546,7 +6546,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="14"/>
+      <c r="M184" s="13"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6579,7 +6579,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="14"/>
+      <c r="M185" s="13"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6606,7 +6606,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="14"/>
+      <c r="M186" s="13"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6633,7 +6633,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="14"/>
+      <c r="M187" s="13"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6662,7 +6662,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="14"/>
+      <c r="M188" s="13"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6885,7 +6885,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="14">
+      <c r="M196" s="13">
         <v>2</v>
       </c>
     </row>
@@ -6914,7 +6914,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="14"/>
+      <c r="M197" s="13"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6944,7 +6944,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="14"/>
+      <c r="M198" s="13"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6971,7 +6971,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="14"/>
+      <c r="M199" s="13"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -6998,7 +6998,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="14"/>
+      <c r="M200" s="13"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7027,7 +7027,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="14"/>
+      <c r="M201" s="13"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7054,7 +7054,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="14"/>
+      <c r="M202" s="13"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7083,7 +7083,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="14"/>
+      <c r="M203" s="13"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7110,7 +7110,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="14"/>
+      <c r="M204" s="13"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7137,7 +7137,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="14"/>
+      <c r="M205" s="13"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7164,7 +7164,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="14"/>
+      <c r="M206" s="13"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7191,7 +7191,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="14"/>
+      <c r="M207" s="13"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7221,7 +7221,7 @@
       <c r="K208" t="s">
         <v>225</v>
       </c>
-      <c r="M208" s="14"/>
+      <c r="M208" s="13"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7251,7 +7251,7 @@
       <c r="K209" t="s">
         <v>225</v>
       </c>
-      <c r="M209" s="14"/>
+      <c r="M209" s="13"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7284,7 +7284,7 @@
       <c r="K210" t="s">
         <v>220</v>
       </c>
-      <c r="M210" s="14">
+      <c r="M210" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -7318,7 +7318,7 @@
       <c r="K211" t="s">
         <v>221</v>
       </c>
-      <c r="M211" s="14"/>
+      <c r="M211" s="13"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7350,7 +7350,7 @@
       <c r="K212" t="s">
         <v>221</v>
       </c>
-      <c r="M212" s="14"/>
+      <c r="M212" s="13"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7382,7 +7382,7 @@
       <c r="K213" t="s">
         <v>221</v>
       </c>
-      <c r="M213" s="14"/>
+      <c r="M213" s="13"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7414,7 +7414,7 @@
       <c r="K214" t="s">
         <v>221</v>
       </c>
-      <c r="M214" s="14"/>
+      <c r="M214" s="13"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7446,7 +7446,7 @@
       <c r="K215" t="s">
         <v>221</v>
       </c>
-      <c r="M215" s="14"/>
+      <c r="M215" s="13"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7478,7 +7478,7 @@
       <c r="K216" t="s">
         <v>221</v>
       </c>
-      <c r="M216" s="14"/>
+      <c r="M216" s="13"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7510,7 +7510,7 @@
       <c r="K217" t="s">
         <v>221</v>
       </c>
-      <c r="M217" s="14"/>
+      <c r="M217" s="13"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7539,7 +7539,7 @@
       <c r="J218" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M218" s="14"/>
+      <c r="M218" s="13"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7568,7 +7568,7 @@
       <c r="J219" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M219" s="14"/>
+      <c r="M219" s="13"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7595,7 +7595,7 @@
       <c r="J220" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M220" s="14">
+      <c r="M220" s="13">
         <v>1</v>
       </c>
     </row>
@@ -7624,7 +7624,7 @@
       <c r="J221" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M221" s="14"/>
+      <c r="M221" s="13"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7651,7 +7651,7 @@
       <c r="J222" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M222" s="14"/>
+      <c r="M222" s="13"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7681,7 +7681,7 @@
       <c r="K223" t="s">
         <v>224</v>
       </c>
-      <c r="M223" s="14"/>
+      <c r="M223" s="13"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7708,7 +7708,7 @@
       <c r="J224" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M224" s="14"/>
+      <c r="M224" s="13"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7735,7 +7735,7 @@
       <c r="J225" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M225" s="14"/>
+      <c r="M225" s="13"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7764,7 +7764,7 @@
       <c r="J226" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M226" s="14"/>
+      <c r="M226" s="13"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7793,7 +7793,7 @@
       <c r="J227" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M227" s="14"/>
+      <c r="M227" s="13"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7824,7 +7824,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="14"/>
+      <c r="M228" s="13"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7855,7 +7855,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="14"/>
+      <c r="M229" s="13"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7891,7 +7891,7 @@
       <c r="K230" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M230" s="14"/>
+      <c r="M230" s="13"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7927,7 +7927,7 @@
       <c r="K231" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M231" s="14"/>
+      <c r="M231" s="13"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7963,7 +7963,7 @@
       <c r="K232" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M232" s="14"/>
+      <c r="M232" s="13"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -7999,7 +7999,7 @@
       <c r="K233" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M233" s="14"/>
+      <c r="M233" s="13"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -8030,7 +8030,7 @@
       <c r="J234" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M234" s="14"/>
+      <c r="M234" s="13"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8066,7 +8066,7 @@
       <c r="K235" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M235" s="14"/>
+      <c r="M235" s="13"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8102,7 +8102,7 @@
       <c r="K236" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M236" s="14"/>
+      <c r="M236" s="13"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8138,7 +8138,7 @@
       <c r="K237" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M237" s="14"/>
+      <c r="M237" s="13"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8171,7 +8171,7 @@
       <c r="J238" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M238" s="14"/>
+      <c r="M238" s="13"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8204,7 +8204,7 @@
       <c r="J239" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M239" s="14"/>
+      <c r="M239" s="13"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8237,7 +8237,7 @@
       <c r="J240" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M240" s="14"/>
+      <c r="M240" s="13"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8264,7 +8264,7 @@
       <c r="J241" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M241" s="14"/>
+      <c r="M241" s="13"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8291,7 +8291,7 @@
       <c r="J242" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M242" s="14"/>
+      <c r="M242" s="13"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8320,7 +8320,7 @@
       <c r="J243" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M243" s="14"/>
+      <c r="M243" s="13"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8349,7 +8349,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="14"/>
+      <c r="M244" s="13"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8378,7 +8378,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="14"/>
+      <c r="M245" s="13"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8407,7 +8407,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="14"/>
+      <c r="M246" s="13"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8436,7 +8436,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="14"/>
+      <c r="M247" s="13"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8465,7 +8465,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="14"/>
+      <c r="M248" s="13"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8494,7 +8494,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="14"/>
+      <c r="M249" s="13"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8523,7 +8523,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="14"/>
+      <c r="M250" s="13"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8550,7 +8550,7 @@
       <c r="J251" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M251" s="14"/>
+      <c r="M251" s="13"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8577,7 +8577,7 @@
       <c r="J252" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M252" s="14"/>
+      <c r="M252" s="13"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8604,7 +8604,7 @@
       <c r="J253" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M253" s="14"/>
+      <c r="M253" s="13"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8634,7 +8634,7 @@
       <c r="K254" t="s">
         <v>224</v>
       </c>
-      <c r="M254" s="14"/>
+      <c r="M254" s="13"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8661,7 +8661,7 @@
       <c r="J255" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M255" s="14"/>
+      <c r="M255" s="13"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8688,7 +8688,7 @@
       <c r="J256" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M256" s="14"/>
+      <c r="M256" s="13"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8715,7 +8715,7 @@
       <c r="J257" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M257" s="14"/>
+      <c r="M257" s="13"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8744,7 +8744,7 @@
       <c r="J258" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M258" s="14"/>
+      <c r="M258" s="13"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8771,7 +8771,7 @@
       <c r="J259" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M259" s="14"/>
+      <c r="M259" s="13"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8800,7 +8800,7 @@
       <c r="J260" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M260" s="14"/>
+      <c r="M260" s="13"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8827,7 +8827,7 @@
       <c r="J261" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M261" s="14"/>
+      <c r="M261" s="13"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8854,7 +8854,7 @@
       <c r="J262" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M262" s="14"/>
+      <c r="M262" s="13"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8881,7 +8881,7 @@
       <c r="J263" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M263" s="14"/>
+      <c r="M263" s="13"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8908,7 +8908,7 @@
       <c r="J264" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M264" s="14"/>
+      <c r="M264" s="13"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8938,7 +8938,7 @@
       <c r="K265" t="s">
         <v>225</v>
       </c>
-      <c r="M265" s="14"/>
+      <c r="M265" s="13"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8968,7 +8968,7 @@
       <c r="K266" t="s">
         <v>225</v>
       </c>
-      <c r="M266" s="14"/>
+      <c r="M266" s="13"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -8998,7 +8998,7 @@
       <c r="K267" t="s">
         <v>225</v>
       </c>
-      <c r="M267" s="14"/>
+      <c r="M267" s="13"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -9028,7 +9028,7 @@
       <c r="K268" t="s">
         <v>220</v>
       </c>
-      <c r="M268" s="14"/>
+      <c r="M268" s="13"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -9060,7 +9060,7 @@
       <c r="K269" t="s">
         <v>221</v>
       </c>
-      <c r="M269" s="14"/>
+      <c r="M269" s="13"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9092,7 +9092,7 @@
       <c r="K270" t="s">
         <v>221</v>
       </c>
-      <c r="M270" s="14"/>
+      <c r="M270" s="13"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9124,7 +9124,7 @@
       <c r="K271" t="s">
         <v>221</v>
       </c>
-      <c r="M271" s="14"/>
+      <c r="M271" s="13"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9156,7 +9156,7 @@
       <c r="K272" t="s">
         <v>221</v>
       </c>
-      <c r="M272" s="14"/>
+      <c r="M272" s="13"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9188,7 +9188,7 @@
       <c r="K273" t="s">
         <v>221</v>
       </c>
-      <c r="M273" s="14"/>
+      <c r="M273" s="13"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9220,7 +9220,7 @@
       <c r="K274" t="s">
         <v>221</v>
       </c>
-      <c r="M274" s="14"/>
+      <c r="M274" s="13"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9252,7 +9252,7 @@
       <c r="K275" t="s">
         <v>221</v>
       </c>
-      <c r="M275" s="14"/>
+      <c r="M275" s="13"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9281,7 +9281,7 @@
       <c r="J276" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M276" s="14"/>
+      <c r="M276" s="13"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9310,7 +9310,7 @@
       <c r="J277" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M277" s="14"/>
+      <c r="M277" s="13"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9332,12 +9332,12 @@
       <c r="G278" s="1"/>
       <c r="H278" s="1"/>
       <c r="I278" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J278" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M278" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M278" s="13"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9359,12 +9359,12 @@
       <c r="G279" s="1"/>
       <c r="H279" s="1"/>
       <c r="I279" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J279" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M279" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M279" s="13"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9386,12 +9386,12 @@
       <c r="G280" s="1"/>
       <c r="H280" s="1"/>
       <c r="I280" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J280" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M280" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M280" s="13"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9413,12 +9413,15 @@
       <c r="G281" s="1"/>
       <c r="H281" s="1"/>
       <c r="I281" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J281" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M281" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K281" t="s">
+        <v>224</v>
+      </c>
+      <c r="M281" s="13"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9440,12 +9443,12 @@
       <c r="G282" s="1"/>
       <c r="H282" s="1"/>
       <c r="I282" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J282" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M282" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M282" s="13"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9467,12 +9470,12 @@
       <c r="G283" s="1"/>
       <c r="H283" s="1"/>
       <c r="I283" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J283" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M283" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M283" s="13"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9496,12 +9499,12 @@
       <c r="G284" s="1"/>
       <c r="H284" s="1"/>
       <c r="I284" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J284" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M284" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M284" s="13"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9525,12 +9528,12 @@
       <c r="G285" s="1"/>
       <c r="H285" s="1"/>
       <c r="I285" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J285" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M285" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M285" s="13"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9561,7 +9564,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="14"/>
+      <c r="M286" s="13"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9592,7 +9595,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="14"/>
+      <c r="M287" s="13"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9620,12 +9623,15 @@
         <v>94</v>
       </c>
       <c r="I288" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J288" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M288" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K288" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="M288" s="13"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9653,12 +9659,15 @@
         <v>95</v>
       </c>
       <c r="I289" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J289" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M289" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K289" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M289" s="13"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9686,12 +9695,15 @@
         <v>5</v>
       </c>
       <c r="I290" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J290" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M290" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K290" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M290" s="13"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9719,12 +9731,15 @@
         <v>6</v>
       </c>
       <c r="I291" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J291" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M291" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K291" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M291" s="13"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9750,12 +9765,12 @@
       </c>
       <c r="H292" s="1"/>
       <c r="I292" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J292" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M292" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M292" s="13"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9783,12 +9798,15 @@
         <v>96</v>
       </c>
       <c r="I293" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J293" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M293" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K293" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M293" s="13"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9816,12 +9834,15 @@
         <v>97</v>
       </c>
       <c r="I294" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J294" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M294" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K294" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M294" s="13"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9849,12 +9870,15 @@
         <v>98</v>
       </c>
       <c r="I295" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J295" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M295" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K295" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="M295" s="13"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9882,12 +9906,12 @@
         <v>99</v>
       </c>
       <c r="I296" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J296" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M296" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M296" s="13"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9915,12 +9939,12 @@
         <v>101</v>
       </c>
       <c r="I297" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J297" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M297" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M297" s="13"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9948,12 +9972,12 @@
         <v>102</v>
       </c>
       <c r="I298" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J298" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M298" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M298" s="13"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -9975,12 +9999,12 @@
       <c r="G299" s="1"/>
       <c r="H299" s="1"/>
       <c r="I299" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J299" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M299" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M299" s="13"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -10002,12 +10026,12 @@
       <c r="G300" s="1"/>
       <c r="H300" s="1"/>
       <c r="I300" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J300" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M300" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M300" s="13"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -10031,12 +10055,12 @@
       <c r="G301" s="1"/>
       <c r="H301" s="1"/>
       <c r="I301" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J301" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M301" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M301" s="13"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -10065,7 +10089,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="14"/>
+      <c r="M302" s="13"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10094,7 +10118,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="14"/>
+      <c r="M303" s="13"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10123,7 +10147,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="14"/>
+      <c r="M304" s="13"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10152,7 +10176,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="14"/>
+      <c r="M305" s="13"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10181,7 +10205,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="14"/>
+      <c r="M306" s="13"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10210,7 +10234,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="14"/>
+      <c r="M307" s="13"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10239,7 +10263,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="14"/>
+      <c r="M308" s="13"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10261,12 +10285,12 @@
       <c r="G309" s="1"/>
       <c r="H309" s="1"/>
       <c r="I309" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J309" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M309" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M309" s="13"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10288,12 +10312,12 @@
       <c r="G310" s="1"/>
       <c r="H310" s="1"/>
       <c r="I310" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J310" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M310" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M310" s="13"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10315,12 +10339,12 @@
       <c r="G311" s="1"/>
       <c r="H311" s="1"/>
       <c r="I311" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J311" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M311" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M311" s="13"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10342,12 +10366,15 @@
       <c r="G312" s="1"/>
       <c r="H312" s="1"/>
       <c r="I312" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J312" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M312" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="K312" t="s">
+        <v>224</v>
+      </c>
+      <c r="M312" s="13"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10369,12 +10396,12 @@
       <c r="G313" s="1"/>
       <c r="H313" s="1"/>
       <c r="I313" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J313" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M313" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M313" s="13"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10396,12 +10423,12 @@
       <c r="G314" s="1"/>
       <c r="H314" s="1"/>
       <c r="I314" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J314" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M314" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M314" s="13"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10423,12 +10450,12 @@
       <c r="G315" s="1"/>
       <c r="H315" s="1"/>
       <c r="I315" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J315" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M315" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M315" s="13"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10452,12 +10479,12 @@
       <c r="G316" s="1"/>
       <c r="H316" s="1"/>
       <c r="I316" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J316" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M316" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M316" s="13"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10479,12 +10506,12 @@
       <c r="G317" s="1"/>
       <c r="H317" s="1"/>
       <c r="I317" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J317" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M317" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M317" s="13"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10508,12 +10535,12 @@
       <c r="G318" s="1"/>
       <c r="H318" s="1"/>
       <c r="I318" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J318" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M318" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M318" s="13"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10535,12 +10562,12 @@
       <c r="G319" s="1"/>
       <c r="H319" s="1"/>
       <c r="I319" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J319" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M319" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M319" s="13"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10562,12 +10589,12 @@
       <c r="G320" s="1"/>
       <c r="H320" s="1"/>
       <c r="I320" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J320" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M320" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M320" s="13"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10589,12 +10616,12 @@
       <c r="G321" s="1"/>
       <c r="H321" s="1"/>
       <c r="I321" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J321" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M321" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M321" s="13"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10616,12 +10643,12 @@
       <c r="G322" s="1"/>
       <c r="H322" s="1"/>
       <c r="I322" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J322" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M322" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M322" s="13"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10643,12 +10670,12 @@
       <c r="G323" s="1"/>
       <c r="H323" s="1"/>
       <c r="I323" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J323" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M323" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M323" s="13"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10670,12 +10697,12 @@
       <c r="G324" s="1"/>
       <c r="H324" s="1"/>
       <c r="I324" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J324" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M324" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M324" s="13"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10697,12 +10724,12 @@
       <c r="G325" s="1"/>
       <c r="H325" s="1"/>
       <c r="I325" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J325" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M325" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M325" s="13"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10724,12 +10751,15 @@
       <c r="G326" s="1"/>
       <c r="H326" s="1"/>
       <c r="I326" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J326" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M326" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K326" t="s">
+        <v>221</v>
+      </c>
+      <c r="M326" s="13"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10753,12 +10783,15 @@
       <c r="G327" s="1"/>
       <c r="H327" s="1"/>
       <c r="I327" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J327" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M327" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K327" t="s">
+        <v>221</v>
+      </c>
+      <c r="M327" s="13"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10782,12 +10815,15 @@
       <c r="G328" s="1"/>
       <c r="H328" s="1"/>
       <c r="I328" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J328" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M328" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K328" t="s">
+        <v>221</v>
+      </c>
+      <c r="M328" s="13"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10811,12 +10847,15 @@
       <c r="G329" s="1"/>
       <c r="H329" s="1"/>
       <c r="I329" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J329" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M329" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K329" t="s">
+        <v>221</v>
+      </c>
+      <c r="M329" s="13"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10840,12 +10879,15 @@
       <c r="G330" s="1"/>
       <c r="H330" s="1"/>
       <c r="I330" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J330" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M330" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K330" t="s">
+        <v>221</v>
+      </c>
+      <c r="M330" s="13"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10869,12 +10911,15 @@
       <c r="G331" s="1"/>
       <c r="H331" s="1"/>
       <c r="I331" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J331" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M331" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K331" t="s">
+        <v>221</v>
+      </c>
+      <c r="M331" s="13"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10898,12 +10943,15 @@
       <c r="G332" s="1"/>
       <c r="H332" s="1"/>
       <c r="I332" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J332" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M332" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K332" t="s">
+        <v>221</v>
+      </c>
+      <c r="M332" s="13"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10927,12 +10975,12 @@
       <c r="G333" s="1"/>
       <c r="H333" s="1"/>
       <c r="I333" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J333" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M333" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M333" s="13"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -10956,12 +11004,12 @@
       <c r="G334" s="1"/>
       <c r="H334" s="1"/>
       <c r="I334" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J334" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M334" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M334" s="13"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -10985,12 +11033,12 @@
       <c r="G335" s="1"/>
       <c r="H335" s="1"/>
       <c r="I335" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J335" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M335" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="M335" s="13"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11165,7 +11213,7 @@
       <c r="J342" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M342" s="14">
+      <c r="M342" s="13">
         <v>1</v>
       </c>
     </row>
@@ -11192,7 +11240,7 @@
       <c r="J343" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M343" s="14"/>
+      <c r="M343" s="13"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11217,7 +11265,7 @@
       <c r="J344" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M344" s="14"/>
+      <c r="M344" s="13"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11242,7 +11290,7 @@
       <c r="J345" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M345" s="14"/>
+      <c r="M345" s="13"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11267,7 +11315,7 @@
       <c r="J346" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M346" s="14"/>
+      <c r="M346" s="13"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11292,7 +11340,7 @@
       <c r="J347" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M347" s="14"/>
+      <c r="M347" s="13"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11319,7 +11367,7 @@
       <c r="J348" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M348" s="14"/>
+      <c r="M348" s="13"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11346,7 +11394,7 @@
       <c r="J349" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M349" s="14"/>
+      <c r="M349" s="13"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11375,7 +11423,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="14"/>
+      <c r="M350" s="13"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11404,7 +11452,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="14"/>
+      <c r="M351" s="13"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11435,7 +11483,7 @@
       <c r="J352" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M352" s="14"/>
+      <c r="M352" s="13"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11466,7 +11514,7 @@
       <c r="J353" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M353" s="14"/>
+      <c r="M353" s="13"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11497,7 +11545,7 @@
       <c r="J354" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M354" s="14"/>
+      <c r="M354" s="13"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11528,7 +11576,7 @@
       <c r="J355" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M355" s="14"/>
+      <c r="M355" s="13"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11557,7 +11605,7 @@
       <c r="J356" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M356" s="14"/>
+      <c r="M356" s="13"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11588,7 +11636,7 @@
       <c r="J357" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M357" s="14"/>
+      <c r="M357" s="13"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11619,7 +11667,7 @@
       <c r="J358" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M358" s="14"/>
+      <c r="M358" s="13"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11650,7 +11698,7 @@
       <c r="J359" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M359" s="14"/>
+      <c r="M359" s="13"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11681,7 +11729,7 @@
       <c r="J360" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M360" s="14"/>
+      <c r="M360" s="13"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11712,7 +11760,7 @@
       <c r="J361" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M361" s="14"/>
+      <c r="M361" s="13"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11743,7 +11791,7 @@
       <c r="J362" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M362" s="14"/>
+      <c r="M362" s="13"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11768,7 +11816,7 @@
       <c r="J363" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M363" s="14"/>
+      <c r="M363" s="13"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11793,7 +11841,7 @@
       <c r="J364" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M364" s="14"/>
+      <c r="M364" s="13"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11820,7 +11868,7 @@
       <c r="J365" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M365" s="14"/>
+      <c r="M365" s="13"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11847,7 +11895,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="14"/>
+      <c r="M366" s="13"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11874,7 +11922,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="14"/>
+      <c r="M367" s="13"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11901,7 +11949,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="14"/>
+      <c r="M368" s="13"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -11928,7 +11976,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="14"/>
+      <c r="M369" s="13"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -11955,7 +12003,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="14"/>
+      <c r="M370" s="13"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -11982,7 +12030,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="14"/>
+      <c r="M371" s="13"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -12009,7 +12057,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="14"/>
+      <c r="M372" s="13"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -12034,7 +12082,7 @@
       <c r="J373" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M373" s="14"/>
+      <c r="M373" s="13"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -12059,7 +12107,7 @@
       <c r="J374" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M374" s="14"/>
+      <c r="M374" s="13"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -12084,7 +12132,7 @@
       <c r="J375" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M375" s="14"/>
+      <c r="M375" s="13"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12109,7 +12157,7 @@
       <c r="J376" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M376" s="14"/>
+      <c r="M376" s="13"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12134,7 +12182,7 @@
       <c r="J377" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M377" s="14"/>
+      <c r="M377" s="13"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12159,7 +12207,7 @@
       <c r="J378" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M378" s="14"/>
+      <c r="M378" s="13"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12184,7 +12232,7 @@
       <c r="J379" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M379" s="14"/>
+      <c r="M379" s="13"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12211,7 +12259,7 @@
       <c r="J380" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M380" s="14"/>
+      <c r="M380" s="13"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12236,7 +12284,7 @@
       <c r="J381" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M381" s="14"/>
+      <c r="M381" s="13"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12263,7 +12311,7 @@
       <c r="J382" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M382" s="14"/>
+      <c r="M382" s="13"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12288,7 +12336,7 @@
       <c r="J383" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M383" s="14"/>
+      <c r="M383" s="13"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12313,7 +12361,7 @@
       <c r="J384" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M384" s="14"/>
+      <c r="M384" s="13"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12338,7 +12386,7 @@
       <c r="J385" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M385" s="14"/>
+      <c r="M385" s="13"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12363,7 +12411,7 @@
       <c r="J386" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M386" s="14"/>
+      <c r="M386" s="13"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12436,7 +12484,7 @@
       <c r="J389" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M389" s="14">
+      <c r="M389" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -12465,7 +12513,7 @@
       <c r="J390" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M390" s="14"/>
+      <c r="M390" s="13"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12492,7 +12540,7 @@
       <c r="J391" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M391" s="14"/>
+      <c r="M391" s="13"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12519,7 +12567,7 @@
       <c r="J392" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M392" s="14"/>
+      <c r="M392" s="13"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12546,7 +12594,7 @@
       <c r="J393" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M393" s="14"/>
+      <c r="M393" s="13"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12573,7 +12621,7 @@
       <c r="J394" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M394" s="14"/>
+      <c r="M394" s="13"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12600,7 +12648,7 @@
       <c r="J395" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M395" s="14"/>
+      <c r="M395" s="13"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12630,7 +12678,7 @@
       <c r="J396" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M396" s="14">
+      <c r="M396" s="13">
         <v>1</v>
       </c>
     </row>
@@ -12659,7 +12707,7 @@
       <c r="J397" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M397" s="14"/>
+      <c r="M397" s="13"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12686,7 +12734,7 @@
       <c r="J398" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M398" s="14"/>
+      <c r="M398" s="13"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12713,7 +12761,7 @@
       <c r="J399" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M399" s="14"/>
+      <c r="M399" s="13"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12740,7 +12788,7 @@
       <c r="J400" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M400" s="14"/>
+      <c r="M400" s="13"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12767,7 +12815,7 @@
       <c r="J401" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M401" s="14"/>
+      <c r="M401" s="13"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12794,7 +12842,7 @@
       <c r="J402" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M402" s="14"/>
+      <c r="M402" s="13"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12821,7 +12869,7 @@
       <c r="J403" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M403" s="14"/>
+      <c r="M403" s="13"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12848,7 +12896,7 @@
       <c r="J404" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M404" s="14"/>
+      <c r="M404" s="13"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12875,7 +12923,7 @@
       <c r="J405" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M405" s="14"/>
+      <c r="M405" s="13"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -12902,7 +12950,7 @@
       <c r="J406" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M406" s="14"/>
+      <c r="M406" s="13"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -12929,7 +12977,7 @@
       <c r="J407" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M407" s="14"/>
+      <c r="M407" s="13"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -12958,7 +13006,7 @@
       <c r="J408" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M408" s="14"/>
+      <c r="M408" s="13"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -12985,7 +13033,7 @@
       <c r="J409" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M409" s="14"/>
+      <c r="M409" s="13"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -13014,7 +13062,7 @@
       <c r="J410" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M410" s="14"/>
+      <c r="M410" s="13"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -13041,7 +13089,7 @@
       <c r="J411" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M411" s="14"/>
+      <c r="M411" s="13"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -13068,7 +13116,7 @@
       <c r="J412" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M412" s="14"/>
+      <c r="M412" s="13"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13095,7 +13143,7 @@
       <c r="J413" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M413" s="14"/>
+      <c r="M413" s="13"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13122,7 +13170,7 @@
       <c r="J414" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M414" s="14"/>
+      <c r="M414" s="13"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13152,7 +13200,7 @@
       <c r="J415" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M415" s="14">
+      <c r="M415" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -13181,7 +13229,7 @@
       <c r="J416" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M416" s="14"/>
+      <c r="M416" s="13"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13210,7 +13258,7 @@
       <c r="J417" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M417" s="14"/>
+      <c r="M417" s="13"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13239,7 +13287,7 @@
       <c r="J418" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M418" s="14"/>
+      <c r="M418" s="13"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13268,7 +13316,7 @@
       <c r="J419" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M419" s="14"/>
+      <c r="M419" s="13"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13297,7 +13345,7 @@
       <c r="J420" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M420" s="14"/>
+      <c r="M420" s="13"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13327,7 +13375,7 @@
       <c r="J421" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M421" s="14">
+      <c r="M421" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13356,7 +13404,7 @@
       <c r="J422" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M422" s="14"/>
+      <c r="M422" s="13"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13383,7 +13431,7 @@
       <c r="J423" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M423" s="14"/>
+      <c r="M423" s="13"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13410,7 +13458,7 @@
       <c r="J424" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M424" s="14"/>
+      <c r="M424" s="13"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13437,7 +13485,7 @@
       <c r="J425" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M425" s="14"/>
+      <c r="M425" s="13"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13464,7 +13512,7 @@
       <c r="J426" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M426" s="14"/>
+      <c r="M426" s="13"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13491,7 +13539,7 @@
       <c r="J427" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M427" s="14"/>
+      <c r="M427" s="13"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13518,7 +13566,7 @@
       <c r="J428" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M428" s="14"/>
+      <c r="M428" s="13"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13545,7 +13593,7 @@
       <c r="J429" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M429" s="14"/>
+      <c r="M429" s="13"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13572,7 +13620,7 @@
       <c r="J430" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M430" s="14"/>
+      <c r="M430" s="13"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13599,7 +13647,7 @@
       <c r="J431" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M431" s="14"/>
+      <c r="M431" s="13"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13626,7 +13674,7 @@
       <c r="J432" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M432" s="14"/>
+      <c r="M432" s="13"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13655,7 +13703,7 @@
       <c r="J433" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M433" s="14"/>
+      <c r="M433" s="13"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13682,7 +13730,7 @@
       <c r="J434" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M434" s="14"/>
+      <c r="M434" s="13"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13711,7 +13759,7 @@
       <c r="J435" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M435" s="14"/>
+      <c r="M435" s="13"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13738,7 +13786,7 @@
       <c r="J436" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M436" s="14"/>
+      <c r="M436" s="13"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13765,7 +13813,7 @@
       <c r="J437" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M437" s="14"/>
+      <c r="M437" s="13"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13792,7 +13840,7 @@
       <c r="J438" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M438" s="14"/>
+      <c r="M438" s="13"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13819,7 +13867,7 @@
       <c r="J439" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M439" s="14"/>
+      <c r="M439" s="13"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13853,7 +13901,7 @@
       <c r="J440" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M440" s="14">
+      <c r="M440" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13886,7 +13934,7 @@
       <c r="J441" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M441" s="14"/>
+      <c r="M441" s="13"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -13917,7 +13965,7 @@
       <c r="J442" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M442" s="14"/>
+      <c r="M442" s="13"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -13948,7 +13996,7 @@
       <c r="J443" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M443" s="14"/>
+      <c r="M443" s="13"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -13979,7 +14027,7 @@
       <c r="J444" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M444" s="14"/>
+      <c r="M444" s="13"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -14010,7 +14058,7 @@
       <c r="J445" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M445" s="14"/>
+      <c r="M445" s="13"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -14041,7 +14089,7 @@
       <c r="J446" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M446" s="14"/>
+      <c r="M446" s="13"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -14072,7 +14120,7 @@
       <c r="J447" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M447" s="14"/>
+      <c r="M447" s="13"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14103,7 +14151,7 @@
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="14"/>
+      <c r="M448" s="13"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14134,7 +14182,7 @@
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="14"/>
+      <c r="M449" s="13"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14163,7 +14211,7 @@
       <c r="J450" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M450" s="14"/>
+      <c r="M450" s="13"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14192,7 +14240,7 @@
       <c r="J451" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M451" s="14"/>
+      <c r="M451" s="13"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14221,7 +14269,7 @@
       <c r="J452" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M452" s="14"/>
+      <c r="M452" s="13"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14250,7 +14298,7 @@
       <c r="J453" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M453" s="14"/>
+      <c r="M453" s="13"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14279,7 +14327,7 @@
       <c r="J454" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M454" s="14"/>
+      <c r="M454" s="13"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14306,7 +14354,7 @@
       <c r="J455" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M455" s="14"/>
+      <c r="M455" s="13"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14333,7 +14381,7 @@
       <c r="J456" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M456" s="14"/>
+      <c r="M456" s="13"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14360,7 +14408,7 @@
       <c r="J457" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M457" s="14"/>
+      <c r="M457" s="13"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14389,7 +14437,7 @@
       <c r="J458" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M458" s="14"/>
+      <c r="M458" s="13"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14418,7 +14466,7 @@
       <c r="J459" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M459" s="14"/>
+      <c r="M459" s="13"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14447,7 +14495,7 @@
       <c r="J460" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M460" s="14"/>
+      <c r="M460" s="13"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14476,7 +14524,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="14"/>
+      <c r="M461" s="13"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14810,7 +14858,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="15">
+      <c r="M474" s="12">
         <v>1</v>
       </c>
     </row>
@@ -14839,7 +14887,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="15"/>
+      <c r="M475" s="12"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14866,7 +14914,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="15"/>
+      <c r="M476" s="12"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -14893,7 +14941,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="15"/>
+      <c r="M477" s="12"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -14920,7 +14968,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="15"/>
+      <c r="M478" s="12"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -14947,7 +14995,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="15"/>
+      <c r="M479" s="12"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -14974,7 +15022,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="15"/>
+      <c r="M480" s="12"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15001,7 +15049,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="15"/>
+      <c r="M481" s="12"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15028,7 +15076,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="15"/>
+      <c r="M482" s="12"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15055,7 +15103,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="15"/>
+      <c r="M483" s="12"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15215,7 +15263,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="15">
+      <c r="M489" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15242,7 +15290,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="15"/>
+      <c r="M490" s="12"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15267,7 +15315,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="15"/>
+      <c r="M491" s="12"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15292,7 +15340,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="15"/>
+      <c r="M492" s="12"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15317,7 +15365,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="15"/>
+      <c r="M493" s="12"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15344,7 +15392,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="15"/>
+      <c r="M494" s="12"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15371,7 +15419,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="15"/>
+      <c r="M495" s="12"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15398,7 +15446,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="15"/>
+      <c r="M496" s="12"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15425,7 +15473,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="15"/>
+      <c r="M497" s="12"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15478,7 +15526,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="15">
+      <c r="M499" s="12">
         <v>1</v>
       </c>
     </row>
@@ -15505,7 +15553,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="15"/>
+      <c r="M500" s="12"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15530,7 +15578,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="15"/>
+      <c r="M501" s="12"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15555,7 +15603,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="15"/>
+      <c r="M502" s="12"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15580,7 +15628,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="15"/>
+      <c r="M503" s="12"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15605,7 +15653,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="15"/>
+      <c r="M504" s="12"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15632,7 +15680,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="15"/>
+      <c r="M505" s="12"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15657,7 +15705,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="15"/>
+      <c r="M506" s="12"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15684,7 +15732,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="15"/>
+      <c r="M507" s="12"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15709,7 +15757,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="15"/>
+      <c r="M508" s="12"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15734,7 +15782,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="15"/>
+      <c r="M509" s="12"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15759,7 +15807,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="15"/>
+      <c r="M510" s="12"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15784,7 +15832,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="15"/>
+      <c r="M511" s="12"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15811,7 +15859,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="15"/>
+      <c r="M512" s="12"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15838,7 +15886,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="15"/>
+      <c r="M513" s="12"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15863,7 +15911,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="15"/>
+      <c r="M514" s="12"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -15888,7 +15936,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="15"/>
+      <c r="M515" s="12"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -15916,7 +15964,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="15">
+      <c r="M516" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15945,7 +15993,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="15"/>
+      <c r="M517" s="12"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -15972,7 +16020,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="15"/>
+      <c r="M518" s="12"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -15999,7 +16047,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="15"/>
+      <c r="M519" s="12"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16028,7 +16076,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="15"/>
+      <c r="M520" s="12"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16057,7 +16105,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="15"/>
+      <c r="M521" s="12"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16086,7 +16134,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="15"/>
+      <c r="M522" s="12"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16115,7 +16163,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="15"/>
+      <c r="M523" s="12"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16144,7 +16192,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="15"/>
+      <c r="M524" s="12"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16173,7 +16221,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="15"/>
+      <c r="M525" s="12"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16200,7 +16248,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="15"/>
+      <c r="M526" s="12"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16227,7 +16275,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="15"/>
+      <c r="M527" s="12"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16252,6 +16300,11 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16268,11 +16321,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart -> X Axis -> Label
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4055" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4060" uniqueCount="228">
   <si>
     <t>Chart</t>
   </si>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>{Left/Right/Top/Bottom}</t>
+  </si>
+  <si>
+    <t>Known issues: [ 1777562 ] Axis label order and text flow</t>
   </si>
 </sst>
 </file>
@@ -1203,10 +1206,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I395" sqref="I395"/>
+      <selection pane="bottomLeft" activeCell="E419" sqref="E419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12726,10 +12729,10 @@
       <c r="G396" s="1"/>
       <c r="H396" s="1"/>
       <c r="I396" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J396" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M396" s="13">
         <v>1</v>
@@ -12755,10 +12758,10 @@
       <c r="G397" s="1"/>
       <c r="H397" s="1"/>
       <c r="I397" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J397" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M397" s="13"/>
     </row>
@@ -12782,10 +12785,10 @@
       <c r="G398" s="1"/>
       <c r="H398" s="1"/>
       <c r="I398" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J398" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M398" s="13"/>
     </row>
@@ -12809,10 +12812,13 @@
       <c r="G399" s="1"/>
       <c r="H399" s="1"/>
       <c r="I399" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J399" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="K399" t="s">
+        <v>224</v>
       </c>
       <c r="M399" s="13"/>
     </row>
@@ -12836,10 +12842,10 @@
       <c r="G400" s="1"/>
       <c r="H400" s="1"/>
       <c r="I400" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J400" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M400" s="13"/>
     </row>
@@ -12863,10 +12869,10 @@
       <c r="G401" s="1"/>
       <c r="H401" s="1"/>
       <c r="I401" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J401" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M401" s="13"/>
     </row>
@@ -12890,10 +12896,10 @@
       <c r="G402" s="1"/>
       <c r="H402" s="1"/>
       <c r="I402" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J402" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M402" s="13"/>
     </row>
@@ -12917,10 +12923,10 @@
       <c r="G403" s="1"/>
       <c r="H403" s="1"/>
       <c r="I403" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J403" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M403" s="13"/>
     </row>
@@ -12944,10 +12950,13 @@
       <c r="G404" s="1"/>
       <c r="H404" s="1"/>
       <c r="I404" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J404" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="K404" t="s">
+        <v>224</v>
       </c>
       <c r="M404" s="13"/>
     </row>
@@ -12971,10 +12980,10 @@
       <c r="G405" s="1"/>
       <c r="H405" s="1"/>
       <c r="I405" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J405" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M405" s="13"/>
     </row>
@@ -12998,10 +13007,10 @@
       <c r="G406" s="1"/>
       <c r="H406" s="1"/>
       <c r="I406" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J406" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M406" s="13"/>
     </row>
@@ -13025,10 +13034,10 @@
       <c r="G407" s="1"/>
       <c r="H407" s="1"/>
       <c r="I407" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J407" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M407" s="13"/>
     </row>
@@ -13054,10 +13063,10 @@
       <c r="G408" s="1"/>
       <c r="H408" s="1"/>
       <c r="I408" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J408" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M408" s="13"/>
     </row>
@@ -13081,10 +13090,10 @@
       <c r="G409" s="1"/>
       <c r="H409" s="1"/>
       <c r="I409" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J409" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M409" s="13"/>
     </row>
@@ -13110,10 +13119,10 @@
       <c r="G410" s="1"/>
       <c r="H410" s="1"/>
       <c r="I410" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J410" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M410" s="13"/>
     </row>
@@ -13137,10 +13146,10 @@
       <c r="G411" s="1"/>
       <c r="H411" s="1"/>
       <c r="I411" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J411" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M411" s="13"/>
     </row>
@@ -13164,10 +13173,10 @@
       <c r="G412" s="1"/>
       <c r="H412" s="1"/>
       <c r="I412" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J412" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M412" s="13"/>
     </row>
@@ -13191,10 +13200,10 @@
       <c r="G413" s="1"/>
       <c r="H413" s="1"/>
       <c r="I413" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J413" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M413" s="13"/>
     </row>
@@ -13218,10 +13227,10 @@
       <c r="G414" s="1"/>
       <c r="H414" s="1"/>
       <c r="I414" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J414" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M414" s="13"/>
       <c r="N414">
@@ -13248,10 +13257,10 @@
       <c r="G415" s="1"/>
       <c r="H415" s="1"/>
       <c r="I415" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J415" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M415" s="13">
         <v>0.5</v>
@@ -13277,10 +13286,13 @@
       <c r="G416" s="1"/>
       <c r="H416" s="1"/>
       <c r="I416" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J416" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="K416" t="s">
+        <v>227</v>
       </c>
       <c r="M416" s="13"/>
     </row>
@@ -13306,10 +13318,13 @@
       <c r="G417" s="1"/>
       <c r="H417" s="1"/>
       <c r="I417" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J417" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="K417" t="s">
+        <v>227</v>
       </c>
       <c r="M417" s="13"/>
     </row>
@@ -13335,10 +13350,13 @@
       <c r="G418" s="1"/>
       <c r="H418" s="1"/>
       <c r="I418" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J418" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="K418" t="s">
+        <v>227</v>
       </c>
       <c r="M418" s="13"/>
     </row>
@@ -13364,10 +13382,10 @@
       <c r="G419" s="1"/>
       <c r="H419" s="1"/>
       <c r="I419" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J419" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M419" s="13"/>
     </row>
@@ -13393,10 +13411,10 @@
       <c r="G420" s="1"/>
       <c r="H420" s="1"/>
       <c r="I420" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J420" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M420" s="13"/>
       <c r="N420">

</xml_diff>

<commit_message>
Added feature: Chart -> Axis -> Scale (direct)
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4060" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4065" uniqueCount="228">
   <si>
     <t>Chart</t>
   </si>
@@ -873,17 +873,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1207,9 +1207,9 @@
   <dimension ref="A1:N530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E419" sqref="E419"/>
+      <selection pane="bottomLeft" activeCell="I450" sqref="I450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1229,16 +1229,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1334,7 +1334,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1359,7 +1359,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1384,7 +1384,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1409,7 +1409,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1434,7 +1434,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1459,7 +1459,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1484,7 +1484,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="13"/>
+      <c r="M10" s="14"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2105,7 +2105,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="13"/>
+      <c r="M34" s="14"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="13">
+      <c r="M43" s="14">
         <v>2</v>
       </c>
     </row>
@@ -2434,7 +2434,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="13"/>
+      <c r="M44" s="14"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2466,7 +2466,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="13"/>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2498,7 +2498,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="13"/>
+      <c r="M46" s="14"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2530,7 +2530,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="13"/>
+      <c r="M47" s="14"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2562,7 +2562,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="13"/>
+      <c r="M48" s="14"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2594,7 +2594,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="13"/>
+      <c r="M49" s="14"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2626,7 +2626,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="13"/>
+      <c r="M50" s="14"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2815,7 +2815,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="13">
+      <c r="M57" s="14">
         <v>3</v>
       </c>
     </row>
@@ -2844,7 +2844,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="13"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2871,7 +2871,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="13"/>
+      <c r="M59" s="14"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2898,7 +2898,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="13"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3996,7 +3996,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="13">
+      <c r="M98" s="14">
         <v>2</v>
       </c>
     </row>
@@ -4023,7 +4023,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="13"/>
+      <c r="M99" s="14"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4051,7 +4051,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="13"/>
+      <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4076,7 +4076,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="13"/>
+      <c r="M101" s="14"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4103,7 +4103,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="13"/>
+      <c r="M102" s="14"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4130,7 +4130,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="13"/>
+      <c r="M103" s="14"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4159,7 +4159,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="13"/>
+      <c r="M104" s="14"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4188,7 +4188,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="13"/>
+      <c r="M105" s="14"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4222,7 +4222,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="13"/>
+      <c r="M106" s="14"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4256,7 +4256,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="13"/>
+      <c r="M107" s="14"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4290,7 +4290,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="13"/>
+      <c r="M108" s="14"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4324,7 +4324,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="13"/>
+      <c r="M109" s="14"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4353,7 +4353,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="13"/>
+      <c r="M110" s="14"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4387,7 +4387,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="13"/>
+      <c r="M111" s="14"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4421,7 +4421,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="13"/>
+      <c r="M112" s="14"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4455,7 +4455,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="13"/>
+      <c r="M113" s="14"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4486,7 +4486,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="13"/>
+      <c r="M114" s="14"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4517,7 +4517,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="13"/>
+      <c r="M115" s="14"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4548,7 +4548,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="13"/>
+      <c r="M116" s="14"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4573,7 +4573,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="13"/>
+      <c r="M117" s="14"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4600,7 +4600,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="13"/>
+      <c r="M118" s="14"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4834,7 +4834,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="13">
+      <c r="M127" s="14">
         <v>1</v>
       </c>
     </row>
@@ -4861,7 +4861,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="13"/>
+      <c r="M128" s="14"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4889,7 +4889,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="13"/>
+      <c r="M129" s="14"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4914,7 +4914,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="13"/>
+      <c r="M130" s="14"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4939,7 +4939,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="13"/>
+      <c r="M131" s="14"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4966,7 +4966,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="13"/>
+      <c r="M132" s="14"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4993,7 +4993,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="13"/>
+      <c r="M133" s="14"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5022,7 +5022,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="13"/>
+      <c r="M134" s="14"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5051,7 +5051,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="13"/>
+      <c r="M135" s="14"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5085,7 +5085,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="13"/>
+      <c r="M136" s="14"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5119,7 +5119,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="13"/>
+      <c r="M137" s="14"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5153,7 +5153,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="13"/>
+      <c r="M138" s="14"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5187,7 +5187,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="13"/>
+      <c r="M139" s="14"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5216,7 +5216,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="13"/>
+      <c r="M140" s="14"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5250,7 +5250,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="13"/>
+      <c r="M141" s="14"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5284,7 +5284,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="13"/>
+      <c r="M142" s="14"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5316,7 +5316,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="13"/>
+      <c r="M143" s="14"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5347,7 +5347,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="13"/>
+      <c r="M144" s="14"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5378,7 +5378,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="13"/>
+      <c r="M145" s="14"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5409,7 +5409,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="13"/>
+      <c r="M146" s="14"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5434,7 +5434,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="13"/>
+      <c r="M147" s="14"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5459,7 +5459,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="13"/>
+      <c r="M148" s="14"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5486,7 +5486,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="13"/>
+      <c r="M149" s="14"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5513,7 +5513,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="13"/>
+      <c r="M150" s="14"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5540,7 +5540,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="13"/>
+      <c r="M151" s="14"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5567,7 +5567,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="13"/>
+      <c r="M152" s="14"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5594,7 +5594,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="13"/>
+      <c r="M153" s="14"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5621,7 +5621,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="13"/>
+      <c r="M154" s="14"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5648,7 +5648,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="13"/>
+      <c r="M155" s="14"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5675,7 +5675,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="13"/>
+      <c r="M156" s="14"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5703,7 +5703,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="13"/>
+      <c r="M157" s="14"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5733,7 +5733,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="13"/>
+      <c r="M158" s="14"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5763,7 +5763,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="13"/>
+      <c r="M159" s="14"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5793,7 +5793,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="13"/>
+      <c r="M160" s="14"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5823,7 +5823,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="13"/>
+      <c r="M161" s="14"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5853,7 +5853,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="13"/>
+      <c r="M162" s="14"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5883,7 +5883,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="13"/>
+      <c r="M163" s="14"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5913,7 +5913,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="13"/>
+      <c r="M164" s="14"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5943,7 +5943,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="13">
+      <c r="M165" s="14">
         <v>1</v>
       </c>
     </row>
@@ -5972,7 +5972,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="13"/>
+      <c r="M166" s="14"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5999,7 +5999,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="13"/>
+      <c r="M167" s="14"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6029,7 +6029,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="13"/>
+      <c r="M168" s="14"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6056,7 +6056,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="13"/>
+      <c r="M169" s="14"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6083,7 +6083,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="13"/>
+      <c r="M170" s="14"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6112,7 +6112,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="13"/>
+      <c r="M171" s="14"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6141,7 +6141,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="13"/>
+      <c r="M172" s="14"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6172,7 +6172,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="13"/>
+      <c r="M173" s="14"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6203,7 +6203,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="13"/>
+      <c r="M174" s="14"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6239,7 +6239,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="13"/>
+      <c r="M175" s="14"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6275,7 +6275,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="13"/>
+      <c r="M176" s="14"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6311,7 +6311,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="13"/>
+      <c r="M177" s="14"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6347,7 +6347,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="13"/>
+      <c r="M178" s="14"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6378,7 +6378,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="13"/>
+      <c r="M179" s="14"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6414,7 +6414,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="13"/>
+      <c r="M180" s="14"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6450,7 +6450,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="13"/>
+      <c r="M181" s="14"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6486,7 +6486,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="13"/>
+      <c r="M182" s="14"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6519,7 +6519,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="13"/>
+      <c r="M183" s="14"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6552,7 +6552,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="13"/>
+      <c r="M184" s="14"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6585,7 +6585,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="13"/>
+      <c r="M185" s="14"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6612,7 +6612,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="13"/>
+      <c r="M186" s="14"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6639,7 +6639,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="13"/>
+      <c r="M187" s="14"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6668,7 +6668,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="13"/>
+      <c r="M188" s="14"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6891,7 +6891,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="13">
+      <c r="M196" s="14">
         <v>2</v>
       </c>
     </row>
@@ -6920,7 +6920,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="13"/>
+      <c r="M197" s="14"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6950,7 +6950,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="13"/>
+      <c r="M198" s="14"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6977,7 +6977,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="13"/>
+      <c r="M199" s="14"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -7004,7 +7004,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="13"/>
+      <c r="M200" s="14"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7033,7 +7033,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="13"/>
+      <c r="M201" s="14"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7060,7 +7060,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="13"/>
+      <c r="M202" s="14"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7089,7 +7089,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="13"/>
+      <c r="M203" s="14"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7116,7 +7116,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="13"/>
+      <c r="M204" s="14"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7143,7 +7143,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="13"/>
+      <c r="M205" s="14"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7170,7 +7170,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="13"/>
+      <c r="M206" s="14"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7197,7 +7197,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="13"/>
+      <c r="M207" s="14"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7227,7 +7227,7 @@
       <c r="K208" t="s">
         <v>225</v>
       </c>
-      <c r="M208" s="13"/>
+      <c r="M208" s="14"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7257,7 +7257,7 @@
       <c r="K209" t="s">
         <v>225</v>
       </c>
-      <c r="M209" s="13"/>
+      <c r="M209" s="14"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7290,7 +7290,7 @@
       <c r="K210" t="s">
         <v>220</v>
       </c>
-      <c r="M210" s="13">
+      <c r="M210" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -7324,7 +7324,7 @@
       <c r="K211" t="s">
         <v>221</v>
       </c>
-      <c r="M211" s="13"/>
+      <c r="M211" s="14"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7356,7 +7356,7 @@
       <c r="K212" t="s">
         <v>221</v>
       </c>
-      <c r="M212" s="13"/>
+      <c r="M212" s="14"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7388,7 +7388,7 @@
       <c r="K213" t="s">
         <v>221</v>
       </c>
-      <c r="M213" s="13"/>
+      <c r="M213" s="14"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7420,7 +7420,7 @@
       <c r="K214" t="s">
         <v>221</v>
       </c>
-      <c r="M214" s="13"/>
+      <c r="M214" s="14"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7452,7 +7452,7 @@
       <c r="K215" t="s">
         <v>221</v>
       </c>
-      <c r="M215" s="13"/>
+      <c r="M215" s="14"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7484,7 +7484,7 @@
       <c r="K216" t="s">
         <v>221</v>
       </c>
-      <c r="M216" s="13"/>
+      <c r="M216" s="14"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7516,7 +7516,7 @@
       <c r="K217" t="s">
         <v>221</v>
       </c>
-      <c r="M217" s="13"/>
+      <c r="M217" s="14"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7545,7 +7545,7 @@
       <c r="J218" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M218" s="13"/>
+      <c r="M218" s="14"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7574,7 +7574,7 @@
       <c r="J219" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M219" s="13"/>
+      <c r="M219" s="14"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7601,7 +7601,7 @@
       <c r="J220" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M220" s="13">
+      <c r="M220" s="14">
         <v>1</v>
       </c>
     </row>
@@ -7630,7 +7630,7 @@
       <c r="J221" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M221" s="13"/>
+      <c r="M221" s="14"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7657,7 +7657,7 @@
       <c r="J222" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M222" s="13"/>
+      <c r="M222" s="14"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7687,7 +7687,7 @@
       <c r="K223" t="s">
         <v>224</v>
       </c>
-      <c r="M223" s="13"/>
+      <c r="M223" s="14"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7714,7 +7714,7 @@
       <c r="J224" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M224" s="13"/>
+      <c r="M224" s="14"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7741,7 +7741,7 @@
       <c r="J225" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M225" s="13"/>
+      <c r="M225" s="14"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7770,7 +7770,7 @@
       <c r="J226" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M226" s="13"/>
+      <c r="M226" s="14"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7799,7 +7799,7 @@
       <c r="J227" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M227" s="13"/>
+      <c r="M227" s="14"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7830,7 +7830,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="13"/>
+      <c r="M228" s="14"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7861,7 +7861,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="13"/>
+      <c r="M229" s="14"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7897,7 +7897,7 @@
       <c r="K230" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M230" s="13"/>
+      <c r="M230" s="14"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7933,7 +7933,7 @@
       <c r="K231" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M231" s="13"/>
+      <c r="M231" s="14"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7969,7 +7969,7 @@
       <c r="K232" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M232" s="13"/>
+      <c r="M232" s="14"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -8005,7 +8005,7 @@
       <c r="K233" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M233" s="13"/>
+      <c r="M233" s="14"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -8036,7 +8036,7 @@
       <c r="J234" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M234" s="13"/>
+      <c r="M234" s="14"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8072,7 +8072,7 @@
       <c r="K235" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M235" s="13"/>
+      <c r="M235" s="14"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8108,7 +8108,7 @@
       <c r="K236" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M236" s="13"/>
+      <c r="M236" s="14"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8144,7 +8144,7 @@
       <c r="K237" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M237" s="13"/>
+      <c r="M237" s="14"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8177,7 +8177,7 @@
       <c r="J238" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M238" s="13"/>
+      <c r="M238" s="14"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8210,7 +8210,7 @@
       <c r="J239" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M239" s="13"/>
+      <c r="M239" s="14"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8243,7 +8243,7 @@
       <c r="J240" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M240" s="13"/>
+      <c r="M240" s="14"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8270,7 +8270,7 @@
       <c r="J241" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M241" s="13"/>
+      <c r="M241" s="14"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8297,7 +8297,7 @@
       <c r="J242" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M242" s="13"/>
+      <c r="M242" s="14"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8326,7 +8326,7 @@
       <c r="J243" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M243" s="13"/>
+      <c r="M243" s="14"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8355,7 +8355,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="13"/>
+      <c r="M244" s="14"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8384,7 +8384,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="13"/>
+      <c r="M245" s="14"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8413,7 +8413,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="13"/>
+      <c r="M246" s="14"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8442,7 +8442,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="13"/>
+      <c r="M247" s="14"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8471,7 +8471,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="13"/>
+      <c r="M248" s="14"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8500,7 +8500,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="13"/>
+      <c r="M249" s="14"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8529,7 +8529,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="13"/>
+      <c r="M250" s="14"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8556,7 +8556,7 @@
       <c r="J251" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M251" s="13"/>
+      <c r="M251" s="14"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8583,7 +8583,7 @@
       <c r="J252" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M252" s="13"/>
+      <c r="M252" s="14"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8610,7 +8610,7 @@
       <c r="J253" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M253" s="13"/>
+      <c r="M253" s="14"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8640,7 +8640,7 @@
       <c r="K254" t="s">
         <v>224</v>
       </c>
-      <c r="M254" s="13"/>
+      <c r="M254" s="14"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8667,7 +8667,7 @@
       <c r="J255" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M255" s="13"/>
+      <c r="M255" s="14"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8694,7 +8694,7 @@
       <c r="J256" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M256" s="13"/>
+      <c r="M256" s="14"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8721,7 +8721,7 @@
       <c r="J257" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M257" s="13"/>
+      <c r="M257" s="14"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8750,7 +8750,7 @@
       <c r="J258" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M258" s="13"/>
+      <c r="M258" s="14"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8777,7 +8777,7 @@
       <c r="J259" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M259" s="13"/>
+      <c r="M259" s="14"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8806,7 +8806,7 @@
       <c r="J260" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M260" s="13"/>
+      <c r="M260" s="14"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8833,7 +8833,7 @@
       <c r="J261" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M261" s="13"/>
+      <c r="M261" s="14"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8860,7 +8860,7 @@
       <c r="J262" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M262" s="13"/>
+      <c r="M262" s="14"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8887,7 +8887,7 @@
       <c r="J263" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M263" s="13"/>
+      <c r="M263" s="14"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8914,7 +8914,7 @@
       <c r="J264" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M264" s="13"/>
+      <c r="M264" s="14"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8944,7 +8944,7 @@
       <c r="K265" t="s">
         <v>225</v>
       </c>
-      <c r="M265" s="13"/>
+      <c r="M265" s="14"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8974,7 +8974,7 @@
       <c r="K266" t="s">
         <v>225</v>
       </c>
-      <c r="M266" s="13"/>
+      <c r="M266" s="14"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -9004,7 +9004,7 @@
       <c r="K267" t="s">
         <v>225</v>
       </c>
-      <c r="M267" s="13"/>
+      <c r="M267" s="14"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -9034,7 +9034,7 @@
       <c r="K268" t="s">
         <v>220</v>
       </c>
-      <c r="M268" s="13"/>
+      <c r="M268" s="14"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -9066,7 +9066,7 @@
       <c r="K269" t="s">
         <v>221</v>
       </c>
-      <c r="M269" s="13"/>
+      <c r="M269" s="14"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9098,7 +9098,7 @@
       <c r="K270" t="s">
         <v>221</v>
       </c>
-      <c r="M270" s="13"/>
+      <c r="M270" s="14"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9130,7 +9130,7 @@
       <c r="K271" t="s">
         <v>221</v>
       </c>
-      <c r="M271" s="13"/>
+      <c r="M271" s="14"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9162,7 +9162,7 @@
       <c r="K272" t="s">
         <v>221</v>
       </c>
-      <c r="M272" s="13"/>
+      <c r="M272" s="14"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9194,7 +9194,7 @@
       <c r="K273" t="s">
         <v>221</v>
       </c>
-      <c r="M273" s="13"/>
+      <c r="M273" s="14"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9226,7 +9226,7 @@
       <c r="K274" t="s">
         <v>221</v>
       </c>
-      <c r="M274" s="13"/>
+      <c r="M274" s="14"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9258,7 +9258,7 @@
       <c r="K275" t="s">
         <v>221</v>
       </c>
-      <c r="M275" s="13"/>
+      <c r="M275" s="14"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9287,7 +9287,7 @@
       <c r="J276" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M276" s="13"/>
+      <c r="M276" s="14"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9316,7 +9316,7 @@
       <c r="J277" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M277" s="13"/>
+      <c r="M277" s="14"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9343,7 +9343,7 @@
       <c r="J278" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M278" s="13"/>
+      <c r="M278" s="14"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9370,7 +9370,7 @@
       <c r="J279" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M279" s="13"/>
+      <c r="M279" s="14"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9397,7 +9397,7 @@
       <c r="J280" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M280" s="13"/>
+      <c r="M280" s="14"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9427,7 +9427,7 @@
       <c r="K281" t="s">
         <v>224</v>
       </c>
-      <c r="M281" s="13"/>
+      <c r="M281" s="14"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9454,7 +9454,7 @@
       <c r="J282" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M282" s="13"/>
+      <c r="M282" s="14"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9481,7 +9481,7 @@
       <c r="J283" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M283" s="13"/>
+      <c r="M283" s="14"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9510,7 +9510,7 @@
       <c r="J284" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M284" s="13"/>
+      <c r="M284" s="14"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9539,7 +9539,7 @@
       <c r="J285" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M285" s="13"/>
+      <c r="M285" s="14"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9570,7 +9570,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="13"/>
+      <c r="M286" s="14"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9601,7 +9601,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="13"/>
+      <c r="M287" s="14"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9637,7 +9637,7 @@
       <c r="K288" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M288" s="13"/>
+      <c r="M288" s="14"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9673,7 +9673,7 @@
       <c r="K289" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M289" s="13"/>
+      <c r="M289" s="14"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9709,7 +9709,7 @@
       <c r="K290" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M290" s="13"/>
+      <c r="M290" s="14"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9745,7 +9745,7 @@
       <c r="K291" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M291" s="13"/>
+      <c r="M291" s="14"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9776,7 +9776,7 @@
       <c r="J292" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M292" s="13"/>
+      <c r="M292" s="14"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9812,7 +9812,7 @@
       <c r="K293" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M293" s="13"/>
+      <c r="M293" s="14"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9848,7 +9848,7 @@
       <c r="K294" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M294" s="13"/>
+      <c r="M294" s="14"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9884,7 +9884,7 @@
       <c r="K295" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M295" s="13"/>
+      <c r="M295" s="14"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9917,7 +9917,7 @@
       <c r="J296" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M296" s="13"/>
+      <c r="M296" s="14"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9950,7 +9950,7 @@
       <c r="J297" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M297" s="13"/>
+      <c r="M297" s="14"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9983,7 +9983,7 @@
       <c r="J298" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M298" s="13"/>
+      <c r="M298" s="14"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -10010,7 +10010,7 @@
       <c r="J299" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M299" s="13"/>
+      <c r="M299" s="14"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -10037,7 +10037,7 @@
       <c r="J300" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M300" s="13"/>
+      <c r="M300" s="14"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -10066,7 +10066,7 @@
       <c r="J301" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M301" s="13"/>
+      <c r="M301" s="14"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -10095,7 +10095,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="13"/>
+      <c r="M302" s="14"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10124,7 +10124,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="13"/>
+      <c r="M303" s="14"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10153,7 +10153,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="13"/>
+      <c r="M304" s="14"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10182,7 +10182,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="13"/>
+      <c r="M305" s="14"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10211,7 +10211,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="13"/>
+      <c r="M306" s="14"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10240,7 +10240,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="13"/>
+      <c r="M307" s="14"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10269,7 +10269,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="13"/>
+      <c r="M308" s="14"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10296,7 +10296,7 @@
       <c r="J309" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M309" s="13"/>
+      <c r="M309" s="14"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10323,7 +10323,7 @@
       <c r="J310" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M310" s="13"/>
+      <c r="M310" s="14"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10350,7 +10350,7 @@
       <c r="J311" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M311" s="13"/>
+      <c r="M311" s="14"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10380,7 +10380,7 @@
       <c r="K312" t="s">
         <v>224</v>
       </c>
-      <c r="M312" s="13"/>
+      <c r="M312" s="14"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10407,7 +10407,7 @@
       <c r="J313" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M313" s="13"/>
+      <c r="M313" s="14"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10434,7 +10434,7 @@
       <c r="J314" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M314" s="13"/>
+      <c r="M314" s="14"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10461,7 +10461,7 @@
       <c r="J315" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M315" s="13"/>
+      <c r="M315" s="14"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10490,7 +10490,7 @@
       <c r="J316" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M316" s="13"/>
+      <c r="M316" s="14"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10517,7 +10517,7 @@
       <c r="J317" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M317" s="13"/>
+      <c r="M317" s="14"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10546,7 +10546,7 @@
       <c r="J318" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M318" s="13"/>
+      <c r="M318" s="14"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10573,7 +10573,7 @@
       <c r="J319" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M319" s="13"/>
+      <c r="M319" s="14"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10600,7 +10600,7 @@
       <c r="J320" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M320" s="13"/>
+      <c r="M320" s="14"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10627,7 +10627,7 @@
       <c r="J321" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M321" s="13"/>
+      <c r="M321" s="14"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10654,7 +10654,7 @@
       <c r="J322" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M322" s="13"/>
+      <c r="M322" s="14"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10681,7 +10681,7 @@
       <c r="J323" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M323" s="13"/>
+      <c r="M323" s="14"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10708,7 +10708,7 @@
       <c r="J324" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M324" s="13"/>
+      <c r="M324" s="14"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10735,7 +10735,7 @@
       <c r="J325" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M325" s="13"/>
+      <c r="M325" s="14"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10765,7 +10765,7 @@
       <c r="K326" t="s">
         <v>221</v>
       </c>
-      <c r="M326" s="13"/>
+      <c r="M326" s="14"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10797,7 +10797,7 @@
       <c r="K327" t="s">
         <v>221</v>
       </c>
-      <c r="M327" s="13"/>
+      <c r="M327" s="14"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10829,7 +10829,7 @@
       <c r="K328" t="s">
         <v>221</v>
       </c>
-      <c r="M328" s="13"/>
+      <c r="M328" s="14"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10861,7 +10861,7 @@
       <c r="K329" t="s">
         <v>221</v>
       </c>
-      <c r="M329" s="13"/>
+      <c r="M329" s="14"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10893,7 +10893,7 @@
       <c r="K330" t="s">
         <v>221</v>
       </c>
-      <c r="M330" s="13"/>
+      <c r="M330" s="14"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10925,7 +10925,7 @@
       <c r="K331" t="s">
         <v>221</v>
       </c>
-      <c r="M331" s="13"/>
+      <c r="M331" s="14"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10957,7 +10957,7 @@
       <c r="K332" t="s">
         <v>221</v>
       </c>
-      <c r="M332" s="13"/>
+      <c r="M332" s="14"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10986,7 +10986,7 @@
       <c r="J333" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M333" s="13"/>
+      <c r="M333" s="14"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -11015,7 +11015,7 @@
       <c r="J334" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M334" s="13"/>
+      <c r="M334" s="14"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -11044,7 +11044,7 @@
       <c r="J335" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M335" s="13"/>
+      <c r="M335" s="14"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11219,7 +11219,7 @@
       <c r="J342" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M342" s="13">
+      <c r="M342" s="14">
         <v>1</v>
       </c>
     </row>
@@ -11246,7 +11246,7 @@
       <c r="J343" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M343" s="13"/>
+      <c r="M343" s="14"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11271,7 +11271,7 @@
       <c r="J344" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M344" s="13"/>
+      <c r="M344" s="14"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11299,7 +11299,7 @@
       <c r="K345" t="s">
         <v>224</v>
       </c>
-      <c r="M345" s="13"/>
+      <c r="M345" s="14"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11324,7 +11324,7 @@
       <c r="J346" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M346" s="13"/>
+      <c r="M346" s="14"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11349,7 +11349,7 @@
       <c r="J347" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M347" s="13"/>
+      <c r="M347" s="14"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11376,7 +11376,7 @@
       <c r="J348" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M348" s="13"/>
+      <c r="M348" s="14"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11403,7 +11403,7 @@
       <c r="J349" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M349" s="13"/>
+      <c r="M349" s="14"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11432,7 +11432,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="13"/>
+      <c r="M350" s="14"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11461,7 +11461,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="13"/>
+      <c r="M351" s="14"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11495,7 +11495,7 @@
       <c r="K352" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M352" s="13"/>
+      <c r="M352" s="14"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11529,7 +11529,7 @@
       <c r="K353" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M353" s="13"/>
+      <c r="M353" s="14"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11563,7 +11563,7 @@
       <c r="K354" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M354" s="13"/>
+      <c r="M354" s="14"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11597,7 +11597,7 @@
       <c r="K355" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M355" s="13"/>
+      <c r="M355" s="14"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11626,7 +11626,7 @@
       <c r="J356" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M356" s="13"/>
+      <c r="M356" s="14"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11660,7 +11660,7 @@
       <c r="K357" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M357" s="13"/>
+      <c r="M357" s="14"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11694,7 +11694,7 @@
       <c r="K358" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M358" s="13"/>
+      <c r="M358" s="14"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11728,7 +11728,7 @@
       <c r="K359" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M359" s="13"/>
+      <c r="M359" s="14"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11759,7 +11759,7 @@
       <c r="J360" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M360" s="13"/>
+      <c r="M360" s="14"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11790,7 +11790,7 @@
       <c r="J361" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M361" s="13"/>
+      <c r="M361" s="14"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11821,7 +11821,7 @@
       <c r="J362" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M362" s="13"/>
+      <c r="M362" s="14"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11846,7 +11846,7 @@
       <c r="J363" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M363" s="13"/>
+      <c r="M363" s="14"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11871,7 +11871,7 @@
       <c r="J364" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M364" s="13"/>
+      <c r="M364" s="14"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11898,7 +11898,7 @@
       <c r="J365" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M365" s="13"/>
+      <c r="M365" s="14"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11925,7 +11925,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="13"/>
+      <c r="M366" s="14"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11952,7 +11952,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="13"/>
+      <c r="M367" s="14"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11979,7 +11979,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="13"/>
+      <c r="M368" s="14"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -12006,7 +12006,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="13"/>
+      <c r="M369" s="14"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -12033,7 +12033,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="13"/>
+      <c r="M370" s="14"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -12060,7 +12060,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="13"/>
+      <c r="M371" s="14"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -12087,7 +12087,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="13"/>
+      <c r="M372" s="14"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -12112,7 +12112,7 @@
       <c r="J373" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M373" s="13"/>
+      <c r="M373" s="14"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -12137,7 +12137,7 @@
       <c r="J374" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M374" s="13"/>
+      <c r="M374" s="14"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -12162,7 +12162,7 @@
       <c r="J375" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M375" s="13"/>
+      <c r="M375" s="14"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12190,7 +12190,7 @@
       <c r="K376" t="s">
         <v>224</v>
       </c>
-      <c r="M376" s="13"/>
+      <c r="M376" s="14"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12215,7 +12215,7 @@
       <c r="J377" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M377" s="13"/>
+      <c r="M377" s="14"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12240,7 +12240,7 @@
       <c r="J378" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M378" s="13"/>
+      <c r="M378" s="14"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12265,7 +12265,7 @@
       <c r="J379" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M379" s="13"/>
+      <c r="M379" s="14"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12292,7 +12292,7 @@
       <c r="J380" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M380" s="13"/>
+      <c r="M380" s="14"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12317,7 +12317,7 @@
       <c r="J381" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M381" s="13"/>
+      <c r="M381" s="14"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12344,7 +12344,7 @@
       <c r="J382" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M382" s="13"/>
+      <c r="M382" s="14"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12369,7 +12369,7 @@
       <c r="J383" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M383" s="13"/>
+      <c r="M383" s="14"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12394,7 +12394,7 @@
       <c r="J384" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M384" s="13"/>
+      <c r="M384" s="14"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12419,7 +12419,7 @@
       <c r="J385" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M385" s="13"/>
+      <c r="M385" s="14"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12444,7 +12444,7 @@
       <c r="J386" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M386" s="13"/>
+      <c r="M386" s="14"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12525,7 +12525,7 @@
       <c r="K389" t="s">
         <v>221</v>
       </c>
-      <c r="M389" s="13">
+      <c r="M389" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -12557,7 +12557,7 @@
       <c r="K390" t="s">
         <v>221</v>
       </c>
-      <c r="M390" s="13"/>
+      <c r="M390" s="14"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12587,7 +12587,7 @@
       <c r="K391" t="s">
         <v>221</v>
       </c>
-      <c r="M391" s="13"/>
+      <c r="M391" s="14"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12617,7 +12617,7 @@
       <c r="K392" t="s">
         <v>221</v>
       </c>
-      <c r="M392" s="13"/>
+      <c r="M392" s="14"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12647,7 +12647,7 @@
       <c r="K393" t="s">
         <v>221</v>
       </c>
-      <c r="M393" s="13"/>
+      <c r="M393" s="14"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12677,7 +12677,7 @@
       <c r="K394" t="s">
         <v>221</v>
       </c>
-      <c r="M394" s="13"/>
+      <c r="M394" s="14"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12704,7 +12704,7 @@
       <c r="J395" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M395" s="13"/>
+      <c r="M395" s="14"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12734,7 +12734,7 @@
       <c r="J396" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M396" s="13">
+      <c r="M396" s="14">
         <v>1</v>
       </c>
     </row>
@@ -12763,7 +12763,7 @@
       <c r="J397" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M397" s="13"/>
+      <c r="M397" s="14"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12790,7 +12790,7 @@
       <c r="J398" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M398" s="13"/>
+      <c r="M398" s="14"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12820,7 +12820,7 @@
       <c r="K399" t="s">
         <v>224</v>
       </c>
-      <c r="M399" s="13"/>
+      <c r="M399" s="14"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12847,7 +12847,7 @@
       <c r="J400" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M400" s="13"/>
+      <c r="M400" s="14"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12874,7 +12874,7 @@
       <c r="J401" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M401" s="13"/>
+      <c r="M401" s="14"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12901,7 +12901,7 @@
       <c r="J402" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M402" s="13"/>
+      <c r="M402" s="14"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12928,7 +12928,7 @@
       <c r="J403" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M403" s="13"/>
+      <c r="M403" s="14"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12958,7 +12958,7 @@
       <c r="K404" t="s">
         <v>224</v>
       </c>
-      <c r="M404" s="13"/>
+      <c r="M404" s="14"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12985,7 +12985,7 @@
       <c r="J405" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M405" s="13"/>
+      <c r="M405" s="14"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -13012,7 +13012,7 @@
       <c r="J406" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M406" s="13"/>
+      <c r="M406" s="14"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -13039,7 +13039,7 @@
       <c r="J407" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M407" s="13"/>
+      <c r="M407" s="14"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -13068,7 +13068,7 @@
       <c r="J408" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M408" s="13"/>
+      <c r="M408" s="14"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -13095,7 +13095,7 @@
       <c r="J409" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M409" s="13"/>
+      <c r="M409" s="14"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -13124,7 +13124,7 @@
       <c r="J410" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M410" s="13"/>
+      <c r="M410" s="14"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -13151,7 +13151,7 @@
       <c r="J411" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M411" s="13"/>
+      <c r="M411" s="14"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -13178,7 +13178,7 @@
       <c r="J412" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M412" s="13"/>
+      <c r="M412" s="14"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13205,7 +13205,7 @@
       <c r="J413" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M413" s="13"/>
+      <c r="M413" s="14"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13232,7 +13232,7 @@
       <c r="J414" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M414" s="13"/>
+      <c r="M414" s="14"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13262,7 +13262,7 @@
       <c r="J415" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M415" s="13">
+      <c r="M415" s="14">
         <v>0.5</v>
       </c>
     </row>
@@ -13294,7 +13294,7 @@
       <c r="K416" t="s">
         <v>227</v>
       </c>
-      <c r="M416" s="13"/>
+      <c r="M416" s="14"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13326,7 +13326,7 @@
       <c r="K417" t="s">
         <v>227</v>
       </c>
-      <c r="M417" s="13"/>
+      <c r="M417" s="14"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13358,7 +13358,7 @@
       <c r="K418" t="s">
         <v>227</v>
       </c>
-      <c r="M418" s="13"/>
+      <c r="M418" s="14"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13387,7 +13387,7 @@
       <c r="J419" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M419" s="13"/>
+      <c r="M419" s="14"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13416,7 +13416,7 @@
       <c r="J420" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M420" s="13"/>
+      <c r="M420" s="14"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13441,12 +13441,12 @@
       <c r="G421" s="1"/>
       <c r="H421" s="1"/>
       <c r="I421" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J421" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M421" s="13">
+        <v>210</v>
+      </c>
+      <c r="M421" s="14">
         <v>1</v>
       </c>
     </row>
@@ -13470,12 +13470,12 @@
       <c r="G422" s="1"/>
       <c r="H422" s="1"/>
       <c r="I422" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J422" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M422" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M422" s="14"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13497,12 +13497,12 @@
       <c r="G423" s="1"/>
       <c r="H423" s="1"/>
       <c r="I423" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J423" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M423" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M423" s="14"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13524,12 +13524,15 @@
       <c r="G424" s="1"/>
       <c r="H424" s="1"/>
       <c r="I424" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J424" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M424" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K424" t="s">
+        <v>224</v>
+      </c>
+      <c r="M424" s="14"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13551,12 +13554,12 @@
       <c r="G425" s="1"/>
       <c r="H425" s="1"/>
       <c r="I425" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J425" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M425" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M425" s="14"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13578,12 +13581,12 @@
       <c r="G426" s="1"/>
       <c r="H426" s="1"/>
       <c r="I426" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J426" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M426" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M426" s="14"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13605,12 +13608,12 @@
       <c r="G427" s="1"/>
       <c r="H427" s="1"/>
       <c r="I427" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J427" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M427" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M427" s="14"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13632,12 +13635,12 @@
       <c r="G428" s="1"/>
       <c r="H428" s="1"/>
       <c r="I428" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J428" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M428" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M428" s="14"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13659,12 +13662,15 @@
       <c r="G429" s="1"/>
       <c r="H429" s="1"/>
       <c r="I429" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J429" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M429" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="K429" t="s">
+        <v>224</v>
+      </c>
+      <c r="M429" s="14"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13686,12 +13692,12 @@
       <c r="G430" s="1"/>
       <c r="H430" s="1"/>
       <c r="I430" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J430" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M430" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M430" s="14"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13713,12 +13719,12 @@
       <c r="G431" s="1"/>
       <c r="H431" s="1"/>
       <c r="I431" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J431" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M431" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M431" s="14"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13740,12 +13746,12 @@
       <c r="G432" s="1"/>
       <c r="H432" s="1"/>
       <c r="I432" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J432" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M432" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M432" s="14"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13769,12 +13775,12 @@
       <c r="G433" s="1"/>
       <c r="H433" s="1"/>
       <c r="I433" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J433" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M433" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M433" s="14"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13796,12 +13802,12 @@
       <c r="G434" s="1"/>
       <c r="H434" s="1"/>
       <c r="I434" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J434" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M434" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M434" s="14"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13825,12 +13831,12 @@
       <c r="G435" s="1"/>
       <c r="H435" s="1"/>
       <c r="I435" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J435" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M435" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M435" s="14"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13852,12 +13858,12 @@
       <c r="G436" s="1"/>
       <c r="H436" s="1"/>
       <c r="I436" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J436" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M436" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M436" s="14"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13879,12 +13885,12 @@
       <c r="G437" s="1"/>
       <c r="H437" s="1"/>
       <c r="I437" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J437" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M437" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M437" s="14"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13906,12 +13912,12 @@
       <c r="G438" s="1"/>
       <c r="H438" s="1"/>
       <c r="I438" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J438" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M438" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="M438" s="14"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13933,12 +13939,12 @@
       <c r="G439" s="1"/>
       <c r="H439" s="1"/>
       <c r="I439" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J439" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M439" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M439" s="14"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13967,12 +13973,12 @@
       </c>
       <c r="H440" s="1"/>
       <c r="I440" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J440" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M440" s="13">
+        <v>210</v>
+      </c>
+      <c r="M440" s="14">
         <v>1</v>
       </c>
     </row>
@@ -14000,12 +14006,12 @@
       </c>
       <c r="H441" s="1"/>
       <c r="I441" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J441" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M441" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M441" s="14"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -14031,12 +14037,12 @@
       </c>
       <c r="H442" s="1"/>
       <c r="I442" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J442" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M442" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M442" s="14"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -14062,12 +14068,12 @@
       </c>
       <c r="H443" s="1"/>
       <c r="I443" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J443" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M443" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M443" s="14"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -14093,12 +14099,12 @@
       </c>
       <c r="H444" s="1"/>
       <c r="I444" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J444" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M444" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M444" s="14"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -14124,12 +14130,12 @@
       </c>
       <c r="H445" s="1"/>
       <c r="I445" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J445" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M445" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M445" s="14"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -14155,12 +14161,12 @@
       </c>
       <c r="H446" s="1"/>
       <c r="I446" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J446" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M446" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M446" s="14"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -14186,12 +14192,12 @@
       </c>
       <c r="H447" s="1"/>
       <c r="I447" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J447" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M447" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M447" s="14"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14217,12 +14223,12 @@
       </c>
       <c r="H448" s="1"/>
       <c r="I448" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J448" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M448" s="13"/>
+      <c r="M448" s="14"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14248,12 +14254,12 @@
       </c>
       <c r="H449" s="1"/>
       <c r="I449" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J449" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M449" s="13"/>
+      <c r="M449" s="14"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14277,12 +14283,12 @@
       <c r="G450" s="1"/>
       <c r="H450" s="1"/>
       <c r="I450" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J450" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M450" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M450" s="14"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14306,12 +14312,12 @@
       <c r="G451" s="1"/>
       <c r="H451" s="1"/>
       <c r="I451" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J451" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M451" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M451" s="14"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14335,12 +14341,12 @@
       <c r="G452" s="1"/>
       <c r="H452" s="1"/>
       <c r="I452" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J452" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M452" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M452" s="14"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14364,12 +14370,12 @@
       <c r="G453" s="1"/>
       <c r="H453" s="1"/>
       <c r="I453" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J453" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M453" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M453" s="14"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14393,12 +14399,12 @@
       <c r="G454" s="1"/>
       <c r="H454" s="1"/>
       <c r="I454" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J454" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M454" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M454" s="14"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14420,12 +14426,12 @@
       <c r="G455" s="1"/>
       <c r="H455" s="1"/>
       <c r="I455" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J455" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M455" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M455" s="14"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14447,12 +14453,15 @@
       <c r="G456" s="1"/>
       <c r="H456" s="1"/>
       <c r="I456" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J456" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M456" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K456" t="s">
+        <v>227</v>
+      </c>
+      <c r="M456" s="14"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14474,12 +14483,15 @@
       <c r="G457" s="1"/>
       <c r="H457" s="1"/>
       <c r="I457" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J457" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M457" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K457" t="s">
+        <v>227</v>
+      </c>
+      <c r="M457" s="14"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14503,12 +14515,15 @@
       <c r="G458" s="1"/>
       <c r="H458" s="1"/>
       <c r="I458" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J458" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M458" s="13"/>
+        <v>211</v>
+      </c>
+      <c r="K458" t="s">
+        <v>227</v>
+      </c>
+      <c r="M458" s="14"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14532,12 +14547,12 @@
       <c r="G459" s="1"/>
       <c r="H459" s="1"/>
       <c r="I459" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J459" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M459" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M459" s="14"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14561,12 +14576,12 @@
       <c r="G460" s="1"/>
       <c r="H460" s="1"/>
       <c r="I460" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J460" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M460" s="13"/>
+        <v>210</v>
+      </c>
+      <c r="M460" s="14"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14595,7 +14610,7 @@
       <c r="J461" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M461" s="13"/>
+      <c r="M461" s="14"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14929,7 +14944,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="12">
+      <c r="M474" s="15">
         <v>1</v>
       </c>
     </row>
@@ -14958,7 +14973,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="12"/>
+      <c r="M475" s="15"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -14985,7 +15000,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="12"/>
+      <c r="M476" s="15"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -15012,7 +15027,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="12"/>
+      <c r="M477" s="15"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -15039,7 +15054,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="12"/>
+      <c r="M478" s="15"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -15066,7 +15081,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="12"/>
+      <c r="M479" s="15"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -15093,7 +15108,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="12"/>
+      <c r="M480" s="15"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15120,7 +15135,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="12"/>
+      <c r="M481" s="15"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15147,7 +15162,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="12"/>
+      <c r="M482" s="15"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15174,7 +15189,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="12"/>
+      <c r="M483" s="15"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15334,7 +15349,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="12">
+      <c r="M489" s="15">
         <v>2</v>
       </c>
     </row>
@@ -15361,7 +15376,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="12"/>
+      <c r="M490" s="15"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15386,7 +15401,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="12"/>
+      <c r="M491" s="15"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15411,7 +15426,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="12"/>
+      <c r="M492" s="15"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15436,7 +15451,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="12"/>
+      <c r="M493" s="15"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15463,7 +15478,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="12"/>
+      <c r="M494" s="15"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15490,7 +15505,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="12"/>
+      <c r="M495" s="15"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15517,7 +15532,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="12"/>
+      <c r="M496" s="15"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15544,7 +15559,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="12"/>
+      <c r="M497" s="15"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15597,7 +15612,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="12">
+      <c r="M499" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15624,7 +15639,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="12"/>
+      <c r="M500" s="15"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15649,7 +15664,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="12"/>
+      <c r="M501" s="15"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15674,7 +15689,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="12"/>
+      <c r="M502" s="15"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15699,7 +15714,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="12"/>
+      <c r="M503" s="15"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15724,7 +15739,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="12"/>
+      <c r="M504" s="15"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15751,7 +15766,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="12"/>
+      <c r="M505" s="15"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15776,7 +15791,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="12"/>
+      <c r="M506" s="15"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15803,7 +15818,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="12"/>
+      <c r="M507" s="15"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15828,7 +15843,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="12"/>
+      <c r="M508" s="15"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15853,7 +15868,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="12"/>
+      <c r="M509" s="15"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15878,7 +15893,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="12"/>
+      <c r="M510" s="15"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15903,7 +15918,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="12"/>
+      <c r="M511" s="15"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15930,7 +15945,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="12"/>
+      <c r="M512" s="15"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15957,7 +15972,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="12"/>
+      <c r="M513" s="15"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15982,7 +15997,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="12"/>
+      <c r="M514" s="15"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -16007,7 +16022,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="12"/>
+      <c r="M515" s="15"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -16035,7 +16050,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="12">
+      <c r="M516" s="15">
         <v>2</v>
       </c>
     </row>
@@ -16064,7 +16079,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="12"/>
+      <c r="M517" s="15"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -16091,7 +16106,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="12"/>
+      <c r="M518" s="15"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -16118,7 +16133,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="12"/>
+      <c r="M519" s="15"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16147,7 +16162,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="12"/>
+      <c r="M520" s="15"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16176,7 +16191,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="12"/>
+      <c r="M521" s="15"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16205,7 +16220,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="12"/>
+      <c r="M522" s="15"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16234,7 +16249,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="12"/>
+      <c r="M523" s="15"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16263,7 +16278,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="12"/>
+      <c r="M524" s="15"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16292,7 +16307,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="12"/>
+      <c r="M525" s="15"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16319,7 +16334,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="12"/>
+      <c r="M526" s="15"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16346,7 +16361,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="12"/>
+      <c r="M527" s="15"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16371,11 +16386,6 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16392,6 +16402,11 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Fixed bubble chart conversion
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -770,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -846,11 +846,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -873,16 +882,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1207,9 +1219,9 @@
   <dimension ref="A1:N530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I450" sqref="I450"/>
+      <selection pane="bottomLeft" activeCell="I470" sqref="I470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1229,16 +1241,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1279,7 +1291,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1309,7 +1321,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1334,7 +1346,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1359,7 +1371,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1384,7 +1396,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1409,7 +1421,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1434,7 +1446,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1459,7 +1471,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1484,7 +1496,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="13"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2105,7 +2117,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2137,7 +2149,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="14"/>
+      <c r="M34" s="13"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2402,7 +2414,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M43" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2434,7 +2446,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="14"/>
+      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2466,7 +2478,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="14"/>
+      <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2498,7 +2510,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="14"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2530,7 +2542,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="14"/>
+      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2562,7 +2574,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="14"/>
+      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2594,7 +2606,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="14"/>
+      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2626,7 +2638,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2815,7 +2827,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="14">
+      <c r="M57" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2844,7 +2856,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="14"/>
+      <c r="M58" s="13"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2871,7 +2883,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="14"/>
+      <c r="M59" s="13"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2898,7 +2910,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="14"/>
+      <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -3996,7 +4008,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="14">
+      <c r="M98" s="13">
         <v>2</v>
       </c>
     </row>
@@ -4023,7 +4035,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="14"/>
+      <c r="M99" s="13"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4051,7 +4063,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="14"/>
+      <c r="M100" s="13"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4076,7 +4088,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="14"/>
+      <c r="M101" s="13"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4103,7 +4115,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="14"/>
+      <c r="M102" s="13"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4130,7 +4142,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="14"/>
+      <c r="M103" s="13"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4159,7 +4171,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="14"/>
+      <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4188,7 +4200,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="14"/>
+      <c r="M105" s="13"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4222,7 +4234,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="14"/>
+      <c r="M106" s="13"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4256,7 +4268,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="14"/>
+      <c r="M107" s="13"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4290,7 +4302,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="14"/>
+      <c r="M108" s="13"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4324,7 +4336,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="14"/>
+      <c r="M109" s="13"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4353,7 +4365,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="14"/>
+      <c r="M110" s="13"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4387,7 +4399,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="14"/>
+      <c r="M111" s="13"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4421,7 +4433,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="14"/>
+      <c r="M112" s="13"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4455,7 +4467,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="14"/>
+      <c r="M113" s="13"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4486,7 +4498,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="14"/>
+      <c r="M114" s="13"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4517,7 +4529,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="14"/>
+      <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4548,7 +4560,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="14"/>
+      <c r="M116" s="13"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4573,7 +4585,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="14"/>
+      <c r="M117" s="13"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4600,7 +4612,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="14"/>
+      <c r="M118" s="13"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4834,7 +4846,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="14">
+      <c r="M127" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4861,7 +4873,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="14"/>
+      <c r="M128" s="13"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4889,7 +4901,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="14"/>
+      <c r="M129" s="13"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4914,7 +4926,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="14"/>
+      <c r="M130" s="13"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4939,7 +4951,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="14"/>
+      <c r="M131" s="13"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4966,7 +4978,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="14"/>
+      <c r="M132" s="13"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -4993,7 +5005,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="14"/>
+      <c r="M133" s="13"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5022,7 +5034,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="14"/>
+      <c r="M134" s="13"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5051,7 +5063,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="14"/>
+      <c r="M135" s="13"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5085,7 +5097,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="14"/>
+      <c r="M136" s="13"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5119,7 +5131,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="14"/>
+      <c r="M137" s="13"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5153,7 +5165,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="14"/>
+      <c r="M138" s="13"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5187,7 +5199,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="14"/>
+      <c r="M139" s="13"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5216,7 +5228,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="14"/>
+      <c r="M140" s="13"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5250,7 +5262,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="14"/>
+      <c r="M141" s="13"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5284,7 +5296,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="14"/>
+      <c r="M142" s="13"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5316,7 +5328,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="14"/>
+      <c r="M143" s="13"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5347,7 +5359,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="14"/>
+      <c r="M144" s="13"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5378,7 +5390,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="14"/>
+      <c r="M145" s="13"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5409,7 +5421,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="14"/>
+      <c r="M146" s="13"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5434,7 +5446,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="14"/>
+      <c r="M147" s="13"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5459,7 +5471,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="14"/>
+      <c r="M148" s="13"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5486,7 +5498,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="14"/>
+      <c r="M149" s="13"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5513,7 +5525,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="14"/>
+      <c r="M150" s="13"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5540,7 +5552,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="14"/>
+      <c r="M151" s="13"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5567,7 +5579,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="14"/>
+      <c r="M152" s="13"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5594,7 +5606,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="14"/>
+      <c r="M153" s="13"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5621,7 +5633,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="14"/>
+      <c r="M154" s="13"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5648,7 +5660,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="14"/>
+      <c r="M155" s="13"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5675,7 +5687,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="14"/>
+      <c r="M156" s="13"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5703,7 +5715,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="14"/>
+      <c r="M157" s="13"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5733,7 +5745,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="14"/>
+      <c r="M158" s="13"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5763,7 +5775,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="14"/>
+      <c r="M159" s="13"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5793,7 +5805,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="14"/>
+      <c r="M160" s="13"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5823,7 +5835,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="14"/>
+      <c r="M161" s="13"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5853,7 +5865,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="14"/>
+      <c r="M162" s="13"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5883,7 +5895,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="14"/>
+      <c r="M163" s="13"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5913,7 +5925,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="14"/>
+      <c r="M164" s="13"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5943,7 +5955,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="14">
+      <c r="M165" s="13">
         <v>1</v>
       </c>
     </row>
@@ -5972,7 +5984,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="14"/>
+      <c r="M166" s="13"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -5999,7 +6011,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="14"/>
+      <c r="M167" s="13"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6029,7 +6041,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="14"/>
+      <c r="M168" s="13"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6056,7 +6068,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="14"/>
+      <c r="M169" s="13"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6083,7 +6095,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="14"/>
+      <c r="M170" s="13"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6112,7 +6124,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="14"/>
+      <c r="M171" s="13"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6141,7 +6153,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="14"/>
+      <c r="M172" s="13"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6172,7 +6184,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="14"/>
+      <c r="M173" s="13"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6203,7 +6215,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="14"/>
+      <c r="M174" s="13"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6239,7 +6251,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="14"/>
+      <c r="M175" s="13"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6275,7 +6287,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="14"/>
+      <c r="M176" s="13"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6311,7 +6323,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="14"/>
+      <c r="M177" s="13"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6347,7 +6359,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="14"/>
+      <c r="M178" s="13"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6378,7 +6390,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="14"/>
+      <c r="M179" s="13"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6414,7 +6426,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="14"/>
+      <c r="M180" s="13"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6450,7 +6462,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="14"/>
+      <c r="M181" s="13"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6486,7 +6498,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="14"/>
+      <c r="M182" s="13"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6519,7 +6531,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="14"/>
+      <c r="M183" s="13"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6552,7 +6564,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="14"/>
+      <c r="M184" s="13"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6585,7 +6597,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="14"/>
+      <c r="M185" s="13"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6612,7 +6624,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="14"/>
+      <c r="M186" s="13"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6639,7 +6651,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="14"/>
+      <c r="M187" s="13"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6668,7 +6680,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="14"/>
+      <c r="M188" s="13"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6891,7 +6903,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="14">
+      <c r="M196" s="13">
         <v>2</v>
       </c>
     </row>
@@ -6920,7 +6932,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="14"/>
+      <c r="M197" s="13"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6950,7 +6962,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="14"/>
+      <c r="M198" s="13"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6977,7 +6989,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="14"/>
+      <c r="M199" s="13"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -7004,7 +7016,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="14"/>
+      <c r="M200" s="13"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7033,7 +7045,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="14"/>
+      <c r="M201" s="13"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7060,7 +7072,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="14"/>
+      <c r="M202" s="13"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7089,7 +7101,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="14"/>
+      <c r="M203" s="13"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7116,7 +7128,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="14"/>
+      <c r="M204" s="13"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7143,7 +7155,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="14"/>
+      <c r="M205" s="13"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7170,7 +7182,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="14"/>
+      <c r="M206" s="13"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7197,7 +7209,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="14"/>
+      <c r="M207" s="13"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7227,7 +7239,7 @@
       <c r="K208" t="s">
         <v>225</v>
       </c>
-      <c r="M208" s="14"/>
+      <c r="M208" s="13"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7257,7 +7269,7 @@
       <c r="K209" t="s">
         <v>225</v>
       </c>
-      <c r="M209" s="14"/>
+      <c r="M209" s="13"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7290,7 +7302,7 @@
       <c r="K210" t="s">
         <v>220</v>
       </c>
-      <c r="M210" s="14">
+      <c r="M210" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -7324,7 +7336,7 @@
       <c r="K211" t="s">
         <v>221</v>
       </c>
-      <c r="M211" s="14"/>
+      <c r="M211" s="13"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7356,7 +7368,7 @@
       <c r="K212" t="s">
         <v>221</v>
       </c>
-      <c r="M212" s="14"/>
+      <c r="M212" s="13"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7388,7 +7400,7 @@
       <c r="K213" t="s">
         <v>221</v>
       </c>
-      <c r="M213" s="14"/>
+      <c r="M213" s="13"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7420,7 +7432,7 @@
       <c r="K214" t="s">
         <v>221</v>
       </c>
-      <c r="M214" s="14"/>
+      <c r="M214" s="13"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7452,7 +7464,7 @@
       <c r="K215" t="s">
         <v>221</v>
       </c>
-      <c r="M215" s="14"/>
+      <c r="M215" s="13"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7484,7 +7496,7 @@
       <c r="K216" t="s">
         <v>221</v>
       </c>
-      <c r="M216" s="14"/>
+      <c r="M216" s="13"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7516,7 +7528,7 @@
       <c r="K217" t="s">
         <v>221</v>
       </c>
-      <c r="M217" s="14"/>
+      <c r="M217" s="13"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7545,7 +7557,7 @@
       <c r="J218" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M218" s="14"/>
+      <c r="M218" s="13"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7574,7 +7586,7 @@
       <c r="J219" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M219" s="14"/>
+      <c r="M219" s="13"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7601,7 +7613,7 @@
       <c r="J220" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M220" s="14">
+      <c r="M220" s="13">
         <v>1</v>
       </c>
     </row>
@@ -7630,7 +7642,7 @@
       <c r="J221" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M221" s="14"/>
+      <c r="M221" s="13"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7657,7 +7669,7 @@
       <c r="J222" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M222" s="14"/>
+      <c r="M222" s="13"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7687,7 +7699,7 @@
       <c r="K223" t="s">
         <v>224</v>
       </c>
-      <c r="M223" s="14"/>
+      <c r="M223" s="13"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7714,7 +7726,7 @@
       <c r="J224" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M224" s="14"/>
+      <c r="M224" s="13"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7741,7 +7753,7 @@
       <c r="J225" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M225" s="14"/>
+      <c r="M225" s="13"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7770,7 +7782,7 @@
       <c r="J226" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M226" s="14"/>
+      <c r="M226" s="13"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7799,7 +7811,7 @@
       <c r="J227" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M227" s="14"/>
+      <c r="M227" s="13"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7830,7 +7842,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="14"/>
+      <c r="M228" s="13"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7861,7 +7873,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="14"/>
+      <c r="M229" s="13"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7897,7 +7909,7 @@
       <c r="K230" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M230" s="14"/>
+      <c r="M230" s="13"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7933,7 +7945,7 @@
       <c r="K231" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M231" s="14"/>
+      <c r="M231" s="13"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7969,7 +7981,7 @@
       <c r="K232" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M232" s="14"/>
+      <c r="M232" s="13"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -8005,7 +8017,7 @@
       <c r="K233" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M233" s="14"/>
+      <c r="M233" s="13"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -8036,7 +8048,7 @@
       <c r="J234" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M234" s="14"/>
+      <c r="M234" s="13"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8072,7 +8084,7 @@
       <c r="K235" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M235" s="14"/>
+      <c r="M235" s="13"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8108,7 +8120,7 @@
       <c r="K236" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M236" s="14"/>
+      <c r="M236" s="13"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8144,7 +8156,7 @@
       <c r="K237" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M237" s="14"/>
+      <c r="M237" s="13"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8177,7 +8189,7 @@
       <c r="J238" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M238" s="14"/>
+      <c r="M238" s="13"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8210,7 +8222,7 @@
       <c r="J239" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M239" s="14"/>
+      <c r="M239" s="13"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8243,7 +8255,7 @@
       <c r="J240" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M240" s="14"/>
+      <c r="M240" s="13"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8270,7 +8282,7 @@
       <c r="J241" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M241" s="14"/>
+      <c r="M241" s="13"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8297,7 +8309,7 @@
       <c r="J242" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M242" s="14"/>
+      <c r="M242" s="13"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8326,7 +8338,7 @@
       <c r="J243" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M243" s="14"/>
+      <c r="M243" s="13"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8355,7 +8367,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="14"/>
+      <c r="M244" s="13"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8384,7 +8396,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="14"/>
+      <c r="M245" s="13"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8413,7 +8425,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="14"/>
+      <c r="M246" s="13"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8442,7 +8454,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="14"/>
+      <c r="M247" s="13"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8471,7 +8483,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="14"/>
+      <c r="M248" s="13"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8500,7 +8512,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="14"/>
+      <c r="M249" s="13"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8529,7 +8541,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="14"/>
+      <c r="M250" s="13"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8556,7 +8568,7 @@
       <c r="J251" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M251" s="14"/>
+      <c r="M251" s="13"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8583,7 +8595,7 @@
       <c r="J252" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M252" s="14"/>
+      <c r="M252" s="13"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8610,7 +8622,7 @@
       <c r="J253" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M253" s="14"/>
+      <c r="M253" s="13"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8640,7 +8652,7 @@
       <c r="K254" t="s">
         <v>224</v>
       </c>
-      <c r="M254" s="14"/>
+      <c r="M254" s="13"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8667,7 +8679,7 @@
       <c r="J255" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M255" s="14"/>
+      <c r="M255" s="13"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8694,7 +8706,7 @@
       <c r="J256" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M256" s="14"/>
+      <c r="M256" s="13"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8721,7 +8733,7 @@
       <c r="J257" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M257" s="14"/>
+      <c r="M257" s="13"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8750,7 +8762,7 @@
       <c r="J258" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M258" s="14"/>
+      <c r="M258" s="13"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8777,7 +8789,7 @@
       <c r="J259" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M259" s="14"/>
+      <c r="M259" s="13"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8806,7 +8818,7 @@
       <c r="J260" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M260" s="14"/>
+      <c r="M260" s="13"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8833,7 +8845,7 @@
       <c r="J261" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M261" s="14"/>
+      <c r="M261" s="13"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8860,7 +8872,7 @@
       <c r="J262" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M262" s="14"/>
+      <c r="M262" s="13"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8887,7 +8899,7 @@
       <c r="J263" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M263" s="14"/>
+      <c r="M263" s="13"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8914,7 +8926,7 @@
       <c r="J264" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M264" s="14"/>
+      <c r="M264" s="13"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8944,7 +8956,7 @@
       <c r="K265" t="s">
         <v>225</v>
       </c>
-      <c r="M265" s="14"/>
+      <c r="M265" s="13"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8974,7 +8986,7 @@
       <c r="K266" t="s">
         <v>225</v>
       </c>
-      <c r="M266" s="14"/>
+      <c r="M266" s="13"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -9004,7 +9016,7 @@
       <c r="K267" t="s">
         <v>225</v>
       </c>
-      <c r="M267" s="14"/>
+      <c r="M267" s="13"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -9034,7 +9046,7 @@
       <c r="K268" t="s">
         <v>220</v>
       </c>
-      <c r="M268" s="14"/>
+      <c r="M268" s="13"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -9066,7 +9078,7 @@
       <c r="K269" t="s">
         <v>221</v>
       </c>
-      <c r="M269" s="14"/>
+      <c r="M269" s="13"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9098,7 +9110,7 @@
       <c r="K270" t="s">
         <v>221</v>
       </c>
-      <c r="M270" s="14"/>
+      <c r="M270" s="13"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9130,7 +9142,7 @@
       <c r="K271" t="s">
         <v>221</v>
       </c>
-      <c r="M271" s="14"/>
+      <c r="M271" s="13"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9162,7 +9174,7 @@
       <c r="K272" t="s">
         <v>221</v>
       </c>
-      <c r="M272" s="14"/>
+      <c r="M272" s="13"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9194,7 +9206,7 @@
       <c r="K273" t="s">
         <v>221</v>
       </c>
-      <c r="M273" s="14"/>
+      <c r="M273" s="13"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9226,7 +9238,7 @@
       <c r="K274" t="s">
         <v>221</v>
       </c>
-      <c r="M274" s="14"/>
+      <c r="M274" s="13"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9258,7 +9270,7 @@
       <c r="K275" t="s">
         <v>221</v>
       </c>
-      <c r="M275" s="14"/>
+      <c r="M275" s="13"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9287,7 +9299,7 @@
       <c r="J276" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M276" s="14"/>
+      <c r="M276" s="13"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9316,7 +9328,7 @@
       <c r="J277" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M277" s="14"/>
+      <c r="M277" s="13"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9343,7 +9355,7 @@
       <c r="J278" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M278" s="14"/>
+      <c r="M278" s="13"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9370,7 +9382,7 @@
       <c r="J279" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M279" s="14"/>
+      <c r="M279" s="13"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9397,7 +9409,7 @@
       <c r="J280" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M280" s="14"/>
+      <c r="M280" s="13"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9427,7 +9439,7 @@
       <c r="K281" t="s">
         <v>224</v>
       </c>
-      <c r="M281" s="14"/>
+      <c r="M281" s="13"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9454,7 +9466,7 @@
       <c r="J282" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M282" s="14"/>
+      <c r="M282" s="13"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9481,7 +9493,7 @@
       <c r="J283" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M283" s="14"/>
+      <c r="M283" s="13"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9510,7 +9522,7 @@
       <c r="J284" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M284" s="14"/>
+      <c r="M284" s="13"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9539,7 +9551,7 @@
       <c r="J285" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M285" s="14"/>
+      <c r="M285" s="13"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9570,7 +9582,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="14"/>
+      <c r="M286" s="13"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9601,7 +9613,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="14"/>
+      <c r="M287" s="13"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9637,7 +9649,7 @@
       <c r="K288" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M288" s="14"/>
+      <c r="M288" s="13"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9673,7 +9685,7 @@
       <c r="K289" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M289" s="14"/>
+      <c r="M289" s="13"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9709,7 +9721,7 @@
       <c r="K290" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M290" s="14"/>
+      <c r="M290" s="13"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9745,7 +9757,7 @@
       <c r="K291" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M291" s="14"/>
+      <c r="M291" s="13"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9776,7 +9788,7 @@
       <c r="J292" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M292" s="14"/>
+      <c r="M292" s="13"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9812,7 +9824,7 @@
       <c r="K293" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M293" s="14"/>
+      <c r="M293" s="13"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9848,7 +9860,7 @@
       <c r="K294" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M294" s="14"/>
+      <c r="M294" s="13"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9884,7 +9896,7 @@
       <c r="K295" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M295" s="14"/>
+      <c r="M295" s="13"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9917,7 +9929,7 @@
       <c r="J296" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M296" s="14"/>
+      <c r="M296" s="13"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9950,7 +9962,7 @@
       <c r="J297" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M297" s="14"/>
+      <c r="M297" s="13"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9983,7 +9995,7 @@
       <c r="J298" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M298" s="14"/>
+      <c r="M298" s="13"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -10010,7 +10022,7 @@
       <c r="J299" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M299" s="14"/>
+      <c r="M299" s="13"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -10037,7 +10049,7 @@
       <c r="J300" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M300" s="14"/>
+      <c r="M300" s="13"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -10066,7 +10078,7 @@
       <c r="J301" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M301" s="14"/>
+      <c r="M301" s="13"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -10095,7 +10107,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="14"/>
+      <c r="M302" s="13"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10124,7 +10136,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="14"/>
+      <c r="M303" s="13"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10153,7 +10165,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="14"/>
+      <c r="M304" s="13"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10182,7 +10194,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="14"/>
+      <c r="M305" s="13"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10211,7 +10223,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="14"/>
+      <c r="M306" s="13"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10240,7 +10252,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="14"/>
+      <c r="M307" s="13"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10269,7 +10281,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="14"/>
+      <c r="M308" s="13"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10296,7 +10308,7 @@
       <c r="J309" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M309" s="14"/>
+      <c r="M309" s="13"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10323,7 +10335,7 @@
       <c r="J310" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M310" s="14"/>
+      <c r="M310" s="13"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10350,7 +10362,7 @@
       <c r="J311" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M311" s="14"/>
+      <c r="M311" s="13"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10380,7 +10392,7 @@
       <c r="K312" t="s">
         <v>224</v>
       </c>
-      <c r="M312" s="14"/>
+      <c r="M312" s="13"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10407,7 +10419,7 @@
       <c r="J313" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M313" s="14"/>
+      <c r="M313" s="13"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10434,7 +10446,7 @@
       <c r="J314" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M314" s="14"/>
+      <c r="M314" s="13"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10461,7 +10473,7 @@
       <c r="J315" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M315" s="14"/>
+      <c r="M315" s="13"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10490,7 +10502,7 @@
       <c r="J316" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M316" s="14"/>
+      <c r="M316" s="13"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10517,7 +10529,7 @@
       <c r="J317" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M317" s="14"/>
+      <c r="M317" s="13"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10546,7 +10558,7 @@
       <c r="J318" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M318" s="14"/>
+      <c r="M318" s="13"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10573,7 +10585,7 @@
       <c r="J319" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M319" s="14"/>
+      <c r="M319" s="13"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10600,7 +10612,7 @@
       <c r="J320" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M320" s="14"/>
+      <c r="M320" s="13"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10627,7 +10639,7 @@
       <c r="J321" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M321" s="14"/>
+      <c r="M321" s="13"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10654,7 +10666,7 @@
       <c r="J322" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M322" s="14"/>
+      <c r="M322" s="13"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10681,7 +10693,7 @@
       <c r="J323" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M323" s="14"/>
+      <c r="M323" s="13"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10708,7 +10720,7 @@
       <c r="J324" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M324" s="14"/>
+      <c r="M324" s="13"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10735,7 +10747,7 @@
       <c r="J325" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M325" s="14"/>
+      <c r="M325" s="13"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10765,7 +10777,7 @@
       <c r="K326" t="s">
         <v>221</v>
       </c>
-      <c r="M326" s="14"/>
+      <c r="M326" s="13"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10797,7 +10809,7 @@
       <c r="K327" t="s">
         <v>221</v>
       </c>
-      <c r="M327" s="14"/>
+      <c r="M327" s="13"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10829,7 +10841,7 @@
       <c r="K328" t="s">
         <v>221</v>
       </c>
-      <c r="M328" s="14"/>
+      <c r="M328" s="13"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10861,7 +10873,7 @@
       <c r="K329" t="s">
         <v>221</v>
       </c>
-      <c r="M329" s="14"/>
+      <c r="M329" s="13"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10893,7 +10905,7 @@
       <c r="K330" t="s">
         <v>221</v>
       </c>
-      <c r="M330" s="14"/>
+      <c r="M330" s="13"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10925,7 +10937,7 @@
       <c r="K331" t="s">
         <v>221</v>
       </c>
-      <c r="M331" s="14"/>
+      <c r="M331" s="13"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10957,7 +10969,7 @@
       <c r="K332" t="s">
         <v>221</v>
       </c>
-      <c r="M332" s="14"/>
+      <c r="M332" s="13"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10986,7 +10998,7 @@
       <c r="J333" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M333" s="14"/>
+      <c r="M333" s="13"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -11015,7 +11027,7 @@
       <c r="J334" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M334" s="14"/>
+      <c r="M334" s="13"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -11044,7 +11056,7 @@
       <c r="J335" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M335" s="14"/>
+      <c r="M335" s="13"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11219,7 +11231,7 @@
       <c r="J342" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M342" s="14">
+      <c r="M342" s="13">
         <v>1</v>
       </c>
     </row>
@@ -11246,7 +11258,7 @@
       <c r="J343" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M343" s="14"/>
+      <c r="M343" s="13"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11271,7 +11283,7 @@
       <c r="J344" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M344" s="14"/>
+      <c r="M344" s="13"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11299,7 +11311,7 @@
       <c r="K345" t="s">
         <v>224</v>
       </c>
-      <c r="M345" s="14"/>
+      <c r="M345" s="13"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11324,7 +11336,7 @@
       <c r="J346" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M346" s="14"/>
+      <c r="M346" s="13"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11349,7 +11361,7 @@
       <c r="J347" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M347" s="14"/>
+      <c r="M347" s="13"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11376,7 +11388,7 @@
       <c r="J348" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M348" s="14"/>
+      <c r="M348" s="13"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11403,7 +11415,7 @@
       <c r="J349" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M349" s="14"/>
+      <c r="M349" s="13"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11432,7 +11444,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="14"/>
+      <c r="M350" s="13"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11461,7 +11473,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="14"/>
+      <c r="M351" s="13"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11495,7 +11507,7 @@
       <c r="K352" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M352" s="14"/>
+      <c r="M352" s="13"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11529,7 +11541,7 @@
       <c r="K353" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M353" s="14"/>
+      <c r="M353" s="13"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11563,7 +11575,7 @@
       <c r="K354" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M354" s="14"/>
+      <c r="M354" s="13"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11597,7 +11609,7 @@
       <c r="K355" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M355" s="14"/>
+      <c r="M355" s="13"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11626,7 +11638,7 @@
       <c r="J356" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M356" s="14"/>
+      <c r="M356" s="13"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11660,7 +11672,7 @@
       <c r="K357" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M357" s="14"/>
+      <c r="M357" s="13"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11694,7 +11706,7 @@
       <c r="K358" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M358" s="14"/>
+      <c r="M358" s="13"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11728,7 +11740,7 @@
       <c r="K359" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M359" s="14"/>
+      <c r="M359" s="13"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11759,7 +11771,7 @@
       <c r="J360" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M360" s="14"/>
+      <c r="M360" s="13"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11790,7 +11802,7 @@
       <c r="J361" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M361" s="14"/>
+      <c r="M361" s="13"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11821,7 +11833,7 @@
       <c r="J362" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M362" s="14"/>
+      <c r="M362" s="13"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11846,7 +11858,7 @@
       <c r="J363" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M363" s="14"/>
+      <c r="M363" s="13"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11871,7 +11883,7 @@
       <c r="J364" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M364" s="14"/>
+      <c r="M364" s="13"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11898,7 +11910,7 @@
       <c r="J365" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M365" s="14"/>
+      <c r="M365" s="13"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11925,7 +11937,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="14"/>
+      <c r="M366" s="13"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11952,7 +11964,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="14"/>
+      <c r="M367" s="13"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11979,7 +11991,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="14"/>
+      <c r="M368" s="13"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -12006,7 +12018,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="14"/>
+      <c r="M369" s="13"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -12033,7 +12045,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="14"/>
+      <c r="M370" s="13"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -12060,7 +12072,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="14"/>
+      <c r="M371" s="13"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -12087,7 +12099,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="14"/>
+      <c r="M372" s="13"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -12112,7 +12124,7 @@
       <c r="J373" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M373" s="14"/>
+      <c r="M373" s="13"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -12137,7 +12149,7 @@
       <c r="J374" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M374" s="14"/>
+      <c r="M374" s="13"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -12162,7 +12174,7 @@
       <c r="J375" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M375" s="14"/>
+      <c r="M375" s="13"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12190,7 +12202,7 @@
       <c r="K376" t="s">
         <v>224</v>
       </c>
-      <c r="M376" s="14"/>
+      <c r="M376" s="13"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12215,7 +12227,7 @@
       <c r="J377" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M377" s="14"/>
+      <c r="M377" s="13"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12240,7 +12252,7 @@
       <c r="J378" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M378" s="14"/>
+      <c r="M378" s="13"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12265,7 +12277,7 @@
       <c r="J379" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M379" s="14"/>
+      <c r="M379" s="13"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12292,7 +12304,7 @@
       <c r="J380" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M380" s="14"/>
+      <c r="M380" s="13"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12317,7 +12329,7 @@
       <c r="J381" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M381" s="14"/>
+      <c r="M381" s="13"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12344,7 +12356,7 @@
       <c r="J382" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M382" s="14"/>
+      <c r="M382" s="13"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12369,7 +12381,7 @@
       <c r="J383" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M383" s="14"/>
+      <c r="M383" s="13"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12394,7 +12406,7 @@
       <c r="J384" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M384" s="14"/>
+      <c r="M384" s="13"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12419,7 +12431,7 @@
       <c r="J385" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M385" s="14"/>
+      <c r="M385" s="13"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12444,7 +12456,7 @@
       <c r="J386" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M386" s="14"/>
+      <c r="M386" s="13"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12525,7 +12537,7 @@
       <c r="K389" t="s">
         <v>221</v>
       </c>
-      <c r="M389" s="14">
+      <c r="M389" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -12557,7 +12569,7 @@
       <c r="K390" t="s">
         <v>221</v>
       </c>
-      <c r="M390" s="14"/>
+      <c r="M390" s="13"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12587,7 +12599,7 @@
       <c r="K391" t="s">
         <v>221</v>
       </c>
-      <c r="M391" s="14"/>
+      <c r="M391" s="13"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12617,7 +12629,7 @@
       <c r="K392" t="s">
         <v>221</v>
       </c>
-      <c r="M392" s="14"/>
+      <c r="M392" s="13"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12647,7 +12659,7 @@
       <c r="K393" t="s">
         <v>221</v>
       </c>
-      <c r="M393" s="14"/>
+      <c r="M393" s="13"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12677,7 +12689,7 @@
       <c r="K394" t="s">
         <v>221</v>
       </c>
-      <c r="M394" s="14"/>
+      <c r="M394" s="13"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12704,7 +12716,7 @@
       <c r="J395" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M395" s="14"/>
+      <c r="M395" s="13"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12734,7 +12746,7 @@
       <c r="J396" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M396" s="14">
+      <c r="M396" s="13">
         <v>1</v>
       </c>
     </row>
@@ -12763,7 +12775,7 @@
       <c r="J397" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M397" s="14"/>
+      <c r="M397" s="13"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12790,7 +12802,7 @@
       <c r="J398" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M398" s="14"/>
+      <c r="M398" s="13"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12820,7 +12832,7 @@
       <c r="K399" t="s">
         <v>224</v>
       </c>
-      <c r="M399" s="14"/>
+      <c r="M399" s="13"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12847,7 +12859,7 @@
       <c r="J400" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M400" s="14"/>
+      <c r="M400" s="13"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12874,7 +12886,7 @@
       <c r="J401" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M401" s="14"/>
+      <c r="M401" s="13"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12901,7 +12913,7 @@
       <c r="J402" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M402" s="14"/>
+      <c r="M402" s="13"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12928,7 +12940,7 @@
       <c r="J403" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M403" s="14"/>
+      <c r="M403" s="13"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12958,7 +12970,7 @@
       <c r="K404" t="s">
         <v>224</v>
       </c>
-      <c r="M404" s="14"/>
+      <c r="M404" s="13"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12985,7 +12997,7 @@
       <c r="J405" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M405" s="14"/>
+      <c r="M405" s="13"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -13012,7 +13024,7 @@
       <c r="J406" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M406" s="14"/>
+      <c r="M406" s="13"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -13039,7 +13051,7 @@
       <c r="J407" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M407" s="14"/>
+      <c r="M407" s="13"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -13068,7 +13080,7 @@
       <c r="J408" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M408" s="14"/>
+      <c r="M408" s="13"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -13095,7 +13107,7 @@
       <c r="J409" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M409" s="14"/>
+      <c r="M409" s="13"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -13124,7 +13136,7 @@
       <c r="J410" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M410" s="14"/>
+      <c r="M410" s="13"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -13151,7 +13163,7 @@
       <c r="J411" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M411" s="14"/>
+      <c r="M411" s="13"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -13178,7 +13190,7 @@
       <c r="J412" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M412" s="14"/>
+      <c r="M412" s="13"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13205,7 +13217,7 @@
       <c r="J413" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M413" s="14"/>
+      <c r="M413" s="13"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13232,7 +13244,7 @@
       <c r="J414" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M414" s="14"/>
+      <c r="M414" s="13"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13262,7 +13274,7 @@
       <c r="J415" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M415" s="14">
+      <c r="M415" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -13294,7 +13306,7 @@
       <c r="K416" t="s">
         <v>227</v>
       </c>
-      <c r="M416" s="14"/>
+      <c r="M416" s="13"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13326,7 +13338,7 @@
       <c r="K417" t="s">
         <v>227</v>
       </c>
-      <c r="M417" s="14"/>
+      <c r="M417" s="13"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13358,7 +13370,7 @@
       <c r="K418" t="s">
         <v>227</v>
       </c>
-      <c r="M418" s="14"/>
+      <c r="M418" s="13"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13387,7 +13399,7 @@
       <c r="J419" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M419" s="14"/>
+      <c r="M419" s="13"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13416,7 +13428,7 @@
       <c r="J420" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M420" s="14"/>
+      <c r="M420" s="13"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13446,7 +13458,7 @@
       <c r="J421" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M421" s="14">
+      <c r="M421" s="13">
         <v>1</v>
       </c>
     </row>
@@ -13475,7 +13487,7 @@
       <c r="J422" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M422" s="14"/>
+      <c r="M422" s="13"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13502,7 +13514,7 @@
       <c r="J423" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M423" s="14"/>
+      <c r="M423" s="13"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13532,7 +13544,7 @@
       <c r="K424" t="s">
         <v>224</v>
       </c>
-      <c r="M424" s="14"/>
+      <c r="M424" s="13"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13559,7 +13571,7 @@
       <c r="J425" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M425" s="14"/>
+      <c r="M425" s="13"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13586,7 +13598,7 @@
       <c r="J426" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M426" s="14"/>
+      <c r="M426" s="13"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13613,7 +13625,7 @@
       <c r="J427" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M427" s="14"/>
+      <c r="M427" s="13"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13640,7 +13652,7 @@
       <c r="J428" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M428" s="14"/>
+      <c r="M428" s="13"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13670,7 +13682,7 @@
       <c r="K429" t="s">
         <v>224</v>
       </c>
-      <c r="M429" s="14"/>
+      <c r="M429" s="13"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13697,7 +13709,7 @@
       <c r="J430" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M430" s="14"/>
+      <c r="M430" s="13"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13724,7 +13736,7 @@
       <c r="J431" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M431" s="14"/>
+      <c r="M431" s="13"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13751,7 +13763,7 @@
       <c r="J432" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M432" s="14"/>
+      <c r="M432" s="13"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13780,7 +13792,7 @@
       <c r="J433" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M433" s="14"/>
+      <c r="M433" s="13"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13807,7 +13819,7 @@
       <c r="J434" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M434" s="14"/>
+      <c r="M434" s="13"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13836,7 +13848,7 @@
       <c r="J435" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M435" s="14"/>
+      <c r="M435" s="13"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13863,7 +13875,7 @@
       <c r="J436" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M436" s="14"/>
+      <c r="M436" s="13"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13890,7 +13902,7 @@
       <c r="J437" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M437" s="14"/>
+      <c r="M437" s="13"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13917,7 +13929,7 @@
       <c r="J438" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M438" s="14"/>
+      <c r="M438" s="13"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13944,7 +13956,7 @@
       <c r="J439" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M439" s="14"/>
+      <c r="M439" s="13"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13978,7 +13990,7 @@
       <c r="J440" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M440" s="14">
+      <c r="M440" s="13">
         <v>1</v>
       </c>
     </row>
@@ -14011,7 +14023,7 @@
       <c r="J441" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M441" s="14"/>
+      <c r="M441" s="13"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -14042,7 +14054,7 @@
       <c r="J442" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M442" s="14"/>
+      <c r="M442" s="13"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -14073,7 +14085,7 @@
       <c r="J443" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M443" s="14"/>
+      <c r="M443" s="13"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -14104,7 +14116,7 @@
       <c r="J444" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M444" s="14"/>
+      <c r="M444" s="13"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -14135,7 +14147,7 @@
       <c r="J445" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M445" s="14"/>
+      <c r="M445" s="13"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -14166,7 +14178,7 @@
       <c r="J446" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M446" s="14"/>
+      <c r="M446" s="13"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -14197,7 +14209,7 @@
       <c r="J447" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M447" s="14"/>
+      <c r="M447" s="13"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14226,9 +14238,9 @@
         <v>210</v>
       </c>
       <c r="J448" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M448" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M448" s="13"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14257,9 +14269,9 @@
         <v>210</v>
       </c>
       <c r="J449" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M449" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M449" s="13"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14288,7 +14300,7 @@
       <c r="J450" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M450" s="14"/>
+      <c r="M450" s="13"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14317,7 +14329,7 @@
       <c r="J451" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M451" s="14"/>
+      <c r="M451" s="13"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14346,7 +14358,7 @@
       <c r="J452" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M452" s="14"/>
+      <c r="M452" s="13"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14375,7 +14387,7 @@
       <c r="J453" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M453" s="14"/>
+      <c r="M453" s="13"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14404,7 +14416,7 @@
       <c r="J454" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M454" s="14"/>
+      <c r="M454" s="13"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14431,7 +14443,7 @@
       <c r="J455" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M455" s="14"/>
+      <c r="M455" s="13"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14452,16 +14464,13 @@
       <c r="F456" s="1"/>
       <c r="G456" s="1"/>
       <c r="H456" s="1"/>
-      <c r="I456" s="4" t="s">
-        <v>211</v>
+      <c r="I456" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="J456" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="K456" t="s">
-        <v>227</v>
-      </c>
-      <c r="M456" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M456" s="13"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14491,7 +14500,7 @@
       <c r="K457" t="s">
         <v>227</v>
       </c>
-      <c r="M457" s="14"/>
+      <c r="M457" s="13"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14523,7 +14532,7 @@
       <c r="K458" t="s">
         <v>227</v>
       </c>
-      <c r="M458" s="14"/>
+      <c r="M458" s="13"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14547,12 +14556,15 @@
       <c r="G459" s="1"/>
       <c r="H459" s="1"/>
       <c r="I459" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J459" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="M459" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="K459" t="s">
+        <v>227</v>
+      </c>
+      <c r="M459" s="13"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14581,7 +14593,7 @@
       <c r="J460" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M460" s="14"/>
+      <c r="M460" s="13"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14605,12 +14617,12 @@
       <c r="G461" s="1"/>
       <c r="H461" s="1"/>
       <c r="I461" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J461" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M461" s="14"/>
+        <v>210</v>
+      </c>
+      <c r="M461" s="13"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14841,10 +14853,10 @@
       <c r="G470" s="1"/>
       <c r="H470" s="1"/>
       <c r="I470" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J470" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="471" spans="1:13">
@@ -14865,10 +14877,10 @@
       <c r="G471" s="1"/>
       <c r="H471" s="1"/>
       <c r="I471" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J471" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="472" spans="1:13">
@@ -14889,10 +14901,10 @@
       <c r="G472" s="1"/>
       <c r="H472" s="1"/>
       <c r="I472" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J472" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="473" spans="1:13">
@@ -14913,10 +14925,10 @@
       <c r="G473" s="1"/>
       <c r="H473" s="1"/>
       <c r="I473" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J473" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="474" spans="1:13">
@@ -14944,7 +14956,7 @@
       <c r="J474" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M474" s="15">
+      <c r="M474" s="12">
         <v>1</v>
       </c>
     </row>
@@ -14973,7 +14985,7 @@
       <c r="J475" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M475" s="15"/>
+      <c r="M475" s="12"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -15000,7 +15012,7 @@
       <c r="J476" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M476" s="15"/>
+      <c r="M476" s="12"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -15027,7 +15039,7 @@
       <c r="J477" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M477" s="15"/>
+      <c r="M477" s="12"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -15054,7 +15066,7 @@
       <c r="J478" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M478" s="15"/>
+      <c r="M478" s="12"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -15081,7 +15093,7 @@
       <c r="J479" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M479" s="15"/>
+      <c r="M479" s="12"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -15108,7 +15120,7 @@
       <c r="J480" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M480" s="15"/>
+      <c r="M480" s="12"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15135,7 +15147,7 @@
       <c r="J481" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M481" s="15"/>
+      <c r="M481" s="12"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15162,7 +15174,7 @@
       <c r="J482" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M482" s="15"/>
+      <c r="M482" s="12"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15189,7 +15201,7 @@
       <c r="J483" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M483" s="15"/>
+      <c r="M483" s="12"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15349,7 +15361,7 @@
       <c r="J489" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M489" s="15">
+      <c r="M489" s="12">
         <v>2</v>
       </c>
     </row>
@@ -15376,7 +15388,7 @@
       <c r="J490" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M490" s="15"/>
+      <c r="M490" s="12"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15401,7 +15413,7 @@
       <c r="J491" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M491" s="15"/>
+      <c r="M491" s="12"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15426,7 +15438,7 @@
       <c r="J492" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M492" s="15"/>
+      <c r="M492" s="12"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15451,7 +15463,7 @@
       <c r="J493" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M493" s="15"/>
+      <c r="M493" s="12"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15478,7 +15490,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="15"/>
+      <c r="M494" s="12"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15505,7 +15517,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="15"/>
+      <c r="M495" s="12"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15532,7 +15544,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="15"/>
+      <c r="M496" s="12"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15559,7 +15571,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="15"/>
+      <c r="M497" s="12"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15612,7 +15624,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="15">
+      <c r="M499" s="12">
         <v>1</v>
       </c>
     </row>
@@ -15639,7 +15651,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="15"/>
+      <c r="M500" s="12"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15664,7 +15676,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="15"/>
+      <c r="M501" s="12"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15689,7 +15701,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="15"/>
+      <c r="M502" s="12"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15714,7 +15726,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="15"/>
+      <c r="M503" s="12"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15739,7 +15751,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="15"/>
+      <c r="M504" s="12"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15766,7 +15778,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="15"/>
+      <c r="M505" s="12"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15791,7 +15803,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="15"/>
+      <c r="M506" s="12"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15818,7 +15830,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="15"/>
+      <c r="M507" s="12"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15843,7 +15855,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="15"/>
+      <c r="M508" s="12"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15868,7 +15880,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="15"/>
+      <c r="M509" s="12"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15893,7 +15905,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="15"/>
+      <c r="M510" s="12"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15918,7 +15930,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="15"/>
+      <c r="M511" s="12"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15945,7 +15957,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="15"/>
+      <c r="M512" s="12"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15972,7 +15984,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="15"/>
+      <c r="M513" s="12"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -15997,7 +16009,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="15"/>
+      <c r="M514" s="12"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -16022,7 +16034,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="15"/>
+      <c r="M515" s="12"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -16050,7 +16062,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="15">
+      <c r="M516" s="12">
         <v>2</v>
       </c>
     </row>
@@ -16079,7 +16091,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="15"/>
+      <c r="M517" s="12"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -16106,7 +16118,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="15"/>
+      <c r="M518" s="12"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -16133,7 +16145,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="15"/>
+      <c r="M519" s="12"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16162,7 +16174,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="15"/>
+      <c r="M520" s="12"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16191,7 +16203,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="15"/>
+      <c r="M521" s="12"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16220,7 +16232,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="15"/>
+      <c r="M522" s="12"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16249,7 +16261,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="15"/>
+      <c r="M523" s="12"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16278,7 +16290,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="15"/>
+      <c r="M524" s="12"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16307,7 +16319,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="15"/>
+      <c r="M525" s="12"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16334,7 +16346,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="15"/>
+      <c r="M526" s="12"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16361,7 +16373,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="15"/>
+      <c r="M527" s="12"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16386,6 +16398,11 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16402,11 +16419,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart -> Data Series -> Line
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4065" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4069" uniqueCount="228">
   <si>
     <t>Chart</t>
   </si>
@@ -882,10 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,7 +891,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1218,10 +1218,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I470" sqref="I470"/>
+      <selection pane="bottomLeft" activeCell="I493" sqref="I493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1241,16 +1241,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1346,7 +1346,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1371,7 +1371,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1396,7 +1396,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1421,7 +1421,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1446,7 +1446,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1471,7 +1471,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1496,7 +1496,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="13"/>
+      <c r="M10" s="15"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2117,7 +2117,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="13"/>
+      <c r="M34" s="15"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="13">
+      <c r="M43" s="15">
         <v>2</v>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="13"/>
+      <c r="M44" s="15"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2478,7 +2478,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="13"/>
+      <c r="M45" s="15"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2510,7 +2510,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="13"/>
+      <c r="M46" s="15"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2542,7 +2542,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="13"/>
+      <c r="M47" s="15"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2574,7 +2574,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="13"/>
+      <c r="M48" s="15"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2606,7 +2606,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="13"/>
+      <c r="M49" s="15"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2638,7 +2638,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="13"/>
+      <c r="M50" s="15"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2827,7 +2827,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="13">
+      <c r="M57" s="15">
         <v>3</v>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="13"/>
+      <c r="M58" s="15"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2883,7 +2883,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="13"/>
+      <c r="M59" s="15"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2910,7 +2910,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="13"/>
+      <c r="M60" s="15"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -4008,7 +4008,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="13">
+      <c r="M98" s="15">
         <v>2</v>
       </c>
     </row>
@@ -4035,7 +4035,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="13"/>
+      <c r="M99" s="15"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4063,7 +4063,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="13"/>
+      <c r="M100" s="15"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4088,7 +4088,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="13"/>
+      <c r="M101" s="15"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4115,7 +4115,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="13"/>
+      <c r="M102" s="15"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4142,7 +4142,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="13"/>
+      <c r="M103" s="15"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4171,7 +4171,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="13"/>
+      <c r="M104" s="15"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4200,7 +4200,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="13"/>
+      <c r="M105" s="15"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4234,7 +4234,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="13"/>
+      <c r="M106" s="15"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4268,7 +4268,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="13"/>
+      <c r="M107" s="15"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4302,7 +4302,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="13"/>
+      <c r="M108" s="15"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4336,7 +4336,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="13"/>
+      <c r="M109" s="15"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4365,7 +4365,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="13"/>
+      <c r="M110" s="15"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4399,7 +4399,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="13"/>
+      <c r="M111" s="15"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4433,7 +4433,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="13"/>
+      <c r="M112" s="15"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4467,7 +4467,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="13"/>
+      <c r="M113" s="15"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4498,7 +4498,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="13"/>
+      <c r="M114" s="15"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4529,7 +4529,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="13"/>
+      <c r="M115" s="15"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4560,7 +4560,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="13"/>
+      <c r="M116" s="15"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4585,7 +4585,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="13"/>
+      <c r="M117" s="15"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4612,7 +4612,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="13"/>
+      <c r="M118" s="15"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4846,7 +4846,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="13">
+      <c r="M127" s="15">
         <v>1</v>
       </c>
     </row>
@@ -4873,7 +4873,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="13"/>
+      <c r="M128" s="15"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4901,7 +4901,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="13"/>
+      <c r="M129" s="15"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4926,7 +4926,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="13"/>
+      <c r="M130" s="15"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4951,7 +4951,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="13"/>
+      <c r="M131" s="15"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4978,7 +4978,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="13"/>
+      <c r="M132" s="15"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -5005,7 +5005,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="13"/>
+      <c r="M133" s="15"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5034,7 +5034,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="13"/>
+      <c r="M134" s="15"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5063,7 +5063,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="13"/>
+      <c r="M135" s="15"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5097,7 +5097,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="13"/>
+      <c r="M136" s="15"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5131,7 +5131,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="13"/>
+      <c r="M137" s="15"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5165,7 +5165,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="13"/>
+      <c r="M138" s="15"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5199,7 +5199,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="13"/>
+      <c r="M139" s="15"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5228,7 +5228,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="13"/>
+      <c r="M140" s="15"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5262,7 +5262,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="13"/>
+      <c r="M141" s="15"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5296,7 +5296,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="13"/>
+      <c r="M142" s="15"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5328,7 +5328,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="13"/>
+      <c r="M143" s="15"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5359,7 +5359,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="13"/>
+      <c r="M144" s="15"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5390,7 +5390,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="13"/>
+      <c r="M145" s="15"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5421,7 +5421,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="13"/>
+      <c r="M146" s="15"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5446,7 +5446,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="13"/>
+      <c r="M147" s="15"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5471,7 +5471,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="13"/>
+      <c r="M148" s="15"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5498,7 +5498,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="13"/>
+      <c r="M149" s="15"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5525,7 +5525,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="13"/>
+      <c r="M150" s="15"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5552,7 +5552,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="13"/>
+      <c r="M151" s="15"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5579,7 +5579,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="13"/>
+      <c r="M152" s="15"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5606,7 +5606,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="13"/>
+      <c r="M153" s="15"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5633,7 +5633,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="13"/>
+      <c r="M154" s="15"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5660,7 +5660,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="13"/>
+      <c r="M155" s="15"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5687,7 +5687,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="13"/>
+      <c r="M156" s="15"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5715,7 +5715,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="13"/>
+      <c r="M157" s="15"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5745,7 +5745,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="13"/>
+      <c r="M158" s="15"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5775,7 +5775,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="13"/>
+      <c r="M159" s="15"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5805,7 +5805,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="13"/>
+      <c r="M160" s="15"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5835,7 +5835,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="13"/>
+      <c r="M161" s="15"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5865,7 +5865,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="13"/>
+      <c r="M162" s="15"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5895,7 +5895,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="13"/>
+      <c r="M163" s="15"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5925,7 +5925,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="13"/>
+      <c r="M164" s="15"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5955,7 +5955,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="13">
+      <c r="M165" s="15">
         <v>1</v>
       </c>
     </row>
@@ -5984,7 +5984,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="13"/>
+      <c r="M166" s="15"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -6011,7 +6011,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="13"/>
+      <c r="M167" s="15"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6041,7 +6041,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="13"/>
+      <c r="M168" s="15"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6068,7 +6068,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="13"/>
+      <c r="M169" s="15"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6095,7 +6095,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="13"/>
+      <c r="M170" s="15"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6124,7 +6124,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="13"/>
+      <c r="M171" s="15"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6153,7 +6153,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="13"/>
+      <c r="M172" s="15"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6184,7 +6184,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="13"/>
+      <c r="M173" s="15"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6215,7 +6215,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="13"/>
+      <c r="M174" s="15"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6251,7 +6251,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="13"/>
+      <c r="M175" s="15"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6287,7 +6287,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="13"/>
+      <c r="M176" s="15"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6323,7 +6323,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="13"/>
+      <c r="M177" s="15"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6359,7 +6359,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="13"/>
+      <c r="M178" s="15"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6390,7 +6390,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="13"/>
+      <c r="M179" s="15"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6426,7 +6426,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="13"/>
+      <c r="M180" s="15"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6462,7 +6462,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="13"/>
+      <c r="M181" s="15"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6498,7 +6498,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="13"/>
+      <c r="M182" s="15"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6531,7 +6531,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="13"/>
+      <c r="M183" s="15"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6564,7 +6564,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="13"/>
+      <c r="M184" s="15"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6597,7 +6597,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="13"/>
+      <c r="M185" s="15"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6624,7 +6624,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="13"/>
+      <c r="M186" s="15"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6651,7 +6651,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="13"/>
+      <c r="M187" s="15"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6680,7 +6680,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="13"/>
+      <c r="M188" s="15"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6903,7 +6903,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="13">
+      <c r="M196" s="15">
         <v>2</v>
       </c>
     </row>
@@ -6932,7 +6932,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="13"/>
+      <c r="M197" s="15"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6962,7 +6962,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="13"/>
+      <c r="M198" s="15"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6989,7 +6989,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="13"/>
+      <c r="M199" s="15"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -7016,7 +7016,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="13"/>
+      <c r="M200" s="15"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7045,7 +7045,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="13"/>
+      <c r="M201" s="15"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7072,7 +7072,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="13"/>
+      <c r="M202" s="15"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7101,7 +7101,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="13"/>
+      <c r="M203" s="15"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7128,7 +7128,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="13"/>
+      <c r="M204" s="15"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7155,7 +7155,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="13"/>
+      <c r="M205" s="15"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7182,7 +7182,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="13"/>
+      <c r="M206" s="15"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7209,7 +7209,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="13"/>
+      <c r="M207" s="15"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7239,7 +7239,7 @@
       <c r="K208" t="s">
         <v>225</v>
       </c>
-      <c r="M208" s="13"/>
+      <c r="M208" s="15"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7269,7 +7269,7 @@
       <c r="K209" t="s">
         <v>225</v>
       </c>
-      <c r="M209" s="13"/>
+      <c r="M209" s="15"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7302,7 +7302,7 @@
       <c r="K210" t="s">
         <v>220</v>
       </c>
-      <c r="M210" s="13">
+      <c r="M210" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -7336,7 +7336,7 @@
       <c r="K211" t="s">
         <v>221</v>
       </c>
-      <c r="M211" s="13"/>
+      <c r="M211" s="15"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7368,7 +7368,7 @@
       <c r="K212" t="s">
         <v>221</v>
       </c>
-      <c r="M212" s="13"/>
+      <c r="M212" s="15"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7400,7 +7400,7 @@
       <c r="K213" t="s">
         <v>221</v>
       </c>
-      <c r="M213" s="13"/>
+      <c r="M213" s="15"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7432,7 +7432,7 @@
       <c r="K214" t="s">
         <v>221</v>
       </c>
-      <c r="M214" s="13"/>
+      <c r="M214" s="15"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7464,7 +7464,7 @@
       <c r="K215" t="s">
         <v>221</v>
       </c>
-      <c r="M215" s="13"/>
+      <c r="M215" s="15"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7496,7 +7496,7 @@
       <c r="K216" t="s">
         <v>221</v>
       </c>
-      <c r="M216" s="13"/>
+      <c r="M216" s="15"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7528,7 +7528,7 @@
       <c r="K217" t="s">
         <v>221</v>
       </c>
-      <c r="M217" s="13"/>
+      <c r="M217" s="15"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7557,7 +7557,7 @@
       <c r="J218" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M218" s="13"/>
+      <c r="M218" s="15"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7586,7 +7586,7 @@
       <c r="J219" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M219" s="13"/>
+      <c r="M219" s="15"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7613,7 +7613,7 @@
       <c r="J220" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M220" s="13">
+      <c r="M220" s="15">
         <v>1</v>
       </c>
     </row>
@@ -7642,7 +7642,7 @@
       <c r="J221" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M221" s="13"/>
+      <c r="M221" s="15"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7669,7 +7669,7 @@
       <c r="J222" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M222" s="13"/>
+      <c r="M222" s="15"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7699,7 +7699,7 @@
       <c r="K223" t="s">
         <v>224</v>
       </c>
-      <c r="M223" s="13"/>
+      <c r="M223" s="15"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7726,7 +7726,7 @@
       <c r="J224" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M224" s="13"/>
+      <c r="M224" s="15"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7753,7 +7753,7 @@
       <c r="J225" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M225" s="13"/>
+      <c r="M225" s="15"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7782,7 +7782,7 @@
       <c r="J226" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M226" s="13"/>
+      <c r="M226" s="15"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7811,7 +7811,7 @@
       <c r="J227" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M227" s="13"/>
+      <c r="M227" s="15"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7842,7 +7842,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="13"/>
+      <c r="M228" s="15"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7873,7 +7873,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="13"/>
+      <c r="M229" s="15"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7909,7 +7909,7 @@
       <c r="K230" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M230" s="13"/>
+      <c r="M230" s="15"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7945,7 +7945,7 @@
       <c r="K231" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M231" s="13"/>
+      <c r="M231" s="15"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7981,7 +7981,7 @@
       <c r="K232" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M232" s="13"/>
+      <c r="M232" s="15"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -8017,7 +8017,7 @@
       <c r="K233" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M233" s="13"/>
+      <c r="M233" s="15"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -8048,7 +8048,7 @@
       <c r="J234" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M234" s="13"/>
+      <c r="M234" s="15"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8084,7 +8084,7 @@
       <c r="K235" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M235" s="13"/>
+      <c r="M235" s="15"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8120,7 +8120,7 @@
       <c r="K236" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M236" s="13"/>
+      <c r="M236" s="15"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8156,7 +8156,7 @@
       <c r="K237" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M237" s="13"/>
+      <c r="M237" s="15"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8189,7 +8189,7 @@
       <c r="J238" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M238" s="13"/>
+      <c r="M238" s="15"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8222,7 +8222,7 @@
       <c r="J239" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M239" s="13"/>
+      <c r="M239" s="15"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8255,7 +8255,7 @@
       <c r="J240" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M240" s="13"/>
+      <c r="M240" s="15"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8282,7 +8282,7 @@
       <c r="J241" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M241" s="13"/>
+      <c r="M241" s="15"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8309,7 +8309,7 @@
       <c r="J242" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M242" s="13"/>
+      <c r="M242" s="15"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8338,7 +8338,7 @@
       <c r="J243" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M243" s="13"/>
+      <c r="M243" s="15"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8367,7 +8367,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="13"/>
+      <c r="M244" s="15"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8396,7 +8396,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="13"/>
+      <c r="M245" s="15"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8425,7 +8425,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="13"/>
+      <c r="M246" s="15"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8454,7 +8454,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="13"/>
+      <c r="M247" s="15"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8483,7 +8483,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="13"/>
+      <c r="M248" s="15"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8512,7 +8512,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="13"/>
+      <c r="M249" s="15"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8541,7 +8541,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="13"/>
+      <c r="M250" s="15"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8568,7 +8568,7 @@
       <c r="J251" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M251" s="13"/>
+      <c r="M251" s="15"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8595,7 +8595,7 @@
       <c r="J252" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M252" s="13"/>
+      <c r="M252" s="15"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8622,7 +8622,7 @@
       <c r="J253" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M253" s="13"/>
+      <c r="M253" s="15"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8652,7 +8652,7 @@
       <c r="K254" t="s">
         <v>224</v>
       </c>
-      <c r="M254" s="13"/>
+      <c r="M254" s="15"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8679,7 +8679,7 @@
       <c r="J255" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M255" s="13"/>
+      <c r="M255" s="15"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8706,7 +8706,7 @@
       <c r="J256" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M256" s="13"/>
+      <c r="M256" s="15"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8733,7 +8733,7 @@
       <c r="J257" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M257" s="13"/>
+      <c r="M257" s="15"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8762,7 +8762,7 @@
       <c r="J258" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M258" s="13"/>
+      <c r="M258" s="15"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8789,7 +8789,7 @@
       <c r="J259" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M259" s="13"/>
+      <c r="M259" s="15"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8818,7 +8818,7 @@
       <c r="J260" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M260" s="13"/>
+      <c r="M260" s="15"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8845,7 +8845,7 @@
       <c r="J261" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M261" s="13"/>
+      <c r="M261" s="15"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8872,7 +8872,7 @@
       <c r="J262" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M262" s="13"/>
+      <c r="M262" s="15"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8899,7 +8899,7 @@
       <c r="J263" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M263" s="13"/>
+      <c r="M263" s="15"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8926,7 +8926,7 @@
       <c r="J264" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M264" s="13"/>
+      <c r="M264" s="15"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8956,7 +8956,7 @@
       <c r="K265" t="s">
         <v>225</v>
       </c>
-      <c r="M265" s="13"/>
+      <c r="M265" s="15"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8986,7 +8986,7 @@
       <c r="K266" t="s">
         <v>225</v>
       </c>
-      <c r="M266" s="13"/>
+      <c r="M266" s="15"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -9016,7 +9016,7 @@
       <c r="K267" t="s">
         <v>225</v>
       </c>
-      <c r="M267" s="13"/>
+      <c r="M267" s="15"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -9046,7 +9046,7 @@
       <c r="K268" t="s">
         <v>220</v>
       </c>
-      <c r="M268" s="13"/>
+      <c r="M268" s="15"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -9078,7 +9078,7 @@
       <c r="K269" t="s">
         <v>221</v>
       </c>
-      <c r="M269" s="13"/>
+      <c r="M269" s="15"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9110,7 +9110,7 @@
       <c r="K270" t="s">
         <v>221</v>
       </c>
-      <c r="M270" s="13"/>
+      <c r="M270" s="15"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9142,7 +9142,7 @@
       <c r="K271" t="s">
         <v>221</v>
       </c>
-      <c r="M271" s="13"/>
+      <c r="M271" s="15"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9174,7 +9174,7 @@
       <c r="K272" t="s">
         <v>221</v>
       </c>
-      <c r="M272" s="13"/>
+      <c r="M272" s="15"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9206,7 +9206,7 @@
       <c r="K273" t="s">
         <v>221</v>
       </c>
-      <c r="M273" s="13"/>
+      <c r="M273" s="15"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9238,7 +9238,7 @@
       <c r="K274" t="s">
         <v>221</v>
       </c>
-      <c r="M274" s="13"/>
+      <c r="M274" s="15"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9270,7 +9270,7 @@
       <c r="K275" t="s">
         <v>221</v>
       </c>
-      <c r="M275" s="13"/>
+      <c r="M275" s="15"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9299,7 +9299,7 @@
       <c r="J276" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M276" s="13"/>
+      <c r="M276" s="15"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9328,7 +9328,7 @@
       <c r="J277" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M277" s="13"/>
+      <c r="M277" s="15"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9355,7 +9355,7 @@
       <c r="J278" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M278" s="13"/>
+      <c r="M278" s="15"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9382,7 +9382,7 @@
       <c r="J279" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M279" s="13"/>
+      <c r="M279" s="15"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9409,7 +9409,7 @@
       <c r="J280" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M280" s="13"/>
+      <c r="M280" s="15"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9439,7 +9439,7 @@
       <c r="K281" t="s">
         <v>224</v>
       </c>
-      <c r="M281" s="13"/>
+      <c r="M281" s="15"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9466,7 +9466,7 @@
       <c r="J282" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M282" s="13"/>
+      <c r="M282" s="15"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9493,7 +9493,7 @@
       <c r="J283" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M283" s="13"/>
+      <c r="M283" s="15"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9522,7 +9522,7 @@
       <c r="J284" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M284" s="13"/>
+      <c r="M284" s="15"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9551,7 +9551,7 @@
       <c r="J285" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M285" s="13"/>
+      <c r="M285" s="15"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9582,7 +9582,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="13"/>
+      <c r="M286" s="15"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9613,7 +9613,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="13"/>
+      <c r="M287" s="15"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9649,7 +9649,7 @@
       <c r="K288" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M288" s="13"/>
+      <c r="M288" s="15"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9685,7 +9685,7 @@
       <c r="K289" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M289" s="13"/>
+      <c r="M289" s="15"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9721,7 +9721,7 @@
       <c r="K290" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M290" s="13"/>
+      <c r="M290" s="15"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9757,7 +9757,7 @@
       <c r="K291" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M291" s="13"/>
+      <c r="M291" s="15"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9788,7 +9788,7 @@
       <c r="J292" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M292" s="13"/>
+      <c r="M292" s="15"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9824,7 +9824,7 @@
       <c r="K293" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M293" s="13"/>
+      <c r="M293" s="15"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9860,7 +9860,7 @@
       <c r="K294" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M294" s="13"/>
+      <c r="M294" s="15"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9896,7 +9896,7 @@
       <c r="K295" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M295" s="13"/>
+      <c r="M295" s="15"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9929,7 +9929,7 @@
       <c r="J296" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M296" s="13"/>
+      <c r="M296" s="15"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9962,7 +9962,7 @@
       <c r="J297" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M297" s="13"/>
+      <c r="M297" s="15"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -9995,7 +9995,7 @@
       <c r="J298" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M298" s="13"/>
+      <c r="M298" s="15"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -10022,7 +10022,7 @@
       <c r="J299" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M299" s="13"/>
+      <c r="M299" s="15"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -10049,7 +10049,7 @@
       <c r="J300" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M300" s="13"/>
+      <c r="M300" s="15"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -10078,7 +10078,7 @@
       <c r="J301" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M301" s="13"/>
+      <c r="M301" s="15"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -10107,7 +10107,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="13"/>
+      <c r="M302" s="15"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10136,7 +10136,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="13"/>
+      <c r="M303" s="15"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10165,7 +10165,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="13"/>
+      <c r="M304" s="15"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10194,7 +10194,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="13"/>
+      <c r="M305" s="15"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10223,7 +10223,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="13"/>
+      <c r="M306" s="15"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10252,7 +10252,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="13"/>
+      <c r="M307" s="15"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10281,7 +10281,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="13"/>
+      <c r="M308" s="15"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10308,7 +10308,7 @@
       <c r="J309" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M309" s="13"/>
+      <c r="M309" s="15"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10335,7 +10335,7 @@
       <c r="J310" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M310" s="13"/>
+      <c r="M310" s="15"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10362,7 +10362,7 @@
       <c r="J311" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M311" s="13"/>
+      <c r="M311" s="15"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10392,7 +10392,7 @@
       <c r="K312" t="s">
         <v>224</v>
       </c>
-      <c r="M312" s="13"/>
+      <c r="M312" s="15"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10419,7 +10419,7 @@
       <c r="J313" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M313" s="13"/>
+      <c r="M313" s="15"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10446,7 +10446,7 @@
       <c r="J314" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M314" s="13"/>
+      <c r="M314" s="15"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10473,7 +10473,7 @@
       <c r="J315" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M315" s="13"/>
+      <c r="M315" s="15"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10502,7 +10502,7 @@
       <c r="J316" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M316" s="13"/>
+      <c r="M316" s="15"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10529,7 +10529,7 @@
       <c r="J317" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M317" s="13"/>
+      <c r="M317" s="15"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10558,7 +10558,7 @@
       <c r="J318" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M318" s="13"/>
+      <c r="M318" s="15"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10585,7 +10585,7 @@
       <c r="J319" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M319" s="13"/>
+      <c r="M319" s="15"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10612,7 +10612,7 @@
       <c r="J320" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M320" s="13"/>
+      <c r="M320" s="15"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10639,7 +10639,7 @@
       <c r="J321" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M321" s="13"/>
+      <c r="M321" s="15"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10666,7 +10666,7 @@
       <c r="J322" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M322" s="13"/>
+      <c r="M322" s="15"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10693,7 +10693,7 @@
       <c r="J323" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M323" s="13"/>
+      <c r="M323" s="15"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10720,7 +10720,7 @@
       <c r="J324" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M324" s="13"/>
+      <c r="M324" s="15"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10747,7 +10747,7 @@
       <c r="J325" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M325" s="13"/>
+      <c r="M325" s="15"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10777,7 +10777,7 @@
       <c r="K326" t="s">
         <v>221</v>
       </c>
-      <c r="M326" s="13"/>
+      <c r="M326" s="15"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10809,7 +10809,7 @@
       <c r="K327" t="s">
         <v>221</v>
       </c>
-      <c r="M327" s="13"/>
+      <c r="M327" s="15"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10841,7 +10841,7 @@
       <c r="K328" t="s">
         <v>221</v>
       </c>
-      <c r="M328" s="13"/>
+      <c r="M328" s="15"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10873,7 +10873,7 @@
       <c r="K329" t="s">
         <v>221</v>
       </c>
-      <c r="M329" s="13"/>
+      <c r="M329" s="15"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10905,7 +10905,7 @@
       <c r="K330" t="s">
         <v>221</v>
       </c>
-      <c r="M330" s="13"/>
+      <c r="M330" s="15"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10937,7 +10937,7 @@
       <c r="K331" t="s">
         <v>221</v>
       </c>
-      <c r="M331" s="13"/>
+      <c r="M331" s="15"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10969,7 +10969,7 @@
       <c r="K332" t="s">
         <v>221</v>
       </c>
-      <c r="M332" s="13"/>
+      <c r="M332" s="15"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -10998,7 +10998,7 @@
       <c r="J333" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M333" s="13"/>
+      <c r="M333" s="15"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -11027,7 +11027,7 @@
       <c r="J334" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M334" s="13"/>
+      <c r="M334" s="15"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -11056,7 +11056,7 @@
       <c r="J335" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M335" s="13"/>
+      <c r="M335" s="15"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11231,7 +11231,7 @@
       <c r="J342" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M342" s="13">
+      <c r="M342" s="15">
         <v>1</v>
       </c>
     </row>
@@ -11258,7 +11258,7 @@
       <c r="J343" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M343" s="13"/>
+      <c r="M343" s="15"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11283,7 +11283,7 @@
       <c r="J344" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M344" s="13"/>
+      <c r="M344" s="15"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11311,7 +11311,7 @@
       <c r="K345" t="s">
         <v>224</v>
       </c>
-      <c r="M345" s="13"/>
+      <c r="M345" s="15"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11336,7 +11336,7 @@
       <c r="J346" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M346" s="13"/>
+      <c r="M346" s="15"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11361,7 +11361,7 @@
       <c r="J347" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M347" s="13"/>
+      <c r="M347" s="15"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11388,7 +11388,7 @@
       <c r="J348" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M348" s="13"/>
+      <c r="M348" s="15"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11415,7 +11415,7 @@
       <c r="J349" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M349" s="13"/>
+      <c r="M349" s="15"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11444,7 +11444,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="13"/>
+      <c r="M350" s="15"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11473,7 +11473,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="13"/>
+      <c r="M351" s="15"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11507,7 +11507,7 @@
       <c r="K352" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M352" s="13"/>
+      <c r="M352" s="15"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11541,7 +11541,7 @@
       <c r="K353" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M353" s="13"/>
+      <c r="M353" s="15"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11575,7 +11575,7 @@
       <c r="K354" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M354" s="13"/>
+      <c r="M354" s="15"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11609,7 +11609,7 @@
       <c r="K355" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M355" s="13"/>
+      <c r="M355" s="15"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11638,7 +11638,7 @@
       <c r="J356" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M356" s="13"/>
+      <c r="M356" s="15"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11672,7 +11672,7 @@
       <c r="K357" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M357" s="13"/>
+      <c r="M357" s="15"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11706,7 +11706,7 @@
       <c r="K358" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M358" s="13"/>
+      <c r="M358" s="15"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11740,7 +11740,7 @@
       <c r="K359" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M359" s="13"/>
+      <c r="M359" s="15"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11771,7 +11771,7 @@
       <c r="J360" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M360" s="13"/>
+      <c r="M360" s="15"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11802,7 +11802,7 @@
       <c r="J361" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M361" s="13"/>
+      <c r="M361" s="15"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11833,7 +11833,7 @@
       <c r="J362" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M362" s="13"/>
+      <c r="M362" s="15"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11858,7 +11858,7 @@
       <c r="J363" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M363" s="13"/>
+      <c r="M363" s="15"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11883,7 +11883,7 @@
       <c r="J364" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M364" s="13"/>
+      <c r="M364" s="15"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11910,7 +11910,7 @@
       <c r="J365" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M365" s="13"/>
+      <c r="M365" s="15"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11937,7 +11937,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="13"/>
+      <c r="M366" s="15"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11964,7 +11964,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="13"/>
+      <c r="M367" s="15"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -11991,7 +11991,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="13"/>
+      <c r="M368" s="15"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -12018,7 +12018,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="13"/>
+      <c r="M369" s="15"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -12045,7 +12045,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="13"/>
+      <c r="M370" s="15"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -12072,7 +12072,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="13"/>
+      <c r="M371" s="15"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -12099,7 +12099,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="13"/>
+      <c r="M372" s="15"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -12124,7 +12124,7 @@
       <c r="J373" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M373" s="13"/>
+      <c r="M373" s="15"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -12149,7 +12149,7 @@
       <c r="J374" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M374" s="13"/>
+      <c r="M374" s="15"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -12174,7 +12174,7 @@
       <c r="J375" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M375" s="13"/>
+      <c r="M375" s="15"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12202,7 +12202,7 @@
       <c r="K376" t="s">
         <v>224</v>
       </c>
-      <c r="M376" s="13"/>
+      <c r="M376" s="15"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12227,7 +12227,7 @@
       <c r="J377" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M377" s="13"/>
+      <c r="M377" s="15"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12252,7 +12252,7 @@
       <c r="J378" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M378" s="13"/>
+      <c r="M378" s="15"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12277,7 +12277,7 @@
       <c r="J379" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M379" s="13"/>
+      <c r="M379" s="15"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12304,7 +12304,7 @@
       <c r="J380" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M380" s="13"/>
+      <c r="M380" s="15"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12329,7 +12329,7 @@
       <c r="J381" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M381" s="13"/>
+      <c r="M381" s="15"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12356,7 +12356,7 @@
       <c r="J382" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M382" s="13"/>
+      <c r="M382" s="15"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12381,7 +12381,7 @@
       <c r="J383" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M383" s="13"/>
+      <c r="M383" s="15"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12406,7 +12406,7 @@
       <c r="J384" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M384" s="13"/>
+      <c r="M384" s="15"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12431,7 +12431,7 @@
       <c r="J385" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M385" s="13"/>
+      <c r="M385" s="15"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12456,7 +12456,7 @@
       <c r="J386" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M386" s="13"/>
+      <c r="M386" s="15"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12537,7 +12537,7 @@
       <c r="K389" t="s">
         <v>221</v>
       </c>
-      <c r="M389" s="13">
+      <c r="M389" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -12569,7 +12569,7 @@
       <c r="K390" t="s">
         <v>221</v>
       </c>
-      <c r="M390" s="13"/>
+      <c r="M390" s="15"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12599,7 +12599,7 @@
       <c r="K391" t="s">
         <v>221</v>
       </c>
-      <c r="M391" s="13"/>
+      <c r="M391" s="15"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12629,7 +12629,7 @@
       <c r="K392" t="s">
         <v>221</v>
       </c>
-      <c r="M392" s="13"/>
+      <c r="M392" s="15"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12659,7 +12659,7 @@
       <c r="K393" t="s">
         <v>221</v>
       </c>
-      <c r="M393" s="13"/>
+      <c r="M393" s="15"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12689,7 +12689,7 @@
       <c r="K394" t="s">
         <v>221</v>
       </c>
-      <c r="M394" s="13"/>
+      <c r="M394" s="15"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12716,7 +12716,7 @@
       <c r="J395" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M395" s="13"/>
+      <c r="M395" s="15"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12746,7 +12746,7 @@
       <c r="J396" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M396" s="13">
+      <c r="M396" s="15">
         <v>1</v>
       </c>
     </row>
@@ -12775,7 +12775,7 @@
       <c r="J397" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M397" s="13"/>
+      <c r="M397" s="15"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12802,7 +12802,7 @@
       <c r="J398" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M398" s="13"/>
+      <c r="M398" s="15"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12832,7 +12832,7 @@
       <c r="K399" t="s">
         <v>224</v>
       </c>
-      <c r="M399" s="13"/>
+      <c r="M399" s="15"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12859,7 +12859,7 @@
       <c r="J400" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M400" s="13"/>
+      <c r="M400" s="15"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12886,7 +12886,7 @@
       <c r="J401" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M401" s="13"/>
+      <c r="M401" s="15"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12913,7 +12913,7 @@
       <c r="J402" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M402" s="13"/>
+      <c r="M402" s="15"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12940,7 +12940,7 @@
       <c r="J403" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M403" s="13"/>
+      <c r="M403" s="15"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12970,7 +12970,7 @@
       <c r="K404" t="s">
         <v>224</v>
       </c>
-      <c r="M404" s="13"/>
+      <c r="M404" s="15"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -12997,7 +12997,7 @@
       <c r="J405" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M405" s="13"/>
+      <c r="M405" s="15"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -13024,7 +13024,7 @@
       <c r="J406" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M406" s="13"/>
+      <c r="M406" s="15"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -13051,7 +13051,7 @@
       <c r="J407" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M407" s="13"/>
+      <c r="M407" s="15"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -13080,7 +13080,7 @@
       <c r="J408" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M408" s="13"/>
+      <c r="M408" s="15"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -13107,7 +13107,7 @@
       <c r="J409" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M409" s="13"/>
+      <c r="M409" s="15"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -13136,7 +13136,7 @@
       <c r="J410" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M410" s="13"/>
+      <c r="M410" s="15"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -13163,7 +13163,7 @@
       <c r="J411" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M411" s="13"/>
+      <c r="M411" s="15"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -13190,7 +13190,7 @@
       <c r="J412" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M412" s="13"/>
+      <c r="M412" s="15"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13217,7 +13217,7 @@
       <c r="J413" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M413" s="13"/>
+      <c r="M413" s="15"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13244,7 +13244,7 @@
       <c r="J414" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M414" s="13"/>
+      <c r="M414" s="15"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13274,7 +13274,7 @@
       <c r="J415" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M415" s="13">
+      <c r="M415" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -13306,7 +13306,7 @@
       <c r="K416" t="s">
         <v>227</v>
       </c>
-      <c r="M416" s="13"/>
+      <c r="M416" s="15"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13338,7 +13338,7 @@
       <c r="K417" t="s">
         <v>227</v>
       </c>
-      <c r="M417" s="13"/>
+      <c r="M417" s="15"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13370,7 +13370,7 @@
       <c r="K418" t="s">
         <v>227</v>
       </c>
-      <c r="M418" s="13"/>
+      <c r="M418" s="15"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13399,7 +13399,7 @@
       <c r="J419" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M419" s="13"/>
+      <c r="M419" s="15"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13428,7 +13428,7 @@
       <c r="J420" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M420" s="13"/>
+      <c r="M420" s="15"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13458,7 +13458,7 @@
       <c r="J421" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M421" s="13">
+      <c r="M421" s="15">
         <v>1</v>
       </c>
     </row>
@@ -13487,7 +13487,7 @@
       <c r="J422" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M422" s="13"/>
+      <c r="M422" s="15"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13514,7 +13514,7 @@
       <c r="J423" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M423" s="13"/>
+      <c r="M423" s="15"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13544,7 +13544,7 @@
       <c r="K424" t="s">
         <v>224</v>
       </c>
-      <c r="M424" s="13"/>
+      <c r="M424" s="15"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13571,7 +13571,7 @@
       <c r="J425" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M425" s="13"/>
+      <c r="M425" s="15"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13598,7 +13598,7 @@
       <c r="J426" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M426" s="13"/>
+      <c r="M426" s="15"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13625,7 +13625,7 @@
       <c r="J427" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M427" s="13"/>
+      <c r="M427" s="15"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13652,7 +13652,7 @@
       <c r="J428" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M428" s="13"/>
+      <c r="M428" s="15"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13682,7 +13682,7 @@
       <c r="K429" t="s">
         <v>224</v>
       </c>
-      <c r="M429" s="13"/>
+      <c r="M429" s="15"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13709,7 +13709,7 @@
       <c r="J430" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M430" s="13"/>
+      <c r="M430" s="15"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13736,7 +13736,7 @@
       <c r="J431" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M431" s="13"/>
+      <c r="M431" s="15"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13763,7 +13763,7 @@
       <c r="J432" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M432" s="13"/>
+      <c r="M432" s="15"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13792,7 +13792,7 @@
       <c r="J433" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M433" s="13"/>
+      <c r="M433" s="15"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13819,7 +13819,7 @@
       <c r="J434" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M434" s="13"/>
+      <c r="M434" s="15"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13848,7 +13848,7 @@
       <c r="J435" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M435" s="13"/>
+      <c r="M435" s="15"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13875,7 +13875,7 @@
       <c r="J436" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M436" s="13"/>
+      <c r="M436" s="15"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13902,7 +13902,7 @@
       <c r="J437" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M437" s="13"/>
+      <c r="M437" s="15"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13929,7 +13929,7 @@
       <c r="J438" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M438" s="13"/>
+      <c r="M438" s="15"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13956,7 +13956,7 @@
       <c r="J439" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M439" s="13"/>
+      <c r="M439" s="15"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13990,7 +13990,7 @@
       <c r="J440" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M440" s="13">
+      <c r="M440" s="15">
         <v>1</v>
       </c>
     </row>
@@ -14023,7 +14023,7 @@
       <c r="J441" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M441" s="13"/>
+      <c r="M441" s="15"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -14054,7 +14054,7 @@
       <c r="J442" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M442" s="13"/>
+      <c r="M442" s="15"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -14085,7 +14085,7 @@
       <c r="J443" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M443" s="13"/>
+      <c r="M443" s="15"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -14116,7 +14116,7 @@
       <c r="J444" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M444" s="13"/>
+      <c r="M444" s="15"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -14147,7 +14147,7 @@
       <c r="J445" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M445" s="13"/>
+      <c r="M445" s="15"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -14178,7 +14178,7 @@
       <c r="J446" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M446" s="13"/>
+      <c r="M446" s="15"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -14209,7 +14209,7 @@
       <c r="J447" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M447" s="13"/>
+      <c r="M447" s="15"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14240,7 +14240,7 @@
       <c r="J448" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M448" s="13"/>
+      <c r="M448" s="15"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14271,7 +14271,7 @@
       <c r="J449" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M449" s="13"/>
+      <c r="M449" s="15"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14300,7 +14300,7 @@
       <c r="J450" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M450" s="13"/>
+      <c r="M450" s="15"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14329,7 +14329,7 @@
       <c r="J451" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M451" s="13"/>
+      <c r="M451" s="15"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14358,7 +14358,7 @@
       <c r="J452" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M452" s="13"/>
+      <c r="M452" s="15"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14387,7 +14387,7 @@
       <c r="J453" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M453" s="13"/>
+      <c r="M453" s="15"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14416,7 +14416,7 @@
       <c r="J454" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M454" s="13"/>
+      <c r="M454" s="15"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14443,7 +14443,7 @@
       <c r="J455" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M455" s="13"/>
+      <c r="M455" s="15"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14464,13 +14464,13 @@
       <c r="F456" s="1"/>
       <c r="G456" s="1"/>
       <c r="H456" s="1"/>
-      <c r="I456" s="16" t="s">
+      <c r="I456" s="12" t="s">
         <v>210</v>
       </c>
       <c r="J456" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M456" s="13"/>
+      <c r="M456" s="15"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14500,7 +14500,7 @@
       <c r="K457" t="s">
         <v>227</v>
       </c>
-      <c r="M457" s="13"/>
+      <c r="M457" s="15"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14532,7 +14532,7 @@
       <c r="K458" t="s">
         <v>227</v>
       </c>
-      <c r="M458" s="13"/>
+      <c r="M458" s="15"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14564,7 +14564,7 @@
       <c r="K459" t="s">
         <v>227</v>
       </c>
-      <c r="M459" s="13"/>
+      <c r="M459" s="15"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14593,7 +14593,7 @@
       <c r="J460" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M460" s="13"/>
+      <c r="M460" s="15"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14622,7 +14622,7 @@
       <c r="J461" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M461" s="13"/>
+      <c r="M461" s="15"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14951,12 +14951,12 @@
       <c r="G474" s="1"/>
       <c r="H474" s="1"/>
       <c r="I474" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J474" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M474" s="12">
+        <v>210</v>
+      </c>
+      <c r="M474" s="16">
         <v>1</v>
       </c>
     </row>
@@ -14980,12 +14980,12 @@
       <c r="G475" s="1"/>
       <c r="H475" s="1"/>
       <c r="I475" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J475" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M475" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M475" s="16"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -15007,12 +15007,12 @@
       <c r="G476" s="1"/>
       <c r="H476" s="1"/>
       <c r="I476" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J476" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M476" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M476" s="16"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -15034,12 +15034,15 @@
       <c r="G477" s="1"/>
       <c r="H477" s="1"/>
       <c r="I477" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J477" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M477" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="K477" t="s">
+        <v>224</v>
+      </c>
+      <c r="M477" s="16"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -15061,12 +15064,12 @@
       <c r="G478" s="1"/>
       <c r="H478" s="1"/>
       <c r="I478" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J478" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M478" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M478" s="16"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -15088,12 +15091,12 @@
       <c r="G479" s="1"/>
       <c r="H479" s="1"/>
       <c r="I479" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J479" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M479" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M479" s="16"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -15115,12 +15118,12 @@
       <c r="G480" s="1"/>
       <c r="H480" s="1"/>
       <c r="I480" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J480" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M480" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M480" s="16"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15142,12 +15145,12 @@
       <c r="G481" s="1"/>
       <c r="H481" s="1"/>
       <c r="I481" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J481" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M481" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M481" s="16"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15169,12 +15172,15 @@
       <c r="G482" s="1"/>
       <c r="H482" s="1"/>
       <c r="I482" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J482" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M482" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="K482" t="s">
+        <v>224</v>
+      </c>
+      <c r="M482" s="16"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15196,12 +15202,12 @@
       <c r="G483" s="1"/>
       <c r="H483" s="1"/>
       <c r="I483" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M483" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M483" s="16"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15223,10 +15229,10 @@
       <c r="G484" s="1"/>
       <c r="H484" s="1"/>
       <c r="I484" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M484" s="1"/>
     </row>
@@ -15250,10 +15256,10 @@
       <c r="G485" s="1"/>
       <c r="H485" s="1"/>
       <c r="I485" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M485" s="1"/>
     </row>
@@ -15277,10 +15283,10 @@
       <c r="G486" s="1"/>
       <c r="H486" s="1"/>
       <c r="I486" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M486" s="1"/>
     </row>
@@ -15304,10 +15310,13 @@
       <c r="G487" s="1"/>
       <c r="H487" s="1"/>
       <c r="I487" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="K487" t="s">
+        <v>224</v>
       </c>
       <c r="M487" s="1"/>
     </row>
@@ -15331,10 +15340,10 @@
       <c r="G488" s="1"/>
       <c r="H488" s="1"/>
       <c r="I488" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M488" s="1"/>
     </row>
@@ -15356,12 +15365,12 @@
       <c r="G489" s="1"/>
       <c r="H489" s="1"/>
       <c r="I489" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M489" s="12">
+        <v>210</v>
+      </c>
+      <c r="M489" s="16">
         <v>2</v>
       </c>
     </row>
@@ -15383,12 +15392,12 @@
       <c r="G490" s="1"/>
       <c r="H490" s="1"/>
       <c r="I490" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M490" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M490" s="16"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15408,12 +15417,12 @@
       <c r="G491" s="1"/>
       <c r="H491" s="1"/>
       <c r="I491" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M491" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M491" s="16"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15433,12 +15442,15 @@
       <c r="G492" s="1"/>
       <c r="H492" s="1"/>
       <c r="I492" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M492" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="K492" t="s">
+        <v>224</v>
+      </c>
+      <c r="M492" s="16"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15458,12 +15470,12 @@
       <c r="G493" s="1"/>
       <c r="H493" s="1"/>
       <c r="I493" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M493" s="12"/>
+        <v>210</v>
+      </c>
+      <c r="M493" s="16"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15490,7 +15502,7 @@
       <c r="J494" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M494" s="12"/>
+      <c r="M494" s="16"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15517,7 +15529,7 @@
       <c r="J495" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M495" s="12"/>
+      <c r="M495" s="16"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15544,7 +15556,7 @@
       <c r="J496" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M496" s="12"/>
+      <c r="M496" s="16"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15571,7 +15583,7 @@
       <c r="J497" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M497" s="12"/>
+      <c r="M497" s="16"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15624,7 +15636,7 @@
       <c r="J499" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M499" s="12">
+      <c r="M499" s="16">
         <v>1</v>
       </c>
     </row>
@@ -15651,7 +15663,7 @@
       <c r="J500" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M500" s="12"/>
+      <c r="M500" s="16"/>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15676,7 +15688,7 @@
       <c r="J501" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M501" s="12"/>
+      <c r="M501" s="16"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15701,7 +15713,7 @@
       <c r="J502" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M502" s="12"/>
+      <c r="M502" s="16"/>
     </row>
     <row r="503" spans="1:14" ht="15" customHeight="1">
       <c r="A503" s="1" t="s">
@@ -15726,7 +15738,7 @@
       <c r="J503" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M503" s="12"/>
+      <c r="M503" s="16"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15751,7 +15763,7 @@
       <c r="J504" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M504" s="12"/>
+      <c r="M504" s="16"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15778,7 +15790,7 @@
       <c r="J505" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M505" s="12"/>
+      <c r="M505" s="16"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15803,7 +15815,7 @@
       <c r="J506" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M506" s="12"/>
+      <c r="M506" s="16"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15830,7 +15842,7 @@
       <c r="J507" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M507" s="12"/>
+      <c r="M507" s="16"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15855,7 +15867,7 @@
       <c r="J508" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M508" s="12"/>
+      <c r="M508" s="16"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15880,7 +15892,7 @@
       <c r="J509" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M509" s="12"/>
+      <c r="M509" s="16"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15905,7 +15917,7 @@
       <c r="J510" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M510" s="12"/>
+      <c r="M510" s="16"/>
     </row>
     <row r="511" spans="1:14">
       <c r="A511" s="1" t="s">
@@ -15930,7 +15942,7 @@
       <c r="J511" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M511" s="12"/>
+      <c r="M511" s="16"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15957,7 +15969,7 @@
       <c r="J512" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M512" s="12"/>
+      <c r="M512" s="16"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15984,7 +15996,7 @@
       <c r="J513" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M513" s="12"/>
+      <c r="M513" s="16"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -16009,7 +16021,7 @@
       <c r="J514" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M514" s="12"/>
+      <c r="M514" s="16"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -16034,7 +16046,7 @@
       <c r="J515" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M515" s="12"/>
+      <c r="M515" s="16"/>
       <c r="N515">
         <v>1</v>
       </c>
@@ -16062,7 +16074,7 @@
       <c r="J516" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M516" s="12">
+      <c r="M516" s="16">
         <v>2</v>
       </c>
     </row>
@@ -16091,7 +16103,7 @@
       <c r="J517" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M517" s="12"/>
+      <c r="M517" s="16"/>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -16118,7 +16130,7 @@
       <c r="J518" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M518" s="12"/>
+      <c r="M518" s="16"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -16145,7 +16157,7 @@
       <c r="J519" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M519" s="12"/>
+      <c r="M519" s="16"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16174,7 +16186,7 @@
       <c r="J520" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M520" s="12"/>
+      <c r="M520" s="16"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16203,7 +16215,7 @@
       <c r="J521" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M521" s="12"/>
+      <c r="M521" s="16"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16232,7 +16244,7 @@
       <c r="J522" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M522" s="12"/>
+      <c r="M522" s="16"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16261,7 +16273,7 @@
       <c r="J523" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M523" s="12"/>
+      <c r="M523" s="16"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16290,7 +16302,7 @@
       <c r="J524" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M524" s="12"/>
+      <c r="M524" s="16"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16319,7 +16331,7 @@
       <c r="J525" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M525" s="12"/>
+      <c r="M525" s="16"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16346,7 +16358,7 @@
       <c r="J526" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="12"/>
+      <c r="M526" s="16"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="2" t="s">
@@ -16373,7 +16385,7 @@
       <c r="J527" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="12"/>
+      <c r="M527" s="16"/>
     </row>
     <row r="528" spans="1:14">
       <c r="M528">
@@ -16398,11 +16410,6 @@
   </sheetData>
   <autoFilter ref="I1:J527"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M516:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -16419,6 +16426,11 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart -> Data Series -> Area. Added feature: Chart -> Data Series -> Transparency. Added feature: Chart -> Data Series -> Characters. Added feature: Chart -> Data Series -> Font Effects. Added feature: Chart -> Data Series -> Data Labels.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$527</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$553</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4069" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4282" uniqueCount="230">
   <si>
     <t>Chart</t>
   </si>
@@ -707,6 +707,12 @@
   </si>
   <si>
     <t>Known issues: [ 1777562 ] Axis label order and text flow</t>
+  </si>
+  <si>
+    <t>Known Issues: [ 1779234 ] Chart point width and height</t>
+  </si>
+  <si>
+    <t>not: "From file..." and "Gallery"</t>
   </si>
 </sst>
 </file>
@@ -859,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -885,17 +891,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,12 +1225,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N530"/>
+  <dimension ref="A1:N555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I493" sqref="I493"/>
+      <selection pane="bottomLeft" activeCell="D542" sqref="D542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1241,16 +1250,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -14956,7 +14965,7 @@
       <c r="J474" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M474" s="16">
+      <c r="M474" s="14">
         <v>1</v>
       </c>
     </row>
@@ -14985,7 +14994,7 @@
       <c r="J475" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M475" s="16"/>
+      <c r="M475" s="14"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -15012,7 +15021,7 @@
       <c r="J476" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M476" s="16"/>
+      <c r="M476" s="14"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -15042,7 +15051,7 @@
       <c r="K477" t="s">
         <v>224</v>
       </c>
-      <c r="M477" s="16"/>
+      <c r="M477" s="14"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -15069,7 +15078,7 @@
       <c r="J478" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M478" s="16"/>
+      <c r="M478" s="14"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -15096,7 +15105,7 @@
       <c r="J479" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M479" s="16"/>
+      <c r="M479" s="14"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -15123,7 +15132,7 @@
       <c r="J480" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M480" s="16"/>
+      <c r="M480" s="14"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15150,7 +15159,7 @@
       <c r="J481" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M481" s="16"/>
+      <c r="M481" s="14"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15180,7 +15189,7 @@
       <c r="K482" t="s">
         <v>224</v>
       </c>
-      <c r="M482" s="16"/>
+      <c r="M482" s="14"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15207,7 +15216,7 @@
       <c r="J483" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M483" s="16"/>
+      <c r="M483" s="14"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15370,7 +15379,7 @@
       <c r="J489" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M489" s="16">
+      <c r="M489" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15397,7 +15406,7 @@
       <c r="J490" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M490" s="16"/>
+      <c r="M490" s="14"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15422,7 +15431,7 @@
       <c r="J491" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M491" s="16"/>
+      <c r="M491" s="14"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15450,7 +15459,7 @@
       <c r="K492" t="s">
         <v>224</v>
       </c>
-      <c r="M492" s="16"/>
+      <c r="M492" s="14"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15475,7 +15484,7 @@
       <c r="J493" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M493" s="16"/>
+      <c r="M493" s="14"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15497,12 +15506,15 @@
       <c r="G494" s="1"/>
       <c r="H494" s="1"/>
       <c r="I494" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M494" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="K494" t="s">
+        <v>229</v>
+      </c>
+      <c r="M494" s="14"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15524,12 +15536,15 @@
       <c r="G495" s="1"/>
       <c r="H495" s="1"/>
       <c r="I495" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J495" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M495" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="K495" t="s">
+        <v>228</v>
+      </c>
+      <c r="M495" s="14"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15551,12 +15566,15 @@
       <c r="G496" s="1"/>
       <c r="H496" s="1"/>
       <c r="I496" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M496" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="K496" t="s">
+        <v>228</v>
+      </c>
+      <c r="M496" s="14"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15578,25 +15596,26 @@
       <c r="G497" s="1"/>
       <c r="H497" s="1"/>
       <c r="I497" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M497" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="K497" t="s">
+        <v>228</v>
+      </c>
+      <c r="M497" s="14"/>
       <c r="N497">
         <v>2</v>
       </c>
     </row>
     <row r="498" spans="1:14">
-      <c r="A498" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A498" s="1"/>
       <c r="B498" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C498" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D498" s="6" t="s">
         <v>135</v>
@@ -15606,12 +15625,12 @@
       <c r="G498" s="1"/>
       <c r="H498" s="1"/>
       <c r="I498" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M498" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="M498" s="13"/>
     </row>
     <row r="499" spans="1:14">
       <c r="A499" s="1" t="s">
@@ -15621,24 +15640,24 @@
         <v>178</v>
       </c>
       <c r="C499" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D499" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E499" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E499" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F499" s="1"/>
       <c r="G499" s="1"/>
       <c r="H499" s="1"/>
       <c r="I499" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M499" s="16">
-        <v>1</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="M499" s="1"/>
     </row>
     <row r="500" spans="1:14">
       <c r="A500" s="1" t="s">
@@ -15648,22 +15667,26 @@
         <v>178</v>
       </c>
       <c r="C500" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D500" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E500" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F500" s="1"/>
       <c r="G500" s="1"/>
       <c r="H500" s="1"/>
       <c r="I500" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M500" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M500" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="501" spans="1:14">
       <c r="A501" s="1" t="s">
@@ -15673,22 +15696,26 @@
         <v>178</v>
       </c>
       <c r="C501" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D501" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E501" s="1"/>
-      <c r="F501" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="G501" s="1"/>
       <c r="H501" s="1"/>
       <c r="I501" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M501" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M501" s="14"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15698,24 +15725,28 @@
         <v>178</v>
       </c>
       <c r="C502" s="1" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D502" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E502" s="1"/>
-      <c r="F502" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="G502" s="1"/>
       <c r="H502" s="1"/>
       <c r="I502" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M502" s="16"/>
-    </row>
-    <row r="503" spans="1:14" ht="15" customHeight="1">
+        <v>211</v>
+      </c>
+      <c r="M502" s="14"/>
+    </row>
+    <row r="503" spans="1:14">
       <c r="A503" s="1" t="s">
         <v>0</v>
       </c>
@@ -15723,22 +15754,31 @@
         <v>178</v>
       </c>
       <c r="C503" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D503" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E503" s="1"/>
-      <c r="F503" s="1"/>
-      <c r="G503" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G503" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="H503" s="1"/>
       <c r="I503" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J503" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M503" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="K503" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="M503" s="14"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15748,22 +15788,31 @@
         <v>178</v>
       </c>
       <c r="C504" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D504" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E504" s="1"/>
-      <c r="F504" s="1"/>
-      <c r="G504" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G504" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="H504" s="1"/>
       <c r="I504" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J504" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M504" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="K504" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="M504" s="14"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15773,24 +15822,31 @@
         <v>178</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D505" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="E505" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F505" s="1"/>
-      <c r="G505" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G505" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H505" s="1"/>
       <c r="I505" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J505" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M505" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="K505" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M505" s="14"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15800,22 +15856,31 @@
         <v>178</v>
       </c>
       <c r="C506" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D506" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E506" s="1"/>
-      <c r="F506" s="1"/>
-      <c r="G506" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E506" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G506" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H506" s="1"/>
       <c r="I506" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J506" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M506" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="K506" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="M506" s="14"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15825,24 +15890,26 @@
         <v>178</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D507" s="1" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="E507" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F507" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="G507" s="1"/>
       <c r="H507" s="1"/>
       <c r="I507" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J507" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M507" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M507" s="14"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15852,22 +15919,31 @@
         <v>178</v>
       </c>
       <c r="C508" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D508" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E508" s="1"/>
-      <c r="F508" s="1"/>
-      <c r="G508" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G508" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="H508" s="1"/>
       <c r="I508" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J508" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M508" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="K508" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M508" s="14"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15877,22 +15953,31 @@
         <v>178</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D509" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E509" s="1"/>
-      <c r="F509" s="1"/>
-      <c r="G509" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E509" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G509" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H509" s="1"/>
       <c r="I509" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J509" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M509" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="K509" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M509" s="14"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -15902,24 +15987,33 @@
         <v>178</v>
       </c>
       <c r="C510" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D510" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E510" s="1"/>
-      <c r="F510" s="1"/>
-      <c r="G510" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E510" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G510" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="H510" s="1"/>
       <c r="I510" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J510" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M510" s="16"/>
-    </row>
-    <row r="511" spans="1:14">
+        <v>210</v>
+      </c>
+      <c r="K510" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="M510" s="14"/>
+    </row>
+    <row r="511" spans="1:14" ht="15" customHeight="1">
       <c r="A511" s="1" t="s">
         <v>0</v>
       </c>
@@ -15927,22 +16021,28 @@
         <v>178</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D511" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E511" s="1"/>
-      <c r="F511" s="1"/>
-      <c r="G511" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G511" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="H511" s="1"/>
       <c r="I511" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J511" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M511" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M511" s="14"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -15952,24 +16052,28 @@
         <v>178</v>
       </c>
       <c r="C512" s="1" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="D512" s="1" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="E512" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F512" s="1"/>
-      <c r="G512" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="F512" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G512" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="H512" s="1"/>
       <c r="I512" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J512" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M512" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M512" s="14"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -15979,24 +16083,28 @@
         <v>178</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="D513" s="1" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="E513" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F513" s="1"/>
-      <c r="G513" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G513" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="H513" s="1"/>
       <c r="I513" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J513" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M513" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M513" s="14"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -16006,22 +16114,22 @@
         <v>178</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D514" s="1" t="s">
-        <v>186</v>
+        <v>85</v>
+      </c>
+      <c r="D514" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="E514" s="1"/>
       <c r="F514" s="1"/>
       <c r="G514" s="1"/>
       <c r="H514" s="1"/>
       <c r="I514" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J514" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M514" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M514" s="14"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -16031,25 +16139,22 @@
         <v>178</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>182</v>
+        <v>85</v>
       </c>
       <c r="D515" s="1" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="E515" s="1"/>
       <c r="F515" s="1"/>
       <c r="G515" s="1"/>
       <c r="H515" s="1"/>
       <c r="I515" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J515" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M515" s="16"/>
-      <c r="N515">
-        <v>1</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="M515" s="14"/>
     </row>
     <row r="516" spans="1:14">
       <c r="A516" s="1" t="s">
@@ -16059,23 +16164,26 @@
         <v>178</v>
       </c>
       <c r="C516" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D516" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E516" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="F516" s="1"/>
       <c r="G516" s="1"/>
       <c r="H516" s="1"/>
       <c r="I516" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J516" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M516" s="16">
-        <v>2</v>
+        <v>210</v>
+      </c>
+      <c r="M516" s="14"/>
+      <c r="N516">
+        <v>1</v>
       </c>
     </row>
     <row r="517" spans="1:14">
@@ -16086,24 +16194,26 @@
         <v>178</v>
       </c>
       <c r="C517" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E517" s="1" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="F517" s="1"/>
       <c r="G517" s="1"/>
       <c r="H517" s="1"/>
       <c r="I517" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J517" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M517" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M517" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="518" spans="1:14">
       <c r="A518" s="1" t="s">
@@ -16113,24 +16223,24 @@
         <v>178</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D518" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E518" s="1" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="F518" s="1"/>
       <c r="G518" s="1"/>
       <c r="H518" s="1"/>
       <c r="I518" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J518" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M518" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M518" s="14"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -16140,24 +16250,24 @@
         <v>178</v>
       </c>
       <c r="C519" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D519" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E519" s="1" t="s">
-        <v>194</v>
+        <v>107</v>
       </c>
       <c r="F519" s="1"/>
       <c r="G519" s="1"/>
       <c r="H519" s="1"/>
       <c r="I519" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J519" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M519" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M519" s="14"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16167,26 +16277,24 @@
         <v>178</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D520" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E520" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F520" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F520" s="1"/>
       <c r="G520" s="1"/>
       <c r="H520" s="1"/>
       <c r="I520" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J520" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M520" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M520" s="14"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16196,26 +16304,24 @@
         <v>178</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D521" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E521" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F521" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F521" s="1"/>
       <c r="G521" s="1"/>
       <c r="H521" s="1"/>
       <c r="I521" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J521" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M521" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M521" s="14"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16225,26 +16331,24 @@
         <v>178</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E522" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F522" s="1" t="s">
-        <v>198</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F522" s="1"/>
       <c r="G522" s="1"/>
       <c r="H522" s="1"/>
       <c r="I522" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J522" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M522" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M522" s="14"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16254,26 +16358,24 @@
         <v>178</v>
       </c>
       <c r="C523" s="1" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="E523" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F523" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="F523" s="1"/>
       <c r="G523" s="1"/>
       <c r="H523" s="1"/>
       <c r="I523" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J523" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M523" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="M523" s="14"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16283,26 +16385,22 @@
         <v>178</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D524" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E524" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F524" s="1" t="s">
-        <v>201</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D524" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E524" s="1"/>
+      <c r="F524" s="1"/>
       <c r="G524" s="1"/>
       <c r="H524" s="1"/>
       <c r="I524" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J524" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M524" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M524" s="14"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16312,26 +16410,22 @@
         <v>178</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>188</v>
+        <v>116</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E525" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F525" s="1" t="s">
-        <v>193</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E525" s="1"/>
+      <c r="F525" s="1"/>
       <c r="G525" s="1"/>
       <c r="H525" s="1"/>
       <c r="I525" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J525" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M525" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="M525" s="14"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16341,76 +16435,744 @@
         <v>178</v>
       </c>
       <c r="C526" s="1" t="s">
-        <v>202</v>
+        <v>116</v>
       </c>
       <c r="D526" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E526" s="1" t="s">
-        <v>204</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E526" s="1"/>
       <c r="F526" s="1"/>
       <c r="G526" s="1"/>
       <c r="H526" s="1"/>
       <c r="I526" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J526" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="M526" s="14"/>
+    </row>
+    <row r="527" spans="1:14">
+      <c r="A527" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C527" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D527" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E527" s="1"/>
+      <c r="F527" s="1"/>
+      <c r="G527" s="1"/>
+      <c r="H527" s="1"/>
+      <c r="I527" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J527" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K527" t="s">
+        <v>224</v>
+      </c>
+      <c r="M527" s="14"/>
+    </row>
+    <row r="528" spans="1:14">
+      <c r="A528" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C528" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D528" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E528" s="1"/>
+      <c r="F528" s="1"/>
+      <c r="G528" s="1"/>
+      <c r="H528" s="1"/>
+      <c r="I528" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J528" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="529" spans="1:10">
+      <c r="A529" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C529" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D529" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E529" s="1"/>
+      <c r="F529" s="1"/>
+      <c r="G529" s="1"/>
+      <c r="H529" s="1"/>
+      <c r="I529" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J529" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="530" spans="1:10">
+      <c r="A530" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D530" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E530" s="1"/>
+      <c r="F530" s="1"/>
+      <c r="G530" s="1"/>
+      <c r="H530" s="1"/>
+      <c r="I530" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J530" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="531" spans="1:10">
+      <c r="A531" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E531" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F531" s="1"/>
+      <c r="G531" s="1"/>
+      <c r="H531" s="1"/>
+      <c r="I531" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J531" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="532" spans="1:10">
+      <c r="A532" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E532" s="1"/>
+      <c r="F532" s="1"/>
+      <c r="G532" s="1"/>
+      <c r="H532" s="1"/>
+      <c r="I532" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J532" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="533" spans="1:10">
+      <c r="A533" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E533" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F533" s="1"/>
+      <c r="G533" s="1"/>
+      <c r="H533" s="1"/>
+      <c r="I533" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J533" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="534" spans="1:10">
+      <c r="A534" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D534" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E534" s="1"/>
+      <c r="F534" s="1"/>
+      <c r="G534" s="1"/>
+      <c r="H534" s="1"/>
+      <c r="I534" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J534" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="535" spans="1:10">
+      <c r="A535" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D535" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E535" s="1"/>
+      <c r="F535" s="1"/>
+      <c r="G535" s="1"/>
+      <c r="H535" s="1"/>
+      <c r="I535" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J535" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10">
+      <c r="A536" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E536" s="1"/>
+      <c r="F536" s="1"/>
+      <c r="G536" s="1"/>
+      <c r="H536" s="1"/>
+      <c r="I536" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J536" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="537" spans="1:10">
+      <c r="A537" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D537" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E537" s="1"/>
+      <c r="F537" s="1"/>
+      <c r="G537" s="1"/>
+      <c r="H537" s="1"/>
+      <c r="I537" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J537" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="538" spans="1:10">
+      <c r="A538" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E538" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F538" s="1"/>
+      <c r="G538" s="1"/>
+      <c r="H538" s="1"/>
+      <c r="I538" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J538" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="539" spans="1:10">
+      <c r="A539" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D539" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E539" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F539" s="1"/>
+      <c r="G539" s="1"/>
+      <c r="H539" s="1"/>
+      <c r="I539" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J539" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="540" spans="1:10">
+      <c r="A540" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E540" s="1"/>
+      <c r="F540" s="1"/>
+      <c r="G540" s="1"/>
+      <c r="H540" s="1"/>
+      <c r="I540" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J540" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="541" spans="1:10">
+      <c r="A541" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E541" s="1"/>
+      <c r="F541" s="1"/>
+      <c r="G541" s="1"/>
+      <c r="H541" s="1"/>
+      <c r="I541" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J541" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="J526" s="4" t="s">
+    </row>
+    <row r="542" spans="1:10">
+      <c r="A542" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D542" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E542" s="1"/>
+      <c r="F542" s="1"/>
+      <c r="G542" s="1"/>
+      <c r="H542" s="1"/>
+      <c r="I542" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M526" s="16"/>
-    </row>
-    <row r="527" spans="1:14">
-      <c r="A527" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B527" s="2" t="s">
+      <c r="J542" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="543" spans="1:10">
+      <c r="A543" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B543" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C527" s="2" t="s">
+      <c r="C543" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D543" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E543" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F543" s="1"/>
+      <c r="G543" s="1"/>
+      <c r="H543" s="1"/>
+      <c r="I543" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J543" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="544" spans="1:10">
+      <c r="A544" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D544" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E544" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F544" s="1"/>
+      <c r="G544" s="1"/>
+      <c r="H544" s="1"/>
+      <c r="I544" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J544" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="545" spans="1:14">
+      <c r="A545" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D545" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E545" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F545" s="1"/>
+      <c r="G545" s="1"/>
+      <c r="H545" s="1"/>
+      <c r="I545" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J545" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="546" spans="1:14">
+      <c r="A546" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D546" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E546" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F546" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G546" s="1"/>
+      <c r="H546" s="1"/>
+      <c r="I546" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J546" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="547" spans="1:14">
+      <c r="A547" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D547" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E547" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F547" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G547" s="1"/>
+      <c r="H547" s="1"/>
+      <c r="I547" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J547" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="548" spans="1:14">
+      <c r="A548" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D548" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E548" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F548" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G548" s="1"/>
+      <c r="H548" s="1"/>
+      <c r="I548" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J548" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="549" spans="1:14">
+      <c r="A549" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D549" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E549" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F549" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G549" s="1"/>
+      <c r="H549" s="1"/>
+      <c r="I549" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J549" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="550" spans="1:14">
+      <c r="A550" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D550" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E550" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F550" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G550" s="1"/>
+      <c r="H550" s="1"/>
+      <c r="I550" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J550" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="551" spans="1:14">
+      <c r="A551" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D551" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E551" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F551" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G551" s="1"/>
+      <c r="H551" s="1"/>
+      <c r="I551" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J551" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="552" spans="1:14">
+      <c r="A552" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C552" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D527" s="2" t="s">
+      <c r="D552" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E527" s="2" t="s">
+      <c r="E552" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F552" s="1"/>
+      <c r="G552" s="1"/>
+      <c r="H552" s="1"/>
+      <c r="I552" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J552" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="553" spans="1:14">
+      <c r="A553" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C553" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D553" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E553" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F527" s="2"/>
-      <c r="G527" s="2"/>
-      <c r="H527" s="2"/>
-      <c r="I527" s="5" t="s">
+      <c r="F553" s="2"/>
+      <c r="G553" s="2"/>
+      <c r="H553" s="2"/>
+      <c r="I553" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="J527" s="5" t="s">
+      <c r="J553" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M527" s="16"/>
-    </row>
-    <row r="528" spans="1:14">
-      <c r="M528">
+      <c r="M553">
         <f>SUM(M2:M527)</f>
         <v>25.5</v>
       </c>
-      <c r="N528">
+      <c r="N553">
         <f>SUM(N1:N527)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="529" spans="14:14">
-      <c r="N529">
+    <row r="554" spans="1:14">
+      <c r="N554">
         <v>3</v>
       </c>
     </row>
-    <row r="530" spans="14:14">
-      <c r="N530" s="8">
+    <row r="555" spans="1:14">
+      <c r="N555" s="8">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:J527"/>
+  <autoFilter ref="I1:J553"/>
   <mergeCells count="21">
-    <mergeCell ref="M516:M527"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
+    <mergeCell ref="M517:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
     <mergeCell ref="M165:M188"/>
@@ -16418,7 +17180,7 @@
     <mergeCell ref="M342:M386"/>
     <mergeCell ref="M396:M414"/>
     <mergeCell ref="M474:M483"/>
-    <mergeCell ref="M499:M515"/>
+    <mergeCell ref="M500:M516"/>
     <mergeCell ref="M489:M497"/>
     <mergeCell ref="M415:M420"/>
     <mergeCell ref="M421:M439"/>
@@ -16426,11 +17188,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Added feature: Chart -> Data Series -> Statistics
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -1227,10 +1227,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N555"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D542" sqref="D542"/>
+      <selection pane="bottomLeft" activeCell="I551" sqref="I551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16821,7 +16821,7 @@
         <v>210</v>
       </c>
       <c r="J541" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="542" spans="1:10">
@@ -16842,10 +16842,10 @@
       <c r="G542" s="1"/>
       <c r="H542" s="1"/>
       <c r="I542" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J542" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="543" spans="1:10">
@@ -16868,10 +16868,10 @@
       <c r="G543" s="1"/>
       <c r="H543" s="1"/>
       <c r="I543" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J543" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="544" spans="1:10">
@@ -16894,10 +16894,10 @@
       <c r="G544" s="1"/>
       <c r="H544" s="1"/>
       <c r="I544" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J544" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="545" spans="1:14">
@@ -16920,10 +16920,10 @@
       <c r="G545" s="1"/>
       <c r="H545" s="1"/>
       <c r="I545" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J545" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="546" spans="1:14">
@@ -16948,10 +16948,10 @@
       <c r="G546" s="1"/>
       <c r="H546" s="1"/>
       <c r="I546" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J546" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="547" spans="1:14">
@@ -16976,10 +16976,10 @@
       <c r="G547" s="1"/>
       <c r="H547" s="1"/>
       <c r="I547" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J547" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="548" spans="1:14">
@@ -17004,10 +17004,10 @@
       <c r="G548" s="1"/>
       <c r="H548" s="1"/>
       <c r="I548" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J548" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="549" spans="1:14">
@@ -17032,10 +17032,10 @@
       <c r="G549" s="1"/>
       <c r="H549" s="1"/>
       <c r="I549" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J549" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="550" spans="1:14">
@@ -17060,10 +17060,10 @@
       <c r="G550" s="1"/>
       <c r="H550" s="1"/>
       <c r="I550" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J550" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="551" spans="1:14">

</xml_diff>

<commit_message>
Added Chart->Data Series->Statistics->Error category->Regression curves
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/Chart Features List.xlsx
+++ b/docs/Developer documentation/Chart Features List.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$553</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$554</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4282" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="232">
   <si>
     <t>Chart</t>
   </si>
@@ -713,6 +713,12 @@
   </si>
   <si>
     <t>not: "From file..." and "Gallery"</t>
+  </si>
+  <si>
+    <t>Regression curves</t>
+  </si>
+  <si>
+    <t>Available only on scatter charts</t>
   </si>
 </sst>
 </file>
@@ -894,17 +900,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,12 +1231,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N555"/>
+  <dimension ref="A1:N556"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A512" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
+      <selection pane="bottomLeft" activeCell="A552" sqref="A552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1250,16 +1256,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="3" t="s">
         <v>207</v>
       </c>
@@ -1300,7 +1306,7 @@
       <c r="K2" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1330,7 +1336,7 @@
       <c r="K3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1355,7 +1361,7 @@
       <c r="J4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1380,7 +1386,7 @@
       <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1405,7 +1411,7 @@
       <c r="J6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M6" s="16"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
@@ -1430,7 +1436,7 @@
       <c r="J7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M7" s="16"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
@@ -1455,7 +1461,7 @@
       <c r="J8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
@@ -1480,7 +1486,7 @@
       <c r="J9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="16"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
@@ -1505,7 +1511,7 @@
       <c r="J10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M10" s="16"/>
+      <c r="M10" s="15"/>
       <c r="N10">
         <v>1</v>
       </c>
@@ -2126,7 +2132,7 @@
       <c r="K33" t="s">
         <v>214</v>
       </c>
-      <c r="M33" s="16">
+      <c r="M33" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2158,7 +2164,7 @@
       <c r="K34" t="s">
         <v>214</v>
       </c>
-      <c r="M34" s="16"/>
+      <c r="M34" s="15"/>
       <c r="N34">
         <v>1</v>
       </c>
@@ -2423,7 +2429,7 @@
       <c r="K43" t="s">
         <v>214</v>
       </c>
-      <c r="M43" s="16">
+      <c r="M43" s="15">
         <v>2</v>
       </c>
     </row>
@@ -2455,7 +2461,7 @@
       <c r="K44" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="16"/>
+      <c r="M44" s="15"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
@@ -2487,7 +2493,7 @@
       <c r="K45" t="s">
         <v>214</v>
       </c>
-      <c r="M45" s="16"/>
+      <c r="M45" s="15"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
@@ -2519,7 +2525,7 @@
       <c r="K46" t="s">
         <v>214</v>
       </c>
-      <c r="M46" s="16"/>
+      <c r="M46" s="15"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
@@ -2551,7 +2557,7 @@
       <c r="K47" t="s">
         <v>214</v>
       </c>
-      <c r="M47" s="16"/>
+      <c r="M47" s="15"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
@@ -2583,7 +2589,7 @@
       <c r="K48" t="s">
         <v>214</v>
       </c>
-      <c r="M48" s="16"/>
+      <c r="M48" s="15"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
@@ -2615,7 +2621,7 @@
       <c r="K49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" s="16"/>
+      <c r="M49" s="15"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
@@ -2647,7 +2653,7 @@
       <c r="K50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" s="16"/>
+      <c r="M50" s="15"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
@@ -2836,7 +2842,7 @@
       <c r="J57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="16">
+      <c r="M57" s="15">
         <v>3</v>
       </c>
     </row>
@@ -2865,7 +2871,7 @@
       <c r="J58" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M58" s="16"/>
+      <c r="M58" s="15"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
@@ -2892,7 +2898,7 @@
       <c r="J59" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="16"/>
+      <c r="M59" s="15"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
@@ -2919,7 +2925,7 @@
       <c r="J60" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M60" s="16"/>
+      <c r="M60" s="15"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
@@ -4017,7 +4023,7 @@
       <c r="J98" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M98" s="16">
+      <c r="M98" s="15">
         <v>2</v>
       </c>
     </row>
@@ -4044,7 +4050,7 @@
       <c r="J99" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M99" s="16"/>
+      <c r="M99" s="15"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100" s="1" t="s">
@@ -4072,7 +4078,7 @@
       <c r="K100" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="M100" s="16"/>
+      <c r="M100" s="15"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
@@ -4097,7 +4103,7 @@
       <c r="J101" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M101" s="16"/>
+      <c r="M101" s="15"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
@@ -4124,7 +4130,7 @@
       <c r="J102" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M102" s="16"/>
+      <c r="M102" s="15"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
@@ -4151,7 +4157,7 @@
       <c r="J103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M103" s="16"/>
+      <c r="M103" s="15"/>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
@@ -4180,7 +4186,7 @@
       <c r="J104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M104" s="16"/>
+      <c r="M104" s="15"/>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
@@ -4209,7 +4215,7 @@
       <c r="J105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M105" s="16"/>
+      <c r="M105" s="15"/>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
@@ -4243,7 +4249,7 @@
       <c r="K106" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M106" s="16"/>
+      <c r="M106" s="15"/>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
@@ -4277,7 +4283,7 @@
       <c r="K107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M107" s="16"/>
+      <c r="M107" s="15"/>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
@@ -4311,7 +4317,7 @@
       <c r="K108" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M108" s="16"/>
+      <c r="M108" s="15"/>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
@@ -4345,7 +4351,7 @@
       <c r="K109" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="16"/>
+      <c r="M109" s="15"/>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
@@ -4374,7 +4380,7 @@
       <c r="J110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M110" s="16"/>
+      <c r="M110" s="15"/>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
@@ -4408,7 +4414,7 @@
       <c r="K111" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M111" s="16"/>
+      <c r="M111" s="15"/>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
@@ -4442,7 +4448,7 @@
       <c r="K112" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M112" s="16"/>
+      <c r="M112" s="15"/>
     </row>
     <row r="113" spans="1:14" ht="30">
       <c r="A113" s="1" t="s">
@@ -4476,7 +4482,7 @@
       <c r="K113" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M113" s="16"/>
+      <c r="M113" s="15"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="1" t="s">
@@ -4507,7 +4513,7 @@
       <c r="J114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M114" s="16"/>
+      <c r="M114" s="15"/>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
@@ -4538,7 +4544,7 @@
       <c r="J115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M115" s="16"/>
+      <c r="M115" s="15"/>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
@@ -4569,7 +4575,7 @@
       <c r="J116" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M116" s="16"/>
+      <c r="M116" s="15"/>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
@@ -4594,7 +4600,7 @@
       <c r="J117" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M117" s="16"/>
+      <c r="M117" s="15"/>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
@@ -4621,7 +4627,7 @@
       <c r="J118" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M118" s="16"/>
+      <c r="M118" s="15"/>
       <c r="N118">
         <v>2</v>
       </c>
@@ -4855,7 +4861,7 @@
       <c r="J127" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M127" s="16">
+      <c r="M127" s="15">
         <v>1</v>
       </c>
     </row>
@@ -4882,7 +4888,7 @@
       <c r="J128" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M128" s="16"/>
+      <c r="M128" s="15"/>
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
@@ -4910,7 +4916,7 @@
       <c r="K129" t="s">
         <v>224</v>
       </c>
-      <c r="M129" s="16"/>
+      <c r="M129" s="15"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
@@ -4935,7 +4941,7 @@
       <c r="J130" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M130" s="16"/>
+      <c r="M130" s="15"/>
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
@@ -4960,7 +4966,7 @@
       <c r="J131" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M131" s="16"/>
+      <c r="M131" s="15"/>
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
@@ -4987,7 +4993,7 @@
       <c r="J132" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M132" s="16"/>
+      <c r="M132" s="15"/>
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
@@ -5014,7 +5020,7 @@
       <c r="J133" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M133" s="16"/>
+      <c r="M133" s="15"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
@@ -5043,7 +5049,7 @@
       <c r="J134" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M134" s="16"/>
+      <c r="M134" s="15"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1">
       <c r="A135" s="1" t="s">
@@ -5072,7 +5078,7 @@
       <c r="J135" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M135" s="16"/>
+      <c r="M135" s="15"/>
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
@@ -5106,7 +5112,7 @@
       <c r="K136" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M136" s="16"/>
+      <c r="M136" s="15"/>
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
@@ -5140,7 +5146,7 @@
       <c r="K137" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M137" s="16"/>
+      <c r="M137" s="15"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
@@ -5174,7 +5180,7 @@
       <c r="K138" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M138" s="16"/>
+      <c r="M138" s="15"/>
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
@@ -5208,7 +5214,7 @@
       <c r="K139" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M139" s="16"/>
+      <c r="M139" s="15"/>
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
@@ -5237,7 +5243,7 @@
       <c r="J140" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M140" s="16"/>
+      <c r="M140" s="15"/>
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
@@ -5271,7 +5277,7 @@
       <c r="K141" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M141" s="16"/>
+      <c r="M141" s="15"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
@@ -5305,7 +5311,7 @@
       <c r="K142" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M142" s="16"/>
+      <c r="M142" s="15"/>
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
@@ -5337,7 +5343,7 @@
         <v>210</v>
       </c>
       <c r="K143" s="10"/>
-      <c r="M143" s="16"/>
+      <c r="M143" s="15"/>
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
@@ -5368,7 +5374,7 @@
       <c r="J144" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M144" s="16"/>
+      <c r="M144" s="15"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
@@ -5399,7 +5405,7 @@
       <c r="J145" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M145" s="16"/>
+      <c r="M145" s="15"/>
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
@@ -5430,7 +5436,7 @@
       <c r="J146" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M146" s="16"/>
+      <c r="M146" s="15"/>
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
@@ -5455,7 +5461,7 @@
       <c r="J147" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M147" s="16"/>
+      <c r="M147" s="15"/>
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
@@ -5480,7 +5486,7 @@
       <c r="J148" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M148" s="16"/>
+      <c r="M148" s="15"/>
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
@@ -5507,7 +5513,7 @@
       <c r="J149" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M149" s="16"/>
+      <c r="M149" s="15"/>
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
@@ -5534,7 +5540,7 @@
       <c r="J150" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M150" s="16"/>
+      <c r="M150" s="15"/>
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
@@ -5561,7 +5567,7 @@
       <c r="J151" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="16"/>
+      <c r="M151" s="15"/>
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
@@ -5588,7 +5594,7 @@
       <c r="J152" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M152" s="16"/>
+      <c r="M152" s="15"/>
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
@@ -5615,7 +5621,7 @@
       <c r="J153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M153" s="16"/>
+      <c r="M153" s="15"/>
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
@@ -5642,7 +5648,7 @@
       <c r="J154" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M154" s="16"/>
+      <c r="M154" s="15"/>
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
@@ -5669,7 +5675,7 @@
       <c r="J155" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M155" s="16"/>
+      <c r="M155" s="15"/>
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
@@ -5696,7 +5702,7 @@
       <c r="J156" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M156" s="16"/>
+      <c r="M156" s="15"/>
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
@@ -5724,7 +5730,7 @@
       <c r="K157" t="s">
         <v>220</v>
       </c>
-      <c r="M157" s="16"/>
+      <c r="M157" s="15"/>
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
@@ -5754,7 +5760,7 @@
       <c r="K158" t="s">
         <v>221</v>
       </c>
-      <c r="M158" s="16"/>
+      <c r="M158" s="15"/>
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
@@ -5784,7 +5790,7 @@
       <c r="K159" t="s">
         <v>221</v>
       </c>
-      <c r="M159" s="16"/>
+      <c r="M159" s="15"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
@@ -5814,7 +5820,7 @@
       <c r="K160" t="s">
         <v>221</v>
       </c>
-      <c r="M160" s="16"/>
+      <c r="M160" s="15"/>
     </row>
     <row r="161" spans="1:14">
       <c r="A161" s="1" t="s">
@@ -5844,7 +5850,7 @@
       <c r="K161" t="s">
         <v>221</v>
       </c>
-      <c r="M161" s="16"/>
+      <c r="M161" s="15"/>
     </row>
     <row r="162" spans="1:14">
       <c r="A162" s="1" t="s">
@@ -5874,7 +5880,7 @@
       <c r="K162" t="s">
         <v>221</v>
       </c>
-      <c r="M162" s="16"/>
+      <c r="M162" s="15"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="1" t="s">
@@ -5904,7 +5910,7 @@
       <c r="K163" t="s">
         <v>221</v>
       </c>
-      <c r="M163" s="16"/>
+      <c r="M163" s="15"/>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" s="1" t="s">
@@ -5934,7 +5940,7 @@
       <c r="K164" t="s">
         <v>221</v>
       </c>
-      <c r="M164" s="16"/>
+      <c r="M164" s="15"/>
       <c r="N164">
         <v>1</v>
       </c>
@@ -5964,7 +5970,7 @@
       <c r="J165" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M165" s="16">
+      <c r="M165" s="15">
         <v>1</v>
       </c>
     </row>
@@ -5993,7 +5999,7 @@
       <c r="J166" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M166" s="16"/>
+      <c r="M166" s="15"/>
     </row>
     <row r="167" spans="1:14">
       <c r="A167" s="1" t="s">
@@ -6020,7 +6026,7 @@
       <c r="J167" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M167" s="16"/>
+      <c r="M167" s="15"/>
     </row>
     <row r="168" spans="1:14">
       <c r="A168" s="1" t="s">
@@ -6050,7 +6056,7 @@
       <c r="K168" t="s">
         <v>224</v>
       </c>
-      <c r="M168" s="16"/>
+      <c r="M168" s="15"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="1" t="s">
@@ -6077,7 +6083,7 @@
       <c r="J169" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M169" s="16"/>
+      <c r="M169" s="15"/>
     </row>
     <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
@@ -6104,7 +6110,7 @@
       <c r="J170" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="16"/>
+      <c r="M170" s="15"/>
     </row>
     <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
@@ -6133,7 +6139,7 @@
       <c r="J171" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M171" s="16"/>
+      <c r="M171" s="15"/>
     </row>
     <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
@@ -6162,7 +6168,7 @@
       <c r="J172" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M172" s="16"/>
+      <c r="M172" s="15"/>
     </row>
     <row r="173" spans="1:14" ht="15" customHeight="1">
       <c r="A173" s="1" t="s">
@@ -6193,7 +6199,7 @@
       <c r="J173" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M173" s="16"/>
+      <c r="M173" s="15"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
@@ -6224,7 +6230,7 @@
       <c r="J174" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M174" s="16"/>
+      <c r="M174" s="15"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="1" t="s">
@@ -6260,7 +6266,7 @@
       <c r="K175" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M175" s="16"/>
+      <c r="M175" s="15"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="1" t="s">
@@ -6296,7 +6302,7 @@
       <c r="K176" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M176" s="16"/>
+      <c r="M176" s="15"/>
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
@@ -6332,7 +6338,7 @@
       <c r="K177" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M177" s="16"/>
+      <c r="M177" s="15"/>
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
@@ -6368,7 +6374,7 @@
       <c r="K178" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M178" s="16"/>
+      <c r="M178" s="15"/>
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
@@ -6399,7 +6405,7 @@
       <c r="J179" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M179" s="16"/>
+      <c r="M179" s="15"/>
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
@@ -6435,7 +6441,7 @@
       <c r="K180" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M180" s="16"/>
+      <c r="M180" s="15"/>
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
@@ -6471,7 +6477,7 @@
       <c r="K181" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M181" s="16"/>
+      <c r="M181" s="15"/>
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
@@ -6507,7 +6513,7 @@
       <c r="K182" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M182" s="16"/>
+      <c r="M182" s="15"/>
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
@@ -6540,7 +6546,7 @@
       <c r="J183" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M183" s="16"/>
+      <c r="M183" s="15"/>
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
@@ -6573,7 +6579,7 @@
       <c r="J184" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M184" s="16"/>
+      <c r="M184" s="15"/>
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
@@ -6606,7 +6612,7 @@
       <c r="J185" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M185" s="16"/>
+      <c r="M185" s="15"/>
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
@@ -6633,7 +6639,7 @@
       <c r="J186" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M186" s="16"/>
+      <c r="M186" s="15"/>
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
@@ -6660,7 +6666,7 @@
       <c r="J187" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M187" s="16"/>
+      <c r="M187" s="15"/>
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
@@ -6689,7 +6695,7 @@
       <c r="J188" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M188" s="16"/>
+      <c r="M188" s="15"/>
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
@@ -6912,7 +6918,7 @@
       <c r="J196" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M196" s="16">
+      <c r="M196" s="15">
         <v>2</v>
       </c>
     </row>
@@ -6941,7 +6947,7 @@
       <c r="J197" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M197" s="16"/>
+      <c r="M197" s="15"/>
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
@@ -6971,7 +6977,7 @@
       <c r="K198" t="s">
         <v>224</v>
       </c>
-      <c r="M198" s="16"/>
+      <c r="M198" s="15"/>
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
@@ -6998,7 +7004,7 @@
       <c r="J199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M199" s="16"/>
+      <c r="M199" s="15"/>
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
@@ -7025,7 +7031,7 @@
       <c r="J200" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M200" s="16"/>
+      <c r="M200" s="15"/>
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
@@ -7054,7 +7060,7 @@
       <c r="J201" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M201" s="16"/>
+      <c r="M201" s="15"/>
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
@@ -7081,7 +7087,7 @@
       <c r="J202" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M202" s="16"/>
+      <c r="M202" s="15"/>
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
@@ -7110,7 +7116,7 @@
       <c r="J203" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M203" s="16"/>
+      <c r="M203" s="15"/>
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
@@ -7137,7 +7143,7 @@
       <c r="J204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M204" s="16"/>
+      <c r="M204" s="15"/>
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
@@ -7164,7 +7170,7 @@
       <c r="J205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M205" s="16"/>
+      <c r="M205" s="15"/>
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
@@ -7191,7 +7197,7 @@
       <c r="J206" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M206" s="16"/>
+      <c r="M206" s="15"/>
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
@@ -7218,7 +7224,7 @@
       <c r="J207" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M207" s="16"/>
+      <c r="M207" s="15"/>
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
@@ -7248,7 +7254,7 @@
       <c r="K208" t="s">
         <v>225</v>
       </c>
-      <c r="M208" s="16"/>
+      <c r="M208" s="15"/>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1" t="s">
@@ -7278,7 +7284,7 @@
       <c r="K209" t="s">
         <v>225</v>
       </c>
-      <c r="M209" s="16"/>
+      <c r="M209" s="15"/>
       <c r="N209">
         <v>3</v>
       </c>
@@ -7311,7 +7317,7 @@
       <c r="K210" t="s">
         <v>220</v>
       </c>
-      <c r="M210" s="16">
+      <c r="M210" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -7345,7 +7351,7 @@
       <c r="K211" t="s">
         <v>221</v>
       </c>
-      <c r="M211" s="16"/>
+      <c r="M211" s="15"/>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1" t="s">
@@ -7377,7 +7383,7 @@
       <c r="K212" t="s">
         <v>221</v>
       </c>
-      <c r="M212" s="16"/>
+      <c r="M212" s="15"/>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1" t="s">
@@ -7409,7 +7415,7 @@
       <c r="K213" t="s">
         <v>221</v>
       </c>
-      <c r="M213" s="16"/>
+      <c r="M213" s="15"/>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1" t="s">
@@ -7441,7 +7447,7 @@
       <c r="K214" t="s">
         <v>221</v>
       </c>
-      <c r="M214" s="16"/>
+      <c r="M214" s="15"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1" t="s">
@@ -7473,7 +7479,7 @@
       <c r="K215" t="s">
         <v>221</v>
       </c>
-      <c r="M215" s="16"/>
+      <c r="M215" s="15"/>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1" t="s">
@@ -7505,7 +7511,7 @@
       <c r="K216" t="s">
         <v>221</v>
       </c>
-      <c r="M216" s="16"/>
+      <c r="M216" s="15"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1" t="s">
@@ -7537,7 +7543,7 @@
       <c r="K217" t="s">
         <v>221</v>
       </c>
-      <c r="M217" s="16"/>
+      <c r="M217" s="15"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1" t="s">
@@ -7566,7 +7572,7 @@
       <c r="J218" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M218" s="16"/>
+      <c r="M218" s="15"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1" t="s">
@@ -7595,7 +7601,7 @@
       <c r="J219" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M219" s="16"/>
+      <c r="M219" s="15"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1" t="s">
@@ -7622,7 +7628,7 @@
       <c r="J220" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M220" s="16">
+      <c r="M220" s="15">
         <v>1</v>
       </c>
     </row>
@@ -7651,7 +7657,7 @@
       <c r="J221" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M221" s="16"/>
+      <c r="M221" s="15"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1" t="s">
@@ -7678,7 +7684,7 @@
       <c r="J222" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M222" s="16"/>
+      <c r="M222" s="15"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1" t="s">
@@ -7708,7 +7714,7 @@
       <c r="K223" t="s">
         <v>224</v>
       </c>
-      <c r="M223" s="16"/>
+      <c r="M223" s="15"/>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1" t="s">
@@ -7735,7 +7741,7 @@
       <c r="J224" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M224" s="16"/>
+      <c r="M224" s="15"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
@@ -7762,7 +7768,7 @@
       <c r="J225" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M225" s="16"/>
+      <c r="M225" s="15"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="1" t="s">
@@ -7791,7 +7797,7 @@
       <c r="J226" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M226" s="16"/>
+      <c r="M226" s="15"/>
     </row>
     <row r="227" spans="1:13">
       <c r="A227" s="1" t="s">
@@ -7820,7 +7826,7 @@
       <c r="J227" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M227" s="16"/>
+      <c r="M227" s="15"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
@@ -7851,7 +7857,7 @@
       <c r="J228" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M228" s="16"/>
+      <c r="M228" s="15"/>
     </row>
     <row r="229" spans="1:13" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
@@ -7882,7 +7888,7 @@
       <c r="J229" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M229" s="16"/>
+      <c r="M229" s="15"/>
     </row>
     <row r="230" spans="1:13">
       <c r="A230" s="1" t="s">
@@ -7918,7 +7924,7 @@
       <c r="K230" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M230" s="16"/>
+      <c r="M230" s="15"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1" t="s">
@@ -7954,7 +7960,7 @@
       <c r="K231" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M231" s="16"/>
+      <c r="M231" s="15"/>
     </row>
     <row r="232" spans="1:13">
       <c r="A232" s="1" t="s">
@@ -7990,7 +7996,7 @@
       <c r="K232" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M232" s="16"/>
+      <c r="M232" s="15"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1" t="s">
@@ -8026,7 +8032,7 @@
       <c r="K233" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M233" s="16"/>
+      <c r="M233" s="15"/>
     </row>
     <row r="234" spans="1:13">
       <c r="A234" s="1" t="s">
@@ -8057,7 +8063,7 @@
       <c r="J234" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M234" s="16"/>
+      <c r="M234" s="15"/>
     </row>
     <row r="235" spans="1:13">
       <c r="A235" s="1" t="s">
@@ -8093,7 +8099,7 @@
       <c r="K235" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M235" s="16"/>
+      <c r="M235" s="15"/>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1" t="s">
@@ -8129,7 +8135,7 @@
       <c r="K236" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M236" s="16"/>
+      <c r="M236" s="15"/>
     </row>
     <row r="237" spans="1:13">
       <c r="A237" s="1" t="s">
@@ -8165,7 +8171,7 @@
       <c r="K237" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M237" s="16"/>
+      <c r="M237" s="15"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1" t="s">
@@ -8198,7 +8204,7 @@
       <c r="J238" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M238" s="16"/>
+      <c r="M238" s="15"/>
     </row>
     <row r="239" spans="1:13">
       <c r="A239" s="1" t="s">
@@ -8231,7 +8237,7 @@
       <c r="J239" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M239" s="16"/>
+      <c r="M239" s="15"/>
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1" t="s">
@@ -8264,7 +8270,7 @@
       <c r="J240" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M240" s="16"/>
+      <c r="M240" s="15"/>
     </row>
     <row r="241" spans="1:13">
       <c r="A241" s="1" t="s">
@@ -8291,7 +8297,7 @@
       <c r="J241" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M241" s="16"/>
+      <c r="M241" s="15"/>
     </row>
     <row r="242" spans="1:13">
       <c r="A242" s="1" t="s">
@@ -8318,7 +8324,7 @@
       <c r="J242" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M242" s="16"/>
+      <c r="M242" s="15"/>
     </row>
     <row r="243" spans="1:13">
       <c r="A243" s="1" t="s">
@@ -8347,7 +8353,7 @@
       <c r="J243" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M243" s="16"/>
+      <c r="M243" s="15"/>
     </row>
     <row r="244" spans="1:13" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
@@ -8376,7 +8382,7 @@
       <c r="J244" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M244" s="16"/>
+      <c r="M244" s="15"/>
     </row>
     <row r="245" spans="1:13" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
@@ -8405,7 +8411,7 @@
       <c r="J245" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M245" s="16"/>
+      <c r="M245" s="15"/>
     </row>
     <row r="246" spans="1:13" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
@@ -8434,7 +8440,7 @@
       <c r="J246" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M246" s="16"/>
+      <c r="M246" s="15"/>
     </row>
     <row r="247" spans="1:13" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
@@ -8463,7 +8469,7 @@
       <c r="J247" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M247" s="16"/>
+      <c r="M247" s="15"/>
     </row>
     <row r="248" spans="1:13" ht="15" customHeight="1">
       <c r="A248" s="1" t="s">
@@ -8492,7 +8498,7 @@
       <c r="J248" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M248" s="16"/>
+      <c r="M248" s="15"/>
     </row>
     <row r="249" spans="1:13" ht="15" customHeight="1">
       <c r="A249" s="1" t="s">
@@ -8521,7 +8527,7 @@
       <c r="J249" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M249" s="16"/>
+      <c r="M249" s="15"/>
     </row>
     <row r="250" spans="1:13" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
@@ -8550,7 +8556,7 @@
       <c r="J250" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M250" s="16"/>
+      <c r="M250" s="15"/>
     </row>
     <row r="251" spans="1:13">
       <c r="A251" s="1" t="s">
@@ -8577,7 +8583,7 @@
       <c r="J251" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M251" s="16"/>
+      <c r="M251" s="15"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1" t="s">
@@ -8604,7 +8610,7 @@
       <c r="J252" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M252" s="16"/>
+      <c r="M252" s="15"/>
     </row>
     <row r="253" spans="1:13">
       <c r="A253" s="1" t="s">
@@ -8631,7 +8637,7 @@
       <c r="J253" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M253" s="16"/>
+      <c r="M253" s="15"/>
     </row>
     <row r="254" spans="1:13">
       <c r="A254" s="1" t="s">
@@ -8661,7 +8667,7 @@
       <c r="K254" t="s">
         <v>224</v>
       </c>
-      <c r="M254" s="16"/>
+      <c r="M254" s="15"/>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1" t="s">
@@ -8688,7 +8694,7 @@
       <c r="J255" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M255" s="16"/>
+      <c r="M255" s="15"/>
     </row>
     <row r="256" spans="1:13">
       <c r="A256" s="1" t="s">
@@ -8715,7 +8721,7 @@
       <c r="J256" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M256" s="16"/>
+      <c r="M256" s="15"/>
     </row>
     <row r="257" spans="1:13">
       <c r="A257" s="1" t="s">
@@ -8742,7 +8748,7 @@
       <c r="J257" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M257" s="16"/>
+      <c r="M257" s="15"/>
     </row>
     <row r="258" spans="1:13">
       <c r="A258" s="1" t="s">
@@ -8771,7 +8777,7 @@
       <c r="J258" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M258" s="16"/>
+      <c r="M258" s="15"/>
     </row>
     <row r="259" spans="1:13">
       <c r="A259" s="1" t="s">
@@ -8798,7 +8804,7 @@
       <c r="J259" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M259" s="16"/>
+      <c r="M259" s="15"/>
     </row>
     <row r="260" spans="1:13">
       <c r="A260" s="1" t="s">
@@ -8827,7 +8833,7 @@
       <c r="J260" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M260" s="16"/>
+      <c r="M260" s="15"/>
     </row>
     <row r="261" spans="1:13">
       <c r="A261" s="1" t="s">
@@ -8854,7 +8860,7 @@
       <c r="J261" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M261" s="16"/>
+      <c r="M261" s="15"/>
     </row>
     <row r="262" spans="1:13">
       <c r="A262" s="1" t="s">
@@ -8881,7 +8887,7 @@
       <c r="J262" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M262" s="16"/>
+      <c r="M262" s="15"/>
     </row>
     <row r="263" spans="1:13">
       <c r="A263" s="1" t="s">
@@ -8908,7 +8914,7 @@
       <c r="J263" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M263" s="16"/>
+      <c r="M263" s="15"/>
     </row>
     <row r="264" spans="1:13">
       <c r="A264" s="1" t="s">
@@ -8935,7 +8941,7 @@
       <c r="J264" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M264" s="16"/>
+      <c r="M264" s="15"/>
     </row>
     <row r="265" spans="1:13">
       <c r="A265" s="1" t="s">
@@ -8965,7 +8971,7 @@
       <c r="K265" t="s">
         <v>225</v>
       </c>
-      <c r="M265" s="16"/>
+      <c r="M265" s="15"/>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1" t="s">
@@ -8995,7 +9001,7 @@
       <c r="K266" t="s">
         <v>225</v>
       </c>
-      <c r="M266" s="16"/>
+      <c r="M266" s="15"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1" t="s">
@@ -9025,7 +9031,7 @@
       <c r="K267" t="s">
         <v>225</v>
       </c>
-      <c r="M267" s="16"/>
+      <c r="M267" s="15"/>
     </row>
     <row r="268" spans="1:13" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
@@ -9055,7 +9061,7 @@
       <c r="K268" t="s">
         <v>220</v>
       </c>
-      <c r="M268" s="16"/>
+      <c r="M268" s="15"/>
     </row>
     <row r="269" spans="1:13" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
@@ -9087,7 +9093,7 @@
       <c r="K269" t="s">
         <v>221</v>
       </c>
-      <c r="M269" s="16"/>
+      <c r="M269" s="15"/>
     </row>
     <row r="270" spans="1:13" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
@@ -9119,7 +9125,7 @@
       <c r="K270" t="s">
         <v>221</v>
       </c>
-      <c r="M270" s="16"/>
+      <c r="M270" s="15"/>
     </row>
     <row r="271" spans="1:13" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
@@ -9151,7 +9157,7 @@
       <c r="K271" t="s">
         <v>221</v>
       </c>
-      <c r="M271" s="16"/>
+      <c r="M271" s="15"/>
     </row>
     <row r="272" spans="1:13" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
@@ -9183,7 +9189,7 @@
       <c r="K272" t="s">
         <v>221</v>
       </c>
-      <c r="M272" s="16"/>
+      <c r="M272" s="15"/>
     </row>
     <row r="273" spans="1:13" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
@@ -9215,7 +9221,7 @@
       <c r="K273" t="s">
         <v>221</v>
       </c>
-      <c r="M273" s="16"/>
+      <c r="M273" s="15"/>
     </row>
     <row r="274" spans="1:13" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
@@ -9247,7 +9253,7 @@
       <c r="K274" t="s">
         <v>221</v>
       </c>
-      <c r="M274" s="16"/>
+      <c r="M274" s="15"/>
     </row>
     <row r="275" spans="1:13" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
@@ -9279,7 +9285,7 @@
       <c r="K275" t="s">
         <v>221</v>
       </c>
-      <c r="M275" s="16"/>
+      <c r="M275" s="15"/>
     </row>
     <row r="276" spans="1:13" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
@@ -9308,7 +9314,7 @@
       <c r="J276" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M276" s="16"/>
+      <c r="M276" s="15"/>
     </row>
     <row r="277" spans="1:13">
       <c r="A277" s="1" t="s">
@@ -9337,7 +9343,7 @@
       <c r="J277" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M277" s="16"/>
+      <c r="M277" s="15"/>
     </row>
     <row r="278" spans="1:13">
       <c r="A278" s="1" t="s">
@@ -9364,7 +9370,7 @@
       <c r="J278" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M278" s="16"/>
+      <c r="M278" s="15"/>
     </row>
     <row r="279" spans="1:13">
       <c r="A279" s="1" t="s">
@@ -9391,7 +9397,7 @@
       <c r="J279" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M279" s="16"/>
+      <c r="M279" s="15"/>
     </row>
     <row r="280" spans="1:13">
       <c r="A280" s="1" t="s">
@@ -9418,7 +9424,7 @@
       <c r="J280" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M280" s="16"/>
+      <c r="M280" s="15"/>
     </row>
     <row r="281" spans="1:13">
       <c r="A281" s="1" t="s">
@@ -9448,7 +9454,7 @@
       <c r="K281" t="s">
         <v>224</v>
       </c>
-      <c r="M281" s="16"/>
+      <c r="M281" s="15"/>
     </row>
     <row r="282" spans="1:13">
       <c r="A282" s="1" t="s">
@@ -9475,7 +9481,7 @@
       <c r="J282" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M282" s="16"/>
+      <c r="M282" s="15"/>
     </row>
     <row r="283" spans="1:13">
       <c r="A283" s="1" t="s">
@@ -9502,7 +9508,7 @@
       <c r="J283" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M283" s="16"/>
+      <c r="M283" s="15"/>
     </row>
     <row r="284" spans="1:13">
       <c r="A284" s="1" t="s">
@@ -9531,7 +9537,7 @@
       <c r="J284" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M284" s="16"/>
+      <c r="M284" s="15"/>
     </row>
     <row r="285" spans="1:13">
       <c r="A285" s="1" t="s">
@@ -9560,7 +9566,7 @@
       <c r="J285" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M285" s="16"/>
+      <c r="M285" s="15"/>
     </row>
     <row r="286" spans="1:13" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
@@ -9591,7 +9597,7 @@
       <c r="J286" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="16"/>
+      <c r="M286" s="15"/>
     </row>
     <row r="287" spans="1:13" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
@@ -9622,7 +9628,7 @@
       <c r="J287" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M287" s="16"/>
+      <c r="M287" s="15"/>
     </row>
     <row r="288" spans="1:13">
       <c r="A288" s="1" t="s">
@@ -9658,7 +9664,7 @@
       <c r="K288" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M288" s="16"/>
+      <c r="M288" s="15"/>
     </row>
     <row r="289" spans="1:13">
       <c r="A289" s="1" t="s">
@@ -9694,7 +9700,7 @@
       <c r="K289" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M289" s="16"/>
+      <c r="M289" s="15"/>
     </row>
     <row r="290" spans="1:13">
       <c r="A290" s="1" t="s">
@@ -9730,7 +9736,7 @@
       <c r="K290" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M290" s="16"/>
+      <c r="M290" s="15"/>
     </row>
     <row r="291" spans="1:13">
       <c r="A291" s="1" t="s">
@@ -9766,7 +9772,7 @@
       <c r="K291" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M291" s="16"/>
+      <c r="M291" s="15"/>
     </row>
     <row r="292" spans="1:13">
       <c r="A292" s="1" t="s">
@@ -9797,7 +9803,7 @@
       <c r="J292" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M292" s="16"/>
+      <c r="M292" s="15"/>
     </row>
     <row r="293" spans="1:13">
       <c r="A293" s="1" t="s">
@@ -9833,7 +9839,7 @@
       <c r="K293" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M293" s="16"/>
+      <c r="M293" s="15"/>
     </row>
     <row r="294" spans="1:13">
       <c r="A294" s="1" t="s">
@@ -9869,7 +9875,7 @@
       <c r="K294" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M294" s="16"/>
+      <c r="M294" s="15"/>
     </row>
     <row r="295" spans="1:13">
       <c r="A295" s="1" t="s">
@@ -9905,7 +9911,7 @@
       <c r="K295" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M295" s="16"/>
+      <c r="M295" s="15"/>
     </row>
     <row r="296" spans="1:13">
       <c r="A296" s="1" t="s">
@@ -9938,7 +9944,7 @@
       <c r="J296" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M296" s="16"/>
+      <c r="M296" s="15"/>
     </row>
     <row r="297" spans="1:13">
       <c r="A297" s="1" t="s">
@@ -9971,7 +9977,7 @@
       <c r="J297" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M297" s="16"/>
+      <c r="M297" s="15"/>
     </row>
     <row r="298" spans="1:13">
       <c r="A298" s="1" t="s">
@@ -10004,7 +10010,7 @@
       <c r="J298" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M298" s="16"/>
+      <c r="M298" s="15"/>
     </row>
     <row r="299" spans="1:13">
       <c r="A299" s="1" t="s">
@@ -10031,7 +10037,7 @@
       <c r="J299" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M299" s="16"/>
+      <c r="M299" s="15"/>
     </row>
     <row r="300" spans="1:13">
       <c r="A300" s="1" t="s">
@@ -10058,7 +10064,7 @@
       <c r="J300" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M300" s="16"/>
+      <c r="M300" s="15"/>
     </row>
     <row r="301" spans="1:13">
       <c r="A301" s="1" t="s">
@@ -10087,7 +10093,7 @@
       <c r="J301" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M301" s="16"/>
+      <c r="M301" s="15"/>
     </row>
     <row r="302" spans="1:13" ht="15" customHeight="1">
       <c r="A302" s="1" t="s">
@@ -10116,7 +10122,7 @@
       <c r="J302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M302" s="16"/>
+      <c r="M302" s="15"/>
     </row>
     <row r="303" spans="1:13" ht="15" customHeight="1">
       <c r="A303" s="1" t="s">
@@ -10145,7 +10151,7 @@
       <c r="J303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M303" s="16"/>
+      <c r="M303" s="15"/>
     </row>
     <row r="304" spans="1:13" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
@@ -10174,7 +10180,7 @@
       <c r="J304" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M304" s="16"/>
+      <c r="M304" s="15"/>
     </row>
     <row r="305" spans="1:13" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
@@ -10203,7 +10209,7 @@
       <c r="J305" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M305" s="16"/>
+      <c r="M305" s="15"/>
     </row>
     <row r="306" spans="1:13" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
@@ -10232,7 +10238,7 @@
       <c r="J306" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M306" s="16"/>
+      <c r="M306" s="15"/>
     </row>
     <row r="307" spans="1:13" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
@@ -10261,7 +10267,7 @@
       <c r="J307" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M307" s="16"/>
+      <c r="M307" s="15"/>
     </row>
     <row r="308" spans="1:13" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
@@ -10290,7 +10296,7 @@
       <c r="J308" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M308" s="16"/>
+      <c r="M308" s="15"/>
     </row>
     <row r="309" spans="1:13">
       <c r="A309" s="1" t="s">
@@ -10317,7 +10323,7 @@
       <c r="J309" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M309" s="16"/>
+      <c r="M309" s="15"/>
     </row>
     <row r="310" spans="1:13">
       <c r="A310" s="1" t="s">
@@ -10344,7 +10350,7 @@
       <c r="J310" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M310" s="16"/>
+      <c r="M310" s="15"/>
     </row>
     <row r="311" spans="1:13">
       <c r="A311" s="1" t="s">
@@ -10371,7 +10377,7 @@
       <c r="J311" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M311" s="16"/>
+      <c r="M311" s="15"/>
     </row>
     <row r="312" spans="1:13">
       <c r="A312" s="1" t="s">
@@ -10401,7 +10407,7 @@
       <c r="K312" t="s">
         <v>224</v>
       </c>
-      <c r="M312" s="16"/>
+      <c r="M312" s="15"/>
     </row>
     <row r="313" spans="1:13">
       <c r="A313" s="1" t="s">
@@ -10428,7 +10434,7 @@
       <c r="J313" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M313" s="16"/>
+      <c r="M313" s="15"/>
     </row>
     <row r="314" spans="1:13">
       <c r="A314" s="1" t="s">
@@ -10455,7 +10461,7 @@
       <c r="J314" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M314" s="16"/>
+      <c r="M314" s="15"/>
     </row>
     <row r="315" spans="1:13">
       <c r="A315" s="1" t="s">
@@ -10482,7 +10488,7 @@
       <c r="J315" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M315" s="16"/>
+      <c r="M315" s="15"/>
     </row>
     <row r="316" spans="1:13">
       <c r="A316" s="1" t="s">
@@ -10511,7 +10517,7 @@
       <c r="J316" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M316" s="16"/>
+      <c r="M316" s="15"/>
     </row>
     <row r="317" spans="1:13">
       <c r="A317" s="1" t="s">
@@ -10538,7 +10544,7 @@
       <c r="J317" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M317" s="16"/>
+      <c r="M317" s="15"/>
     </row>
     <row r="318" spans="1:13">
       <c r="A318" s="1" t="s">
@@ -10567,7 +10573,7 @@
       <c r="J318" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M318" s="16"/>
+      <c r="M318" s="15"/>
     </row>
     <row r="319" spans="1:13">
       <c r="A319" s="1" t="s">
@@ -10594,7 +10600,7 @@
       <c r="J319" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M319" s="16"/>
+      <c r="M319" s="15"/>
     </row>
     <row r="320" spans="1:13">
       <c r="A320" s="1" t="s">
@@ -10621,7 +10627,7 @@
       <c r="J320" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M320" s="16"/>
+      <c r="M320" s="15"/>
     </row>
     <row r="321" spans="1:14">
       <c r="A321" s="1" t="s">
@@ -10648,7 +10654,7 @@
       <c r="J321" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M321" s="16"/>
+      <c r="M321" s="15"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="1" t="s">
@@ -10675,7 +10681,7 @@
       <c r="J322" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M322" s="16"/>
+      <c r="M322" s="15"/>
     </row>
     <row r="323" spans="1:14">
       <c r="A323" s="1" t="s">
@@ -10702,7 +10708,7 @@
       <c r="J323" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M323" s="16"/>
+      <c r="M323" s="15"/>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="1" t="s">
@@ -10729,7 +10735,7 @@
       <c r="J324" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M324" s="16"/>
+      <c r="M324" s="15"/>
     </row>
     <row r="325" spans="1:14">
       <c r="A325" s="1" t="s">
@@ -10756,7 +10762,7 @@
       <c r="J325" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M325" s="16"/>
+      <c r="M325" s="15"/>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="1" t="s">
@@ -10786,7 +10792,7 @@
       <c r="K326" t="s">
         <v>221</v>
       </c>
-      <c r="M326" s="16"/>
+      <c r="M326" s="15"/>
     </row>
     <row r="327" spans="1:14">
       <c r="A327" s="1" t="s">
@@ -10818,7 +10824,7 @@
       <c r="K327" t="s">
         <v>221</v>
       </c>
-      <c r="M327" s="16"/>
+      <c r="M327" s="15"/>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="1" t="s">
@@ -10850,7 +10856,7 @@
       <c r="K328" t="s">
         <v>221</v>
       </c>
-      <c r="M328" s="16"/>
+      <c r="M328" s="15"/>
     </row>
     <row r="329" spans="1:14">
       <c r="A329" s="1" t="s">
@@ -10882,7 +10888,7 @@
       <c r="K329" t="s">
         <v>221</v>
       </c>
-      <c r="M329" s="16"/>
+      <c r="M329" s="15"/>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="1" t="s">
@@ -10914,7 +10920,7 @@
       <c r="K330" t="s">
         <v>221</v>
       </c>
-      <c r="M330" s="16"/>
+      <c r="M330" s="15"/>
     </row>
     <row r="331" spans="1:14">
       <c r="A331" s="1" t="s">
@@ -10946,7 +10952,7 @@
       <c r="K331" t="s">
         <v>221</v>
       </c>
-      <c r="M331" s="16"/>
+      <c r="M331" s="15"/>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="1" t="s">
@@ -10978,7 +10984,7 @@
       <c r="K332" t="s">
         <v>221</v>
       </c>
-      <c r="M332" s="16"/>
+      <c r="M332" s="15"/>
     </row>
     <row r="333" spans="1:14">
       <c r="A333" s="1" t="s">
@@ -11007,7 +11013,7 @@
       <c r="J333" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M333" s="16"/>
+      <c r="M333" s="15"/>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="1" t="s">
@@ -11036,7 +11042,7 @@
       <c r="J334" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M334" s="16"/>
+      <c r="M334" s="15"/>
     </row>
     <row r="335" spans="1:14">
       <c r="A335" s="1" t="s">
@@ -11065,7 +11071,7 @@
       <c r="J335" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M335" s="16"/>
+      <c r="M335" s="15"/>
       <c r="N335">
         <v>1</v>
       </c>
@@ -11240,7 +11246,7 @@
       <c r="J342" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M342" s="16">
+      <c r="M342" s="15">
         <v>1</v>
       </c>
     </row>
@@ -11267,7 +11273,7 @@
       <c r="J343" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M343" s="16"/>
+      <c r="M343" s="15"/>
     </row>
     <row r="344" spans="1:13">
       <c r="A344" s="1" t="s">
@@ -11292,7 +11298,7 @@
       <c r="J344" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M344" s="16"/>
+      <c r="M344" s="15"/>
     </row>
     <row r="345" spans="1:13">
       <c r="A345" s="1" t="s">
@@ -11320,7 +11326,7 @@
       <c r="K345" t="s">
         <v>224</v>
       </c>
-      <c r="M345" s="16"/>
+      <c r="M345" s="15"/>
     </row>
     <row r="346" spans="1:13">
       <c r="A346" s="1" t="s">
@@ -11345,7 +11351,7 @@
       <c r="J346" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M346" s="16"/>
+      <c r="M346" s="15"/>
     </row>
     <row r="347" spans="1:13">
       <c r="A347" s="1" t="s">
@@ -11370,7 +11376,7 @@
       <c r="J347" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M347" s="16"/>
+      <c r="M347" s="15"/>
     </row>
     <row r="348" spans="1:13">
       <c r="A348" s="1" t="s">
@@ -11397,7 +11403,7 @@
       <c r="J348" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M348" s="16"/>
+      <c r="M348" s="15"/>
     </row>
     <row r="349" spans="1:13">
       <c r="A349" s="1" t="s">
@@ -11424,7 +11430,7 @@
       <c r="J349" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M349" s="16"/>
+      <c r="M349" s="15"/>
     </row>
     <row r="350" spans="1:13" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
@@ -11453,7 +11459,7 @@
       <c r="J350" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M350" s="16"/>
+      <c r="M350" s="15"/>
     </row>
     <row r="351" spans="1:13" ht="15" customHeight="1">
       <c r="A351" s="1" t="s">
@@ -11482,7 +11488,7 @@
       <c r="J351" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M351" s="16"/>
+      <c r="M351" s="15"/>
     </row>
     <row r="352" spans="1:13">
       <c r="A352" s="1" t="s">
@@ -11516,7 +11522,7 @@
       <c r="K352" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M352" s="16"/>
+      <c r="M352" s="15"/>
     </row>
     <row r="353" spans="1:13">
       <c r="A353" s="1" t="s">
@@ -11550,7 +11556,7 @@
       <c r="K353" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M353" s="16"/>
+      <c r="M353" s="15"/>
     </row>
     <row r="354" spans="1:13">
       <c r="A354" s="1" t="s">
@@ -11584,7 +11590,7 @@
       <c r="K354" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M354" s="16"/>
+      <c r="M354" s="15"/>
     </row>
     <row r="355" spans="1:13">
       <c r="A355" s="1" t="s">
@@ -11618,7 +11624,7 @@
       <c r="K355" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M355" s="16"/>
+      <c r="M355" s="15"/>
     </row>
     <row r="356" spans="1:13">
       <c r="A356" s="1" t="s">
@@ -11647,7 +11653,7 @@
       <c r="J356" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M356" s="16"/>
+      <c r="M356" s="15"/>
     </row>
     <row r="357" spans="1:13">
       <c r="A357" s="1" t="s">
@@ -11681,7 +11687,7 @@
       <c r="K357" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M357" s="16"/>
+      <c r="M357" s="15"/>
     </row>
     <row r="358" spans="1:13">
       <c r="A358" s="1" t="s">
@@ -11715,7 +11721,7 @@
       <c r="K358" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M358" s="16"/>
+      <c r="M358" s="15"/>
     </row>
     <row r="359" spans="1:13">
       <c r="A359" s="1" t="s">
@@ -11749,7 +11755,7 @@
       <c r="K359" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M359" s="16"/>
+      <c r="M359" s="15"/>
     </row>
     <row r="360" spans="1:13">
       <c r="A360" s="1" t="s">
@@ -11780,7 +11786,7 @@
       <c r="J360" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M360" s="16"/>
+      <c r="M360" s="15"/>
     </row>
     <row r="361" spans="1:13">
       <c r="A361" s="1" t="s">
@@ -11811,7 +11817,7 @@
       <c r="J361" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M361" s="16"/>
+      <c r="M361" s="15"/>
     </row>
     <row r="362" spans="1:13">
       <c r="A362" s="1" t="s">
@@ -11842,7 +11848,7 @@
       <c r="J362" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M362" s="16"/>
+      <c r="M362" s="15"/>
     </row>
     <row r="363" spans="1:13">
       <c r="A363" s="1" t="s">
@@ -11867,7 +11873,7 @@
       <c r="J363" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M363" s="16"/>
+      <c r="M363" s="15"/>
     </row>
     <row r="364" spans="1:13">
       <c r="A364" s="1" t="s">
@@ -11892,7 +11898,7 @@
       <c r="J364" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M364" s="16"/>
+      <c r="M364" s="15"/>
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="1" t="s">
@@ -11919,7 +11925,7 @@
       <c r="J365" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M365" s="16"/>
+      <c r="M365" s="15"/>
     </row>
     <row r="366" spans="1:13">
       <c r="A366" s="1" t="s">
@@ -11946,7 +11952,7 @@
       <c r="J366" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M366" s="16"/>
+      <c r="M366" s="15"/>
     </row>
     <row r="367" spans="1:13">
       <c r="A367" s="1" t="s">
@@ -11973,7 +11979,7 @@
       <c r="J367" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M367" s="16"/>
+      <c r="M367" s="15"/>
     </row>
     <row r="368" spans="1:13">
       <c r="A368" s="1" t="s">
@@ -12000,7 +12006,7 @@
       <c r="J368" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M368" s="16"/>
+      <c r="M368" s="15"/>
     </row>
     <row r="369" spans="1:13">
       <c r="A369" s="1" t="s">
@@ -12027,7 +12033,7 @@
       <c r="J369" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M369" s="16"/>
+      <c r="M369" s="15"/>
     </row>
     <row r="370" spans="1:13">
       <c r="A370" s="1" t="s">
@@ -12054,7 +12060,7 @@
       <c r="J370" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M370" s="16"/>
+      <c r="M370" s="15"/>
     </row>
     <row r="371" spans="1:13">
       <c r="A371" s="1" t="s">
@@ -12081,7 +12087,7 @@
       <c r="J371" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M371" s="16"/>
+      <c r="M371" s="15"/>
     </row>
     <row r="372" spans="1:13">
       <c r="A372" s="1" t="s">
@@ -12108,7 +12114,7 @@
       <c r="J372" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M372" s="16"/>
+      <c r="M372" s="15"/>
     </row>
     <row r="373" spans="1:13">
       <c r="A373" s="1" t="s">
@@ -12133,7 +12139,7 @@
       <c r="J373" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M373" s="16"/>
+      <c r="M373" s="15"/>
     </row>
     <row r="374" spans="1:13">
       <c r="A374" s="1" t="s">
@@ -12158,7 +12164,7 @@
       <c r="J374" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M374" s="16"/>
+      <c r="M374" s="15"/>
     </row>
     <row r="375" spans="1:13">
       <c r="A375" s="1" t="s">
@@ -12183,7 +12189,7 @@
       <c r="J375" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M375" s="16"/>
+      <c r="M375" s="15"/>
     </row>
     <row r="376" spans="1:13">
       <c r="A376" s="1" t="s">
@@ -12211,7 +12217,7 @@
       <c r="K376" t="s">
         <v>224</v>
       </c>
-      <c r="M376" s="16"/>
+      <c r="M376" s="15"/>
     </row>
     <row r="377" spans="1:13">
       <c r="A377" s="1" t="s">
@@ -12236,7 +12242,7 @@
       <c r="J377" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M377" s="16"/>
+      <c r="M377" s="15"/>
     </row>
     <row r="378" spans="1:13">
       <c r="A378" s="1" t="s">
@@ -12261,7 +12267,7 @@
       <c r="J378" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M378" s="16"/>
+      <c r="M378" s="15"/>
     </row>
     <row r="379" spans="1:13">
       <c r="A379" s="1" t="s">
@@ -12286,7 +12292,7 @@
       <c r="J379" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M379" s="16"/>
+      <c r="M379" s="15"/>
     </row>
     <row r="380" spans="1:13">
       <c r="A380" s="1" t="s">
@@ -12313,7 +12319,7 @@
       <c r="J380" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M380" s="16"/>
+      <c r="M380" s="15"/>
     </row>
     <row r="381" spans="1:13">
       <c r="A381" s="1" t="s">
@@ -12338,7 +12344,7 @@
       <c r="J381" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M381" s="16"/>
+      <c r="M381" s="15"/>
     </row>
     <row r="382" spans="1:13">
       <c r="A382" s="1" t="s">
@@ -12365,7 +12371,7 @@
       <c r="J382" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M382" s="16"/>
+      <c r="M382" s="15"/>
     </row>
     <row r="383" spans="1:13">
       <c r="A383" s="1" t="s">
@@ -12390,7 +12396,7 @@
       <c r="J383" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M383" s="16"/>
+      <c r="M383" s="15"/>
     </row>
     <row r="384" spans="1:13">
       <c r="A384" s="1" t="s">
@@ -12415,7 +12421,7 @@
       <c r="J384" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M384" s="16"/>
+      <c r="M384" s="15"/>
     </row>
     <row r="385" spans="1:14">
       <c r="A385" s="1" t="s">
@@ -12440,7 +12446,7 @@
       <c r="J385" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M385" s="16"/>
+      <c r="M385" s="15"/>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="1" t="s">
@@ -12465,7 +12471,7 @@
       <c r="J386" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M386" s="16"/>
+      <c r="M386" s="15"/>
     </row>
     <row r="387" spans="1:14">
       <c r="A387" s="1" t="s">
@@ -12546,7 +12552,7 @@
       <c r="K389" t="s">
         <v>221</v>
       </c>
-      <c r="M389" s="16">
+      <c r="M389" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -12578,7 +12584,7 @@
       <c r="K390" t="s">
         <v>221</v>
       </c>
-      <c r="M390" s="16"/>
+      <c r="M390" s="15"/>
     </row>
     <row r="391" spans="1:14">
       <c r="A391" s="1" t="s">
@@ -12608,7 +12614,7 @@
       <c r="K391" t="s">
         <v>221</v>
       </c>
-      <c r="M391" s="16"/>
+      <c r="M391" s="15"/>
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="1" t="s">
@@ -12638,7 +12644,7 @@
       <c r="K392" t="s">
         <v>221</v>
       </c>
-      <c r="M392" s="16"/>
+      <c r="M392" s="15"/>
     </row>
     <row r="393" spans="1:14">
       <c r="A393" s="1" t="s">
@@ -12668,7 +12674,7 @@
       <c r="K393" t="s">
         <v>221</v>
       </c>
-      <c r="M393" s="16"/>
+      <c r="M393" s="15"/>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="1" t="s">
@@ -12698,7 +12704,7 @@
       <c r="K394" t="s">
         <v>221</v>
       </c>
-      <c r="M394" s="16"/>
+      <c r="M394" s="15"/>
     </row>
     <row r="395" spans="1:14">
       <c r="A395" s="1" t="s">
@@ -12725,7 +12731,7 @@
       <c r="J395" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M395" s="16"/>
+      <c r="M395" s="15"/>
       <c r="N395">
         <v>0.5</v>
       </c>
@@ -12755,7 +12761,7 @@
       <c r="J396" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M396" s="16">
+      <c r="M396" s="15">
         <v>1</v>
       </c>
     </row>
@@ -12784,7 +12790,7 @@
       <c r="J397" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M397" s="16"/>
+      <c r="M397" s="15"/>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="1" t="s">
@@ -12811,7 +12817,7 @@
       <c r="J398" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M398" s="16"/>
+      <c r="M398" s="15"/>
     </row>
     <row r="399" spans="1:14">
       <c r="A399" s="1" t="s">
@@ -12841,7 +12847,7 @@
       <c r="K399" t="s">
         <v>224</v>
       </c>
-      <c r="M399" s="16"/>
+      <c r="M399" s="15"/>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="1" t="s">
@@ -12868,7 +12874,7 @@
       <c r="J400" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M400" s="16"/>
+      <c r="M400" s="15"/>
     </row>
     <row r="401" spans="1:14">
       <c r="A401" s="1" t="s">
@@ -12895,7 +12901,7 @@
       <c r="J401" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M401" s="16"/>
+      <c r="M401" s="15"/>
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="1" t="s">
@@ -12922,7 +12928,7 @@
       <c r="J402" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M402" s="16"/>
+      <c r="M402" s="15"/>
     </row>
     <row r="403" spans="1:14">
       <c r="A403" s="1" t="s">
@@ -12949,7 +12955,7 @@
       <c r="J403" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M403" s="16"/>
+      <c r="M403" s="15"/>
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="1" t="s">
@@ -12979,7 +12985,7 @@
       <c r="K404" t="s">
         <v>224</v>
       </c>
-      <c r="M404" s="16"/>
+      <c r="M404" s="15"/>
     </row>
     <row r="405" spans="1:14">
       <c r="A405" s="1" t="s">
@@ -13006,7 +13012,7 @@
       <c r="J405" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M405" s="16"/>
+      <c r="M405" s="15"/>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="1" t="s">
@@ -13033,7 +13039,7 @@
       <c r="J406" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M406" s="16"/>
+      <c r="M406" s="15"/>
     </row>
     <row r="407" spans="1:14">
       <c r="A407" s="1" t="s">
@@ -13060,7 +13066,7 @@
       <c r="J407" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M407" s="16"/>
+      <c r="M407" s="15"/>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="1" t="s">
@@ -13089,7 +13095,7 @@
       <c r="J408" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M408" s="16"/>
+      <c r="M408" s="15"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="1" t="s">
@@ -13116,7 +13122,7 @@
       <c r="J409" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M409" s="16"/>
+      <c r="M409" s="15"/>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="1" t="s">
@@ -13145,7 +13151,7 @@
       <c r="J410" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M410" s="16"/>
+      <c r="M410" s="15"/>
     </row>
     <row r="411" spans="1:14">
       <c r="A411" s="1" t="s">
@@ -13172,7 +13178,7 @@
       <c r="J411" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M411" s="16"/>
+      <c r="M411" s="15"/>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="1" t="s">
@@ -13199,7 +13205,7 @@
       <c r="J412" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M412" s="16"/>
+      <c r="M412" s="15"/>
     </row>
     <row r="413" spans="1:14">
       <c r="A413" s="1" t="s">
@@ -13226,7 +13232,7 @@
       <c r="J413" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M413" s="16"/>
+      <c r="M413" s="15"/>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="1" t="s">
@@ -13253,7 +13259,7 @@
       <c r="J414" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M414" s="16"/>
+      <c r="M414" s="15"/>
       <c r="N414">
         <v>1</v>
       </c>
@@ -13283,7 +13289,7 @@
       <c r="J415" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M415" s="16">
+      <c r="M415" s="15">
         <v>0.5</v>
       </c>
     </row>
@@ -13315,7 +13321,7 @@
       <c r="K416" t="s">
         <v>227</v>
       </c>
-      <c r="M416" s="16"/>
+      <c r="M416" s="15"/>
     </row>
     <row r="417" spans="1:14">
       <c r="A417" s="1" t="s">
@@ -13347,7 +13353,7 @@
       <c r="K417" t="s">
         <v>227</v>
       </c>
-      <c r="M417" s="16"/>
+      <c r="M417" s="15"/>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="1" t="s">
@@ -13379,7 +13385,7 @@
       <c r="K418" t="s">
         <v>227</v>
       </c>
-      <c r="M418" s="16"/>
+      <c r="M418" s="15"/>
     </row>
     <row r="419" spans="1:14">
       <c r="A419" s="1" t="s">
@@ -13408,7 +13414,7 @@
       <c r="J419" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M419" s="16"/>
+      <c r="M419" s="15"/>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="1" t="s">
@@ -13437,7 +13443,7 @@
       <c r="J420" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M420" s="16"/>
+      <c r="M420" s="15"/>
       <c r="N420">
         <v>0.5</v>
       </c>
@@ -13467,7 +13473,7 @@
       <c r="J421" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M421" s="16">
+      <c r="M421" s="15">
         <v>1</v>
       </c>
     </row>
@@ -13496,7 +13502,7 @@
       <c r="J422" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M422" s="16"/>
+      <c r="M422" s="15"/>
     </row>
     <row r="423" spans="1:14">
       <c r="A423" s="1" t="s">
@@ -13523,7 +13529,7 @@
       <c r="J423" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M423" s="16"/>
+      <c r="M423" s="15"/>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="1" t="s">
@@ -13553,7 +13559,7 @@
       <c r="K424" t="s">
         <v>224</v>
       </c>
-      <c r="M424" s="16"/>
+      <c r="M424" s="15"/>
     </row>
     <row r="425" spans="1:14">
       <c r="A425" s="1" t="s">
@@ -13580,7 +13586,7 @@
       <c r="J425" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M425" s="16"/>
+      <c r="M425" s="15"/>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="1" t="s">
@@ -13607,7 +13613,7 @@
       <c r="J426" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M426" s="16"/>
+      <c r="M426" s="15"/>
     </row>
     <row r="427" spans="1:14">
       <c r="A427" s="1" t="s">
@@ -13634,7 +13640,7 @@
       <c r="J427" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M427" s="16"/>
+      <c r="M427" s="15"/>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="1" t="s">
@@ -13661,7 +13667,7 @@
       <c r="J428" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M428" s="16"/>
+      <c r="M428" s="15"/>
     </row>
     <row r="429" spans="1:14">
       <c r="A429" s="1" t="s">
@@ -13691,7 +13697,7 @@
       <c r="K429" t="s">
         <v>224</v>
       </c>
-      <c r="M429" s="16"/>
+      <c r="M429" s="15"/>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="1" t="s">
@@ -13718,7 +13724,7 @@
       <c r="J430" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M430" s="16"/>
+      <c r="M430" s="15"/>
     </row>
     <row r="431" spans="1:14">
       <c r="A431" s="1" t="s">
@@ -13745,7 +13751,7 @@
       <c r="J431" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M431" s="16"/>
+      <c r="M431" s="15"/>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="1" t="s">
@@ -13772,7 +13778,7 @@
       <c r="J432" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M432" s="16"/>
+      <c r="M432" s="15"/>
     </row>
     <row r="433" spans="1:14">
       <c r="A433" s="1" t="s">
@@ -13801,7 +13807,7 @@
       <c r="J433" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M433" s="16"/>
+      <c r="M433" s="15"/>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="1" t="s">
@@ -13828,7 +13834,7 @@
       <c r="J434" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M434" s="16"/>
+      <c r="M434" s="15"/>
     </row>
     <row r="435" spans="1:14">
       <c r="A435" s="1" t="s">
@@ -13857,7 +13863,7 @@
       <c r="J435" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M435" s="16"/>
+      <c r="M435" s="15"/>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="1" t="s">
@@ -13884,7 +13890,7 @@
       <c r="J436" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M436" s="16"/>
+      <c r="M436" s="15"/>
     </row>
     <row r="437" spans="1:14">
       <c r="A437" s="1" t="s">
@@ -13911,7 +13917,7 @@
       <c r="J437" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M437" s="16"/>
+      <c r="M437" s="15"/>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="1" t="s">
@@ -13938,7 +13944,7 @@
       <c r="J438" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M438" s="16"/>
+      <c r="M438" s="15"/>
     </row>
     <row r="439" spans="1:14">
       <c r="A439" s="1" t="s">
@@ -13965,7 +13971,7 @@
       <c r="J439" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M439" s="16"/>
+      <c r="M439" s="15"/>
       <c r="N439">
         <v>1</v>
       </c>
@@ -13999,7 +14005,7 @@
       <c r="J440" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M440" s="16">
+      <c r="M440" s="15">
         <v>1</v>
       </c>
     </row>
@@ -14032,7 +14038,7 @@
       <c r="J441" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M441" s="16"/>
+      <c r="M441" s="15"/>
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="1" t="s">
@@ -14063,7 +14069,7 @@
       <c r="J442" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M442" s="16"/>
+      <c r="M442" s="15"/>
     </row>
     <row r="443" spans="1:14">
       <c r="A443" s="1" t="s">
@@ -14094,7 +14100,7 @@
       <c r="J443" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M443" s="16"/>
+      <c r="M443" s="15"/>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="1" t="s">
@@ -14125,7 +14131,7 @@
       <c r="J444" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M444" s="16"/>
+      <c r="M444" s="15"/>
     </row>
     <row r="445" spans="1:14">
       <c r="A445" s="1" t="s">
@@ -14156,7 +14162,7 @@
       <c r="J445" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M445" s="16"/>
+      <c r="M445" s="15"/>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="1" t="s">
@@ -14187,7 +14193,7 @@
       <c r="J446" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M446" s="16"/>
+      <c r="M446" s="15"/>
     </row>
     <row r="447" spans="1:14">
       <c r="A447" s="1" t="s">
@@ -14218,7 +14224,7 @@
       <c r="J447" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M447" s="16"/>
+      <c r="M447" s="15"/>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="1" t="s">
@@ -14249,7 +14255,7 @@
       <c r="J448" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M448" s="16"/>
+      <c r="M448" s="15"/>
     </row>
     <row r="449" spans="1:14">
       <c r="A449" s="1" t="s">
@@ -14280,7 +14286,7 @@
       <c r="J449" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M449" s="16"/>
+      <c r="M449" s="15"/>
     </row>
     <row r="450" spans="1:14">
       <c r="A450" s="1" t="s">
@@ -14309,7 +14315,7 @@
       <c r="J450" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M450" s="16"/>
+      <c r="M450" s="15"/>
     </row>
     <row r="451" spans="1:14">
       <c r="A451" s="1" t="s">
@@ -14338,7 +14344,7 @@
       <c r="J451" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M451" s="16"/>
+      <c r="M451" s="15"/>
     </row>
     <row r="452" spans="1:14">
       <c r="A452" s="1" t="s">
@@ -14367,7 +14373,7 @@
       <c r="J452" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M452" s="16"/>
+      <c r="M452" s="15"/>
     </row>
     <row r="453" spans="1:14">
       <c r="A453" s="1" t="s">
@@ -14396,7 +14402,7 @@
       <c r="J453" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M453" s="16"/>
+      <c r="M453" s="15"/>
     </row>
     <row r="454" spans="1:14">
       <c r="A454" s="1" t="s">
@@ -14425,7 +14431,7 @@
       <c r="J454" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M454" s="16"/>
+      <c r="M454" s="15"/>
     </row>
     <row r="455" spans="1:14">
       <c r="A455" s="1" t="s">
@@ -14452,7 +14458,7 @@
       <c r="J455" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M455" s="16"/>
+      <c r="M455" s="15"/>
     </row>
     <row r="456" spans="1:14">
       <c r="A456" s="1" t="s">
@@ -14479,7 +14485,7 @@
       <c r="J456" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M456" s="16"/>
+      <c r="M456" s="15"/>
     </row>
     <row r="457" spans="1:14">
       <c r="A457" s="1" t="s">
@@ -14509,7 +14515,7 @@
       <c r="K457" t="s">
         <v>227</v>
       </c>
-      <c r="M457" s="16"/>
+      <c r="M457" s="15"/>
     </row>
     <row r="458" spans="1:14">
       <c r="A458" s="1" t="s">
@@ -14541,7 +14547,7 @@
       <c r="K458" t="s">
         <v>227</v>
       </c>
-      <c r="M458" s="16"/>
+      <c r="M458" s="15"/>
     </row>
     <row r="459" spans="1:14">
       <c r="A459" s="1" t="s">
@@ -14573,7 +14579,7 @@
       <c r="K459" t="s">
         <v>227</v>
       </c>
-      <c r="M459" s="16"/>
+      <c r="M459" s="15"/>
     </row>
     <row r="460" spans="1:14">
       <c r="A460" s="1" t="s">
@@ -14602,7 +14608,7 @@
       <c r="J460" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M460" s="16"/>
+      <c r="M460" s="15"/>
     </row>
     <row r="461" spans="1:14">
       <c r="A461" s="1" t="s">
@@ -14631,7 +14637,7 @@
       <c r="J461" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M461" s="16"/>
+      <c r="M461" s="15"/>
       <c r="N461">
         <v>1</v>
       </c>
@@ -14965,7 +14971,7 @@
       <c r="J474" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M474" s="17">
+      <c r="M474" s="14">
         <v>1</v>
       </c>
     </row>
@@ -14994,7 +15000,7 @@
       <c r="J475" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M475" s="17"/>
+      <c r="M475" s="14"/>
     </row>
     <row r="476" spans="1:13">
       <c r="A476" s="1" t="s">
@@ -15021,7 +15027,7 @@
       <c r="J476" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M476" s="17"/>
+      <c r="M476" s="14"/>
     </row>
     <row r="477" spans="1:13">
       <c r="A477" s="1" t="s">
@@ -15051,7 +15057,7 @@
       <c r="K477" t="s">
         <v>224</v>
       </c>
-      <c r="M477" s="17"/>
+      <c r="M477" s="14"/>
     </row>
     <row r="478" spans="1:13">
       <c r="A478" s="1" t="s">
@@ -15078,7 +15084,7 @@
       <c r="J478" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M478" s="17"/>
+      <c r="M478" s="14"/>
     </row>
     <row r="479" spans="1:13">
       <c r="A479" s="1" t="s">
@@ -15105,7 +15111,7 @@
       <c r="J479" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M479" s="17"/>
+      <c r="M479" s="14"/>
     </row>
     <row r="480" spans="1:13">
       <c r="A480" s="1" t="s">
@@ -15132,7 +15138,7 @@
       <c r="J480" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M480" s="17"/>
+      <c r="M480" s="14"/>
     </row>
     <row r="481" spans="1:13">
       <c r="A481" s="1" t="s">
@@ -15159,7 +15165,7 @@
       <c r="J481" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M481" s="17"/>
+      <c r="M481" s="14"/>
     </row>
     <row r="482" spans="1:13">
       <c r="A482" s="1" t="s">
@@ -15189,7 +15195,7 @@
       <c r="K482" t="s">
         <v>224</v>
       </c>
-      <c r="M482" s="17"/>
+      <c r="M482" s="14"/>
     </row>
     <row r="483" spans="1:13">
       <c r="A483" s="1" t="s">
@@ -15216,7 +15222,7 @@
       <c r="J483" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M483" s="17"/>
+      <c r="M483" s="14"/>
     </row>
     <row r="484" spans="1:13">
       <c r="A484" s="1" t="s">
@@ -15379,7 +15385,7 @@
       <c r="J489" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M489" s="17">
+      <c r="M489" s="14">
         <v>2</v>
       </c>
     </row>
@@ -15406,7 +15412,7 @@
       <c r="J490" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M490" s="17"/>
+      <c r="M490" s="14"/>
     </row>
     <row r="491" spans="1:13">
       <c r="A491" s="1" t="s">
@@ -15431,7 +15437,7 @@
       <c r="J491" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M491" s="17"/>
+      <c r="M491" s="14"/>
     </row>
     <row r="492" spans="1:13">
       <c r="A492" s="1" t="s">
@@ -15459,7 +15465,7 @@
       <c r="K492" t="s">
         <v>224</v>
       </c>
-      <c r="M492" s="17"/>
+      <c r="M492" s="14"/>
     </row>
     <row r="493" spans="1:13">
       <c r="A493" s="1" t="s">
@@ -15484,7 +15490,7 @@
       <c r="J493" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M493" s="17"/>
+      <c r="M493" s="14"/>
     </row>
     <row r="494" spans="1:13">
       <c r="A494" s="1" t="s">
@@ -15514,7 +15520,7 @@
       <c r="K494" t="s">
         <v>229</v>
       </c>
-      <c r="M494" s="17"/>
+      <c r="M494" s="14"/>
     </row>
     <row r="495" spans="1:13">
       <c r="A495" s="1" t="s">
@@ -15544,7 +15550,7 @@
       <c r="K495" t="s">
         <v>228</v>
       </c>
-      <c r="M495" s="17"/>
+      <c r="M495" s="14"/>
     </row>
     <row r="496" spans="1:13">
       <c r="A496" s="1" t="s">
@@ -15574,7 +15580,7 @@
       <c r="K496" t="s">
         <v>228</v>
       </c>
-      <c r="M496" s="17"/>
+      <c r="M496" s="14"/>
     </row>
     <row r="497" spans="1:14">
       <c r="A497" s="1" t="s">
@@ -15604,7 +15610,7 @@
       <c r="K497" t="s">
         <v>228</v>
       </c>
-      <c r="M497" s="17"/>
+      <c r="M497" s="14"/>
       <c r="N497">
         <v>2</v>
       </c>
@@ -15684,7 +15690,7 @@
       <c r="J500" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M500" s="17">
+      <c r="M500" s="14">
         <v>1</v>
       </c>
     </row>
@@ -15715,7 +15721,7 @@
       <c r="J501" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M501" s="17"/>
+      <c r="M501" s="14"/>
     </row>
     <row r="502" spans="1:14">
       <c r="A502" s="1" t="s">
@@ -15744,7 +15750,7 @@
       <c r="J502" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M502" s="17"/>
+      <c r="M502" s="14"/>
     </row>
     <row r="503" spans="1:14">
       <c r="A503" s="1" t="s">
@@ -15778,7 +15784,7 @@
       <c r="K503" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M503" s="17"/>
+      <c r="M503" s="14"/>
     </row>
     <row r="504" spans="1:14" ht="15" customHeight="1">
       <c r="A504" s="1" t="s">
@@ -15812,7 +15818,7 @@
       <c r="K504" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M504" s="17"/>
+      <c r="M504" s="14"/>
     </row>
     <row r="505" spans="1:14" ht="15" customHeight="1">
       <c r="A505" s="1" t="s">
@@ -15846,7 +15852,7 @@
       <c r="K505" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M505" s="17"/>
+      <c r="M505" s="14"/>
     </row>
     <row r="506" spans="1:14" ht="15" customHeight="1">
       <c r="A506" s="1" t="s">
@@ -15880,7 +15886,7 @@
       <c r="K506" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M506" s="17"/>
+      <c r="M506" s="14"/>
     </row>
     <row r="507" spans="1:14" ht="15" customHeight="1">
       <c r="A507" s="1" t="s">
@@ -15909,7 +15915,7 @@
       <c r="J507" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M507" s="17"/>
+      <c r="M507" s="14"/>
     </row>
     <row r="508" spans="1:14" ht="15" customHeight="1">
       <c r="A508" s="1" t="s">
@@ -15943,7 +15949,7 @@
       <c r="K508" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M508" s="17"/>
+      <c r="M508" s="14"/>
     </row>
     <row r="509" spans="1:14" ht="15" customHeight="1">
       <c r="A509" s="1" t="s">
@@ -15977,7 +15983,7 @@
       <c r="K509" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M509" s="17"/>
+      <c r="M509" s="14"/>
     </row>
     <row r="510" spans="1:14" ht="15" customHeight="1">
       <c r="A510" s="1" t="s">
@@ -16011,7 +16017,7 @@
       <c r="K510" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M510" s="17"/>
+      <c r="M510" s="14"/>
     </row>
     <row r="511" spans="1:14" ht="15" customHeight="1">
       <c r="A511" s="1" t="s">
@@ -16042,7 +16048,7 @@
       <c r="J511" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M511" s="17"/>
+      <c r="M511" s="14"/>
     </row>
     <row r="512" spans="1:14">
       <c r="A512" s="1" t="s">
@@ -16073,7 +16079,7 @@
       <c r="J512" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M512" s="17"/>
+      <c r="M512" s="14"/>
     </row>
     <row r="513" spans="1:14">
       <c r="A513" s="1" t="s">
@@ -16104,7 +16110,7 @@
       <c r="J513" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M513" s="17"/>
+      <c r="M513" s="14"/>
     </row>
     <row r="514" spans="1:14">
       <c r="A514" s="1" t="s">
@@ -16129,7 +16135,7 @@
       <c r="J514" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M514" s="17"/>
+      <c r="M514" s="14"/>
     </row>
     <row r="515" spans="1:14">
       <c r="A515" s="1" t="s">
@@ -16154,7 +16160,7 @@
       <c r="J515" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M515" s="17"/>
+      <c r="M515" s="14"/>
     </row>
     <row r="516" spans="1:14">
       <c r="A516" s="1" t="s">
@@ -16181,7 +16187,7 @@
       <c r="J516" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M516" s="17"/>
+      <c r="M516" s="14"/>
       <c r="N516">
         <v>1</v>
       </c>
@@ -16211,7 +16217,7 @@
       <c r="J517" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M517" s="17">
+      <c r="M517" s="14">
         <v>2</v>
       </c>
     </row>
@@ -16240,7 +16246,7 @@
       <c r="J518" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M518" s="17"/>
+      <c r="M518" s="14"/>
     </row>
     <row r="519" spans="1:14">
       <c r="A519" s="1" t="s">
@@ -16267,7 +16273,7 @@
       <c r="J519" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M519" s="17"/>
+      <c r="M519" s="14"/>
     </row>
     <row r="520" spans="1:14">
       <c r="A520" s="1" t="s">
@@ -16294,7 +16300,7 @@
       <c r="J520" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M520" s="17"/>
+      <c r="M520" s="14"/>
     </row>
     <row r="521" spans="1:14">
       <c r="A521" s="1" t="s">
@@ -16321,7 +16327,7 @@
       <c r="J521" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M521" s="17"/>
+      <c r="M521" s="14"/>
     </row>
     <row r="522" spans="1:14">
       <c r="A522" s="1" t="s">
@@ -16348,7 +16354,7 @@
       <c r="J522" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M522" s="17"/>
+      <c r="M522" s="14"/>
     </row>
     <row r="523" spans="1:14">
       <c r="A523" s="1" t="s">
@@ -16375,7 +16381,7 @@
       <c r="J523" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M523" s="17"/>
+      <c r="M523" s="14"/>
     </row>
     <row r="524" spans="1:14">
       <c r="A524" s="1" t="s">
@@ -16400,7 +16406,7 @@
       <c r="J524" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M524" s="17"/>
+      <c r="M524" s="14"/>
     </row>
     <row r="525" spans="1:14">
       <c r="A525" s="1" t="s">
@@ -16425,7 +16431,7 @@
       <c r="J525" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M525" s="17"/>
+      <c r="M525" s="14"/>
     </row>
     <row r="526" spans="1:14">
       <c r="A526" s="1" t="s">
@@ -16450,7 +16456,7 @@
       <c r="J526" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M526" s="17"/>
+      <c r="M526" s="14"/>
     </row>
     <row r="527" spans="1:14">
       <c r="A527" s="1" t="s">
@@ -16478,7 +16484,7 @@
       <c r="K527" t="s">
         <v>224</v>
       </c>
-      <c r="M527" s="17"/>
+      <c r="M527" s="14"/>
     </row>
     <row r="528" spans="1:14">
       <c r="A528" s="1" t="s">
@@ -17095,20 +17101,20 @@
       </c>
     </row>
     <row r="552" spans="1:14">
-      <c r="A552" s="1" t="s">
+      <c r="A552" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B552" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D552" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E552" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
+      </c>
+      <c r="E552" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="F552" s="1"/>
       <c r="G552" s="1"/>
@@ -17117,56 +17123,90 @@
         <v>210</v>
       </c>
       <c r="J552" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K552" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="553" spans="1:14">
+      <c r="A553" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D553" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E553" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F553" s="1"/>
+      <c r="G553" s="1"/>
+      <c r="H553" s="1"/>
+      <c r="I553" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J553" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="553" spans="1:14">
-      <c r="A553" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B553" s="2" t="s">
+    <row r="554" spans="1:14">
+      <c r="A554" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B554" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C553" s="2" t="s">
+      <c r="C554" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D553" s="2" t="s">
+      <c r="D554" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E553" s="2" t="s">
+      <c r="E554" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F553" s="2"/>
-      <c r="G553" s="2"/>
-      <c r="H553" s="2"/>
-      <c r="I553" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="J553" s="5" t="s">
+      <c r="F554" s="2"/>
+      <c r="G554" s="2"/>
+      <c r="H554" s="2"/>
+      <c r="I554" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="J554" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M553">
+      <c r="M554">
         <f>SUM(M2:M527)</f>
         <v>25.5</v>
       </c>
-      <c r="N553">
+      <c r="N554">
         <f>SUM(N1:N527)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="554" spans="1:14">
-      <c r="N554">
+    <row r="555" spans="1:14">
+      <c r="N555">
         <v>3</v>
       </c>
     </row>
-    <row r="555" spans="1:14">
-      <c r="N555" s="8">
+    <row r="556" spans="1:14">
+      <c r="N556" s="8">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:J553"/>
+  <autoFilter ref="I1:J554"/>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M2:M10"/>
+    <mergeCell ref="M43:M50"/>
+    <mergeCell ref="M57:M60"/>
     <mergeCell ref="M517:M527"/>
     <mergeCell ref="M98:M118"/>
     <mergeCell ref="M127:M164"/>
@@ -17183,11 +17223,6 @@
     <mergeCell ref="M389:M395"/>
     <mergeCell ref="M196:M209"/>
     <mergeCell ref="M210:M219"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M43:M50"/>
-    <mergeCell ref="M57:M60"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:M1">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>